<commit_message>
special dragon content test
Former-commit-id: c526e542a235af45b3ec0db3305174d3255cce89
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malinares/Projects/Dragon_Android/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="132">
   <si>
     <t>[sku]</t>
   </si>
@@ -396,6 +396,30 @@
   </si>
   <si>
     <t>10;10</t>
+  </si>
+  <si>
+    <t>SEPECIAL DRAGONS</t>
+  </si>
+  <si>
+    <t>{specialDragonTierDefinitions}</t>
+  </si>
+  <si>
+    <t>dragon_robot</t>
+  </si>
+  <si>
+    <t>dragon_electric</t>
+  </si>
+  <si>
+    <t>PF_DragonElectric</t>
+  </si>
+  <si>
+    <t>PF_DragonSonic</t>
+  </si>
+  <si>
+    <t>dragon_sonic</t>
+  </si>
+  <si>
+    <t>PF_DragonHelicopter</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1433,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="105">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1470,7 +1534,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1478,14 +1542,12 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1510,7 +1572,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1525,7 +1587,7 @@
           <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1550,25 +1612,23 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1590,25 +1650,23 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1630,14 +1688,109 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1649,6 +1802,58 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1667,6 +1872,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1685,7 +1891,7 @@
           <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1755,7 +1961,7 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -1790,7 +1996,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1798,7 +2004,9 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -1828,12 +2036,12 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -1868,7 +2076,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1876,12 +2084,14 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1906,7 +2116,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1921,7 +2131,7 @@
           <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1946,7 +2156,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1954,7 +2164,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color auto="1"/>
         </right>
         <top style="thin">
@@ -1964,9 +2174,7 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1988,23 +2196,25 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2026,12 +2236,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -2040,9 +2252,7 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2064,23 +2274,25 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2102,23 +2314,23 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2140,23 +2352,25 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2183,8 +2397,12 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2411,9 +2629,7 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -2446,15 +2662,13 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -2486,98 +2700,23 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2599,14 +2738,12 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -2615,30 +2752,9 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2660,7 +2776,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2674,122 +2790,9 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2811,14 +2814,12 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -2827,7 +2828,9 @@
           <color auto="1"/>
         </bottom>
         <vertical/>
-        <horizontal/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2849,6 +2852,449 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -3700,6 +4146,26 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3845,92 +4311,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table6" displayName="Table6" ref="B19:G25" totalsRowShown="0" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
-  <autoFilter ref="B19:G25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table6" displayName="Table6" ref="B25:G31" totalsRowShown="0" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+  <autoFilter ref="B25:G31"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="{specialDragonStatsUpgradeDefinitions}" dataDxfId="69"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="68"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="67"/>
-    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="66"/>
-    <tableColumn id="4" name="[stat]" dataDxfId="65"/>
-    <tableColumn id="5" name="[percentage]" dataDxfId="64"/>
+    <tableColumn id="1" name="{specialDragonStatsUpgradeDefinitions}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="84"/>
+    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="83"/>
+    <tableColumn id="4" name="[stat]" dataDxfId="82"/>
+    <tableColumn id="5" name="[percentage]" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table63" displayName="Table63" ref="B36:F42" totalsRowShown="0" headerRowBorderDxfId="63" tableBorderDxfId="62" totalsRowBorderDxfId="61">
-  <autoFilter ref="B36:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table63" displayName="Table63" ref="B42:F48" totalsRowShown="0" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+  <autoFilter ref="B42:F48"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPetsUpgradeDefinitions}" dataDxfId="60"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="59"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="58"/>
-    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="57"/>
-    <tableColumn id="4" name="[maxPets]" dataDxfId="56"/>
+    <tableColumn id="1" name="{specialDragonPetsUpgradeDefinitions}" dataDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="75"/>
+    <tableColumn id="3" name="[unlockPricePC]" dataDxfId="74"/>
+    <tableColumn id="4" name="[maxPets]" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B6:BC12" totalsRowShown="0" headerRowBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="B6:BC12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BC18" totalsRowShown="0" headerRowBorderDxfId="72" totalsRowBorderDxfId="71">
+  <autoFilter ref="B12:BC18"/>
   <tableColumns count="54">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="53"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="51"/>
-    <tableColumn id="4" name="[order]" dataDxfId="50"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="49"/>
-    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="48"/>
-    <tableColumn id="7" name="[unlockPricePC]" dataDxfId="47"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="46"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="45"/>
-    <tableColumn id="10" name="[health]" dataDxfId="44"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="43"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="42"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="41"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="40"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="39"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="38"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="37"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="36"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="35"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="34"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="33"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="32"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="31"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="30"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="29"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="28"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="27"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="26"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="25"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="24"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="23"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="22"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="21"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="20"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="19"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="18"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="17"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="16"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="15"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="14"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="13"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="12"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="11"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="10"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="9"/>
-    <tableColumn id="46" name="[force]" dataDxfId="8"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="7"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="6"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="5"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="4"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="3"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="2"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="1"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="70"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="69"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="68"/>
+    <tableColumn id="4" name="[order]" dataDxfId="67"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="66"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="65"/>
+    <tableColumn id="7" name="[unlockPricePC]" dataDxfId="64"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="63"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="62"/>
+    <tableColumn id="10" name="[health]" dataDxfId="61"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="60"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="59"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="58"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="57"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="56"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="55"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="54"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="53"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="52"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="51"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="50"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="49"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="48"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="47"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="46"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="45"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="44"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="43"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="42"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="41"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="40"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="39"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="38"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="37"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="36"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="35"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="34"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="33"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="32"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="31"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="30"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="29"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="28"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="27"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="26"/>
+    <tableColumn id="46" name="[force]" dataDxfId="25"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="24"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="23"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="22"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="21"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="20"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="19"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="18"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B3:L6" totalsRowShown="0" headerRowBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="B3:L6"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="14"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="4" name="[order]" dataDxfId="12"/>
+    <tableColumn id="6" name="[unlockPriceCoins]" dataDxfId="11"/>
+    <tableColumn id="7" name="[unlockPricePC]" dataDxfId="10"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="9"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="8"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="7"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="6"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="5"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4199,1699 +4685,1914 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BC42"/>
+  <dimension ref="A1:BC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" customWidth="1"/>
-    <col min="19" max="20" width="12.85546875" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.5" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="20" width="12.83203125" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.5" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="19.5" customWidth="1"/>
     <col min="31" max="31" width="30" customWidth="1"/>
-    <col min="32" max="32" width="26.7109375" customWidth="1"/>
-    <col min="43" max="43" width="33.140625" customWidth="1"/>
-    <col min="44" max="44" width="29.28515625" customWidth="1"/>
-    <col min="55" max="55" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="26.6640625" customWidth="1"/>
+    <col min="43" max="43" width="33.1640625" customWidth="1"/>
+    <col min="44" max="44" width="29.33203125" customWidth="1"/>
+    <col min="55" max="55" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="F2" s="47" t="s">
+    <row r="1" spans="1:55" ht="24" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:55" ht="128" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B4" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="52">
+        <v>0</v>
+      </c>
+      <c r="E4" s="54">
+        <v>0</v>
+      </c>
+      <c r="F4" s="55">
+        <v>0</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B5" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="82" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="84">
+        <v>1</v>
+      </c>
+      <c r="E5" s="86">
+        <v>2000</v>
+      </c>
+      <c r="F5" s="87">
+        <v>60</v>
+      </c>
+      <c r="G5" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="82" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B6" s="105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="106" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="84">
+        <v>2</v>
+      </c>
+      <c r="E6" s="109">
+        <v>11000</v>
+      </c>
+      <c r="F6" s="110">
+        <v>100</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="100" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="106" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="F8" s="47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:55" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+    <row r="9" spans="1:55" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:55" ht="24" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
     </row>
-    <row r="6" spans="1:55" ht="163.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="6" t="s">
+    <row r="12" spans="1:55" ht="161" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H12" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I12" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M12" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N12" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O12" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P12" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q12" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="T12" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="U12" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="V12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="W12" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="X12" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="Y6" s="22" t="s">
+      <c r="Y12" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AA12" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AB12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="42" t="s">
+      <c r="AC12" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="38" t="s">
+      <c r="AD12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AE6" s="37" t="s">
+      <c r="AE12" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AF6" s="37" t="s">
+      <c r="AF12" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="AG6" s="37" t="s">
+      <c r="AG12" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AH6" s="37" t="s">
+      <c r="AH12" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AI6" s="37" t="s">
+      <c r="AI12" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="AJ6" s="37" t="s">
+      <c r="AJ12" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="AK6" s="37" t="s">
+      <c r="AK12" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="AL6" s="37" t="s">
+      <c r="AL12" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AM6" s="37" t="s">
+      <c r="AM12" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="AN6" s="37" t="s">
+      <c r="AN12" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="AO6" s="37" t="s">
+      <c r="AO12" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="AP6" s="41" t="s">
+      <c r="AP12" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="AQ6" s="43" t="s">
+      <c r="AQ12" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AR6" s="45" t="s">
+      <c r="AR12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AS6" s="44" t="s">
+      <c r="AS12" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="AT6" s="46" t="s">
+      <c r="AT12" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="AU6" s="40" t="s">
+      <c r="AU12" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="AV6" s="39" t="s">
+      <c r="AV12" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="AW6" s="39" t="s">
+      <c r="AW12" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AX6" s="39" t="s">
+      <c r="AX12" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="AY6" s="39" t="s">
+      <c r="AY12" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="39" t="s">
+      <c r="AZ12" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="BA6" s="32" t="s">
+      <c r="BA12" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="BB6" s="32" t="s">
+      <c r="BB12" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="BC6" s="39" t="s">
+      <c r="BC12" s="39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B13" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C13" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D13" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F13" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G13" s="54">
         <v>0</v>
       </c>
-      <c r="H7" s="55">
+      <c r="H13" s="55">
         <v>0</v>
       </c>
-      <c r="I7" s="56">
+      <c r="I13" s="56">
         <v>5</v>
       </c>
-      <c r="J7" s="57">
+      <c r="J13" s="57">
         <v>-2</v>
       </c>
-      <c r="K7" s="58">
+      <c r="K13" s="58">
         <v>170</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L13" s="59">
         <v>1.5</v>
       </c>
-      <c r="M7" s="59">
+      <c r="M13" s="59">
         <v>0</v>
       </c>
-      <c r="N7" s="59">
+      <c r="N13" s="59">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O7" s="60">
+      <c r="O13" s="60">
         <v>30</v>
       </c>
-      <c r="P7" s="60">
+      <c r="P13" s="60">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="61">
+      <c r="Q13" s="61">
         <v>1</v>
       </c>
-      <c r="R7" s="57">
+      <c r="R13" s="57">
         <v>1</v>
       </c>
-      <c r="S7" s="59">
+      <c r="S13" s="59">
         <v>100</v>
       </c>
-      <c r="T7" s="59">
+      <c r="T13" s="59">
         <v>40</v>
       </c>
-      <c r="U7" s="62">
+      <c r="U13" s="62">
         <v>28</v>
       </c>
-      <c r="V7" s="63">
+      <c r="V13" s="63">
         <v>9</v>
       </c>
-      <c r="W7" s="59">
+      <c r="W13" s="59">
         <v>3</v>
       </c>
-      <c r="X7" s="60">
+      <c r="X13" s="60">
         <v>9</v>
       </c>
-      <c r="Y7" s="62">
+      <c r="Y13" s="62">
         <v>8000</v>
       </c>
-      <c r="Z7" s="64">
+      <c r="Z13" s="64">
         <v>2</v>
       </c>
-      <c r="AA7" s="61">
+      <c r="AA13" s="61">
         <v>0.13</v>
       </c>
-      <c r="AB7" s="65">
+      <c r="AB13" s="65">
         <v>0</v>
       </c>
-      <c r="AC7" s="66">
+      <c r="AC13" s="66">
         <v>6</v>
       </c>
-      <c r="AD7" s="68" t="s">
+      <c r="AD13" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AE7" s="69" t="s">
+      <c r="AE13" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="AF7" s="69" t="s">
+      <c r="AF13" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="AG7" s="69"/>
-      <c r="AH7" s="69"/>
-      <c r="AI7" s="69">
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="69"/>
+      <c r="AI13" s="69">
         <v>4.0999999999999996</v>
       </c>
-      <c r="AJ7" s="69">
+      <c r="AJ13" s="69">
         <v>2</v>
       </c>
-      <c r="AK7" s="69">
+      <c r="AK13" s="69">
         <v>2</v>
       </c>
-      <c r="AL7" s="69" t="b">
+      <c r="AL13" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AM7" s="69" t="b">
+      <c r="AM13" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AN7" s="69" t="b">
+      <c r="AN13" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AO7" s="69">
+      <c r="AO13" s="69">
         <v>10</v>
       </c>
-      <c r="AP7" s="70">
+      <c r="AP13" s="70">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AQ7" s="71" t="s">
+      <c r="AQ13" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="AR7" s="72" t="s">
+      <c r="AR13" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="AS7" s="75">
+      <c r="AS13" s="75">
         <v>2E-3</v>
       </c>
-      <c r="AT7" s="76">
+      <c r="AT13" s="76">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU7" s="77">
+      <c r="AU13" s="77">
         <v>260</v>
       </c>
-      <c r="AV7" s="48">
+      <c r="AV13" s="48">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AW7" s="48">
+      <c r="AW13" s="48">
         <v>5</v>
       </c>
-      <c r="AX7" s="48">
+      <c r="AX13" s="48">
         <v>1.7</v>
       </c>
-      <c r="AY7" s="78">
+      <c r="AY13" s="78">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ7" s="78">
+      <c r="AZ13" s="78">
         <v>2.25</v>
       </c>
-      <c r="BA7" s="78">
+      <c r="BA13" s="78">
         <v>0</v>
       </c>
-      <c r="BB7" s="78">
+      <c r="BB13" s="78">
         <v>8</v>
       </c>
-      <c r="BC7" s="48" t="s">
+      <c r="BC13" s="48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B8" s="49" t="s">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B14" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C14" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D14" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F14" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G14" s="54">
         <v>0</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H14" s="55">
         <v>0</v>
       </c>
-      <c r="I8" s="56">
+      <c r="I14" s="56">
         <v>10</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J14" s="57">
         <v>0</v>
       </c>
-      <c r="K8" s="58">
+      <c r="K14" s="58">
         <v>280</v>
       </c>
-      <c r="L8" s="59">
+      <c r="L14" s="59">
         <v>1.9</v>
       </c>
-      <c r="M8" s="59">
+      <c r="M14" s="59">
         <v>0</v>
       </c>
-      <c r="N8" s="59">
+      <c r="N14" s="59">
         <v>1.2E-2</v>
       </c>
-      <c r="O8" s="60">
+      <c r="O14" s="60">
         <v>30</v>
       </c>
-      <c r="P8" s="60">
+      <c r="P14" s="60">
         <v>0.6</v>
       </c>
-      <c r="Q8" s="61">
+      <c r="Q14" s="61">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R8" s="57">
+      <c r="R14" s="57">
         <v>1</v>
       </c>
-      <c r="S8" s="59">
+      <c r="S14" s="59">
         <v>100</v>
       </c>
-      <c r="T8" s="59">
+      <c r="T14" s="59">
         <v>40</v>
       </c>
-      <c r="U8" s="62">
+      <c r="U14" s="62">
         <v>28</v>
       </c>
-      <c r="V8" s="63">
+      <c r="V14" s="63">
         <v>11</v>
       </c>
-      <c r="W8" s="59">
+      <c r="W14" s="59">
         <v>4</v>
       </c>
-      <c r="X8" s="60">
+      <c r="X14" s="60">
         <v>10</v>
       </c>
-      <c r="Y8" s="62">
+      <c r="Y14" s="62">
         <v>10000</v>
       </c>
-      <c r="Z8" s="64">
+      <c r="Z14" s="64">
         <v>3</v>
       </c>
-      <c r="AA8" s="61">
+      <c r="AA14" s="61">
         <v>0.08</v>
       </c>
-      <c r="AB8" s="65">
+      <c r="AB14" s="65">
         <v>0</v>
       </c>
-      <c r="AC8" s="65">
+      <c r="AC14" s="65">
         <v>6</v>
       </c>
-      <c r="AD8" s="68" t="s">
+      <c r="AD14" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="AE8" s="69" t="s">
+      <c r="AE14" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AF8" s="69" t="s">
+      <c r="AF14" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AG8" s="69"/>
-      <c r="AH8" s="69"/>
-      <c r="AI8" s="69">
+      <c r="AG14" s="69"/>
+      <c r="AH14" s="69"/>
+      <c r="AI14" s="69">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AJ8" s="69">
+      <c r="AJ14" s="69">
         <v>2</v>
       </c>
-      <c r="AK8" s="69">
+      <c r="AK14" s="69">
         <v>2</v>
       </c>
-      <c r="AL8" s="69" t="b">
+      <c r="AL14" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AM8" s="69" t="b">
+      <c r="AM14" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AN8" s="69" t="b">
+      <c r="AN14" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AO8" s="69">
+      <c r="AO14" s="69">
         <v>10</v>
       </c>
-      <c r="AP8" s="70">
+      <c r="AP14" s="70">
         <v>0.7</v>
       </c>
-      <c r="AQ8" s="71" t="s">
+      <c r="AQ14" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="AR8" s="72" t="s">
+      <c r="AR14" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="AS8" s="75">
+      <c r="AS14" s="75">
         <v>1.8E-3</v>
       </c>
-      <c r="AT8" s="76">
+      <c r="AT14" s="76">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU8" s="77">
+      <c r="AU14" s="77">
         <v>333</v>
       </c>
-      <c r="AV8" s="48">
+      <c r="AV14" s="48">
         <v>2.5</v>
       </c>
-      <c r="AW8" s="48">
+      <c r="AW14" s="48">
         <v>5</v>
       </c>
-      <c r="AX8" s="48">
+      <c r="AX14" s="48">
         <v>1.7</v>
       </c>
-      <c r="AY8" s="48">
+      <c r="AY14" s="48">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ8" s="48">
+      <c r="AZ14" s="48">
         <v>2.25</v>
       </c>
-      <c r="BA8" s="48">
+      <c r="BA14" s="48">
         <v>9</v>
       </c>
-      <c r="BB8" s="48">
+      <c r="BB14" s="48">
         <v>8</v>
       </c>
-      <c r="BC8" s="48" t="s">
+      <c r="BC14" s="48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B15" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C15" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D15" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E15" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F15" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G15" s="54">
         <v>0</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H15" s="55">
         <v>0</v>
       </c>
-      <c r="I9" s="56">
+      <c r="I15" s="56">
         <v>15</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J15" s="57">
         <v>0</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K15" s="58">
         <v>400</v>
       </c>
-      <c r="L9" s="59">
+      <c r="L15" s="59">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M9" s="59">
+      <c r="M15" s="59">
         <v>0</v>
       </c>
-      <c r="N9" s="59">
+      <c r="N15" s="59">
         <v>1.4E-2</v>
       </c>
-      <c r="O9" s="60">
+      <c r="O15" s="60">
         <v>25</v>
       </c>
-      <c r="P9" s="60">
+      <c r="P15" s="60">
         <v>0.7</v>
       </c>
-      <c r="Q9" s="61">
+      <c r="Q15" s="61">
         <v>1.75</v>
       </c>
-      <c r="R9" s="57">
+      <c r="R15" s="57">
         <v>1</v>
       </c>
-      <c r="S9" s="59">
+      <c r="S15" s="59">
         <v>100</v>
       </c>
-      <c r="T9" s="59">
+      <c r="T15" s="59">
         <v>40</v>
       </c>
-      <c r="U9" s="62">
+      <c r="U15" s="62">
         <v>28</v>
       </c>
-      <c r="V9" s="63">
+      <c r="V15" s="63">
         <v>11.5</v>
       </c>
-      <c r="W9" s="59">
+      <c r="W15" s="59">
         <v>5</v>
       </c>
-      <c r="X9" s="60">
+      <c r="X15" s="60">
         <v>10</v>
       </c>
-      <c r="Y9" s="62">
+      <c r="Y15" s="62">
         <v>20000</v>
       </c>
-      <c r="Z9" s="64">
+      <c r="Z15" s="64">
         <v>4</v>
       </c>
-      <c r="AA9" s="61">
+      <c r="AA15" s="61">
         <v>0.05</v>
       </c>
-      <c r="AB9" s="65">
+      <c r="AB15" s="65">
         <v>0</v>
       </c>
-      <c r="AC9" s="67">
+      <c r="AC15" s="67">
         <v>6</v>
       </c>
-      <c r="AD9" s="68" t="s">
+      <c r="AD15" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="AE9" s="69" t="s">
+      <c r="AE15" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="AF9" s="69" t="s">
+      <c r="AF15" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="AG9" s="69"/>
-      <c r="AH9" s="69"/>
-      <c r="AI9" s="69">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69">
         <v>2.1</v>
       </c>
-      <c r="AJ9" s="69">
+      <c r="AJ15" s="69">
         <v>2</v>
       </c>
-      <c r="AK9" s="69">
+      <c r="AK15" s="69">
         <v>2</v>
       </c>
-      <c r="AL9" s="69" t="b">
+      <c r="AL15" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AM9" s="69" t="b">
+      <c r="AM15" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AN9" s="69" t="b">
+      <c r="AN15" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AO9" s="69">
+      <c r="AO15" s="69">
         <v>10</v>
       </c>
-      <c r="AP9" s="70">
+      <c r="AP15" s="70">
         <v>0.7</v>
       </c>
-      <c r="AQ9" s="73" t="s">
+      <c r="AQ15" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="AR9" s="74" t="s">
+      <c r="AR15" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="AS9" s="75">
+      <c r="AS15" s="75">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AT9" s="76">
+      <c r="AT15" s="76">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU9" s="77">
+      <c r="AU15" s="77">
         <v>475</v>
       </c>
-      <c r="AV9" s="48">
+      <c r="AV15" s="48">
         <v>3.4</v>
       </c>
-      <c r="AW9" s="48">
+      <c r="AW15" s="48">
         <v>5</v>
       </c>
-      <c r="AX9" s="48">
+      <c r="AX15" s="48">
         <v>1.7</v>
       </c>
-      <c r="AY9" s="48">
+      <c r="AY15" s="48">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ9" s="48">
+      <c r="AZ15" s="48">
         <v>2.25</v>
       </c>
-      <c r="BA9" s="48">
+      <c r="BA15" s="48">
         <v>45</v>
       </c>
-      <c r="BB9" s="48">
+      <c r="BB15" s="48">
         <v>15</v>
       </c>
-      <c r="BC9" s="79" t="s">
+      <c r="BC15" s="79" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="49" t="s">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C16" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E16" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F16" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G16" s="54">
         <v>0</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H16" s="55">
         <v>0</v>
       </c>
-      <c r="I10" s="56">
+      <c r="I16" s="56">
         <v>25</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J16" s="57">
         <v>0</v>
       </c>
-      <c r="K10" s="58">
+      <c r="K16" s="58">
         <v>430</v>
       </c>
-      <c r="L10" s="59">
+      <c r="L16" s="59">
         <v>2.4</v>
       </c>
-      <c r="M10" s="59">
+      <c r="M16" s="59">
         <v>0</v>
       </c>
-      <c r="N10" s="59">
+      <c r="N16" s="59">
         <v>1.6E-2</v>
       </c>
-      <c r="O10" s="60">
+      <c r="O16" s="60">
         <v>20</v>
       </c>
-      <c r="P10" s="60">
+      <c r="P16" s="60">
         <v>0.8</v>
       </c>
-      <c r="Q10" s="61">
+      <c r="Q16" s="61">
         <v>2.1</v>
       </c>
-      <c r="R10" s="57">
+      <c r="R16" s="57">
         <v>1</v>
       </c>
-      <c r="S10" s="59">
+      <c r="S16" s="59">
         <v>100</v>
       </c>
-      <c r="T10" s="59">
+      <c r="T16" s="59">
         <v>40</v>
       </c>
-      <c r="U10" s="62">
+      <c r="U16" s="62">
         <v>28</v>
       </c>
-      <c r="V10" s="63">
+      <c r="V16" s="63">
         <v>12</v>
       </c>
-      <c r="W10" s="59">
+      <c r="W16" s="59">
         <v>6</v>
       </c>
-      <c r="X10" s="60">
+      <c r="X16" s="60">
         <v>10</v>
       </c>
-      <c r="Y10" s="62">
+      <c r="Y16" s="62">
         <v>30000</v>
       </c>
-      <c r="Z10" s="64">
+      <c r="Z16" s="64">
         <v>5</v>
       </c>
-      <c r="AA10" s="61">
+      <c r="AA16" s="61">
         <v>0.04</v>
       </c>
-      <c r="AB10" s="65">
+      <c r="AB16" s="65">
         <v>0</v>
       </c>
-      <c r="AC10" s="65">
+      <c r="AC16" s="65">
         <v>6</v>
       </c>
-      <c r="AD10" s="68" t="s">
+      <c r="AD16" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AE10" s="69" t="s">
+      <c r="AE16" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="AF10" s="69" t="s">
+      <c r="AF16" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="69"/>
-      <c r="AI10" s="69">
+      <c r="AG16" s="69"/>
+      <c r="AH16" s="69"/>
+      <c r="AI16" s="69">
         <v>2.1</v>
       </c>
-      <c r="AJ10" s="69">
+      <c r="AJ16" s="69">
         <v>2</v>
       </c>
-      <c r="AK10" s="69">
+      <c r="AK16" s="69">
         <v>2</v>
       </c>
-      <c r="AL10" s="69" t="b">
+      <c r="AL16" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AM10" s="69" t="b">
+      <c r="AM16" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AN10" s="69" t="b">
+      <c r="AN16" s="69" t="b">
         <v>1</v>
       </c>
-      <c r="AO10" s="69">
+      <c r="AO16" s="69">
         <v>10</v>
       </c>
-      <c r="AP10" s="70">
+      <c r="AP16" s="70">
         <v>0.7</v>
       </c>
-      <c r="AQ10" s="73" t="s">
+      <c r="AQ16" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="AR10" s="74" t="s">
+      <c r="AR16" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="AS10" s="75">
+      <c r="AS16" s="75">
         <v>1.5E-3</v>
       </c>
-      <c r="AT10" s="76">
+      <c r="AT16" s="76">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU10" s="77">
+      <c r="AU16" s="77">
         <v>705</v>
       </c>
-      <c r="AV10" s="48">
+      <c r="AV16" s="48">
         <v>4.7</v>
       </c>
-      <c r="AW10" s="48">
+      <c r="AW16" s="48">
         <v>5</v>
       </c>
-      <c r="AX10" s="48">
+      <c r="AX16" s="48">
         <v>1.7</v>
       </c>
-      <c r="AY10" s="48">
+      <c r="AY16" s="48">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ10" s="48">
+      <c r="AZ16" s="48">
         <v>2.25</v>
       </c>
-      <c r="BA10" s="48">
+      <c r="BA16" s="48">
         <v>59</v>
       </c>
-      <c r="BB10" s="48">
+      <c r="BB16" s="48">
         <v>15</v>
       </c>
-      <c r="BC10" s="79" t="s">
+      <c r="BC16" s="79" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B11" s="81" t="s">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B17" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C17" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D17" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E17" s="84">
         <v>1</v>
       </c>
-      <c r="F11" s="85" t="s">
+      <c r="F17" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="86">
+      <c r="G17" s="86">
         <v>2000</v>
       </c>
-      <c r="H11" s="87">
+      <c r="H17" s="87">
         <v>60</v>
       </c>
-      <c r="I11" s="88">
+      <c r="I17" s="88">
         <v>3</v>
       </c>
-      <c r="J11" s="89">
+      <c r="J17" s="89">
         <v>0</v>
       </c>
-      <c r="K11" s="90">
+      <c r="K17" s="90">
         <v>95</v>
       </c>
-      <c r="L11" s="91">
+      <c r="L17" s="91">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M11" s="91">
+      <c r="M17" s="91">
         <v>1</v>
       </c>
-      <c r="N11" s="91">
+      <c r="N17" s="91">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="O11" s="91">
+      <c r="O17" s="91">
         <v>30</v>
       </c>
-      <c r="P11" s="91">
+      <c r="P17" s="91">
         <v>0.5</v>
       </c>
-      <c r="Q11" s="92">
+      <c r="Q17" s="92">
         <v>0.8</v>
       </c>
-      <c r="R11" s="89">
+      <c r="R17" s="89">
         <v>1.7</v>
       </c>
-      <c r="S11" s="91">
+      <c r="S17" s="91">
         <v>100</v>
       </c>
-      <c r="T11" s="91">
+      <c r="T17" s="91">
         <v>20</v>
       </c>
-      <c r="U11" s="93">
+      <c r="U17" s="93">
         <v>10</v>
       </c>
-      <c r="V11" s="89">
+      <c r="V17" s="89">
         <v>8</v>
       </c>
-      <c r="W11" s="91">
+      <c r="W17" s="91">
         <v>3</v>
       </c>
-      <c r="X11" s="91">
+      <c r="X17" s="91">
         <v>9</v>
       </c>
-      <c r="Y11" s="93">
+      <c r="Y17" s="93">
         <v>7000</v>
       </c>
-      <c r="Z11" s="94">
+      <c r="Z17" s="94">
         <v>2</v>
       </c>
-      <c r="AA11" s="95">
+      <c r="AA17" s="95">
         <v>0.19</v>
       </c>
-      <c r="AB11" s="95">
+      <c r="AB17" s="95">
         <v>0</v>
       </c>
-      <c r="AC11" s="95">
+      <c r="AC17" s="95">
         <v>12</v>
       </c>
-      <c r="AD11" s="96" t="s">
+      <c r="AD17" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="AE11" s="97" t="s">
+      <c r="AE17" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="AF11" s="97" t="s">
+      <c r="AF17" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="AG11" s="97"/>
-      <c r="AH11" s="97"/>
-      <c r="AI11" s="97">
+      <c r="AG17" s="97"/>
+      <c r="AH17" s="97"/>
+      <c r="AI17" s="97">
         <v>2.1</v>
       </c>
-      <c r="AJ11" s="97">
+      <c r="AJ17" s="97">
         <v>2</v>
       </c>
-      <c r="AK11" s="97">
+      <c r="AK17" s="97">
         <v>2</v>
       </c>
-      <c r="AL11" s="97" t="b">
+      <c r="AL17" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AM11" s="97" t="b">
+      <c r="AM17" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AN11" s="97" t="b">
+      <c r="AN17" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AO11" s="97">
+      <c r="AO17" s="97">
         <v>10</v>
       </c>
-      <c r="AP11" s="98">
+      <c r="AP17" s="98">
         <v>0.7</v>
       </c>
-      <c r="AQ11" s="99" t="s">
+      <c r="AQ17" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="AR11" s="100" t="s">
+      <c r="AR17" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="AS11" s="101">
+      <c r="AS17" s="101">
         <v>1.9E-3</v>
       </c>
-      <c r="AT11" s="102">
+      <c r="AT17" s="102">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU11" s="103">
+      <c r="AU17" s="103">
         <v>300</v>
       </c>
-      <c r="AV11" s="83">
+      <c r="AV17" s="83">
         <v>2.4</v>
       </c>
-      <c r="AW11" s="83">
+      <c r="AW17" s="83">
         <v>9.5</v>
       </c>
-      <c r="AX11" s="83">
+      <c r="AX17" s="83">
         <v>1.7</v>
       </c>
-      <c r="AY11" s="83">
+      <c r="AY17" s="83">
         <v>1</v>
       </c>
-      <c r="AZ11" s="83">
+      <c r="AZ17" s="83">
         <v>1.6</v>
       </c>
-      <c r="BA11" s="83">
+      <c r="BA17" s="83">
         <v>9</v>
       </c>
-      <c r="BB11" s="83">
+      <c r="BB17" s="83">
         <v>6</v>
       </c>
-      <c r="BC11" s="104" t="s">
+      <c r="BC17" s="104" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="105" t="s">
+    <row r="18" spans="1:55" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C18" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="107" t="s">
+      <c r="D18" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="84">
+      <c r="E18" s="84">
         <v>2</v>
       </c>
-      <c r="F12" s="108" t="s">
+      <c r="F18" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="109">
+      <c r="G18" s="109">
         <v>11000</v>
       </c>
-      <c r="H12" s="110">
+      <c r="H18" s="110">
         <v>100</v>
       </c>
-      <c r="I12" s="111">
+      <c r="I18" s="111">
         <v>5</v>
       </c>
-      <c r="J12" s="112">
+      <c r="J18" s="112">
         <v>0</v>
       </c>
-      <c r="K12" s="113">
+      <c r="K18" s="113">
         <v>80</v>
       </c>
-      <c r="L12" s="114">
+      <c r="L18" s="114">
         <v>1.5</v>
       </c>
-      <c r="M12" s="114">
+      <c r="M18" s="114">
         <v>1</v>
       </c>
-      <c r="N12" s="114">
+      <c r="N18" s="114">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O12" s="114">
+      <c r="O18" s="114">
         <v>30</v>
       </c>
-      <c r="P12" s="114">
+      <c r="P18" s="114">
         <v>0.5</v>
       </c>
-      <c r="Q12" s="115">
+      <c r="Q18" s="115">
         <v>0.85</v>
       </c>
-      <c r="R12" s="112">
+      <c r="R18" s="112">
         <v>2.1</v>
       </c>
-      <c r="S12" s="114">
+      <c r="S18" s="114">
         <v>100</v>
       </c>
-      <c r="T12" s="114">
+      <c r="T18" s="114">
         <v>40</v>
       </c>
-      <c r="U12" s="116">
+      <c r="U18" s="116">
         <v>14</v>
       </c>
-      <c r="V12" s="112">
+      <c r="V18" s="112">
         <v>9</v>
       </c>
-      <c r="W12" s="114">
+      <c r="W18" s="114">
         <v>3</v>
       </c>
-      <c r="X12" s="114">
+      <c r="X18" s="114">
         <v>9</v>
       </c>
-      <c r="Y12" s="116">
+      <c r="Y18" s="116">
         <v>8000</v>
       </c>
-      <c r="Z12" s="117">
+      <c r="Z18" s="117">
         <v>2</v>
       </c>
-      <c r="AA12" s="115">
+      <c r="AA18" s="115">
         <v>0.15</v>
       </c>
-      <c r="AB12" s="115">
+      <c r="AB18" s="115">
         <v>0</v>
       </c>
-      <c r="AC12" s="95">
+      <c r="AC18" s="95">
         <v>12</v>
       </c>
-      <c r="AD12" s="96" t="s">
+      <c r="AD18" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="AE12" s="97" t="s">
+      <c r="AE18" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="AF12" s="97" t="s">
+      <c r="AF18" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="AG12" s="97"/>
-      <c r="AH12" s="97"/>
-      <c r="AI12" s="97">
+      <c r="AG18" s="97"/>
+      <c r="AH18" s="97"/>
+      <c r="AI18" s="97">
         <v>2</v>
       </c>
-      <c r="AJ12" s="97">
+      <c r="AJ18" s="97">
         <v>2</v>
       </c>
-      <c r="AK12" s="97">
+      <c r="AK18" s="97">
         <v>2</v>
       </c>
-      <c r="AL12" s="97" t="b">
+      <c r="AL18" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AM12" s="97" t="b">
+      <c r="AM18" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AN12" s="97" t="b">
+      <c r="AN18" s="97" t="b">
         <v>1</v>
       </c>
-      <c r="AO12" s="97">
+      <c r="AO18" s="97">
         <v>10</v>
       </c>
-      <c r="AP12" s="98">
+      <c r="AP18" s="98">
         <v>0.7</v>
       </c>
-      <c r="AQ12" s="99" t="s">
+      <c r="AQ18" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="AR12" s="100" t="s">
+      <c r="AR18" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="AS12" s="101">
+      <c r="AS18" s="101">
         <v>1.8E-3</v>
       </c>
-      <c r="AT12" s="102">
+      <c r="AT18" s="102">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AU12" s="103">
+      <c r="AU18" s="103">
         <v>322</v>
       </c>
-      <c r="AV12" s="83">
+      <c r="AV18" s="83">
         <v>2.5</v>
       </c>
-      <c r="AW12" s="83">
+      <c r="AW18" s="83">
         <v>9.5</v>
       </c>
-      <c r="AX12" s="83">
+      <c r="AX18" s="83">
         <v>1.7</v>
       </c>
-      <c r="AY12" s="83">
+      <c r="AY18" s="83">
         <v>0.5</v>
       </c>
-      <c r="AZ12" s="83">
+      <c r="AZ18" s="83">
         <v>1.9</v>
       </c>
-      <c r="BA12" s="83">
+      <c r="BA18" s="83">
         <v>9</v>
       </c>
-      <c r="BB12" s="83">
+      <c r="BB18" s="83">
         <v>6</v>
       </c>
-      <c r="BC12" s="104" t="s">
+      <c r="BC18" s="104" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="123" t="s">
+    <row r="19" spans="1:55" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="124"/>
-      <c r="K13" s="125" t="s">
+      <c r="J19" s="124"/>
+      <c r="K19" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="126"/>
-      <c r="M13" s="126"/>
-      <c r="N13" s="126"/>
-      <c r="O13" s="126"/>
-      <c r="P13" s="127"/>
-      <c r="Q13" s="29" t="s">
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
+      <c r="N19" s="126"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="127"/>
+      <c r="Q19" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="128" t="s">
+      <c r="R19" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="129"/>
-      <c r="T13" s="129"/>
-      <c r="U13" s="130"/>
-      <c r="V13" s="131" t="s">
+      <c r="S19" s="129"/>
+      <c r="T19" s="129"/>
+      <c r="U19" s="130"/>
+      <c r="V19" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="132"/>
-      <c r="X13" s="132"/>
-      <c r="Y13" s="133"/>
-      <c r="Z13" s="30"/>
-      <c r="AA13" s="30"/>
-      <c r="AB13" s="30"/>
+      <c r="W19" s="132"/>
+      <c r="X19" s="132"/>
+      <c r="Y19" s="133"/>
+      <c r="Z19" s="30"/>
+      <c r="AA19" s="30"/>
+      <c r="AB19" s="30"/>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
     </row>
-    <row r="16" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
+    <row r="22" spans="1:55" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:55" ht="24" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>99</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F24" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="80" t="s">
+      <c r="G24" s="80" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="187.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+    <row r="25" spans="1:55" ht="185" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C25" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E25" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F25" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B26" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C26" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D26" s="24">
         <v>0</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E26" s="25">
         <v>0</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G26" s="34" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C27" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D27" s="24">
         <v>0</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E27" s="25">
         <v>0</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G27" s="35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B28" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C28" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D28" s="24">
         <v>0</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E28" s="25">
         <v>0</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="35" t="s">
+      <c r="G28" s="35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B23" s="81" t="s">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B29" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C29" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="86">
+      <c r="D29" s="86">
         <v>0</v>
       </c>
-      <c r="E23" s="87">
+      <c r="E29" s="87">
         <v>0</v>
       </c>
-      <c r="F23" s="119" t="s">
+      <c r="F29" s="119" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G29" s="120">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B24" s="81" t="s">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B30" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="118" t="s">
+      <c r="C30" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="86">
+      <c r="D30" s="86">
         <v>2000</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E30" s="87">
         <v>60</v>
       </c>
-      <c r="F24" s="119" t="s">
+      <c r="F30" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G30" s="120">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B25" s="105" t="s">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B31" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="121" t="s">
+      <c r="C31" s="121" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="109">
+      <c r="D31" s="109">
         <v>11000</v>
       </c>
-      <c r="E25" s="110">
+      <c r="E31" s="110">
         <v>100</v>
       </c>
-      <c r="F25" s="119" t="s">
+      <c r="F31" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="G25" s="122">
+      <c r="G31" s="122">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="1" t="s">
+    <row r="32" spans="1:55" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:27" ht="24" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
     </row>
-    <row r="33" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B34" s="1" t="s">
+    <row r="39" spans="2:27" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:27" ht="24" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
     </row>
-    <row r="36" spans="2:27" ht="184.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+    <row r="42" spans="2:27" ht="182" x14ac:dyDescent="0.2">
+      <c r="B42" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C42" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D42" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E42" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F42" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B43" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C43" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D43" s="24">
         <v>0</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E43" s="25">
         <v>0</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F43" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B44" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C44" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D44" s="24">
         <v>0</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E44" s="25">
         <v>0</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F44" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B45" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C45" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D45" s="24">
         <v>0</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E45" s="25">
         <v>0</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F45" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B46" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C46" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D46" s="24">
         <v>0</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E46" s="25">
         <v>0</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F46" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B47" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C47" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D47" s="24">
         <v>2000</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E47" s="25">
         <v>60</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F47" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B48" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C48" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D48" s="27">
         <v>11000</v>
       </c>
-      <c r="E42" s="28">
+      <c r="E48" s="28">
         <v>100</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F48" s="13">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:P19"/>
+    <mergeCell ref="R19:U19"/>
+    <mergeCell ref="V19:Y19"/>
   </mergeCells>
-  <conditionalFormatting sqref="C11:C12 C7">
-    <cfRule type="duplicateValues" dxfId="85" priority="10"/>
+  <conditionalFormatting sqref="C17:C18 C13">
+    <cfRule type="duplicateValues" dxfId="104" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="84" priority="9"/>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="duplicateValues" dxfId="103" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="83" priority="8"/>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="duplicateValues" dxfId="102" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="82" priority="7"/>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="duplicateValues" dxfId="101" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:C25 C20">
-    <cfRule type="duplicateValues" dxfId="81" priority="11"/>
+  <conditionalFormatting sqref="C30:C31 C26">
+    <cfRule type="duplicateValues" dxfId="100" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="duplicateValues" dxfId="80" priority="12"/>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="duplicateValues" dxfId="99" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="duplicateValues" dxfId="79" priority="13"/>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="duplicateValues" dxfId="98" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="duplicateValues" dxfId="78" priority="14"/>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="duplicateValues" dxfId="97" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C42 C37">
-    <cfRule type="duplicateValues" dxfId="77" priority="3"/>
+  <conditionalFormatting sqref="C47:C48 C43">
+    <cfRule type="duplicateValues" dxfId="96" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="duplicateValues" dxfId="76" priority="4"/>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="duplicateValues" dxfId="95" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="duplicateValues" dxfId="75" priority="5"/>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="duplicateValues" dxfId="94" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="duplicateValues" dxfId="74" priority="6"/>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="duplicateValues" dxfId="93" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BC7:BC12">
-    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
+  <conditionalFormatting sqref="BC13:BC18">
+    <cfRule type="duplicateValues" dxfId="92" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C6">
+    <cfRule type="duplicateValues" dxfId="91" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D7:D12">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D18">
       <formula1>INDIRECT("dragonTierDefinitions['[sku']]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP Special dragon content
Former-commit-id: ac9078f06f2130c4535a47dcb3768f48dc9f70bb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>[sku]</t>
   </si>
@@ -50,12 +50,6 @@
     <t>dragon_fat</t>
   </si>
   <si>
-    <t>dragon_bug</t>
-  </si>
-  <si>
-    <t>dragon_chinese</t>
-  </si>
-  <si>
     <t>[order]</t>
   </si>
   <si>
@@ -95,21 +89,6 @@
     <t>tier_2</t>
   </si>
   <si>
-    <t>PF_DragonChineseResults</t>
-  </si>
-  <si>
-    <t>PF_DragonChineseMenu</t>
-  </si>
-  <si>
-    <t>PF_DragonChinese</t>
-  </si>
-  <si>
-    <t>PF_DragonBugMenu</t>
-  </si>
-  <si>
-    <t>PF_DragonBug</t>
-  </si>
-  <si>
     <t>PF_DragonFatMenu</t>
   </si>
   <si>
@@ -405,6 +384,15 @@
   </si>
   <si>
     <t>[upgradeLevelToUnlock]</t>
+  </si>
+  <si>
+    <t>{specialDragonPowerDefinitions}</t>
+  </si>
+  <si>
+    <t>[type]</t>
+  </si>
+  <si>
+    <t>special</t>
   </si>
 </sst>
 </file>
@@ -1164,6 +1152,24 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1196,24 +1202,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,29 +1229,94 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1300,6 +1353,31 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1337,96 +1415,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1510,13 +1498,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1526,6 +1507,13 @@
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -3804,11 +3792,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:S6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35">
-  <autoFilter ref="B3:S6"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35">
+  <autoFilter ref="B3:T6"/>
+  <tableColumns count="19">
     <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="34"/>
     <tableColumn id="2" name="[sku]"/>
+    <tableColumn id="3" name="[type]"/>
     <tableColumn id="5" name="[order]" dataDxfId="33"/>
     <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="32"/>
     <tableColumn id="8" name="[unlockPricePC]" dataDxfId="31"/>
@@ -3831,14 +3820,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="15"/>
     <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="4"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="2"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="3">
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="13"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="12"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="11">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4111,8 +4100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,7 +4174,7 @@
   <sheetData>
     <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4215,57 +4204,60 @@
     </row>
     <row r="3" spans="1:54" ht="147" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="61" t="s">
+      <c r="D3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="83" t="s">
+      <c r="O3" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="P3" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="83" t="s">
+      <c r="Q3" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="80" t="s">
+      <c r="R3" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="80" t="s">
+      <c r="S3" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="80" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="N3" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="81" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="81" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="S3" s="71" t="s">
+      <c r="T3" s="71" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4274,30 +4266,33 @@
         <v>2</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="64">
+        <v>81</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="64">
         <v>0</v>
       </c>
-      <c r="E4" s="65">
+      <c r="F4" s="65">
         <v>200</v>
       </c>
-      <c r="F4" s="66">
+      <c r="G4" s="66">
         <v>400</v>
       </c>
-      <c r="G4" s="78"/>
       <c r="H4" s="78"/>
       <c r="I4" s="78"/>
-      <c r="J4" s="76"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="76"/>
       <c r="L4" s="76"/>
-      <c r="M4" s="84"/>
+      <c r="M4" s="76"/>
       <c r="N4" s="84"/>
       <c r="O4" s="84"/>
-      <c r="P4" s="74"/>
+      <c r="P4" s="84"/>
       <c r="Q4" s="74"/>
       <c r="R4" s="74"/>
-      <c r="S4" s="72" t="s">
+      <c r="S4" s="74"/>
+      <c r="T4" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4306,30 +4301,57 @@
         <v>2</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="64">
+        <v>79</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="64">
         <v>1</v>
       </c>
-      <c r="E5" s="65">
+      <c r="F5" s="65">
         <v>200</v>
       </c>
-      <c r="F5" s="66">
+      <c r="G5" s="66">
         <v>400</v>
       </c>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="72" t="s">
+      <c r="H5" s="78">
+        <v>30</v>
+      </c>
+      <c r="I5" s="78">
+        <v>0</v>
+      </c>
+      <c r="J5" s="78">
+        <v>100</v>
+      </c>
+      <c r="K5" s="76">
+        <v>30</v>
+      </c>
+      <c r="L5" s="76">
+        <v>0</v>
+      </c>
+      <c r="M5" s="76">
+        <v>100</v>
+      </c>
+      <c r="N5" s="84">
+        <v>30</v>
+      </c>
+      <c r="O5" s="84">
+        <v>0</v>
+      </c>
+      <c r="P5" s="84">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="74">
+        <v>1</v>
+      </c>
+      <c r="R5" s="74">
+        <v>1</v>
+      </c>
+      <c r="S5" s="74">
+        <v>1</v>
+      </c>
+      <c r="T5" s="72" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4338,30 +4360,33 @@
         <v>2</v>
       </c>
       <c r="C6" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="64">
+        <v>80</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="64">
         <v>2</v>
       </c>
-      <c r="E6" s="69">
+      <c r="F6" s="69">
         <v>200</v>
       </c>
-      <c r="F6" s="70">
+      <c r="G6" s="70">
         <v>400</v>
       </c>
-      <c r="G6" s="79"/>
       <c r="H6" s="79"/>
       <c r="I6" s="79"/>
-      <c r="J6" s="77"/>
+      <c r="J6" s="79"/>
       <c r="K6" s="77"/>
       <c r="L6" s="77"/>
-      <c r="M6" s="85"/>
+      <c r="M6" s="77"/>
       <c r="N6" s="85"/>
       <c r="O6" s="85"/>
-      <c r="P6" s="75"/>
+      <c r="P6" s="85"/>
       <c r="Q6" s="75"/>
       <c r="R6" s="75"/>
-      <c r="S6" s="73" t="s">
+      <c r="S6" s="75"/>
+      <c r="T6" s="73" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4426,7 +4451,7 @@
     <row r="9" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -4485,160 +4510,160 @@
     </row>
     <row r="12" spans="1:54" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="Q12" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="AB12" s="28" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="AC12" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AD12" s="23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AE12" s="23" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="AF12" s="23" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="AG12" s="23" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="AH12" s="23" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="AI12" s="23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="AJ12" s="23" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AK12" s="23" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AL12" s="23" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AM12" s="23" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="AN12" s="23" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AO12" s="27" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AP12" s="29" t="s">
         <v>3</v>
       </c>
       <c r="AQ12" s="31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AR12" s="30" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AS12" s="32" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AT12" s="26" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AU12" s="25" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AV12" s="25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="AW12" s="25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AX12" s="25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="AY12" s="25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="AZ12" s="22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="BA12" s="22" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="BB12" s="25" t="s">
         <v>1</v>
@@ -4649,459 +4674,201 @@
         <v>2</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G13" s="39">
         <v>0</v>
       </c>
-      <c r="H13" s="40">
-        <v>5</v>
-      </c>
-      <c r="I13" s="41">
-        <v>-2</v>
-      </c>
-      <c r="J13" s="42">
-        <v>170</v>
-      </c>
-      <c r="K13" s="43">
-        <v>1.5</v>
-      </c>
-      <c r="L13" s="43">
-        <v>0</v>
-      </c>
-      <c r="M13" s="43">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="N13" s="44">
-        <v>30</v>
-      </c>
-      <c r="O13" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="P13" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="41">
-        <v>1</v>
-      </c>
-      <c r="R13" s="43">
-        <v>100</v>
-      </c>
-      <c r="S13" s="43">
-        <v>40</v>
-      </c>
-      <c r="T13" s="46">
-        <v>28</v>
-      </c>
-      <c r="U13" s="47">
-        <v>9</v>
-      </c>
-      <c r="V13" s="43">
-        <v>3</v>
-      </c>
-      <c r="W13" s="44">
-        <v>9</v>
-      </c>
-      <c r="X13" s="46">
-        <v>8000</v>
-      </c>
-      <c r="Y13" s="48">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="45">
-        <v>0.13</v>
-      </c>
-      <c r="AA13" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="50">
-        <v>6</v>
-      </c>
-      <c r="AC13" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD13" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE13" s="52" t="s">
-        <v>36</v>
-      </c>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="46"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="51"/>
+      <c r="AD13" s="52"/>
+      <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
       <c r="AG13" s="52"/>
-      <c r="AH13" s="52">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="AI13" s="52">
-        <v>2</v>
-      </c>
-      <c r="AJ13" s="52">
-        <v>2</v>
-      </c>
-      <c r="AK13" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM13" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN13" s="52">
-        <v>10</v>
-      </c>
-      <c r="AO13" s="53">
-        <v>0.55999999999999994</v>
-      </c>
+      <c r="AH13" s="52"/>
+      <c r="AI13" s="52"/>
+      <c r="AJ13" s="52"/>
+      <c r="AK13" s="52"/>
+      <c r="AL13" s="52"/>
+      <c r="AM13" s="52"/>
+      <c r="AN13" s="52"/>
+      <c r="AO13" s="53"/>
       <c r="AP13" s="54"/>
       <c r="AQ13" s="55"/>
-      <c r="AR13" s="56">
-        <v>2E-3</v>
-      </c>
-      <c r="AS13" s="57">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AT13" s="58">
-        <v>260</v>
-      </c>
-      <c r="AU13" s="33">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AV13" s="33">
-        <v>5</v>
-      </c>
-      <c r="AW13" s="33">
-        <v>1.7</v>
-      </c>
-      <c r="AX13" s="59">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AY13" s="59">
-        <v>2.25</v>
-      </c>
-      <c r="AZ13" s="59">
-        <v>0</v>
-      </c>
-      <c r="BA13" s="59">
-        <v>8</v>
-      </c>
-      <c r="BB13" s="33" t="s">
-        <v>4</v>
-      </c>
+      <c r="AR13" s="56"/>
+      <c r="AS13" s="57"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="33"/>
+      <c r="AV13" s="33"/>
+      <c r="AW13" s="33"/>
+      <c r="AX13" s="59"/>
+      <c r="AY13" s="59"/>
+      <c r="AZ13" s="59"/>
+      <c r="BA13" s="59"/>
+      <c r="BB13" s="33"/>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B14" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G14" s="39">
         <v>10</v>
       </c>
-      <c r="H14" s="40">
-        <v>10</v>
-      </c>
-      <c r="I14" s="41">
-        <v>0</v>
-      </c>
-      <c r="J14" s="42">
-        <v>280</v>
-      </c>
-      <c r="K14" s="43">
-        <v>1.9</v>
-      </c>
-      <c r="L14" s="43">
-        <v>0</v>
-      </c>
-      <c r="M14" s="43">
-        <v>1.2E-2</v>
-      </c>
-      <c r="N14" s="44">
-        <v>30</v>
-      </c>
-      <c r="O14" s="44">
-        <v>0.6</v>
-      </c>
-      <c r="P14" s="45">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q14" s="41">
-        <v>1</v>
-      </c>
-      <c r="R14" s="43">
-        <v>100</v>
-      </c>
-      <c r="S14" s="43">
-        <v>40</v>
-      </c>
-      <c r="T14" s="46">
-        <v>28</v>
-      </c>
-      <c r="U14" s="47">
-        <v>11</v>
-      </c>
-      <c r="V14" s="43">
-        <v>4</v>
-      </c>
-      <c r="W14" s="44">
-        <v>10</v>
-      </c>
-      <c r="X14" s="46">
-        <v>10000</v>
-      </c>
-      <c r="Y14" s="48">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="45">
-        <v>0.08</v>
-      </c>
-      <c r="AA14" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="50">
-        <v>6</v>
-      </c>
-      <c r="AC14" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD14" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE14" s="52" t="s">
-        <v>34</v>
-      </c>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="46"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="50"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="52"/>
+      <c r="AE14" s="52"/>
       <c r="AF14" s="52"/>
       <c r="AG14" s="52"/>
-      <c r="AH14" s="52">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AI14" s="52">
-        <v>2</v>
-      </c>
-      <c r="AJ14" s="52">
-        <v>2</v>
-      </c>
-      <c r="AK14" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM14" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN14" s="52">
-        <v>10</v>
-      </c>
-      <c r="AO14" s="53">
-        <v>0.7</v>
-      </c>
+      <c r="AH14" s="52"/>
+      <c r="AI14" s="52"/>
+      <c r="AJ14" s="52"/>
+      <c r="AK14" s="52"/>
+      <c r="AL14" s="52"/>
+      <c r="AM14" s="52"/>
+      <c r="AN14" s="52"/>
+      <c r="AO14" s="53"/>
       <c r="AP14" s="54"/>
       <c r="AQ14" s="55"/>
-      <c r="AR14" s="56">
-        <v>1.8E-3</v>
-      </c>
-      <c r="AS14" s="57">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AT14" s="58">
-        <v>333</v>
-      </c>
-      <c r="AU14" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="AV14" s="33">
-        <v>5</v>
-      </c>
-      <c r="AW14" s="33">
-        <v>1.7</v>
-      </c>
-      <c r="AX14" s="59">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AY14" s="59">
-        <v>2.25</v>
-      </c>
-      <c r="AZ14" s="59">
-        <v>9</v>
-      </c>
-      <c r="BA14" s="59">
-        <v>8</v>
-      </c>
-      <c r="BB14" s="33" t="s">
-        <v>5</v>
-      </c>
+      <c r="AR14" s="56"/>
+      <c r="AS14" s="57"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="33"/>
+      <c r="AV14" s="33"/>
+      <c r="AW14" s="33"/>
+      <c r="AX14" s="59"/>
+      <c r="AY14" s="59"/>
+      <c r="AZ14" s="59"/>
+      <c r="BA14" s="59"/>
+      <c r="BB14" s="33"/>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" s="39">
         <v>20</v>
       </c>
-      <c r="H15" s="40">
-        <v>15</v>
-      </c>
-      <c r="I15" s="41">
-        <v>0</v>
-      </c>
-      <c r="J15" s="42">
-        <v>400</v>
-      </c>
-      <c r="K15" s="43">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L15" s="43">
-        <v>0</v>
-      </c>
-      <c r="M15" s="43">
-        <v>1.4E-2</v>
-      </c>
-      <c r="N15" s="44">
-        <v>25</v>
-      </c>
-      <c r="O15" s="44">
-        <v>0.7</v>
-      </c>
-      <c r="P15" s="45">
-        <v>1.75</v>
-      </c>
-      <c r="Q15" s="41">
-        <v>1</v>
-      </c>
-      <c r="R15" s="43">
-        <v>100</v>
-      </c>
-      <c r="S15" s="43">
-        <v>40</v>
-      </c>
-      <c r="T15" s="46">
-        <v>28</v>
-      </c>
-      <c r="U15" s="47">
-        <v>11.5</v>
-      </c>
-      <c r="V15" s="43">
-        <v>5</v>
-      </c>
-      <c r="W15" s="44">
-        <v>10</v>
-      </c>
-      <c r="X15" s="46">
-        <v>20000</v>
-      </c>
-      <c r="Y15" s="48">
-        <v>4</v>
-      </c>
-      <c r="Z15" s="45">
-        <v>0.05</v>
-      </c>
-      <c r="AA15" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="50">
-        <v>6</v>
-      </c>
-      <c r="AC15" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD15" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE15" s="52" t="s">
-        <v>31</v>
-      </c>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="50"/>
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="52"/>
+      <c r="AE15" s="52"/>
       <c r="AF15" s="52"/>
       <c r="AG15" s="52"/>
-      <c r="AH15" s="52">
-        <v>2.1</v>
-      </c>
-      <c r="AI15" s="52">
-        <v>2</v>
-      </c>
-      <c r="AJ15" s="52">
-        <v>2</v>
-      </c>
-      <c r="AK15" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL15" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM15" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN15" s="52">
-        <v>10</v>
-      </c>
-      <c r="AO15" s="53">
-        <v>0.7</v>
-      </c>
+      <c r="AH15" s="52"/>
+      <c r="AI15" s="52"/>
+      <c r="AJ15" s="52"/>
+      <c r="AK15" s="52"/>
+      <c r="AL15" s="52"/>
+      <c r="AM15" s="52"/>
+      <c r="AN15" s="52"/>
+      <c r="AO15" s="53"/>
       <c r="AP15" s="54"/>
       <c r="AQ15" s="55"/>
-      <c r="AR15" s="56">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="AS15" s="57">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AT15" s="58">
-        <v>475</v>
-      </c>
-      <c r="AU15" s="33">
-        <v>3.4</v>
-      </c>
-      <c r="AV15" s="33">
-        <v>5</v>
-      </c>
-      <c r="AW15" s="33">
-        <v>1.7</v>
-      </c>
-      <c r="AX15" s="59">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AY15" s="59">
-        <v>2.25</v>
-      </c>
-      <c r="AZ15" s="59">
-        <v>45</v>
-      </c>
-      <c r="BA15" s="59">
-        <v>15</v>
-      </c>
-      <c r="BB15" s="33" t="s">
-        <v>6</v>
-      </c>
+      <c r="AR15" s="56"/>
+      <c r="AS15" s="57"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="33"/>
+      <c r="AV15" s="33"/>
+      <c r="AW15" s="33"/>
+      <c r="AX15" s="59"/>
+      <c r="AY15" s="59"/>
+      <c r="AZ15" s="59"/>
+      <c r="BA15" s="59"/>
+      <c r="BB15" s="33"/>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -5109,190 +4876,104 @@
         <v>2</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G16" s="39">
         <v>30</v>
       </c>
-      <c r="H16" s="40">
-        <v>25</v>
-      </c>
-      <c r="I16" s="41">
-        <v>0</v>
-      </c>
-      <c r="J16" s="42">
-        <v>430</v>
-      </c>
-      <c r="K16" s="43">
-        <v>2.4</v>
-      </c>
-      <c r="L16" s="43">
-        <v>0</v>
-      </c>
-      <c r="M16" s="43">
-        <v>1.6E-2</v>
-      </c>
-      <c r="N16" s="44">
-        <v>20</v>
-      </c>
-      <c r="O16" s="44">
-        <v>0.8</v>
-      </c>
-      <c r="P16" s="45">
-        <v>2.1</v>
-      </c>
-      <c r="Q16" s="41">
-        <v>1</v>
-      </c>
-      <c r="R16" s="43">
-        <v>100</v>
-      </c>
-      <c r="S16" s="43">
-        <v>40</v>
-      </c>
-      <c r="T16" s="46">
-        <v>28</v>
-      </c>
-      <c r="U16" s="47">
-        <v>12</v>
-      </c>
-      <c r="V16" s="43">
-        <v>6</v>
-      </c>
-      <c r="W16" s="44">
-        <v>10</v>
-      </c>
-      <c r="X16" s="46">
-        <v>30000</v>
-      </c>
-      <c r="Y16" s="48">
-        <v>5</v>
-      </c>
-      <c r="Z16" s="45">
-        <v>0.04</v>
-      </c>
-      <c r="AA16" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="50">
-        <v>6</v>
-      </c>
-      <c r="AC16" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD16" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE16" s="52" t="s">
-        <v>28</v>
-      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="49"/>
+      <c r="AB16" s="50"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="52"/>
+      <c r="AE16" s="52"/>
       <c r="AF16" s="52"/>
       <c r="AG16" s="52"/>
-      <c r="AH16" s="52">
-        <v>2.1</v>
-      </c>
-      <c r="AI16" s="52">
-        <v>2</v>
-      </c>
-      <c r="AJ16" s="52">
-        <v>2</v>
-      </c>
-      <c r="AK16" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL16" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM16" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN16" s="52">
-        <v>10</v>
-      </c>
-      <c r="AO16" s="53">
-        <v>0.7</v>
-      </c>
+      <c r="AH16" s="52"/>
+      <c r="AI16" s="52"/>
+      <c r="AJ16" s="52"/>
+      <c r="AK16" s="52"/>
+      <c r="AL16" s="52"/>
+      <c r="AM16" s="52"/>
+      <c r="AN16" s="52"/>
+      <c r="AO16" s="53"/>
       <c r="AP16" s="54"/>
       <c r="AQ16" s="55"/>
-      <c r="AR16" s="56">
-        <v>1.5E-3</v>
-      </c>
-      <c r="AS16" s="57">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AT16" s="58">
-        <v>705</v>
-      </c>
-      <c r="AU16" s="33">
-        <v>4.7</v>
-      </c>
-      <c r="AV16" s="33">
-        <v>5</v>
-      </c>
-      <c r="AW16" s="33">
-        <v>1.7</v>
-      </c>
-      <c r="AX16" s="59">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AY16" s="59">
-        <v>2.25</v>
-      </c>
-      <c r="AZ16" s="59">
-        <v>59</v>
-      </c>
-      <c r="BA16" s="59">
-        <v>15</v>
-      </c>
-      <c r="BB16" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="AR16" s="56"/>
+      <c r="AS16" s="57"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="33"/>
+      <c r="AV16" s="33"/>
+      <c r="AW16" s="33"/>
+      <c r="AX16" s="59"/>
+      <c r="AY16" s="59"/>
+      <c r="AZ16" s="59"/>
+      <c r="BA16" s="59"/>
+      <c r="BB16" s="33"/>
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G17" s="39">
         <v>0</v>
       </c>
       <c r="H17" s="40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I17" s="41">
+        <v>-2</v>
+      </c>
+      <c r="J17" s="42">
+        <v>170</v>
+      </c>
+      <c r="K17" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="43">
         <v>0</v>
       </c>
-      <c r="J17" s="42">
-        <v>95</v>
-      </c>
-      <c r="K17" s="43">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L17" s="43">
-        <v>1</v>
-      </c>
       <c r="M17" s="43">
-        <v>8.5000000000000006E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N17" s="44">
         <v>30</v>
@@ -5301,22 +4982,22 @@
         <v>0.5</v>
       </c>
       <c r="P17" s="45">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="41">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="R17" s="43">
         <v>100</v>
       </c>
       <c r="S17" s="43">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="T17" s="46">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="U17" s="47">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V17" s="43">
         <v>3</v>
@@ -5325,33 +5006,33 @@
         <v>9</v>
       </c>
       <c r="X17" s="46">
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="Y17" s="48">
         <v>2</v>
       </c>
       <c r="Z17" s="45">
-        <v>0.19</v>
+        <v>0.13</v>
       </c>
       <c r="AA17" s="49">
         <v>0</v>
       </c>
       <c r="AB17" s="50">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AC17" s="51" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AD17" s="52" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AE17" s="52" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AF17" s="52"/>
       <c r="AG17" s="52"/>
       <c r="AH17" s="52">
-        <v>2.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AI17" s="52">
         <v>2</v>
@@ -5372,42 +5053,42 @@
         <v>10</v>
       </c>
       <c r="AO17" s="53">
-        <v>0.7</v>
+        <v>0.55999999999999994</v>
       </c>
       <c r="AP17" s="54"/>
       <c r="AQ17" s="55"/>
       <c r="AR17" s="56">
-        <v>1.9E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="AS17" s="57">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT17" s="58">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="AU17" s="33">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AV17" s="33">
-        <v>9.5</v>
+        <v>5</v>
       </c>
       <c r="AW17" s="33">
         <v>1.7</v>
       </c>
       <c r="AX17" s="59">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AY17" s="59">
-        <v>1.6</v>
+        <v>2.25</v>
       </c>
       <c r="AZ17" s="59">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BA17" s="59">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BB17" s="33" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">
@@ -5415,217 +5096,475 @@
         <v>2</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G18" s="39">
         <v>10</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="46"/>
-      <c r="U18" s="47"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="44"/>
-      <c r="X18" s="46"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="45"/>
-      <c r="AA18" s="49"/>
-      <c r="AB18" s="50"/>
-      <c r="AC18" s="51"/>
-      <c r="AD18" s="52"/>
-      <c r="AE18" s="52"/>
+      <c r="H18" s="40">
+        <v>10</v>
+      </c>
+      <c r="I18" s="41">
+        <v>0</v>
+      </c>
+      <c r="J18" s="42">
+        <v>280</v>
+      </c>
+      <c r="K18" s="43">
+        <v>1.9</v>
+      </c>
+      <c r="L18" s="43">
+        <v>0</v>
+      </c>
+      <c r="M18" s="43">
+        <v>1.2E-2</v>
+      </c>
+      <c r="N18" s="44">
+        <v>30</v>
+      </c>
+      <c r="O18" s="44">
+        <v>0.6</v>
+      </c>
+      <c r="P18" s="45">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q18" s="41">
+        <v>1</v>
+      </c>
+      <c r="R18" s="43">
+        <v>125</v>
+      </c>
+      <c r="S18" s="43">
+        <v>40</v>
+      </c>
+      <c r="T18" s="46">
+        <v>28</v>
+      </c>
+      <c r="U18" s="47">
+        <v>11</v>
+      </c>
+      <c r="V18" s="43">
+        <v>4</v>
+      </c>
+      <c r="W18" s="44">
+        <v>10</v>
+      </c>
+      <c r="X18" s="46">
+        <v>10000</v>
+      </c>
+      <c r="Y18" s="48">
+        <v>3</v>
+      </c>
+      <c r="Z18" s="45">
+        <v>0.08</v>
+      </c>
+      <c r="AA18" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="50">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD18" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE18" s="52" t="s">
+        <v>27</v>
+      </c>
       <c r="AF18" s="52"/>
       <c r="AG18" s="52"/>
-      <c r="AH18" s="52"/>
-      <c r="AI18" s="52"/>
-      <c r="AJ18" s="52"/>
-      <c r="AK18" s="52"/>
-      <c r="AL18" s="52"/>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="52"/>
-      <c r="AO18" s="53"/>
+      <c r="AH18" s="52">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI18" s="52">
+        <v>2</v>
+      </c>
+      <c r="AJ18" s="52">
+        <v>2</v>
+      </c>
+      <c r="AK18" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM18" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="52">
+        <v>10</v>
+      </c>
+      <c r="AO18" s="53">
+        <v>0.7</v>
+      </c>
       <c r="AP18" s="54"/>
       <c r="AQ18" s="55"/>
-      <c r="AR18" s="56"/>
-      <c r="AS18" s="57"/>
-      <c r="AT18" s="58"/>
-      <c r="AU18" s="33"/>
-      <c r="AV18" s="33"/>
-      <c r="AW18" s="33"/>
-      <c r="AX18" s="59"/>
-      <c r="AY18" s="59"/>
-      <c r="AZ18" s="59"/>
-      <c r="BA18" s="59"/>
-      <c r="BB18" s="33"/>
+      <c r="AR18" s="56">
+        <v>1.8E-3</v>
+      </c>
+      <c r="AS18" s="57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT18" s="58">
+        <v>333</v>
+      </c>
+      <c r="AU18" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="AV18" s="33">
+        <v>5</v>
+      </c>
+      <c r="AW18" s="33">
+        <v>1.7</v>
+      </c>
+      <c r="AX18" s="59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AY18" s="59">
+        <v>2.25</v>
+      </c>
+      <c r="AZ18" s="59">
+        <v>9</v>
+      </c>
+      <c r="BA18" s="59">
+        <v>8</v>
+      </c>
+      <c r="BB18" s="33" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G19" s="39">
         <v>20</v>
       </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="47"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="45"/>
-      <c r="AA19" s="49"/>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="52"/>
-      <c r="AE19" s="52"/>
+      <c r="H19" s="40">
+        <v>15</v>
+      </c>
+      <c r="I19" s="41">
+        <v>0</v>
+      </c>
+      <c r="J19" s="42">
+        <v>400</v>
+      </c>
+      <c r="K19" s="43">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L19" s="43">
+        <v>0</v>
+      </c>
+      <c r="M19" s="43">
+        <v>1.4E-2</v>
+      </c>
+      <c r="N19" s="44">
+        <v>25</v>
+      </c>
+      <c r="O19" s="44">
+        <v>0.7</v>
+      </c>
+      <c r="P19" s="45">
+        <v>1.75</v>
+      </c>
+      <c r="Q19" s="41">
+        <v>1</v>
+      </c>
+      <c r="R19" s="43">
+        <v>150</v>
+      </c>
+      <c r="S19" s="43">
+        <v>40</v>
+      </c>
+      <c r="T19" s="46">
+        <v>28</v>
+      </c>
+      <c r="U19" s="47">
+        <v>11.5</v>
+      </c>
+      <c r="V19" s="43">
+        <v>5</v>
+      </c>
+      <c r="W19" s="44">
+        <v>10</v>
+      </c>
+      <c r="X19" s="46">
+        <v>20000</v>
+      </c>
+      <c r="Y19" s="48">
+        <v>4</v>
+      </c>
+      <c r="Z19" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="AA19" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="50">
+        <v>6</v>
+      </c>
+      <c r="AC19" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD19" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE19" s="52" t="s">
+        <v>24</v>
+      </c>
       <c r="AF19" s="52"/>
       <c r="AG19" s="52"/>
-      <c r="AH19" s="52"/>
-      <c r="AI19" s="52"/>
-      <c r="AJ19" s="52"/>
-      <c r="AK19" s="52"/>
-      <c r="AL19" s="52"/>
-      <c r="AM19" s="52"/>
-      <c r="AN19" s="52"/>
-      <c r="AO19" s="53"/>
+      <c r="AH19" s="52">
+        <v>2.1</v>
+      </c>
+      <c r="AI19" s="52">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="52">
+        <v>2</v>
+      </c>
+      <c r="AK19" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="52">
+        <v>10</v>
+      </c>
+      <c r="AO19" s="53">
+        <v>0.7</v>
+      </c>
       <c r="AP19" s="54"/>
       <c r="AQ19" s="55"/>
-      <c r="AR19" s="56"/>
-      <c r="AS19" s="57"/>
-      <c r="AT19" s="58"/>
-      <c r="AU19" s="33"/>
-      <c r="AV19" s="33"/>
-      <c r="AW19" s="33"/>
-      <c r="AX19" s="59"/>
-      <c r="AY19" s="59"/>
-      <c r="AZ19" s="59"/>
-      <c r="BA19" s="59"/>
-      <c r="BB19" s="33"/>
+      <c r="AR19" s="56">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AS19" s="57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT19" s="58">
+        <v>475</v>
+      </c>
+      <c r="AU19" s="33">
+        <v>3.4</v>
+      </c>
+      <c r="AV19" s="33">
+        <v>5</v>
+      </c>
+      <c r="AW19" s="33">
+        <v>1.7</v>
+      </c>
+      <c r="AX19" s="59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AY19" s="59">
+        <v>2.25</v>
+      </c>
+      <c r="AZ19" s="59">
+        <v>45</v>
+      </c>
+      <c r="BA19" s="59">
+        <v>15</v>
+      </c>
+      <c r="BB19" s="33" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G20" s="39">
         <v>30</v>
       </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="46"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="44"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="49"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="52"/>
-      <c r="AE20" s="52"/>
+      <c r="H20" s="40">
+        <v>25</v>
+      </c>
+      <c r="I20" s="41">
+        <v>0</v>
+      </c>
+      <c r="J20" s="42">
+        <v>430</v>
+      </c>
+      <c r="K20" s="43">
+        <v>2.4</v>
+      </c>
+      <c r="L20" s="43">
+        <v>0</v>
+      </c>
+      <c r="M20" s="43">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N20" s="44">
+        <v>20</v>
+      </c>
+      <c r="O20" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="P20" s="45">
+        <v>2.1</v>
+      </c>
+      <c r="Q20" s="41">
+        <v>1</v>
+      </c>
+      <c r="R20" s="43">
+        <v>175</v>
+      </c>
+      <c r="S20" s="43">
+        <v>40</v>
+      </c>
+      <c r="T20" s="46">
+        <v>28</v>
+      </c>
+      <c r="U20" s="47">
+        <v>12</v>
+      </c>
+      <c r="V20" s="43">
+        <v>6</v>
+      </c>
+      <c r="W20" s="44">
+        <v>10</v>
+      </c>
+      <c r="X20" s="46">
+        <v>30000</v>
+      </c>
+      <c r="Y20" s="48">
+        <v>5</v>
+      </c>
+      <c r="Z20" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="AA20" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="50">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD20" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE20" s="52" t="s">
+        <v>21</v>
+      </c>
       <c r="AF20" s="52"/>
       <c r="AG20" s="52"/>
-      <c r="AH20" s="52"/>
-      <c r="AI20" s="52"/>
-      <c r="AJ20" s="52"/>
-      <c r="AK20" s="52"/>
-      <c r="AL20" s="52"/>
-      <c r="AM20" s="52"/>
-      <c r="AN20" s="52"/>
-      <c r="AO20" s="53"/>
+      <c r="AH20" s="52">
+        <v>2.1</v>
+      </c>
+      <c r="AI20" s="52">
+        <v>2</v>
+      </c>
+      <c r="AJ20" s="52">
+        <v>2</v>
+      </c>
+      <c r="AK20" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="52">
+        <v>10</v>
+      </c>
+      <c r="AO20" s="53">
+        <v>0.7</v>
+      </c>
       <c r="AP20" s="54"/>
       <c r="AQ20" s="55"/>
-      <c r="AR20" s="56"/>
-      <c r="AS20" s="57"/>
-      <c r="AT20" s="58"/>
-      <c r="AU20" s="33"/>
-      <c r="AV20" s="33"/>
-      <c r="AW20" s="33"/>
-      <c r="AX20" s="59"/>
-      <c r="AY20" s="59"/>
-      <c r="AZ20" s="59"/>
-      <c r="BA20" s="59"/>
-      <c r="BB20" s="33"/>
+      <c r="AR20" s="56">
+        <v>1.5E-3</v>
+      </c>
+      <c r="AS20" s="57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT20" s="58">
+        <v>705</v>
+      </c>
+      <c r="AU20" s="33">
+        <v>4.7</v>
+      </c>
+      <c r="AV20" s="33">
+        <v>5</v>
+      </c>
+      <c r="AW20" s="33">
+        <v>1.7</v>
+      </c>
+      <c r="AX20" s="59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AY20" s="59">
+        <v>2.25</v>
+      </c>
+      <c r="AZ20" s="59">
+        <v>59</v>
+      </c>
+      <c r="BA20" s="59">
+        <v>15</v>
+      </c>
+      <c r="BB20" s="33" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B21" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G21" s="39">
         <v>0</v>
@@ -5683,169 +5622,83 @@
         <v>2</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G22" s="39">
         <v>10</v>
       </c>
-      <c r="H22" s="40">
-        <v>5</v>
-      </c>
-      <c r="I22" s="41">
-        <v>0</v>
-      </c>
-      <c r="J22" s="42">
-        <v>80</v>
-      </c>
-      <c r="K22" s="43">
-        <v>1.5</v>
-      </c>
-      <c r="L22" s="43">
-        <v>1</v>
-      </c>
-      <c r="M22" s="43">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="N22" s="44">
-        <v>30</v>
-      </c>
-      <c r="O22" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="P22" s="45">
-        <v>0.85</v>
-      </c>
-      <c r="Q22" s="41">
-        <v>2.1</v>
-      </c>
-      <c r="R22" s="43">
-        <v>100</v>
-      </c>
-      <c r="S22" s="43">
-        <v>40</v>
-      </c>
-      <c r="T22" s="46">
-        <v>14</v>
-      </c>
-      <c r="U22" s="47">
-        <v>9</v>
-      </c>
-      <c r="V22" s="43">
-        <v>3</v>
-      </c>
-      <c r="W22" s="44">
-        <v>9</v>
-      </c>
-      <c r="X22" s="46">
-        <v>8000</v>
-      </c>
-      <c r="Y22" s="48">
-        <v>2</v>
-      </c>
-      <c r="Z22" s="45">
-        <v>0.15</v>
-      </c>
-      <c r="AA22" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="50">
-        <v>12</v>
-      </c>
-      <c r="AC22" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD22" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE22" s="52" t="s">
-        <v>23</v>
-      </c>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="49"/>
+      <c r="AB22" s="50"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="52"/>
+      <c r="AE22" s="52"/>
       <c r="AF22" s="52"/>
       <c r="AG22" s="52"/>
-      <c r="AH22" s="52">
-        <v>2</v>
-      </c>
-      <c r="AI22" s="52">
-        <v>2</v>
-      </c>
-      <c r="AJ22" s="52">
-        <v>2</v>
-      </c>
-      <c r="AK22" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL22" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM22" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN22" s="52">
-        <v>10</v>
-      </c>
-      <c r="AO22" s="53">
-        <v>0.7</v>
-      </c>
+      <c r="AH22" s="52"/>
+      <c r="AI22" s="52"/>
+      <c r="AJ22" s="52"/>
+      <c r="AK22" s="52"/>
+      <c r="AL22" s="52"/>
+      <c r="AM22" s="52"/>
+      <c r="AN22" s="52"/>
+      <c r="AO22" s="53"/>
       <c r="AP22" s="54"/>
       <c r="AQ22" s="55"/>
-      <c r="AR22" s="56">
-        <v>1.8E-3</v>
-      </c>
-      <c r="AS22" s="57">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AT22" s="58">
-        <v>322</v>
-      </c>
-      <c r="AU22" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="AV22" s="33">
-        <v>9.5</v>
-      </c>
-      <c r="AW22" s="33">
-        <v>1.7</v>
-      </c>
-      <c r="AX22" s="59">
-        <v>0.5</v>
-      </c>
-      <c r="AY22" s="59">
-        <v>1.9</v>
-      </c>
-      <c r="AZ22" s="59">
-        <v>9</v>
-      </c>
-      <c r="BA22" s="59">
-        <v>6</v>
-      </c>
-      <c r="BB22" s="33" t="s">
-        <v>9</v>
-      </c>
+      <c r="AR22" s="56"/>
+      <c r="AS22" s="57"/>
+      <c r="AT22" s="58"/>
+      <c r="AU22" s="33"/>
+      <c r="AV22" s="33"/>
+      <c r="AW22" s="33"/>
+      <c r="AX22" s="59"/>
+      <c r="AY22" s="59"/>
+      <c r="AZ22" s="59"/>
+      <c r="BA22" s="59"/>
+      <c r="BB22" s="33"/>
     </row>
     <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G23" s="39">
         <v>20</v>
@@ -5904,16 +5757,16 @@
         <v>2</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" s="39">
         <v>30</v>
@@ -5974,33 +5827,33 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="87"/>
-      <c r="K25" s="88" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="89"/>
-      <c r="M25" s="89"/>
-      <c r="N25" s="89"/>
-      <c r="O25" s="89"/>
-      <c r="P25" s="90"/>
+      <c r="I25" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="93"/>
+      <c r="K25" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="96"/>
       <c r="Q25" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="R25" s="91" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="92"/>
-      <c r="T25" s="92"/>
-      <c r="U25" s="93"/>
-      <c r="V25" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="W25" s="95"/>
-      <c r="X25" s="95"/>
-      <c r="Y25" s="96"/>
+      <c r="R25" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="S25" s="98"/>
+      <c r="T25" s="98"/>
+      <c r="U25" s="99"/>
+      <c r="V25" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="W25" s="101"/>
+      <c r="X25" s="101"/>
+      <c r="Y25" s="102"/>
       <c r="Z25" s="21"/>
       <c r="AA25" s="21"/>
       <c r="AB25" s="21"/>
@@ -6008,7 +5861,7 @@
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -6019,37 +5872,37 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="30" spans="1:54" ht="147" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E30" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="F30" s="100" t="s">
-        <v>89</v>
+        <v>119</v>
+      </c>
+      <c r="F30" s="89" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="97" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="98">
+      <c r="C31" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="87">
         <v>5</v>
       </c>
-      <c r="F31" s="99" t="str">
+      <c r="F31" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_1</v>
       </c>
@@ -6058,16 +5911,16 @@
       <c r="B32" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="97" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="98">
+      <c r="C32" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="87">
         <v>15</v>
       </c>
-      <c r="F32" s="99" t="str">
+      <c r="F32" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_2</v>
       </c>
@@ -6076,16 +5929,16 @@
       <c r="B33" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="97" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="98">
+      <c r="C33" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="87">
         <v>25</v>
       </c>
-      <c r="F33" s="99" t="str">
+      <c r="F33" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_3</v>
       </c>
@@ -6094,16 +5947,16 @@
       <c r="B34" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="97" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="98" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="98">
+      <c r="C34" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="87">
         <v>5</v>
       </c>
-      <c r="F34" s="99" t="str">
+      <c r="F34" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_1</v>
       </c>
@@ -6112,16 +5965,16 @@
       <c r="B35" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="97" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="98" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="98">
+      <c r="C35" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="87">
         <v>15</v>
       </c>
-      <c r="F35" s="99" t="str">
+      <c r="F35" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_2</v>
       </c>
@@ -6130,16 +5983,16 @@
       <c r="B36" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="97" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="98" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="98">
+      <c r="C36" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="87">
         <v>25</v>
       </c>
-      <c r="F36" s="99" t="str">
+      <c r="F36" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_3</v>
       </c>
@@ -6148,16 +6001,16 @@
       <c r="B37" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="97" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="98">
+      <c r="C37" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="87">
         <v>5</v>
       </c>
-      <c r="F37" s="99" t="str">
+      <c r="F37" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_1</v>
       </c>
@@ -6166,16 +6019,16 @@
       <c r="B38" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="97" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="98">
+      <c r="C38" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="87">
         <v>15</v>
       </c>
-      <c r="F38" s="99" t="str">
+      <c r="F38" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_2</v>
       </c>
@@ -6184,16 +6037,16 @@
       <c r="B39" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="101" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="102" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="102">
+      <c r="C39" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="91">
         <v>25</v>
       </c>
-      <c r="F39" s="99" t="str">
+      <c r="F39" s="88" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_3</v>
       </c>
@@ -6206,31 +6059,37 @@
     <mergeCell ref="V25:Y25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="13" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB13">
-    <cfRule type="duplicateValues" dxfId="12" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="38"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C6">
-    <cfRule type="duplicateValues" dxfId="11" priority="20"/>
+  <conditionalFormatting sqref="C4:D6">
+    <cfRule type="duplicateValues" dxfId="8" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S6">
-    <cfRule type="duplicateValues" dxfId="10" priority="19"/>
+  <conditionalFormatting sqref="T4:T6">
+    <cfRule type="duplicateValues" dxfId="7" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="8" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB14:BB24">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  <conditionalFormatting sqref="BB14:BB16 BB21:BB24">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB17">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB18:BB20">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">

</xml_diff>

<commit_message>
WIP special dragons base stats
Former-commit-id: fcd0a028adff8ab1191eae68ae9037cc9b9d51ea
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
   <si>
     <t>[sku]</t>
   </si>
@@ -393,13 +394,85 @@
   </si>
   <si>
     <t>special</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Min bonus</t>
+  </si>
+  <si>
+    <t>Max bonus</t>
+  </si>
+  <si>
+    <t>ELECTRIC</t>
+  </si>
+  <si>
+    <t>TIER</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Energy base</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Health upgrade</t>
+  </si>
+  <si>
+    <t>Current tier</t>
+  </si>
+  <si>
+    <t>Energy base upgrade</t>
+  </si>
+  <si>
+    <t>Force upgrade</t>
+  </si>
+  <si>
+    <t>(HP)</t>
+  </si>
+  <si>
+    <t>(BOOST)</t>
+  </si>
+  <si>
+    <t>(SPEED)</t>
+  </si>
+  <si>
+    <t>Inc. Bonus</t>
+  </si>
+  <si>
+    <t>Tier 1</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>Tier 2</t>
+  </si>
+  <si>
+    <t>Tier 3</t>
+  </si>
+  <si>
+    <t>Tier 4</t>
+  </si>
+  <si>
+    <t>Upgrades</t>
+  </si>
+  <si>
+    <t>DIF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,8 +510,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,6 +631,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1203,11 +1296,45 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="97">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3729,90 +3856,992 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HP Min-Max Per Tier</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$12:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8EF-4FE4-82E3-26959BA93B53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>HP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$12:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D8EF-4FE4-82E3-26959BA93B53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="398241056"/>
+        <c:axId val="398241472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="398241056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398241472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="398241472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398241056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="93" totalsRowBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="96" totalsRowBorderDxfId="95">
   <autoFilter ref="B12:BB24"/>
   <tableColumns count="53">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="91"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="90"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="89"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="88"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="87"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="86"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="85"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="84"/>
-    <tableColumn id="10" name="[health]" dataDxfId="83"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="82"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="81"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="80"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="79"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="78"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="77"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="76"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="75"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="74"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="73"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="72"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="71"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="70"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="69"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="68"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="67"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="66"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="65"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="64"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="63"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="62"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="61"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="60"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="59"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="57"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="56"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="55"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="54"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="53"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="52"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="51"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="50"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="49"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="48"/>
-    <tableColumn id="46" name="[force]" dataDxfId="47"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="46"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="45"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="44"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="43"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="42"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="41"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="40"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="39"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="94"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="93"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="92"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="91"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="90"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="89"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="88"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="87"/>
+    <tableColumn id="10" name="[health]" dataDxfId="86"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="85"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="84"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="83"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="82"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="81"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="80"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="79"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="78"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="77"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="76"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="75"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="74"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="73"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="72"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="71"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="70"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="69"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="68"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="67"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="66"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="65"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="64"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="63"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="62"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="61"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="60"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="59"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="58"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="57"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="56"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="55"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="54"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="53"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="52"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="51"/>
+    <tableColumn id="46" name="[force]" dataDxfId="50"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="49"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="48"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="47"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="46"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="45"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="44"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="43"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
   <autoFilter ref="B3:T6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="34"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="37"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="33"/>
-    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="32"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="31"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="30"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="29"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="28"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="27"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="26"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="25"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="24"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="23"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="22"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="21"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="20"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="19"/>
+    <tableColumn id="5" name="[order]" dataDxfId="36"/>
+    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="35"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="34"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="33"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="32"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="31"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="30"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="29"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="28"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="27"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="26"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="25"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="24"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="23"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="22"/>
     <tableColumn id="65" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3820,14 +4849,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="13"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="12"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="11">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="16"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="15"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="14">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4100,8 +5129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6059,37 +7088,37 @@
     <mergeCell ref="V25:Y25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="10" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB13">
-    <cfRule type="duplicateValues" dxfId="9" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="8" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T6">
-    <cfRule type="duplicateValues" dxfId="7" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="5" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB14:BB16 BB21:BB24">
-    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB17">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB18:BB20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -6104,4 +7133,320 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E1:X15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:24" ht="21" x14ac:dyDescent="0.35">
+      <c r="E1" s="106" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F3" s="104"/>
+      <c r="G3" s="107" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="L3" s="104" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q3" s="104" t="s">
+        <v>129</v>
+      </c>
+      <c r="V3" s="104" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F4" s="105"/>
+      <c r="G4" s="105">
+        <v>1</v>
+      </c>
+      <c r="H4" s="105">
+        <v>2</v>
+      </c>
+      <c r="I4" s="105">
+        <v>3</v>
+      </c>
+      <c r="J4" s="105">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="103">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S4" s="103">
+        <v>30</v>
+      </c>
+      <c r="W4" t="s">
+        <v>145</v>
+      </c>
+      <c r="X4" s="103">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F5" s="105" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="108">
+        <v>100</v>
+      </c>
+      <c r="H5" s="108">
+        <v>200</v>
+      </c>
+      <c r="I5" s="108">
+        <v>300</v>
+      </c>
+      <c r="J5" s="108">
+        <v>400</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" s="103">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>124</v>
+      </c>
+      <c r="S5" s="103">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>124</v>
+      </c>
+      <c r="X5" s="103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F6" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="108">
+        <v>100</v>
+      </c>
+      <c r="H6" s="108">
+        <v>125</v>
+      </c>
+      <c r="I6" s="108">
+        <v>150</v>
+      </c>
+      <c r="J6" s="108">
+        <v>200</v>
+      </c>
+      <c r="M6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="103">
+        <v>100</v>
+      </c>
+      <c r="R6" t="s">
+        <v>125</v>
+      </c>
+      <c r="S6" s="103">
+        <v>100</v>
+      </c>
+      <c r="W6" t="s">
+        <v>125</v>
+      </c>
+      <c r="X6" s="103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F7" s="105" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="M7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N7">
+        <f>ROUND((N6-N5)/N4,1)</f>
+        <v>3.3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>138</v>
+      </c>
+      <c r="S7">
+        <f>ROUND((S6-S5)/S4,1)</f>
+        <v>3.3</v>
+      </c>
+      <c r="W7" t="s">
+        <v>138</v>
+      </c>
+      <c r="X7">
+        <f>ROUND((X6-X5)/X4,1)</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="103">
+        <v>1</v>
+      </c>
+      <c r="L11" s="104" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="109" t="s">
+        <v>140</v>
+      </c>
+      <c r="N11" s="109" t="s">
+        <v>141</v>
+      </c>
+      <c r="O11" s="109" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="5:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="104" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12">
+        <f>G5</f>
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <f>G5+G5*(N6/100)</f>
+        <v>200</v>
+      </c>
+      <c r="O12">
+        <f>N12-M12</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="5:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="103">
+        <v>0</v>
+      </c>
+      <c r="I13" s="110" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="111">
+        <f ca="1">INDIRECT(ADDRESS(5,6+G11)) + (INDIRECT(ADDRESS(5,6+G11)) *(N7/100) *G13)</f>
+        <v>100</v>
+      </c>
+      <c r="L13" s="104" t="s">
+        <v>142</v>
+      </c>
+      <c r="M13">
+        <f>H5</f>
+        <v>200</v>
+      </c>
+      <c r="N13">
+        <f>H5+H5*(N6/100)</f>
+        <v>400</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13:O15" si="0">N13-M13</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="103">
+        <v>0</v>
+      </c>
+      <c r="L14" s="104" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14">
+        <f>I5</f>
+        <v>300</v>
+      </c>
+      <c r="N14">
+        <f>I5+I5*(N6/100)</f>
+        <v>600</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="103">
+        <v>0</v>
+      </c>
+      <c r="L15" s="104" t="s">
+        <v>144</v>
+      </c>
+      <c r="M15">
+        <f>J5</f>
+        <v>400</v>
+      </c>
+      <c r="N15">
+        <f>J5+J5*(N6/100)</f>
+        <v>800</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G3:J3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G13:G15">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>G13&gt;$N$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G$11&gt;4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WIP special dragons stats
Former-commit-id: 87103b6095a855f813b2ce0d74f7b2737c20bf7c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="156">
   <si>
     <t>[sku]</t>
   </si>
@@ -88,9 +88,6 @@
     <t>PF_DragonFatMenu</t>
   </si>
   <si>
-    <t>PF_DragonFat</t>
-  </si>
-  <si>
     <t>tier_1</t>
   </si>
   <si>
@@ -100,21 +97,12 @@
     <t>PF_DragonReptileMenu</t>
   </si>
   <si>
-    <t>PF_DragonReptile</t>
-  </si>
-  <si>
     <t>PF_DragonCrocodileMenu</t>
   </si>
   <si>
-    <t>PF_DragonCrocodile</t>
-  </si>
-  <si>
     <t>PF_DragonBabyMenu</t>
   </si>
   <si>
-    <t>PF_DragonBaby</t>
-  </si>
-  <si>
     <t>[dotAnimationThreshold]</t>
   </si>
   <si>
@@ -503,6 +491,9 @@
   </si>
   <si>
     <t>Electric</t>
+  </si>
+  <si>
+    <t>PF_DragonElectric</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1467,6 +1458,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1506,40 +1533,10 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9828,7 +9825,7 @@
   <dimension ref="A1:BB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9901,7 +9898,7 @@
   <sheetData>
     <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -9931,58 +9928,58 @@
     </row>
     <row r="3" spans="1:54" ht="147" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E3" s="57" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="80" t="s">
+      <c r="L3" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="M3" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="80" t="s">
+      <c r="N3" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="77" t="s">
+      <c r="O3" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="77" t="s">
+      <c r="P3" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="77" t="s">
+      <c r="Q3" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="79" t="s">
+      <c r="R3" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="79" t="s">
+      <c r="S3" s="78" t="s">
         <v>89</v>
-      </c>
-      <c r="P3" s="79" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q3" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="78" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="78" t="s">
-        <v>93</v>
       </c>
       <c r="T3" s="68" t="s">
         <v>1</v>
@@ -9993,10 +9990,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E4" s="61">
         <v>0</v>
@@ -10028,10 +10025,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" s="61">
         <v>1</v>
@@ -10087,10 +10084,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E6" s="61">
         <v>2</v>
@@ -10178,7 +10175,7 @@
     <row r="9" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -10237,7 +10234,7 @@
     </row>
     <row r="12" spans="1:54" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
@@ -10246,76 +10243,76 @@
         <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="K12" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="AB12" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AC12" s="23" t="s">
         <v>10</v>
@@ -10324,37 +10321,37 @@
         <v>11</v>
       </c>
       <c r="AE12" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AF12" s="22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AG12" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AH12" s="22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AI12" s="22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AJ12" s="22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AK12" s="22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AL12" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AM12" s="22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AN12" s="22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AO12" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AP12" s="27" t="s">
         <v>3</v>
@@ -10363,34 +10360,34 @@
         <v>9</v>
       </c>
       <c r="AR12" s="28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AS12" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AT12" s="25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AU12" s="24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV12" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AW12" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AX12" s="24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AY12" s="24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AZ12" s="21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="BA12" s="21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="BB12" s="24" t="s">
         <v>1</v>
@@ -10401,16 +10398,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="37">
         <v>0</v>
@@ -10468,13 +10465,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F14" s="36" t="s">
         <v>18</v>
@@ -10535,13 +10532,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F15" s="36" t="s">
         <v>17</v>
@@ -10603,13 +10600,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F16" s="36" t="s">
         <v>16</v>
@@ -10670,45 +10667,45 @@
         <v>2</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="37">
         <v>0</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="144">
         <v>5</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="121">
         <v>-2</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="145">
         <v>100</v>
       </c>
-      <c r="K17" s="132">
+      <c r="K17" s="119">
         <v>1.5</v>
       </c>
-      <c r="L17" s="132">
+      <c r="L17" s="119">
         <v>0</v>
       </c>
-      <c r="M17" s="132">
+      <c r="M17" s="119">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N17" s="132">
+      <c r="N17" s="119">
         <v>30</v>
       </c>
-      <c r="O17" s="132">
+      <c r="O17" s="119">
         <v>0.5</v>
       </c>
-      <c r="P17" s="43">
+      <c r="P17" s="123">
         <v>1</v>
       </c>
       <c r="Q17" s="39">
@@ -10717,77 +10714,77 @@
       <c r="R17" s="41">
         <v>100</v>
       </c>
-      <c r="S17" s="132">
+      <c r="S17" s="119">
         <v>40</v>
       </c>
-      <c r="T17" s="133">
+      <c r="T17" s="120">
         <v>28</v>
       </c>
-      <c r="U17" s="134">
+      <c r="U17" s="121">
         <v>9</v>
       </c>
-      <c r="V17" s="132">
+      <c r="V17" s="119">
         <v>3</v>
       </c>
-      <c r="W17" s="132">
+      <c r="W17" s="119">
         <v>9</v>
       </c>
-      <c r="X17" s="133">
+      <c r="X17" s="120">
         <v>8000</v>
       </c>
-      <c r="Y17" s="135">
+      <c r="Y17" s="122">
         <v>2</v>
       </c>
-      <c r="Z17" s="136">
+      <c r="Z17" s="123">
         <v>0.13</v>
       </c>
-      <c r="AA17" s="136">
+      <c r="AA17" s="123">
         <v>0</v>
       </c>
-      <c r="AB17" s="135">
+      <c r="AB17" s="122">
         <v>6</v>
       </c>
-      <c r="AC17" s="143" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD17" s="137" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE17" s="137" t="s">
-        <v>27</v>
+      <c r="AC17" s="130" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD17" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE17" s="124" t="s">
+        <v>24</v>
       </c>
       <c r="AF17" s="50"/>
       <c r="AG17" s="50"/>
-      <c r="AH17" s="137">
+      <c r="AH17" s="124">
         <v>4.0999999999999996</v>
       </c>
-      <c r="AI17" s="137">
+      <c r="AI17" s="124">
         <v>2</v>
       </c>
-      <c r="AJ17" s="137">
+      <c r="AJ17" s="124">
         <v>2</v>
       </c>
-      <c r="AK17" s="137" t="b">
+      <c r="AK17" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AL17" s="137" t="b">
+      <c r="AL17" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AM17" s="137" t="b">
+      <c r="AM17" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AN17" s="137">
+      <c r="AN17" s="124">
         <v>10</v>
       </c>
-      <c r="AO17" s="138">
+      <c r="AO17" s="125">
         <v>0.55999999999999994</v>
       </c>
       <c r="AP17" s="51"/>
       <c r="AQ17" s="52"/>
-      <c r="AR17" s="139">
+      <c r="AR17" s="126">
         <v>2E-3</v>
       </c>
-      <c r="AS17" s="140">
+      <c r="AS17" s="127">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT17" s="55">
@@ -10799,22 +10796,22 @@
       <c r="AV17" s="31">
         <v>9.5</v>
       </c>
-      <c r="AW17" s="141">
+      <c r="AW17" s="128">
         <v>1.7</v>
       </c>
-      <c r="AX17" s="142">
+      <c r="AX17" s="129">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AY17" s="142">
+      <c r="AY17" s="129">
         <v>2.25</v>
       </c>
-      <c r="AZ17" s="142">
+      <c r="AZ17" s="129">
         <v>0</v>
       </c>
-      <c r="BA17" s="142">
+      <c r="BA17" s="129">
         <v>8</v>
       </c>
-      <c r="BB17" s="141" t="s">
+      <c r="BB17" s="128" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10823,13 +10820,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F18" s="36" t="s">
         <v>18</v>
@@ -10837,31 +10834,31 @@
       <c r="G18" s="37">
         <v>10</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="144">
         <v>10</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="121">
         <v>0</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="145">
         <v>150</v>
       </c>
-      <c r="K18" s="132">
+      <c r="K18" s="119">
         <v>1.9</v>
       </c>
-      <c r="L18" s="132">
+      <c r="L18" s="119">
         <v>0</v>
       </c>
-      <c r="M18" s="132">
+      <c r="M18" s="119">
         <v>1.2E-2</v>
       </c>
-      <c r="N18" s="132">
+      <c r="N18" s="119">
         <v>30</v>
       </c>
-      <c r="O18" s="132">
+      <c r="O18" s="119">
         <v>0.6</v>
       </c>
-      <c r="P18" s="43">
+      <c r="P18" s="123">
         <v>1.1499999999999999</v>
       </c>
       <c r="Q18" s="39">
@@ -10870,77 +10867,77 @@
       <c r="R18" s="41">
         <v>120</v>
       </c>
-      <c r="S18" s="132">
+      <c r="S18" s="119">
         <v>40</v>
       </c>
-      <c r="T18" s="133">
+      <c r="T18" s="120">
         <v>28</v>
       </c>
-      <c r="U18" s="134">
+      <c r="U18" s="121">
         <v>11</v>
       </c>
-      <c r="V18" s="132">
+      <c r="V18" s="119">
         <v>4</v>
       </c>
-      <c r="W18" s="132">
+      <c r="W18" s="119">
         <v>10</v>
       </c>
-      <c r="X18" s="133">
+      <c r="X18" s="120">
         <v>10000</v>
       </c>
-      <c r="Y18" s="135">
+      <c r="Y18" s="122">
         <v>3</v>
       </c>
-      <c r="Z18" s="136">
+      <c r="Z18" s="123">
         <v>0.08</v>
       </c>
-      <c r="AA18" s="136">
+      <c r="AA18" s="123">
         <v>0</v>
       </c>
-      <c r="AB18" s="135">
+      <c r="AB18" s="122">
         <v>6</v>
       </c>
-      <c r="AC18" s="143" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD18" s="137" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE18" s="137" t="s">
-        <v>25</v>
+      <c r="AC18" s="130" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD18" s="124" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE18" s="124" t="s">
+        <v>23</v>
       </c>
       <c r="AF18" s="50"/>
       <c r="AG18" s="50"/>
-      <c r="AH18" s="137">
+      <c r="AH18" s="124">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AI18" s="137">
+      <c r="AI18" s="124">
         <v>2</v>
       </c>
-      <c r="AJ18" s="137">
+      <c r="AJ18" s="124">
         <v>2</v>
       </c>
-      <c r="AK18" s="137" t="b">
+      <c r="AK18" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AL18" s="137" t="b">
+      <c r="AL18" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AM18" s="137" t="b">
+      <c r="AM18" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AN18" s="137">
+      <c r="AN18" s="124">
         <v>10</v>
       </c>
-      <c r="AO18" s="138">
+      <c r="AO18" s="125">
         <v>0.7</v>
       </c>
       <c r="AP18" s="51"/>
       <c r="AQ18" s="52"/>
-      <c r="AR18" s="139">
+      <c r="AR18" s="126">
         <v>1.8E-3</v>
       </c>
-      <c r="AS18" s="140">
+      <c r="AS18" s="127">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT18" s="55">
@@ -10952,22 +10949,22 @@
       <c r="AV18" s="31">
         <v>9.5</v>
       </c>
-      <c r="AW18" s="141">
+      <c r="AW18" s="128">
         <v>1.7</v>
       </c>
-      <c r="AX18" s="142">
+      <c r="AX18" s="129">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AY18" s="142">
+      <c r="AY18" s="129">
         <v>2.25</v>
       </c>
-      <c r="AZ18" s="142">
+      <c r="AZ18" s="129">
         <v>9</v>
       </c>
-      <c r="BA18" s="142">
+      <c r="BA18" s="129">
         <v>8</v>
       </c>
-      <c r="BB18" s="141" t="s">
+      <c r="BB18" s="128" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10976,13 +10973,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="36" t="s">
         <v>17</v>
@@ -10990,31 +10987,31 @@
       <c r="G19" s="37">
         <v>20</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="144">
         <v>15</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="121">
         <v>0</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="145">
         <v>200</v>
       </c>
-      <c r="K19" s="132">
+      <c r="K19" s="119">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L19" s="132">
+      <c r="L19" s="119">
         <v>0</v>
       </c>
-      <c r="M19" s="132">
+      <c r="M19" s="119">
         <v>1.4E-2</v>
       </c>
-      <c r="N19" s="132">
+      <c r="N19" s="119">
         <v>25</v>
       </c>
-      <c r="O19" s="132">
+      <c r="O19" s="119">
         <v>0.7</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="123">
         <v>1.75</v>
       </c>
       <c r="Q19" s="39">
@@ -11023,77 +11020,77 @@
       <c r="R19" s="41">
         <v>140</v>
       </c>
-      <c r="S19" s="132">
+      <c r="S19" s="119">
         <v>40</v>
       </c>
-      <c r="T19" s="133">
+      <c r="T19" s="120">
         <v>28</v>
       </c>
-      <c r="U19" s="134">
+      <c r="U19" s="121">
         <v>11.5</v>
       </c>
-      <c r="V19" s="132">
+      <c r="V19" s="119">
         <v>5</v>
       </c>
-      <c r="W19" s="132">
+      <c r="W19" s="119">
         <v>10</v>
       </c>
-      <c r="X19" s="133">
+      <c r="X19" s="120">
         <v>20000</v>
       </c>
-      <c r="Y19" s="135">
+      <c r="Y19" s="122">
         <v>4</v>
       </c>
-      <c r="Z19" s="136">
+      <c r="Z19" s="123">
         <v>0.05</v>
       </c>
-      <c r="AA19" s="136">
+      <c r="AA19" s="123">
         <v>0</v>
       </c>
-      <c r="AB19" s="135">
+      <c r="AB19" s="122">
         <v>6</v>
       </c>
-      <c r="AC19" s="143" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD19" s="137" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE19" s="137" t="s">
+      <c r="AC19" s="130" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD19" s="124" t="s">
         <v>22</v>
+      </c>
+      <c r="AE19" s="124" t="s">
+        <v>21</v>
       </c>
       <c r="AF19" s="50"/>
       <c r="AG19" s="50"/>
-      <c r="AH19" s="137">
+      <c r="AH19" s="124">
         <v>2.1</v>
       </c>
-      <c r="AI19" s="137">
+      <c r="AI19" s="124">
         <v>2</v>
       </c>
-      <c r="AJ19" s="137">
+      <c r="AJ19" s="124">
         <v>2</v>
       </c>
-      <c r="AK19" s="137" t="b">
+      <c r="AK19" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AL19" s="137" t="b">
+      <c r="AL19" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AM19" s="137" t="b">
+      <c r="AM19" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AN19" s="137">
+      <c r="AN19" s="124">
         <v>10</v>
       </c>
-      <c r="AO19" s="138">
+      <c r="AO19" s="125">
         <v>0.7</v>
       </c>
       <c r="AP19" s="51"/>
       <c r="AQ19" s="52"/>
-      <c r="AR19" s="139">
+      <c r="AR19" s="126">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AS19" s="140">
+      <c r="AS19" s="127">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT19" s="55">
@@ -11105,22 +11102,22 @@
       <c r="AV19" s="31">
         <v>9.5</v>
       </c>
-      <c r="AW19" s="141">
+      <c r="AW19" s="128">
         <v>1.7</v>
       </c>
-      <c r="AX19" s="142">
+      <c r="AX19" s="129">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AY19" s="142">
+      <c r="AY19" s="129">
         <v>2.25</v>
       </c>
-      <c r="AZ19" s="142">
+      <c r="AZ19" s="129">
         <v>45</v>
       </c>
-      <c r="BA19" s="142">
+      <c r="BA19" s="129">
         <v>15</v>
       </c>
-      <c r="BB19" s="141" t="s">
+      <c r="BB19" s="128" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11129,13 +11126,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F20" s="36" t="s">
         <v>16</v>
@@ -11143,31 +11140,31 @@
       <c r="G20" s="37">
         <v>30</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="144">
         <v>25</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="121">
         <v>0</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J20" s="145">
         <v>250</v>
       </c>
-      <c r="K20" s="132">
+      <c r="K20" s="119">
         <v>2.4</v>
       </c>
-      <c r="L20" s="132">
+      <c r="L20" s="119">
         <v>0</v>
       </c>
-      <c r="M20" s="132">
+      <c r="M20" s="119">
         <v>1.6E-2</v>
       </c>
-      <c r="N20" s="132">
+      <c r="N20" s="119">
         <v>20</v>
       </c>
-      <c r="O20" s="132">
+      <c r="O20" s="119">
         <v>0.8</v>
       </c>
-      <c r="P20" s="43">
+      <c r="P20" s="123">
         <v>2.1</v>
       </c>
       <c r="Q20" s="39">
@@ -11176,77 +11173,77 @@
       <c r="R20" s="41">
         <v>160</v>
       </c>
-      <c r="S20" s="132">
+      <c r="S20" s="119">
         <v>40</v>
       </c>
-      <c r="T20" s="133">
+      <c r="T20" s="120">
         <v>28</v>
       </c>
-      <c r="U20" s="134">
+      <c r="U20" s="121">
         <v>12</v>
       </c>
-      <c r="V20" s="132">
+      <c r="V20" s="119">
         <v>6</v>
       </c>
-      <c r="W20" s="132">
+      <c r="W20" s="119">
         <v>10</v>
       </c>
-      <c r="X20" s="133">
+      <c r="X20" s="120">
         <v>30000</v>
       </c>
-      <c r="Y20" s="135">
+      <c r="Y20" s="122">
         <v>5</v>
       </c>
-      <c r="Z20" s="136">
+      <c r="Z20" s="123">
         <v>0.04</v>
       </c>
-      <c r="AA20" s="136">
+      <c r="AA20" s="123">
         <v>0</v>
       </c>
-      <c r="AB20" s="135">
+      <c r="AB20" s="122">
         <v>6</v>
       </c>
-      <c r="AC20" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD20" s="137" t="s">
+      <c r="AC20" s="130" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD20" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="AE20" s="137" t="s">
+      <c r="AE20" s="124" t="s">
         <v>19</v>
       </c>
       <c r="AF20" s="50"/>
       <c r="AG20" s="50"/>
-      <c r="AH20" s="137">
+      <c r="AH20" s="124">
         <v>2.1</v>
       </c>
-      <c r="AI20" s="137">
+      <c r="AI20" s="124">
         <v>2</v>
       </c>
-      <c r="AJ20" s="137">
+      <c r="AJ20" s="124">
         <v>2</v>
       </c>
-      <c r="AK20" s="137" t="b">
+      <c r="AK20" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AL20" s="137" t="b">
+      <c r="AL20" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AM20" s="137" t="b">
+      <c r="AM20" s="124" t="b">
         <v>1</v>
       </c>
-      <c r="AN20" s="137">
+      <c r="AN20" s="124">
         <v>10</v>
       </c>
-      <c r="AO20" s="138">
+      <c r="AO20" s="125">
         <v>0.7</v>
       </c>
       <c r="AP20" s="51"/>
       <c r="AQ20" s="52"/>
-      <c r="AR20" s="139">
+      <c r="AR20" s="126">
         <v>1.5E-3</v>
       </c>
-      <c r="AS20" s="140">
+      <c r="AS20" s="127">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT20" s="55">
@@ -11258,22 +11255,22 @@
       <c r="AV20" s="31">
         <v>9.5</v>
       </c>
-      <c r="AW20" s="141">
+      <c r="AW20" s="128">
         <v>1.7</v>
       </c>
-      <c r="AX20" s="142">
+      <c r="AX20" s="129">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AY20" s="142">
+      <c r="AY20" s="129">
         <v>2.25</v>
       </c>
-      <c r="AZ20" s="142">
+      <c r="AZ20" s="129">
         <v>59</v>
       </c>
-      <c r="BA20" s="142">
+      <c r="BA20" s="129">
         <v>15</v>
       </c>
-      <c r="BB20" s="141" t="s">
+      <c r="BB20" s="128" t="s">
         <v>7</v>
       </c>
     </row>
@@ -11282,16 +11279,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="37">
         <v>0</v>
@@ -11349,13 +11346,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F22" s="36" t="s">
         <v>18</v>
@@ -11416,13 +11413,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F23" s="36" t="s">
         <v>17</v>
@@ -11484,13 +11481,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F24" s="36" t="s">
         <v>16</v>
@@ -11553,49 +11550,49 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="126" t="s">
+      <c r="H25" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="127"/>
-      <c r="J25" s="128" t="s">
+      <c r="I25" s="139"/>
+      <c r="J25" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="129"/>
-      <c r="L25" s="129"/>
-      <c r="M25" s="129"/>
-      <c r="N25" s="129"/>
-      <c r="O25" s="130"/>
+      <c r="K25" s="141"/>
+      <c r="L25" s="141"/>
+      <c r="M25" s="141"/>
+      <c r="N25" s="141"/>
+      <c r="O25" s="142"/>
       <c r="P25" s="99"/>
-      <c r="Q25" s="122" t="s">
-        <v>149</v>
-      </c>
-      <c r="R25" s="123"/>
-      <c r="S25" s="123"/>
-      <c r="T25" s="123"/>
-      <c r="U25" s="124" t="s">
+      <c r="Q25" s="134" t="s">
+        <v>145</v>
+      </c>
+      <c r="R25" s="135"/>
+      <c r="S25" s="135"/>
+      <c r="T25" s="135"/>
+      <c r="U25" s="136" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="125"/>
-      <c r="W25" s="125"/>
-      <c r="X25" s="125"/>
+      <c r="V25" s="137"/>
+      <c r="W25" s="137"/>
+      <c r="X25" s="137"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="119" t="s">
-        <v>150</v>
-      </c>
-      <c r="AI25" s="120"/>
-      <c r="AJ25" s="120"/>
-      <c r="AK25" s="120"/>
-      <c r="AL25" s="120"/>
-      <c r="AM25" s="120"/>
-      <c r="AN25" s="121"/>
+      <c r="AH25" s="131" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI25" s="132"/>
+      <c r="AJ25" s="132"/>
+      <c r="AK25" s="132"/>
+      <c r="AL25" s="132"/>
+      <c r="AM25" s="132"/>
+      <c r="AN25" s="133"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -11608,19 +11605,19 @@
     </row>
     <row r="30" spans="1:54" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F30" s="86" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
@@ -11628,10 +11625,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="83" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D31" s="84" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E31" s="84">
         <v>5</v>
@@ -11646,10 +11643,10 @@
         <v>2</v>
       </c>
       <c r="C32" s="83" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D32" s="84" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E32" s="84">
         <v>15</v>
@@ -11664,10 +11661,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="83" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D33" s="84" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E33" s="84">
         <v>25</v>
@@ -11682,10 +11679,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="83" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D34" s="84" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E34" s="84">
         <v>5</v>
@@ -11700,10 +11697,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="83" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D35" s="84" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E35" s="84">
         <v>15</v>
@@ -11718,10 +11715,10 @@
         <v>2</v>
       </c>
       <c r="C36" s="83" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D36" s="84" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" s="84">
         <v>25</v>
@@ -11736,10 +11733,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="83" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D37" s="84" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E37" s="84">
         <v>5</v>
@@ -11754,10 +11751,10 @@
         <v>2</v>
       </c>
       <c r="C38" s="83" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D38" s="84" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E38" s="84">
         <v>15</v>
@@ -11772,10 +11769,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="87" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D39" s="88" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E39" s="88">
         <v>25</v>
@@ -11846,7 +11843,7 @@
   <dimension ref="C1:AC63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11863,25 +11860,25 @@
   <sheetData>
     <row r="1" spans="3:29" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="92" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="90"/>
-      <c r="E3" s="131" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
+      <c r="E3" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
       <c r="J3" s="90" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="R3" s="90" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Z3" s="90" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="3:29" x14ac:dyDescent="0.25">
@@ -11899,19 +11896,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="L4" s="89">
         <v>30</v>
       </c>
       <c r="S4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="T4" s="89">
         <v>30</v>
       </c>
       <c r="AA4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="AB4" s="89">
         <v>30</v>
@@ -11919,7 +11916,7 @@
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D5" s="91" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E5" s="93">
         <v>100</v>
@@ -11934,19 +11931,19 @@
         <v>250</v>
       </c>
       <c r="K5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L5" s="89">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="T5" s="89">
         <v>0</v>
       </c>
       <c r="AA5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AB5" s="89">
         <v>0</v>
@@ -11954,7 +11951,7 @@
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D6" s="91" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E6" s="93">
         <v>100</v>
@@ -11969,19 +11966,19 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L6" s="89">
         <v>100</v>
       </c>
       <c r="S6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="T6" s="89">
         <v>50</v>
       </c>
       <c r="AA6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AB6" s="89">
         <v>50</v>
@@ -11989,7 +11986,7 @@
     </row>
     <row r="7" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="102" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E7" s="103">
         <v>240</v>
@@ -12004,21 +12001,21 @@
         <v>270</v>
       </c>
       <c r="K7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>3.3</v>
       </c>
       <c r="S7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>1.7</v>
       </c>
       <c r="AA7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
@@ -12027,7 +12024,7 @@
     </row>
     <row r="8" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="106" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E8" s="104">
         <v>0</v>
@@ -12046,7 +12043,7 @@
     <row r="11" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C11" s="107"/>
       <c r="D11" s="108" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E11" s="109">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -12056,46 +12053,46 @@
       <c r="G11" s="109"/>
       <c r="H11" s="110"/>
       <c r="J11" s="90" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K11" s="94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L11" s="94" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M11" s="94" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N11" s="94"/>
       <c r="O11" s="94"/>
       <c r="P11" s="94"/>
       <c r="R11" s="97" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S11" s="94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="T11" s="94" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="U11" s="94" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="V11" s="94"/>
       <c r="W11" s="94"/>
       <c r="X11" s="94"/>
       <c r="Z11" s="90" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AA11" s="94" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AB11" s="94" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AC11" s="94" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12106,7 +12103,7 @@
       <c r="G12" s="112"/>
       <c r="H12" s="98"/>
       <c r="J12" s="90" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -12121,7 +12118,7 @@
         <v>100</v>
       </c>
       <c r="R12" s="90" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -12136,7 +12133,7 @@
         <v>50</v>
       </c>
       <c r="Z12" s="90" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AV17)/'special dragons'!AU17,1)</f>
@@ -12153,24 +12150,24 @@
     </row>
     <row r="13" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="111" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D13" s="112" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E13" s="113">
         <v>0</v>
       </c>
       <c r="F13" s="112"/>
       <c r="G13" s="95" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H13" s="96">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>100</v>
       </c>
       <c r="J13" s="90" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -12185,7 +12182,7 @@
         <v>150</v>
       </c>
       <c r="R13" s="90" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -12200,7 +12197,7 @@
         <v>60</v>
       </c>
       <c r="Z13" s="90" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AV18)/'special dragons'!AU18,1)</f>
@@ -12217,24 +12214,24 @@
     </row>
     <row r="14" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="111" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D14" s="112" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E14" s="113">
         <v>0</v>
       </c>
       <c r="F14" s="112"/>
       <c r="G14" s="95" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H14" s="96">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>100</v>
       </c>
       <c r="J14" s="90" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -12249,7 +12246,7 @@
         <v>200</v>
       </c>
       <c r="R14" s="90" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -12264,7 +12261,7 @@
         <v>70</v>
       </c>
       <c r="Z14" s="90" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AV19)/'special dragons'!AU19,1)</f>
@@ -12281,24 +12278,24 @@
     </row>
     <row r="15" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="111" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D15" s="112" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E15" s="113">
         <v>0</v>
       </c>
       <c r="F15" s="112"/>
       <c r="G15" s="95" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H15" s="96">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
         <v>10.1</v>
       </c>
       <c r="J15" s="90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -12313,7 +12310,7 @@
         <v>250</v>
       </c>
       <c r="R15" s="90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -12328,7 +12325,7 @@
         <v>80</v>
       </c>
       <c r="Z15" s="90" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AV20)/'special dragons'!AU20,1)</f>
@@ -12346,7 +12343,7 @@
     <row r="16" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C16" s="111"/>
       <c r="D16" s="118" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E16" s="118">
         <f>SUM(E13:E15)</f>
@@ -12762,18 +12759,18 @@
   <sheetData>
     <row r="4" spans="6:9" x14ac:dyDescent="0.25">
       <c r="G4" s="117" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H4" s="117" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I4" s="117" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -12787,7 +12784,7 @@
     </row>
     <row r="6" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G6">
         <v>240</v>
@@ -12801,7 +12798,7 @@
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G7">
         <v>365</v>
@@ -12815,7 +12812,7 @@
     </row>
     <row r="8" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G8">
         <v>410</v>
@@ -12829,7 +12826,7 @@
     </row>
     <row r="9" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G9">
         <f ca="1">tools!H13</f>

</xml_diff>

<commit_message>
WIP fixing alcohol drain
Former-commit-id: 38e582658ba3b40cbe2ddfe4b5e86aeb9f43d404
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5166,7 +5166,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>299</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5475,7 +5475,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>151.9</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5784,7 +5784,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.3</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9827,8 +9827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10745,7 +10745,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="122">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AC17" s="130" t="s">
         <v>155</v>
@@ -10898,7 +10898,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="122">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AC18" s="130" t="s">
         <v>155</v>
@@ -11051,7 +11051,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="122">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AC19" s="130" t="s">
         <v>155</v>
@@ -11204,7 +11204,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="122">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AC20" s="130" t="s">
         <v>155</v>
@@ -11846,7 +11846,7 @@
   <dimension ref="C1:AC63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12077,7 +12077,7 @@
       </c>
       <c r="E11" s="109">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="109"/>
       <c r="G11" s="109"/>
@@ -12186,7 +12186,7 @@
         <v>124</v>
       </c>
       <c r="E13" s="113">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F13" s="112"/>
       <c r="G13" s="95" t="s">
@@ -12194,7 +12194,7 @@
       </c>
       <c r="H13" s="96">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>299</v>
+        <v>100</v>
       </c>
       <c r="J13" s="90" t="s">
         <v>135</v>
@@ -12250,7 +12250,7 @@
         <v>126</v>
       </c>
       <c r="E14" s="113">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F14" s="112"/>
       <c r="G14" s="95" t="s">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="H14" s="96">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>151.9</v>
+        <v>100</v>
       </c>
       <c r="J14" s="90" t="s">
         <v>136</v>
@@ -12314,7 +12314,7 @@
         <v>127</v>
       </c>
       <c r="E15" s="113">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F15" s="112"/>
       <c r="G15" s="95" t="s">
@@ -12322,7 +12322,7 @@
       </c>
       <c r="H15" s="96">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
-        <v>12.3</v>
+        <v>10.1</v>
       </c>
       <c r="J15" s="90" t="s">
         <v>137</v>
@@ -12377,7 +12377,7 @@
       </c>
       <c r="E16" s="118">
         <f>SUM(E13:E15)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F16" s="112"/>
       <c r="G16" s="112"/>
@@ -12860,15 +12860,15 @@
       </c>
       <c r="G9">
         <f ca="1">tools!H13</f>
-        <v>299</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <f ca="1">tools!H14</f>
-        <v>151.9</v>
+        <v>100</v>
       </c>
       <c r="I9">
         <f ca="1">tools!H15</f>
-        <v>12.3</v>
+        <v>10.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP special dragons data
Former-commit-id: 3f044be56e928a780013efbf53cf4434bc003e0e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -1500,9 +1500,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1541,6 +1538,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5691,7 +5691,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9827,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+    <sheetView topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10690,7 +10689,7 @@
       <c r="I17" s="121">
         <v>-2</v>
       </c>
-      <c r="J17" s="132">
+      <c r="J17" s="145">
         <v>100</v>
       </c>
       <c r="K17" s="119">
@@ -10843,7 +10842,7 @@
       <c r="I18" s="121">
         <v>0</v>
       </c>
-      <c r="J18" s="132">
+      <c r="J18" s="145">
         <v>150</v>
       </c>
       <c r="K18" s="119">
@@ -10996,7 +10995,7 @@
       <c r="I19" s="121">
         <v>0</v>
       </c>
-      <c r="J19" s="132">
+      <c r="J19" s="145">
         <v>200</v>
       </c>
       <c r="K19" s="119">
@@ -11149,7 +11148,7 @@
       <c r="I20" s="121">
         <v>0</v>
       </c>
-      <c r="J20" s="132">
+      <c r="J20" s="145">
         <v>250</v>
       </c>
       <c r="K20" s="119">
@@ -11553,44 +11552,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="140" t="s">
+      <c r="H25" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="141"/>
-      <c r="J25" s="142" t="s">
+      <c r="I25" s="140"/>
+      <c r="J25" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="143"/>
-      <c r="L25" s="143"/>
-      <c r="M25" s="143"/>
-      <c r="N25" s="143"/>
-      <c r="O25" s="144"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="142"/>
+      <c r="M25" s="142"/>
+      <c r="N25" s="142"/>
+      <c r="O25" s="143"/>
       <c r="P25" s="99"/>
-      <c r="Q25" s="136" t="s">
+      <c r="Q25" s="135" t="s">
         <v>145</v>
       </c>
-      <c r="R25" s="137"/>
-      <c r="S25" s="137"/>
-      <c r="T25" s="137"/>
-      <c r="U25" s="138" t="s">
+      <c r="R25" s="136"/>
+      <c r="S25" s="136"/>
+      <c r="T25" s="136"/>
+      <c r="U25" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="139"/>
-      <c r="W25" s="139"/>
-      <c r="X25" s="139"/>
+      <c r="V25" s="138"/>
+      <c r="W25" s="138"/>
+      <c r="X25" s="138"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="133" t="s">
+      <c r="AH25" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="AI25" s="134"/>
-      <c r="AJ25" s="134"/>
-      <c r="AK25" s="134"/>
-      <c r="AL25" s="134"/>
-      <c r="AM25" s="134"/>
-      <c r="AN25" s="135"/>
+      <c r="AI25" s="133"/>
+      <c r="AJ25" s="133"/>
+      <c r="AK25" s="133"/>
+      <c r="AL25" s="133"/>
+      <c r="AM25" s="133"/>
+      <c r="AN25" s="134"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
@@ -11845,8 +11844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11868,12 +11867,12 @@
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="90"/>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
       <c r="J3" s="90" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
WIP setting electric dragon stats
Former-commit-id: 2c649bbc9528529bee6fad4e129bb91e0327a9f6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -1500,6 +1500,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1538,9 +1541,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5166,7 +5166,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>497.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5475,7 +5475,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>241.60000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5783,7 +5783,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.1</c:v>
+                  <c:v>18.100000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9826,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10689,7 +10689,7 @@
       <c r="I17" s="121">
         <v>-2</v>
       </c>
-      <c r="J17" s="145">
+      <c r="J17" s="132">
         <v>100</v>
       </c>
       <c r="K17" s="119">
@@ -10717,7 +10717,7 @@
         <v>100</v>
       </c>
       <c r="S17" s="119">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="T17" s="120">
         <v>30</v>
@@ -10842,7 +10842,7 @@
       <c r="I18" s="121">
         <v>0</v>
       </c>
-      <c r="J18" s="145">
+      <c r="J18" s="132">
         <v>150</v>
       </c>
       <c r="K18" s="119">
@@ -10870,7 +10870,7 @@
         <v>120</v>
       </c>
       <c r="S18" s="119">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="T18" s="120">
         <v>30</v>
@@ -10995,7 +10995,7 @@
       <c r="I19" s="121">
         <v>0</v>
       </c>
-      <c r="J19" s="145">
+      <c r="J19" s="132">
         <v>200</v>
       </c>
       <c r="K19" s="119">
@@ -11023,7 +11023,7 @@
         <v>140</v>
       </c>
       <c r="S19" s="119">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="T19" s="120">
         <v>30</v>
@@ -11148,7 +11148,7 @@
       <c r="I20" s="121">
         <v>0</v>
       </c>
-      <c r="J20" s="145">
+      <c r="J20" s="132">
         <v>250</v>
       </c>
       <c r="K20" s="119">
@@ -11176,7 +11176,7 @@
         <v>160</v>
       </c>
       <c r="S20" s="119">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="T20" s="120">
         <v>30</v>
@@ -11552,44 +11552,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="139" t="s">
+      <c r="H25" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="140"/>
-      <c r="J25" s="141" t="s">
+      <c r="I25" s="141"/>
+      <c r="J25" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="142"/>
-      <c r="L25" s="142"/>
-      <c r="M25" s="142"/>
-      <c r="N25" s="142"/>
-      <c r="O25" s="143"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="143"/>
+      <c r="M25" s="143"/>
+      <c r="N25" s="143"/>
+      <c r="O25" s="144"/>
       <c r="P25" s="99"/>
-      <c r="Q25" s="135" t="s">
+      <c r="Q25" s="136" t="s">
         <v>145</v>
       </c>
-      <c r="R25" s="136"/>
-      <c r="S25" s="136"/>
-      <c r="T25" s="136"/>
-      <c r="U25" s="137" t="s">
+      <c r="R25" s="137"/>
+      <c r="S25" s="137"/>
+      <c r="T25" s="137"/>
+      <c r="U25" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="138"/>
-      <c r="W25" s="138"/>
-      <c r="X25" s="138"/>
+      <c r="V25" s="139"/>
+      <c r="W25" s="139"/>
+      <c r="X25" s="139"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="132" t="s">
+      <c r="AH25" s="133" t="s">
         <v>146</v>
       </c>
-      <c r="AI25" s="133"/>
-      <c r="AJ25" s="133"/>
-      <c r="AK25" s="133"/>
-      <c r="AL25" s="133"/>
-      <c r="AM25" s="133"/>
-      <c r="AN25" s="134"/>
+      <c r="AI25" s="134"/>
+      <c r="AJ25" s="134"/>
+      <c r="AK25" s="134"/>
+      <c r="AL25" s="134"/>
+      <c r="AM25" s="134"/>
+      <c r="AN25" s="135"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
@@ -11844,8 +11844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11867,12 +11867,12 @@
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="90"/>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="145" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
       <c r="J3" s="90" t="s">
         <v>121</v>
       </c>
@@ -12076,7 +12076,7 @@
       </c>
       <c r="E11" s="109">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11" s="109"/>
       <c r="G11" s="109"/>
@@ -12185,7 +12185,7 @@
         <v>124</v>
       </c>
       <c r="E13" s="113">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F13" s="112"/>
       <c r="G13" s="95" t="s">
@@ -12193,7 +12193,7 @@
       </c>
       <c r="H13" s="96">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>100</v>
+        <v>497.5</v>
       </c>
       <c r="J13" s="90" t="s">
         <v>135</v>
@@ -12249,7 +12249,7 @@
         <v>126</v>
       </c>
       <c r="E14" s="113">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F14" s="112"/>
       <c r="G14" s="95" t="s">
@@ -12257,7 +12257,7 @@
       </c>
       <c r="H14" s="96">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>100</v>
+        <v>241.60000000000002</v>
       </c>
       <c r="J14" s="90" t="s">
         <v>136</v>
@@ -12313,7 +12313,7 @@
         <v>127</v>
       </c>
       <c r="E15" s="113">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F15" s="112"/>
       <c r="G15" s="95" t="s">
@@ -12321,7 +12321,7 @@
       </c>
       <c r="H15" s="96">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
-        <v>10.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="J15" s="90" t="s">
         <v>137</v>
@@ -12376,7 +12376,7 @@
       </c>
       <c r="E16" s="118">
         <f>SUM(E13:E15)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16" s="112"/>
       <c r="G16" s="112"/>
@@ -12859,15 +12859,15 @@
       </c>
       <c r="G9">
         <f ca="1">tools!H13</f>
-        <v>100</v>
+        <v>497.5</v>
       </c>
       <c r="H9">
         <f ca="1">tools!H14</f>
-        <v>100</v>
+        <v>241.60000000000002</v>
       </c>
       <c r="I9">
         <f ca="1">tools!H15</f>
-        <v>10.1</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP electric dragon stats
Former-commit-id: 9ac8d3bdd3095433b635a7fd67fa6ba292f9942b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9827,7 +9827,7 @@
   <dimension ref="A1:BB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10711,16 +10711,16 @@
         <v>0.6</v>
       </c>
       <c r="Q17" s="39">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R17" s="41">
         <v>100</v>
       </c>
       <c r="S17" s="119">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T17" s="120">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U17" s="121">
         <v>9</v>
@@ -10864,16 +10864,16 @@
         <v>0.95</v>
       </c>
       <c r="Q18" s="39">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R18" s="41">
         <v>120</v>
       </c>
       <c r="S18" s="119">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T18" s="120">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U18" s="121">
         <v>11</v>
@@ -11017,16 +11017,16 @@
         <v>1.55</v>
       </c>
       <c r="Q19" s="39">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R19" s="41">
         <v>140</v>
       </c>
       <c r="S19" s="119">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T19" s="120">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U19" s="121">
         <v>11.5</v>
@@ -11170,16 +11170,16 @@
         <v>2</v>
       </c>
       <c r="Q20" s="39">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="R20" s="41">
         <v>160</v>
       </c>
       <c r="S20" s="119">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T20" s="120">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U20" s="121">
         <v>12</v>

</xml_diff>

<commit_message>
WIP electric dragon setting stats
Former-commit-id: 411a28c114d5db596ff088e473a0f02a5371f10e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9826,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="P7" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10885,7 +10885,7 @@
         <v>10</v>
       </c>
       <c r="X18" s="120">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="Y18" s="48">
         <v>3</v>
@@ -11038,7 +11038,7 @@
         <v>10</v>
       </c>
       <c r="X19" s="120">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="Y19" s="48">
         <v>4</v>
@@ -11191,7 +11191,7 @@
         <v>10</v>
       </c>
       <c r="X20" s="120">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="Y20" s="48">
         <v>5</v>

</xml_diff>

<commit_message>
WIP electric dragon stats, 1st version
Former-commit-id: 68503d9a6c42654edf7105657d0ed9d5a55d348e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9826,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P7" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" topLeftCell="AQ7" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11158,7 +11158,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="119">
-        <v>1.6E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="N20" s="119">
         <v>20</v>
@@ -11167,7 +11167,7 @@
         <v>0.8</v>
       </c>
       <c r="P20" s="123">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="Q20" s="39">
         <v>1.2</v>
@@ -11845,7 +11845,7 @@
   <dimension ref="C1:AC63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
WIP Helicopter stats added (right now a copy from Electric)
Former-commit-id: 389e06354c18f59aa00cda4dbf8f48dd9adb2dbe
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="158">
   <si>
     <t>[sku]</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>PF_DragonHelicopter</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1494,9 +1497,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1542,11 +1542,37 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
+  <dxfs count="97">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -9456,89 +9482,89 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="83" totalsRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="85" totalsRowBorderDxfId="84">
   <autoFilter ref="B12:BB24"/>
   <tableColumns count="53">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="81"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="80"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="79"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="78"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="77"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="76"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="75"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="74"/>
-    <tableColumn id="10" name="[health]" dataDxfId="73"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="72"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="71"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="70"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="69"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="68"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="67"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="66"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="65"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="64"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="63"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="62"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="61"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="60"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="59"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="58"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="57"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="56"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="55"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="54"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="53"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="52"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="51"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="50"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="49"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="48"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="47"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="46"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="45"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="44"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="43"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="42"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="41"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="40"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="39"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="38"/>
-    <tableColumn id="46" name="[force]" dataDxfId="37"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="36"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="35"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="34"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="33"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="32"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="31"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="30"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="29"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="83"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="82"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="81"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="80"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="79"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="78"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="77"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="76"/>
+    <tableColumn id="10" name="[health]" dataDxfId="75"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="74"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="73"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="72"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="71"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="70"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="69"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="68"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="67"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="66"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="65"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="64"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="63"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="62"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="61"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="60"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="59"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="58"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="57"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="56"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="55"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="54"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="53"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="52"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="51"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="50"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="49"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="48"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="47"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="46"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="45"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="44"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="43"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="42"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="41"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="40"/>
+    <tableColumn id="46" name="[force]" dataDxfId="39"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="38"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="37"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="36"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="35"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="34"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="33"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="32"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
   <autoFilter ref="B3:T6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="24"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="26"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="23"/>
-    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="22"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="21"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="20"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="19"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="18"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="17"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="16"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="15"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="14"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="13"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="12"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="11"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="10"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="9"/>
+    <tableColumn id="5" name="[order]" dataDxfId="25"/>
+    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="24"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="23"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="22"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="21"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="20"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="19"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="18"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="17"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="16"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="15"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="14"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="13"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="12"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="11"/>
     <tableColumn id="65" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9546,14 +9572,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="5"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="3"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="2"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="1">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="7"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="5"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="4"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9826,8 +9852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ7" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AT13" sqref="AT13:AW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10414,53 +10440,139 @@
       <c r="G13" s="37">
         <v>0</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="42"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="48"/>
-      <c r="AC13" s="49"/>
-      <c r="AD13" s="50"/>
-      <c r="AE13" s="50"/>
+      <c r="H13" s="130">
+        <v>3</v>
+      </c>
+      <c r="I13" s="121">
+        <v>-2</v>
+      </c>
+      <c r="J13" s="145">
+        <v>100</v>
+      </c>
+      <c r="K13" s="119">
+        <v>1.5</v>
+      </c>
+      <c r="L13" s="119">
+        <v>0</v>
+      </c>
+      <c r="M13" s="119">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N13" s="119">
+        <v>30</v>
+      </c>
+      <c r="O13" s="119">
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="123">
+        <v>0.6</v>
+      </c>
+      <c r="Q13" s="121">
+        <v>1.2</v>
+      </c>
+      <c r="R13" s="119">
+        <v>100</v>
+      </c>
+      <c r="S13" s="119">
+        <v>25</v>
+      </c>
+      <c r="T13" s="120">
+        <v>35</v>
+      </c>
+      <c r="U13" s="121">
+        <v>9</v>
+      </c>
+      <c r="V13" s="119">
+        <v>3</v>
+      </c>
+      <c r="W13" s="119">
+        <v>9</v>
+      </c>
+      <c r="X13" s="120">
+        <v>8500</v>
+      </c>
+      <c r="Y13" s="122">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="123">
+        <v>0.13</v>
+      </c>
+      <c r="AA13" s="123">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="122">
+        <v>12</v>
+      </c>
+      <c r="AC13" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD13" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE13" s="124" t="s">
+        <v>24</v>
+      </c>
       <c r="AF13" s="50"/>
       <c r="AG13" s="50"/>
-      <c r="AH13" s="50"/>
-      <c r="AI13" s="50"/>
-      <c r="AJ13" s="50"/>
-      <c r="AK13" s="50"/>
-      <c r="AL13" s="50"/>
-      <c r="AM13" s="50"/>
-      <c r="AN13" s="50"/>
-      <c r="AO13" s="101"/>
+      <c r="AH13" s="124">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AI13" s="124">
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="124">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="124">
+        <v>10</v>
+      </c>
+      <c r="AO13" s="125">
+        <v>0.55999999999999994</v>
+      </c>
       <c r="AP13" s="51"/>
       <c r="AQ13" s="52"/>
-      <c r="AR13" s="53"/>
-      <c r="AS13" s="54"/>
-      <c r="AT13" s="55"/>
-      <c r="AU13" s="31"/>
-      <c r="AV13" s="31"/>
-      <c r="AW13" s="31"/>
-      <c r="AX13" s="56"/>
-      <c r="AY13" s="56"/>
-      <c r="AZ13" s="56"/>
-      <c r="BA13" s="56"/>
-      <c r="BB13" s="31"/>
+      <c r="AR13" s="126">
+        <v>2E-3</v>
+      </c>
+      <c r="AS13" s="127">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT13" s="146">
+        <v>240</v>
+      </c>
+      <c r="AU13" s="128">
+        <v>2.5</v>
+      </c>
+      <c r="AV13" s="128">
+        <v>9.5</v>
+      </c>
+      <c r="AW13" s="128">
+        <v>1.7</v>
+      </c>
+      <c r="AX13" s="129">
+        <v>0.7</v>
+      </c>
+      <c r="AY13" s="129">
+        <v>1.2</v>
+      </c>
+      <c r="AZ13" s="129">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="129">
+        <v>8</v>
+      </c>
+      <c r="BB13" s="128" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B14" s="32" t="s">
@@ -10481,53 +10593,139 @@
       <c r="G14" s="37">
         <v>10</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="43"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="49"/>
-      <c r="AD14" s="50"/>
-      <c r="AE14" s="50"/>
+      <c r="H14" s="130">
+        <v>8</v>
+      </c>
+      <c r="I14" s="121">
+        <v>0</v>
+      </c>
+      <c r="J14" s="145">
+        <v>150</v>
+      </c>
+      <c r="K14" s="119">
+        <v>1.9</v>
+      </c>
+      <c r="L14" s="119">
+        <v>0</v>
+      </c>
+      <c r="M14" s="119">
+        <v>1.2E-2</v>
+      </c>
+      <c r="N14" s="119">
+        <v>30</v>
+      </c>
+      <c r="O14" s="119">
+        <v>0.6</v>
+      </c>
+      <c r="P14" s="123">
+        <v>0.95</v>
+      </c>
+      <c r="Q14" s="121">
+        <v>1.2</v>
+      </c>
+      <c r="R14" s="119">
+        <v>120</v>
+      </c>
+      <c r="S14" s="119">
+        <v>25</v>
+      </c>
+      <c r="T14" s="120">
+        <v>35</v>
+      </c>
+      <c r="U14" s="121">
+        <v>11</v>
+      </c>
+      <c r="V14" s="119">
+        <v>4</v>
+      </c>
+      <c r="W14" s="119">
+        <v>10</v>
+      </c>
+      <c r="X14" s="120">
+        <v>15000</v>
+      </c>
+      <c r="Y14" s="122">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="123">
+        <v>0.08</v>
+      </c>
+      <c r="AA14" s="123">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="122">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD14" s="124" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE14" s="124" t="s">
+        <v>23</v>
+      </c>
       <c r="AF14" s="50"/>
       <c r="AG14" s="50"/>
-      <c r="AH14" s="50"/>
-      <c r="AI14" s="50"/>
-      <c r="AJ14" s="50"/>
-      <c r="AK14" s="50"/>
-      <c r="AL14" s="50"/>
-      <c r="AM14" s="50"/>
-      <c r="AN14" s="50"/>
-      <c r="AO14" s="101"/>
+      <c r="AH14" s="124">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI14" s="124">
+        <v>2</v>
+      </c>
+      <c r="AJ14" s="124">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="124">
+        <v>10</v>
+      </c>
+      <c r="AO14" s="125">
+        <v>0.7</v>
+      </c>
       <c r="AP14" s="51"/>
       <c r="AQ14" s="52"/>
-      <c r="AR14" s="53"/>
-      <c r="AS14" s="54"/>
-      <c r="AT14" s="55"/>
-      <c r="AU14" s="31"/>
-      <c r="AV14" s="31"/>
-      <c r="AW14" s="31"/>
-      <c r="AX14" s="56"/>
-      <c r="AY14" s="56"/>
-      <c r="AZ14" s="56"/>
-      <c r="BA14" s="56"/>
-      <c r="BB14" s="31"/>
+      <c r="AR14" s="126">
+        <v>1.8E-3</v>
+      </c>
+      <c r="AS14" s="127">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT14" s="146">
+        <v>255</v>
+      </c>
+      <c r="AU14" s="128">
+        <v>2.5</v>
+      </c>
+      <c r="AV14" s="128">
+        <v>9.5</v>
+      </c>
+      <c r="AW14" s="128">
+        <v>1.7</v>
+      </c>
+      <c r="AX14" s="129">
+        <v>0.7</v>
+      </c>
+      <c r="AY14" s="129">
+        <v>1.2</v>
+      </c>
+      <c r="AZ14" s="129">
+        <v>9</v>
+      </c>
+      <c r="BA14" s="129">
+        <v>8</v>
+      </c>
+      <c r="BB14" s="128" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B15" s="32" t="s">
@@ -10548,53 +10746,139 @@
       <c r="G15" s="37">
         <v>20</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="42"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="47"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="49"/>
-      <c r="AD15" s="50"/>
-      <c r="AE15" s="50"/>
+      <c r="H15" s="130">
+        <v>17</v>
+      </c>
+      <c r="I15" s="121">
+        <v>0</v>
+      </c>
+      <c r="J15" s="145">
+        <v>200</v>
+      </c>
+      <c r="K15" s="119">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L15" s="119">
+        <v>0</v>
+      </c>
+      <c r="M15" s="119">
+        <v>1.4E-2</v>
+      </c>
+      <c r="N15" s="119">
+        <v>25</v>
+      </c>
+      <c r="O15" s="119">
+        <v>0.7</v>
+      </c>
+      <c r="P15" s="123">
+        <v>1.55</v>
+      </c>
+      <c r="Q15" s="121">
+        <v>1.2</v>
+      </c>
+      <c r="R15" s="119">
+        <v>140</v>
+      </c>
+      <c r="S15" s="119">
+        <v>25</v>
+      </c>
+      <c r="T15" s="120">
+        <v>35</v>
+      </c>
+      <c r="U15" s="121">
+        <v>11.5</v>
+      </c>
+      <c r="V15" s="119">
+        <v>5</v>
+      </c>
+      <c r="W15" s="119">
+        <v>10</v>
+      </c>
+      <c r="X15" s="120">
+        <v>27000</v>
+      </c>
+      <c r="Y15" s="122">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="123">
+        <v>0.05</v>
+      </c>
+      <c r="AA15" s="123">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="122">
+        <v>12</v>
+      </c>
+      <c r="AC15" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD15" s="124" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE15" s="124" t="s">
+        <v>21</v>
+      </c>
       <c r="AF15" s="50"/>
       <c r="AG15" s="50"/>
-      <c r="AH15" s="50"/>
-      <c r="AI15" s="50"/>
-      <c r="AJ15" s="50"/>
-      <c r="AK15" s="50"/>
-      <c r="AL15" s="50"/>
-      <c r="AM15" s="50"/>
-      <c r="AN15" s="50"/>
-      <c r="AO15" s="101"/>
+      <c r="AH15" s="124">
+        <v>2.1</v>
+      </c>
+      <c r="AI15" s="124">
+        <v>2</v>
+      </c>
+      <c r="AJ15" s="124">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM15" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="124">
+        <v>10</v>
+      </c>
+      <c r="AO15" s="125">
+        <v>0.7</v>
+      </c>
       <c r="AP15" s="51"/>
       <c r="AQ15" s="52"/>
-      <c r="AR15" s="53"/>
-      <c r="AS15" s="54"/>
-      <c r="AT15" s="55"/>
-      <c r="AU15" s="31"/>
-      <c r="AV15" s="31"/>
-      <c r="AW15" s="31"/>
-      <c r="AX15" s="56"/>
-      <c r="AY15" s="56"/>
-      <c r="AZ15" s="56"/>
-      <c r="BA15" s="56"/>
-      <c r="BB15" s="31"/>
+      <c r="AR15" s="126">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AS15" s="127">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT15" s="146">
+        <v>270</v>
+      </c>
+      <c r="AU15" s="128">
+        <v>2.5</v>
+      </c>
+      <c r="AV15" s="128">
+        <v>9.5</v>
+      </c>
+      <c r="AW15" s="128">
+        <v>1.7</v>
+      </c>
+      <c r="AX15" s="129">
+        <v>0.7</v>
+      </c>
+      <c r="AY15" s="129">
+        <v>1.2</v>
+      </c>
+      <c r="AZ15" s="129">
+        <v>45</v>
+      </c>
+      <c r="BA15" s="129">
+        <v>15</v>
+      </c>
+      <c r="BB15" s="128" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -10616,53 +10900,139 @@
       <c r="G16" s="37">
         <v>30</v>
       </c>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="44"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="42"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="46"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="47"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="49"/>
-      <c r="AD16" s="50"/>
-      <c r="AE16" s="50"/>
+      <c r="H16" s="130">
+        <v>25</v>
+      </c>
+      <c r="I16" s="121">
+        <v>0</v>
+      </c>
+      <c r="J16" s="145">
+        <v>250</v>
+      </c>
+      <c r="K16" s="119">
+        <v>2.4</v>
+      </c>
+      <c r="L16" s="119">
+        <v>0</v>
+      </c>
+      <c r="M16" s="119">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N16" s="119">
+        <v>20</v>
+      </c>
+      <c r="O16" s="119">
+        <v>0.8</v>
+      </c>
+      <c r="P16" s="123">
+        <v>1.9</v>
+      </c>
+      <c r="Q16" s="121">
+        <v>1.2</v>
+      </c>
+      <c r="R16" s="119">
+        <v>160</v>
+      </c>
+      <c r="S16" s="119">
+        <v>25</v>
+      </c>
+      <c r="T16" s="120">
+        <v>35</v>
+      </c>
+      <c r="U16" s="121">
+        <v>12</v>
+      </c>
+      <c r="V16" s="119">
+        <v>6</v>
+      </c>
+      <c r="W16" s="119">
+        <v>10</v>
+      </c>
+      <c r="X16" s="120">
+        <v>45000</v>
+      </c>
+      <c r="Y16" s="122">
+        <v>5</v>
+      </c>
+      <c r="Z16" s="123">
+        <v>0.04</v>
+      </c>
+      <c r="AA16" s="123">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="122">
+        <v>12</v>
+      </c>
+      <c r="AC16" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD16" s="124" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE16" s="124" t="s">
+        <v>19</v>
+      </c>
       <c r="AF16" s="50"/>
       <c r="AG16" s="50"/>
-      <c r="AH16" s="50"/>
-      <c r="AI16" s="50"/>
-      <c r="AJ16" s="50"/>
-      <c r="AK16" s="50"/>
-      <c r="AL16" s="50"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="50"/>
-      <c r="AO16" s="101"/>
+      <c r="AH16" s="124">
+        <v>2.1</v>
+      </c>
+      <c r="AI16" s="124">
+        <v>2</v>
+      </c>
+      <c r="AJ16" s="124">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="124">
+        <v>10</v>
+      </c>
+      <c r="AO16" s="125">
+        <v>0.7</v>
+      </c>
       <c r="AP16" s="51"/>
       <c r="AQ16" s="52"/>
-      <c r="AR16" s="53"/>
-      <c r="AS16" s="54"/>
-      <c r="AT16" s="55"/>
-      <c r="AU16" s="31"/>
-      <c r="AV16" s="31"/>
-      <c r="AW16" s="31"/>
-      <c r="AX16" s="56"/>
-      <c r="AY16" s="56"/>
-      <c r="AZ16" s="56"/>
-      <c r="BA16" s="56"/>
-      <c r="BB16" s="31"/>
+      <c r="AR16" s="126">
+        <v>1.5E-3</v>
+      </c>
+      <c r="AS16" s="127">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AT16" s="146">
+        <v>285</v>
+      </c>
+      <c r="AU16" s="128">
+        <v>2.5</v>
+      </c>
+      <c r="AV16" s="128">
+        <v>9.5</v>
+      </c>
+      <c r="AW16" s="128">
+        <v>1.7</v>
+      </c>
+      <c r="AX16" s="129">
+        <v>0.7</v>
+      </c>
+      <c r="AY16" s="129">
+        <v>1.2</v>
+      </c>
+      <c r="AZ16" s="129">
+        <v>59</v>
+      </c>
+      <c r="BA16" s="129">
+        <v>15</v>
+      </c>
+      <c r="BB16" s="128" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B17" s="32" t="s">
@@ -10683,13 +11053,13 @@
       <c r="G17" s="37">
         <v>0</v>
       </c>
-      <c r="H17" s="131">
+      <c r="H17" s="130">
         <v>3</v>
       </c>
       <c r="I17" s="121">
         <v>-2</v>
       </c>
-      <c r="J17" s="132">
+      <c r="J17" s="131">
         <v>100</v>
       </c>
       <c r="K17" s="119">
@@ -10746,7 +11116,7 @@
       <c r="AB17" s="122">
         <v>12</v>
       </c>
-      <c r="AC17" s="130" t="s">
+      <c r="AC17" s="49" t="s">
         <v>155</v>
       </c>
       <c r="AD17" s="124" t="s">
@@ -10836,13 +11206,13 @@
       <c r="G18" s="37">
         <v>10</v>
       </c>
-      <c r="H18" s="131">
+      <c r="H18" s="130">
         <v>8</v>
       </c>
       <c r="I18" s="121">
         <v>0</v>
       </c>
-      <c r="J18" s="132">
+      <c r="J18" s="131">
         <v>150</v>
       </c>
       <c r="K18" s="119">
@@ -10899,7 +11269,7 @@
       <c r="AB18" s="122">
         <v>12</v>
       </c>
-      <c r="AC18" s="130" t="s">
+      <c r="AC18" s="49" t="s">
         <v>155</v>
       </c>
       <c r="AD18" s="124" t="s">
@@ -10989,13 +11359,13 @@
       <c r="G19" s="37">
         <v>20</v>
       </c>
-      <c r="H19" s="131">
+      <c r="H19" s="130">
         <v>17</v>
       </c>
       <c r="I19" s="121">
         <v>0</v>
       </c>
-      <c r="J19" s="132">
+      <c r="J19" s="131">
         <v>200</v>
       </c>
       <c r="K19" s="119">
@@ -11052,7 +11422,7 @@
       <c r="AB19" s="122">
         <v>12</v>
       </c>
-      <c r="AC19" s="130" t="s">
+      <c r="AC19" s="49" t="s">
         <v>155</v>
       </c>
       <c r="AD19" s="124" t="s">
@@ -11142,13 +11512,13 @@
       <c r="G20" s="37">
         <v>30</v>
       </c>
-      <c r="H20" s="131">
+      <c r="H20" s="130">
         <v>25</v>
       </c>
       <c r="I20" s="121">
         <v>0</v>
       </c>
-      <c r="J20" s="132">
+      <c r="J20" s="131">
         <v>250</v>
       </c>
       <c r="K20" s="119">
@@ -11205,7 +11575,7 @@
       <c r="AB20" s="122">
         <v>12</v>
       </c>
-      <c r="AC20" s="130" t="s">
+      <c r="AC20" s="49" t="s">
         <v>155</v>
       </c>
       <c r="AD20" s="124" t="s">
@@ -11552,44 +11922,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="140" t="s">
+      <c r="H25" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="141"/>
-      <c r="J25" s="142" t="s">
+      <c r="I25" s="140"/>
+      <c r="J25" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="143"/>
-      <c r="L25" s="143"/>
-      <c r="M25" s="143"/>
-      <c r="N25" s="143"/>
-      <c r="O25" s="144"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="142"/>
+      <c r="M25" s="142"/>
+      <c r="N25" s="142"/>
+      <c r="O25" s="143"/>
       <c r="P25" s="99"/>
-      <c r="Q25" s="136" t="s">
+      <c r="Q25" s="135" t="s">
         <v>145</v>
       </c>
-      <c r="R25" s="137"/>
-      <c r="S25" s="137"/>
-      <c r="T25" s="137"/>
-      <c r="U25" s="138" t="s">
+      <c r="R25" s="136"/>
+      <c r="S25" s="136"/>
+      <c r="T25" s="136"/>
+      <c r="U25" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="139"/>
-      <c r="W25" s="139"/>
-      <c r="X25" s="139"/>
+      <c r="V25" s="138"/>
+      <c r="W25" s="138"/>
+      <c r="X25" s="138"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="133" t="s">
+      <c r="AH25" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="AI25" s="134"/>
-      <c r="AJ25" s="134"/>
-      <c r="AK25" s="134"/>
-      <c r="AL25" s="134"/>
-      <c r="AM25" s="134"/>
-      <c r="AN25" s="135"/>
+      <c r="AI25" s="133"/>
+      <c r="AJ25" s="133"/>
+      <c r="AK25" s="133"/>
+      <c r="AL25" s="133"/>
+      <c r="AM25" s="133"/>
+      <c r="AN25" s="134"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
@@ -11793,37 +12163,40 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="94" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:D6">
+    <cfRule type="duplicateValues" dxfId="94" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T6">
+    <cfRule type="duplicateValues" dxfId="93" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:C36">
+    <cfRule type="duplicateValues" dxfId="92" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C33">
+    <cfRule type="duplicateValues" dxfId="91" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C39">
+    <cfRule type="duplicateValues" dxfId="90" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C24">
+    <cfRule type="duplicateValues" dxfId="89" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB21:BB24">
+    <cfRule type="duplicateValues" dxfId="88" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB17">
+    <cfRule type="duplicateValues" dxfId="87" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB18:BB20">
+    <cfRule type="duplicateValues" dxfId="86" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB13">
-    <cfRule type="duplicateValues" dxfId="93" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="92" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T4:T6">
-    <cfRule type="duplicateValues" dxfId="91" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="90" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="89" priority="47"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="88" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="87" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB14:BB16 BB21:BB24">
-    <cfRule type="duplicateValues" dxfId="86" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB17">
-    <cfRule type="duplicateValues" dxfId="85" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BB18:BB20">
-    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
+  <conditionalFormatting sqref="BB14:BB16">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -11845,7 +12218,7 @@
   <dimension ref="C1:AC63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11867,12 +12240,12 @@
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="90"/>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
       <c r="J3" s="90" t="s">
         <v>121</v>
       </c>
@@ -12763,7 +13136,7 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
WIP Helicopter stats: Heavy drain, make up for incredible boost power
Former-commit-id: cf85814b64ef8fe131c634cc718073fb0a041d75
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="165">
   <si>
     <t>[sku]</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>HELICOPTER</t>
+  </si>
+  <si>
+    <t>PROBAR: Drain casi que no incremente con el tiempo (que sea muy poco), pero ya desde el principio un drain muy bestia</t>
+  </si>
+  <si>
+    <t>El uso del boost ha de matar mucho (metralleta, misiles, bombas…)</t>
+  </si>
+  <si>
+    <t>El boost ha de dudar bastante y regenerar rapido</t>
+  </si>
+  <si>
+    <t>-&gt; Hacer depender la vida del dragon de matar con el boost</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1606,6 +1618,14 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4655,7 +4675,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>415</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4964,7 +4984,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>184.48</c:v>
+                  <c:v>140.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5273,7 +5293,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.4</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6226,7 +6246,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>415</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6535,7 +6555,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>184.48</c:v>
+                  <c:v>140.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6844,7 +6864,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.4</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7115,16 +7135,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7158,16 +7178,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7437,16 +7457,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7480,16 +7500,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7759,16 +7779,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.1</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.7</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>17.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7802,16 +7822,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>6.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4000000000000021</c:v>
+                  <c:v>7.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7000000000000011</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15353,8 +15373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView topLeftCell="AL4" workbookViewId="0">
-      <selection activeCell="AV13" sqref="AV13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16007,16 +16027,16 @@
         <v>0</v>
       </c>
       <c r="J13" s="109">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K13" s="97">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="L13" s="97">
         <v>0</v>
       </c>
       <c r="M13" s="97">
-        <v>8.9999999999999993E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="N13" s="97">
         <v>30</v>
@@ -16031,13 +16051,13 @@
         <v>1.2</v>
       </c>
       <c r="R13" s="97">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="S13" s="97">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T13" s="98">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="U13" s="99">
         <v>9</v>
@@ -16106,17 +16126,17 @@
       <c r="AS13" s="105">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT13" s="110">
-        <v>240</v>
-      </c>
-      <c r="AU13" s="106">
+      <c r="AT13" s="154">
+        <v>100</v>
+      </c>
+      <c r="AU13" s="153">
         <v>2.5</v>
       </c>
-      <c r="AV13" s="106">
-        <v>9.5</v>
-      </c>
-      <c r="AW13" s="106">
-        <v>1.7</v>
+      <c r="AV13" s="153">
+        <v>3</v>
+      </c>
+      <c r="AW13" s="153">
+        <v>0</v>
       </c>
       <c r="AX13" s="107">
         <v>0.7</v>
@@ -16160,16 +16180,16 @@
         <v>0</v>
       </c>
       <c r="J14" s="109">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="K14" s="97">
-        <v>1.9</v>
+        <v>6.4</v>
       </c>
       <c r="L14" s="97">
         <v>0</v>
       </c>
       <c r="M14" s="97">
-        <v>1.2E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="N14" s="97">
         <v>30</v>
@@ -16184,13 +16204,13 @@
         <v>1.2</v>
       </c>
       <c r="R14" s="97">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="S14" s="97">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T14" s="98">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="U14" s="99">
         <v>11</v>
@@ -16259,17 +16279,17 @@
       <c r="AS14" s="105">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT14" s="110">
-        <v>255</v>
-      </c>
-      <c r="AU14" s="106">
+      <c r="AT14" s="154">
+        <v>110</v>
+      </c>
+      <c r="AU14" s="153">
         <v>2.5</v>
       </c>
-      <c r="AV14" s="106">
-        <v>9.5</v>
-      </c>
-      <c r="AW14" s="106">
-        <v>1.7</v>
+      <c r="AV14" s="153">
+        <v>3</v>
+      </c>
+      <c r="AW14" s="153">
+        <v>0</v>
       </c>
       <c r="AX14" s="107">
         <v>0.7</v>
@@ -16313,16 +16333,16 @@
         <v>0</v>
       </c>
       <c r="J15" s="109">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="K15" s="97">
-        <v>2.2999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="L15" s="97">
         <v>0</v>
       </c>
       <c r="M15" s="97">
-        <v>1.4E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="N15" s="97">
         <v>25</v>
@@ -16337,13 +16357,13 @@
         <v>1.2</v>
       </c>
       <c r="R15" s="97">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="S15" s="97">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T15" s="98">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="U15" s="99">
         <v>11.5</v>
@@ -16412,17 +16432,17 @@
       <c r="AS15" s="105">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT15" s="110">
-        <v>270</v>
-      </c>
-      <c r="AU15" s="106">
+      <c r="AT15" s="154">
+        <v>120</v>
+      </c>
+      <c r="AU15" s="153">
         <v>2.5</v>
       </c>
-      <c r="AV15" s="106">
-        <v>9.5</v>
-      </c>
-      <c r="AW15" s="106">
-        <v>1.7</v>
+      <c r="AV15" s="153">
+        <v>3</v>
+      </c>
+      <c r="AW15" s="153">
+        <v>0</v>
       </c>
       <c r="AX15" s="107">
         <v>0.7</v>
@@ -16467,16 +16487,16 @@
         <v>0</v>
       </c>
       <c r="J16" s="109">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="K16" s="97">
-        <v>2.4</v>
+        <v>7.2</v>
       </c>
       <c r="L16" s="97">
         <v>0</v>
       </c>
       <c r="M16" s="97">
-        <v>1.7000000000000001E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="N16" s="97">
         <v>20</v>
@@ -16491,13 +16511,13 @@
         <v>1.2</v>
       </c>
       <c r="R16" s="97">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="S16" s="97">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T16" s="98">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="U16" s="99">
         <v>12</v>
@@ -16566,17 +16586,17 @@
       <c r="AS16" s="105">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT16" s="110">
-        <v>285</v>
-      </c>
-      <c r="AU16" s="106">
+      <c r="AT16" s="154">
+        <v>130</v>
+      </c>
+      <c r="AU16" s="153">
         <v>2.5</v>
       </c>
-      <c r="AV16" s="106">
-        <v>9.5</v>
-      </c>
-      <c r="AW16" s="106">
-        <v>1.7</v>
+      <c r="AV16" s="153">
+        <v>3</v>
+      </c>
+      <c r="AW16" s="153">
+        <v>0</v>
       </c>
       <c r="AX16" s="107">
         <v>0.7</v>
@@ -18124,8 +18144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18356,7 +18376,7 @@
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87"/>
@@ -18465,7 +18485,7 @@
         <v>124</v>
       </c>
       <c r="E13" s="91">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
@@ -18473,7 +18493,7 @@
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>415</v>
+        <v>150</v>
       </c>
       <c r="J13" s="70" t="s">
         <v>135</v>
@@ -18529,7 +18549,7 @@
         <v>126</v>
       </c>
       <c r="E14" s="91">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="90"/>
       <c r="G14" s="75" t="s">
@@ -18537,7 +18557,7 @@
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>184.48</v>
+        <v>140.4</v>
       </c>
       <c r="J14" s="70" t="s">
         <v>136</v>
@@ -18593,7 +18613,7 @@
         <v>127</v>
       </c>
       <c r="E15" s="91">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
@@ -18601,7 +18621,7 @@
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
-        <v>14.4</v>
+        <v>10.7</v>
       </c>
       <c r="J15" s="70" t="s">
         <v>137</v>
@@ -18656,7 +18676,7 @@
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -19072,8 +19092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19149,16 +19169,16 @@
         <v>121</v>
       </c>
       <c r="E5" s="73">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F5" s="73">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G5" s="73">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="H5" s="73">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="K5" t="s">
         <v>117</v>
@@ -19193,16 +19213,16 @@
         <v>122</v>
       </c>
       <c r="E6" s="73">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F6" s="73">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G6" s="73">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H6" s="73">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="K6" t="s">
         <v>118</v>
@@ -19237,16 +19257,16 @@
         <v>123</v>
       </c>
       <c r="E7" s="81">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="F7" s="81">
-        <v>255</v>
+        <v>110</v>
       </c>
       <c r="G7" s="81">
-        <v>270</v>
+        <v>120</v>
       </c>
       <c r="H7" s="81">
-        <v>285</v>
+        <v>130</v>
       </c>
       <c r="K7" t="s">
         <v>131</v>
@@ -19304,7 +19324,7 @@
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87"/>
@@ -19364,45 +19384,45 @@
       </c>
       <c r="K12">
         <f>E5</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="L12">
         <f>E5+E5*(L6/100)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="M12">
         <f>L12-K12</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R12" s="70" t="s">
         <v>132</v>
       </c>
       <c r="S12">
         <f>E6</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="T12">
         <f>E6+E6*(T6/100)</f>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="U12">
         <f>T12-S12</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="Z12" s="70" t="s">
         <v>132</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AV13)/'special dragons'!AU13,1)</f>
-        <v>10.1</v>
+        <v>13.3</v>
       </c>
       <c r="AB12">
         <f>ROUND(((E7+E7*(AB6/100))/'special dragons'!AV13)/'special dragons'!AU13,1)</f>
-        <v>15.2</v>
+        <v>20</v>
       </c>
       <c r="AC12">
         <f>AB12-AA12</f>
-        <v>5.0999999999999996</v>
+        <v>6.6999999999999993</v>
       </c>
     </row>
     <row r="13" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19413,7 +19433,7 @@
         <v>124</v>
       </c>
       <c r="E13" s="91">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
@@ -19421,52 +19441,52 @@
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>415</v>
+        <v>150</v>
       </c>
       <c r="J13" s="70" t="s">
         <v>135</v>
       </c>
       <c r="K13">
         <f>F5</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L13">
         <f>F5+F5*(L6/100)</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:M15" si="0">L13-K13</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="R13" s="70" t="s">
         <v>135</v>
       </c>
       <c r="S13">
         <f>F6</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="T13">
         <f>F6+F6*(T6/100)</f>
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="U13">
         <f t="shared" ref="U13:U15" si="1">T13-S13</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="Z13" s="70" t="s">
         <v>135</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AV14)/'special dragons'!AU14,1)</f>
-        <v>10.7</v>
+        <v>14.7</v>
       </c>
       <c r="AB13">
         <f>ROUND(((F7+F7*(AB6/100))/'special dragons'!AV14)/'special dragons'!AU14,1)</f>
-        <v>16.100000000000001</v>
+        <v>22</v>
       </c>
       <c r="AC13">
         <f>AB13-AA13</f>
-        <v>5.4000000000000021</v>
+        <v>7.3000000000000007</v>
       </c>
     </row>
     <row r="14" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19477,7 +19497,7 @@
         <v>126</v>
       </c>
       <c r="E14" s="91">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F14" s="90"/>
       <c r="G14" s="75" t="s">
@@ -19485,52 +19505,52 @@
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>184.48</v>
+        <v>120</v>
       </c>
       <c r="J14" s="70" t="s">
         <v>136</v>
       </c>
       <c r="K14">
         <f>G5</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="L14">
         <f>G5+G5*(L6/100)</f>
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R14" s="70" t="s">
         <v>136</v>
       </c>
       <c r="S14">
         <f>G6</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="T14">
         <f>G6+G6*(T6/100)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="U14">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="Z14" s="70" t="s">
         <v>136</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AV15)/'special dragons'!AU15,1)</f>
-        <v>11.4</v>
+        <v>16</v>
       </c>
       <c r="AB14">
         <f>ROUND(((G7+G7*(AB6/100))/'special dragons'!AV15)/'special dragons'!AU15,1)</f>
-        <v>17.100000000000001</v>
+        <v>24</v>
       </c>
       <c r="AC14">
         <f>AB14-AA14</f>
-        <v>5.7000000000000011</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19541,7 +19561,7 @@
         <v>127</v>
       </c>
       <c r="E15" s="91">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
@@ -19549,52 +19569,52 @@
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(12+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(12+E11,47,1,1,"special dragons")),1)</f>
-        <v>14.4</v>
+        <v>13.3</v>
       </c>
       <c r="J15" s="70" t="s">
         <v>137</v>
       </c>
       <c r="K15">
         <f>H5</f>
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="L15">
         <f>H5+H5*(L6/100)</f>
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R15" s="70" t="s">
         <v>137</v>
       </c>
       <c r="S15">
         <f>H6</f>
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="T15">
         <f>H6+H6*(T6/100)</f>
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="U15">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="Z15" s="70" t="s">
         <v>137</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AV16)/'special dragons'!AU16,1)</f>
-        <v>12</v>
+        <v>17.3</v>
       </c>
       <c r="AB15">
         <f>ROUND(((H7+H7*(AB6/100))/'special dragons'!AV16)/'special dragons'!AU16,1)</f>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="AC15">
         <f>AB15-AA15</f>
-        <v>6</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.25">
@@ -19604,7 +19624,7 @@
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -19738,7 +19758,7 @@
       <c r="G32" s="90"/>
       <c r="H32" s="78"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="89"/>
       <c r="D33" s="90"/>
       <c r="E33" s="90"/>
@@ -19746,7 +19766,7 @@
       <c r="G33" s="90"/>
       <c r="H33" s="78"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="89"/>
       <c r="D34" s="90"/>
       <c r="E34" s="90"/>
@@ -19754,39 +19774,55 @@
       <c r="G34" s="90"/>
       <c r="H34" s="78"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="89"/>
       <c r="D35" s="90"/>
       <c r="E35" s="90"/>
       <c r="F35" s="90"/>
       <c r="G35" s="90"/>
       <c r="H35" s="78"/>
+      <c r="N35" s="155" t="s">
+        <v>161</v>
+      </c>
+      <c r="O35" s="155"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="89"/>
       <c r="D36" s="90"/>
       <c r="E36" s="90"/>
       <c r="F36" s="90"/>
       <c r="G36" s="90"/>
       <c r="H36" s="78"/>
+      <c r="N36" s="155"/>
+      <c r="O36" s="155" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C37" s="89"/>
       <c r="D37" s="90"/>
       <c r="E37" s="90"/>
       <c r="F37" s="90"/>
       <c r="G37" s="90"/>
       <c r="H37" s="78"/>
+      <c r="N37" s="155"/>
+      <c r="O37" s="155" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="89"/>
       <c r="D38" s="90"/>
       <c r="E38" s="90"/>
       <c r="F38" s="90"/>
       <c r="G38" s="90"/>
       <c r="H38" s="78"/>
+      <c r="N38" s="155"/>
+      <c r="O38" s="156" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="89"/>
       <c r="D39" s="90"/>
       <c r="E39" s="90"/>
@@ -19794,7 +19830,7 @@
       <c r="G39" s="90"/>
       <c r="H39" s="78"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="89"/>
       <c r="D40" s="90"/>
       <c r="E40" s="90"/>
@@ -19802,7 +19838,7 @@
       <c r="G40" s="90"/>
       <c r="H40" s="78"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C41" s="89"/>
       <c r="D41" s="90"/>
       <c r="E41" s="90"/>
@@ -19810,7 +19846,7 @@
       <c r="G41" s="90"/>
       <c r="H41" s="78"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C42" s="89"/>
       <c r="D42" s="90"/>
       <c r="E42" s="90"/>
@@ -19818,7 +19854,7 @@
       <c r="G42" s="90"/>
       <c r="H42" s="78"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C43" s="89"/>
       <c r="D43" s="90"/>
       <c r="E43" s="90"/>
@@ -19826,7 +19862,7 @@
       <c r="G43" s="90"/>
       <c r="H43" s="78"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="89"/>
       <c r="D44" s="90"/>
       <c r="E44" s="90"/>
@@ -19834,7 +19870,7 @@
       <c r="G44" s="90"/>
       <c r="H44" s="78"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="89"/>
       <c r="D45" s="90"/>
       <c r="E45" s="90"/>
@@ -19842,7 +19878,7 @@
       <c r="G45" s="90"/>
       <c r="H45" s="78"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C46" s="89"/>
       <c r="D46" s="90"/>
       <c r="E46" s="90"/>
@@ -19850,7 +19886,7 @@
       <c r="G46" s="90"/>
       <c r="H46" s="78"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="89"/>
       <c r="D47" s="90"/>
       <c r="E47" s="90"/>
@@ -19858,7 +19894,7 @@
       <c r="G47" s="90"/>
       <c r="H47" s="78"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="89"/>
       <c r="D48" s="90"/>
       <c r="E48" s="90"/>
@@ -20102,15 +20138,15 @@
       </c>
       <c r="G9">
         <f ca="1">Electric!H13</f>
-        <v>415</v>
+        <v>150</v>
       </c>
       <c r="H9">
         <f ca="1">Electric!H14</f>
-        <v>184.48</v>
+        <v>140.4</v>
       </c>
       <c r="I9">
         <f ca="1">Electric!H15</f>
-        <v>14.4</v>
+        <v>10.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP setting values for Helicopter
Former-commit-id: bbccd1b3b469524d894c4b324db5c6898178bf3e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -1644,6 +1644,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1682,45 +1721,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4366,7 +4366,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5614,7 +5613,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5936,7 +5934,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6258,7 +6255,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6567,7 +6563,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15477,8 +15472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13:AO20"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16127,56 +16122,56 @@
       <c r="G13" s="36">
         <v>0</v>
       </c>
-      <c r="H13" s="173">
+      <c r="H13" s="160">
         <v>20</v>
       </c>
-      <c r="I13" s="171">
+      <c r="I13" s="158">
         <v>0</v>
       </c>
-      <c r="J13" s="169">
+      <c r="J13" s="156">
         <v>150</v>
       </c>
-      <c r="K13" s="170">
-        <v>6</v>
-      </c>
-      <c r="L13" s="170">
+      <c r="K13" s="157">
+        <v>6.2</v>
+      </c>
+      <c r="L13" s="157">
         <v>0</v>
       </c>
-      <c r="M13" s="170">
+      <c r="M13" s="157">
         <v>1E-4</v>
       </c>
-      <c r="N13" s="170">
+      <c r="N13" s="157">
         <v>30</v>
       </c>
-      <c r="O13" s="170">
+      <c r="O13" s="157">
         <v>0.5</v>
       </c>
       <c r="P13" s="137">
         <v>1.25</v>
       </c>
-      <c r="Q13" s="171">
-        <v>1.2</v>
-      </c>
-      <c r="R13" s="170">
+      <c r="Q13" s="158">
+        <v>1.4</v>
+      </c>
+      <c r="R13" s="157">
         <v>120</v>
       </c>
-      <c r="S13" s="170">
-        <v>20</v>
-      </c>
-      <c r="T13" s="172">
+      <c r="S13" s="157">
         <v>40</v>
       </c>
-      <c r="U13" s="171">
+      <c r="T13" s="159">
+        <v>14</v>
+      </c>
+      <c r="U13" s="158">
         <v>9</v>
       </c>
-      <c r="V13" s="170">
+      <c r="V13" s="157">
         <v>3</v>
       </c>
-      <c r="W13" s="170">
+      <c r="W13" s="157">
         <v>9</v>
       </c>
-      <c r="X13" s="172">
-        <v>9500</v>
+      <c r="X13" s="159">
+        <v>25000</v>
       </c>
       <c r="Y13" s="138">
         <v>2</v>
@@ -16222,15 +16217,15 @@
       <c r="AN13" s="150">
         <v>10</v>
       </c>
-      <c r="AO13" s="167">
+      <c r="AO13" s="154">
         <v>0.55999999999999994</v>
       </c>
       <c r="AP13" s="39"/>
       <c r="AQ13" s="40"/>
-      <c r="AR13" s="176">
+      <c r="AR13" s="163">
         <v>2E-3</v>
       </c>
-      <c r="AS13" s="177">
+      <c r="AS13" s="164">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT13" s="131">
@@ -16249,12 +16244,12 @@
         <v>0.7</v>
       </c>
       <c r="AY13" s="106">
-        <v>1.2</v>
-      </c>
-      <c r="AZ13" s="174">
+        <v>0.8</v>
+      </c>
+      <c r="AZ13" s="161">
         <v>0</v>
       </c>
-      <c r="BA13" s="174">
+      <c r="BA13" s="161">
         <v>8</v>
       </c>
       <c r="BB13" s="105" t="s">
@@ -16280,56 +16275,56 @@
       <c r="G14" s="36">
         <v>10</v>
       </c>
-      <c r="H14" s="173">
+      <c r="H14" s="160">
         <v>22</v>
       </c>
-      <c r="I14" s="171">
+      <c r="I14" s="158">
         <v>0</v>
       </c>
-      <c r="J14" s="169">
+      <c r="J14" s="156">
         <v>200</v>
       </c>
-      <c r="K14" s="170">
-        <v>6.5</v>
-      </c>
-      <c r="L14" s="170">
+      <c r="K14" s="157">
+        <v>6.7</v>
+      </c>
+      <c r="L14" s="157">
         <v>0</v>
       </c>
-      <c r="M14" s="170">
+      <c r="M14" s="157">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="N14" s="170">
+      <c r="N14" s="157">
         <v>30</v>
       </c>
-      <c r="O14" s="170">
+      <c r="O14" s="157">
         <v>0.6</v>
       </c>
       <c r="P14" s="137">
         <v>1.4</v>
       </c>
-      <c r="Q14" s="171">
-        <v>1.2</v>
-      </c>
-      <c r="R14" s="170">
+      <c r="Q14" s="158">
+        <v>1.4</v>
+      </c>
+      <c r="R14" s="157">
         <v>140</v>
       </c>
-      <c r="S14" s="170">
-        <v>20</v>
-      </c>
-      <c r="T14" s="172">
+      <c r="S14" s="157">
         <v>40</v>
       </c>
-      <c r="U14" s="171">
+      <c r="T14" s="159">
+        <v>14</v>
+      </c>
+      <c r="U14" s="158">
         <v>11</v>
       </c>
-      <c r="V14" s="170">
+      <c r="V14" s="157">
         <v>4</v>
       </c>
-      <c r="W14" s="170">
+      <c r="W14" s="157">
         <v>10</v>
       </c>
-      <c r="X14" s="172">
-        <v>18000</v>
+      <c r="X14" s="159">
+        <v>35000</v>
       </c>
       <c r="Y14" s="138">
         <v>3</v>
@@ -16375,15 +16370,15 @@
       <c r="AN14" s="150">
         <v>10</v>
       </c>
-      <c r="AO14" s="167">
+      <c r="AO14" s="154">
         <v>0.7</v>
       </c>
       <c r="AP14" s="39"/>
       <c r="AQ14" s="40"/>
-      <c r="AR14" s="176">
+      <c r="AR14" s="163">
         <v>1.8E-3</v>
       </c>
-      <c r="AS14" s="177">
+      <c r="AS14" s="164">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT14" s="131">
@@ -16402,12 +16397,12 @@
         <v>0.7</v>
       </c>
       <c r="AY14" s="106">
-        <v>1.2</v>
-      </c>
-      <c r="AZ14" s="174">
+        <v>0.8</v>
+      </c>
+      <c r="AZ14" s="161">
         <v>9</v>
       </c>
-      <c r="BA14" s="174">
+      <c r="BA14" s="161">
         <v>8</v>
       </c>
       <c r="BB14" s="105" t="s">
@@ -16433,56 +16428,56 @@
       <c r="G15" s="36">
         <v>20</v>
       </c>
-      <c r="H15" s="173">
+      <c r="H15" s="160">
         <v>24</v>
       </c>
-      <c r="I15" s="171">
+      <c r="I15" s="158">
         <v>0</v>
       </c>
-      <c r="J15" s="169">
+      <c r="J15" s="156">
         <v>250</v>
       </c>
-      <c r="K15" s="170">
-        <v>7</v>
-      </c>
-      <c r="L15" s="170">
+      <c r="K15" s="157">
+        <v>7.2</v>
+      </c>
+      <c r="L15" s="157">
         <v>0</v>
       </c>
-      <c r="M15" s="170">
+      <c r="M15" s="157">
         <v>1E-3</v>
       </c>
-      <c r="N15" s="170">
+      <c r="N15" s="157">
         <v>25</v>
       </c>
-      <c r="O15" s="170">
+      <c r="O15" s="157">
         <v>0.7</v>
       </c>
       <c r="P15" s="137">
         <v>1.55</v>
       </c>
-      <c r="Q15" s="171">
-        <v>1.2</v>
-      </c>
-      <c r="R15" s="170">
+      <c r="Q15" s="158">
+        <v>1.4</v>
+      </c>
+      <c r="R15" s="157">
         <v>160</v>
       </c>
-      <c r="S15" s="170">
-        <v>20</v>
-      </c>
-      <c r="T15" s="172">
+      <c r="S15" s="157">
         <v>40</v>
       </c>
-      <c r="U15" s="171">
+      <c r="T15" s="159">
+        <v>14</v>
+      </c>
+      <c r="U15" s="158">
         <v>11.5</v>
       </c>
-      <c r="V15" s="170">
+      <c r="V15" s="157">
         <v>5</v>
       </c>
-      <c r="W15" s="170">
+      <c r="W15" s="157">
         <v>10</v>
       </c>
-      <c r="X15" s="172">
-        <v>30000</v>
+      <c r="X15" s="159">
+        <v>47000</v>
       </c>
       <c r="Y15" s="138">
         <v>4</v>
@@ -16528,15 +16523,15 @@
       <c r="AN15" s="150">
         <v>10</v>
       </c>
-      <c r="AO15" s="167">
+      <c r="AO15" s="154">
         <v>0.7</v>
       </c>
       <c r="AP15" s="39"/>
       <c r="AQ15" s="40"/>
-      <c r="AR15" s="176">
+      <c r="AR15" s="163">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AS15" s="177">
+      <c r="AS15" s="164">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT15" s="131">
@@ -16555,12 +16550,12 @@
         <v>0.7</v>
       </c>
       <c r="AY15" s="106">
-        <v>1.2</v>
-      </c>
-      <c r="AZ15" s="174">
+        <v>0.8</v>
+      </c>
+      <c r="AZ15" s="161">
         <v>45</v>
       </c>
-      <c r="BA15" s="174">
+      <c r="BA15" s="161">
         <v>15</v>
       </c>
       <c r="BB15" s="105" t="s">
@@ -16587,56 +16582,56 @@
       <c r="G16" s="36">
         <v>30</v>
       </c>
-      <c r="H16" s="173">
+      <c r="H16" s="160">
         <v>25</v>
       </c>
-      <c r="I16" s="171">
+      <c r="I16" s="158">
         <v>0</v>
       </c>
-      <c r="J16" s="169">
+      <c r="J16" s="156">
         <v>300</v>
       </c>
-      <c r="K16" s="170">
-        <v>7.5</v>
-      </c>
-      <c r="L16" s="170">
+      <c r="K16" s="157">
+        <v>7.7</v>
+      </c>
+      <c r="L16" s="157">
         <v>0</v>
       </c>
-      <c r="M16" s="170">
+      <c r="M16" s="157">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N16" s="170">
+      <c r="N16" s="157">
         <v>20</v>
       </c>
-      <c r="O16" s="170">
+      <c r="O16" s="157">
         <v>0.8</v>
       </c>
       <c r="P16" s="137">
         <v>1.75</v>
       </c>
-      <c r="Q16" s="171">
-        <v>1.2</v>
-      </c>
-      <c r="R16" s="170">
+      <c r="Q16" s="158">
+        <v>1.4</v>
+      </c>
+      <c r="R16" s="157">
         <v>180</v>
       </c>
-      <c r="S16" s="170">
-        <v>20</v>
-      </c>
-      <c r="T16" s="172">
+      <c r="S16" s="157">
         <v>40</v>
       </c>
-      <c r="U16" s="171">
+      <c r="T16" s="159">
+        <v>14</v>
+      </c>
+      <c r="U16" s="158">
         <v>12</v>
       </c>
-      <c r="V16" s="170">
+      <c r="V16" s="157">
         <v>6</v>
       </c>
-      <c r="W16" s="170">
+      <c r="W16" s="157">
         <v>10</v>
       </c>
-      <c r="X16" s="172">
-        <v>50000</v>
+      <c r="X16" s="159">
+        <v>83000</v>
       </c>
       <c r="Y16" s="138">
         <v>5</v>
@@ -16682,15 +16677,15 @@
       <c r="AN16" s="150">
         <v>10</v>
       </c>
-      <c r="AO16" s="167">
+      <c r="AO16" s="154">
         <v>0.7</v>
       </c>
       <c r="AP16" s="39"/>
       <c r="AQ16" s="40"/>
-      <c r="AR16" s="176">
+      <c r="AR16" s="163">
         <v>1.5E-3</v>
       </c>
-      <c r="AS16" s="177">
+      <c r="AS16" s="164">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT16" s="131">
@@ -16709,12 +16704,12 @@
         <v>0.7</v>
       </c>
       <c r="AY16" s="106">
-        <v>1.2</v>
-      </c>
-      <c r="AZ16" s="174">
+        <v>0.8</v>
+      </c>
+      <c r="AZ16" s="161">
         <v>59</v>
       </c>
-      <c r="BA16" s="174">
+      <c r="BA16" s="161">
         <v>15</v>
       </c>
       <c r="BB16" s="105" t="s">
@@ -16835,15 +16830,15 @@
       <c r="AN17" s="151">
         <v>10</v>
       </c>
-      <c r="AO17" s="168">
+      <c r="AO17" s="155">
         <v>0.55999999999999994</v>
       </c>
       <c r="AP17" s="124"/>
       <c r="AQ17" s="125"/>
-      <c r="AR17" s="178">
+      <c r="AR17" s="165">
         <v>2E-3</v>
       </c>
-      <c r="AS17" s="179">
+      <c r="AS17" s="166">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT17" s="126">
@@ -16864,10 +16859,10 @@
       <c r="AY17" s="128">
         <v>1.2</v>
       </c>
-      <c r="AZ17" s="175">
+      <c r="AZ17" s="162">
         <v>0</v>
       </c>
-      <c r="BA17" s="175">
+      <c r="BA17" s="162">
         <v>8</v>
       </c>
       <c r="BB17" s="129" t="s">
@@ -16988,15 +16983,15 @@
       <c r="AN18" s="151">
         <v>10</v>
       </c>
-      <c r="AO18" s="168">
+      <c r="AO18" s="155">
         <v>0.7</v>
       </c>
       <c r="AP18" s="124"/>
       <c r="AQ18" s="125"/>
-      <c r="AR18" s="178">
+      <c r="AR18" s="165">
         <v>1.8E-3</v>
       </c>
-      <c r="AS18" s="179">
+      <c r="AS18" s="166">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT18" s="126">
@@ -17017,10 +17012,10 @@
       <c r="AY18" s="128">
         <v>1.2</v>
       </c>
-      <c r="AZ18" s="175">
+      <c r="AZ18" s="162">
         <v>9</v>
       </c>
-      <c r="BA18" s="175">
+      <c r="BA18" s="162">
         <v>8</v>
       </c>
       <c r="BB18" s="129" t="s">
@@ -17141,15 +17136,15 @@
       <c r="AN19" s="151">
         <v>10</v>
       </c>
-      <c r="AO19" s="168">
+      <c r="AO19" s="155">
         <v>0.7</v>
       </c>
       <c r="AP19" s="124"/>
       <c r="AQ19" s="125"/>
-      <c r="AR19" s="178">
+      <c r="AR19" s="165">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AS19" s="179">
+      <c r="AS19" s="166">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT19" s="126">
@@ -17170,10 +17165,10 @@
       <c r="AY19" s="128">
         <v>1.2</v>
       </c>
-      <c r="AZ19" s="175">
+      <c r="AZ19" s="162">
         <v>45</v>
       </c>
-      <c r="BA19" s="175">
+      <c r="BA19" s="162">
         <v>15</v>
       </c>
       <c r="BB19" s="129" t="s">
@@ -17294,15 +17289,15 @@
       <c r="AN20" s="151">
         <v>10</v>
       </c>
-      <c r="AO20" s="168">
+      <c r="AO20" s="155">
         <v>0.7</v>
       </c>
       <c r="AP20" s="124"/>
       <c r="AQ20" s="125"/>
-      <c r="AR20" s="178">
+      <c r="AR20" s="165">
         <v>1.5E-3</v>
       </c>
-      <c r="AS20" s="179">
+      <c r="AS20" s="166">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT20" s="126">
@@ -17323,10 +17318,10 @@
       <c r="AY20" s="128">
         <v>1.2</v>
       </c>
-      <c r="AZ20" s="175">
+      <c r="AZ20" s="162">
         <v>59</v>
       </c>
-      <c r="BA20" s="175">
+      <c r="BA20" s="162">
         <v>15</v>
       </c>
       <c r="BB20" s="129" t="s">
@@ -17953,44 +17948,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="161" t="s">
+      <c r="H25" s="174" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="162"/>
-      <c r="J25" s="163" t="s">
+      <c r="I25" s="175"/>
+      <c r="J25" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="164"/>
-      <c r="L25" s="164"/>
-      <c r="M25" s="164"/>
-      <c r="N25" s="164"/>
-      <c r="O25" s="165"/>
+      <c r="K25" s="177"/>
+      <c r="L25" s="177"/>
+      <c r="M25" s="177"/>
+      <c r="N25" s="177"/>
+      <c r="O25" s="178"/>
       <c r="P25" s="79"/>
-      <c r="Q25" s="157" t="s">
+      <c r="Q25" s="170" t="s">
         <v>145</v>
       </c>
-      <c r="R25" s="158"/>
-      <c r="S25" s="158"/>
-      <c r="T25" s="158"/>
-      <c r="U25" s="159" t="s">
+      <c r="R25" s="171"/>
+      <c r="S25" s="171"/>
+      <c r="T25" s="171"/>
+      <c r="U25" s="172" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="160"/>
-      <c r="W25" s="160"/>
-      <c r="X25" s="160"/>
+      <c r="V25" s="173"/>
+      <c r="W25" s="173"/>
+      <c r="X25" s="173"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="154" t="s">
+      <c r="AH25" s="167" t="s">
         <v>146</v>
       </c>
-      <c r="AI25" s="155"/>
-      <c r="AJ25" s="155"/>
-      <c r="AK25" s="155"/>
-      <c r="AL25" s="155"/>
-      <c r="AM25" s="155"/>
-      <c r="AN25" s="156"/>
+      <c r="AI25" s="168"/>
+      <c r="AJ25" s="168"/>
+      <c r="AK25" s="168"/>
+      <c r="AL25" s="168"/>
+      <c r="AM25" s="168"/>
+      <c r="AN25" s="169"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
@@ -18274,12 +18269,12 @@
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="179" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
       <c r="J3" s="70" t="s">
         <v>121</v>
       </c>
@@ -19199,8 +19194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19222,12 +19217,12 @@
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="179" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
       <c r="J3" s="70" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
WIP setting Helicopter stats
Former-commit-id: 9990816edb2127730381ea95b94c831c121c09b2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -15472,8 +15472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16132,7 +16132,7 @@
         <v>150</v>
       </c>
       <c r="K13" s="157">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="L13" s="157">
         <v>0</v>
@@ -16156,10 +16156,10 @@
         <v>120</v>
       </c>
       <c r="S13" s="157">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T13" s="159">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U13" s="158">
         <v>9</v>
@@ -16171,7 +16171,7 @@
         <v>9</v>
       </c>
       <c r="X13" s="159">
-        <v>25000</v>
+        <v>28000</v>
       </c>
       <c r="Y13" s="138">
         <v>2</v>
@@ -16244,7 +16244,7 @@
         <v>0.7</v>
       </c>
       <c r="AY13" s="106">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AZ13" s="161">
         <v>0</v>
@@ -16285,7 +16285,7 @@
         <v>200</v>
       </c>
       <c r="K14" s="157">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="L14" s="157">
         <v>0</v>
@@ -16309,10 +16309,10 @@
         <v>140</v>
       </c>
       <c r="S14" s="157">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T14" s="159">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U14" s="158">
         <v>11</v>
@@ -16324,7 +16324,7 @@
         <v>10</v>
       </c>
       <c r="X14" s="159">
-        <v>35000</v>
+        <v>38000</v>
       </c>
       <c r="Y14" s="138">
         <v>3</v>
@@ -16397,7 +16397,7 @@
         <v>0.7</v>
       </c>
       <c r="AY14" s="106">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AZ14" s="161">
         <v>9</v>
@@ -16438,7 +16438,7 @@
         <v>250</v>
       </c>
       <c r="K15" s="157">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="L15" s="157">
         <v>0</v>
@@ -16462,10 +16462,10 @@
         <v>160</v>
       </c>
       <c r="S15" s="157">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T15" s="159">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U15" s="158">
         <v>11.5</v>
@@ -16477,7 +16477,7 @@
         <v>10</v>
       </c>
       <c r="X15" s="159">
-        <v>47000</v>
+        <v>50000</v>
       </c>
       <c r="Y15" s="138">
         <v>4</v>
@@ -16550,7 +16550,7 @@
         <v>0.7</v>
       </c>
       <c r="AY15" s="106">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AZ15" s="161">
         <v>45</v>
@@ -16592,7 +16592,7 @@
         <v>300</v>
       </c>
       <c r="K16" s="157">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="L16" s="157">
         <v>0</v>
@@ -16616,10 +16616,10 @@
         <v>180</v>
       </c>
       <c r="S16" s="157">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T16" s="159">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U16" s="158">
         <v>12</v>
@@ -16631,7 +16631,7 @@
         <v>10</v>
       </c>
       <c r="X16" s="159">
-        <v>83000</v>
+        <v>86000</v>
       </c>
       <c r="Y16" s="138">
         <v>5</v>
@@ -16704,7 +16704,7 @@
         <v>0.7</v>
       </c>
       <c r="AY16" s="106">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="161">
         <v>59</v>

</xml_diff>

<commit_message>
WIP Setting Helicopter stats (tier 4)
Former-commit-id: c77a17d13e5c410672c727e781dfd64bc8b98e3f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -15477,8 +15477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView topLeftCell="M7" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16603,7 +16603,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="157">
-        <v>0.03</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="N16" s="157">
         <v>20</v>
@@ -19199,7 +19199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WIP Helicopter HP drain reduced
Former-commit-id: 2bf15bc3b487367453412ba065fe5e5eb36b3c83
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -4366,7 +4366,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4688,7 +4687,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4997,7 +4995,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5614,7 +5611,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5936,7 +5932,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6258,7 +6253,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6567,7 +6561,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7184,7 +7177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7506,7 +7498,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7828,7 +7819,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15477,7 +15467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -16449,7 +16439,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="157">
-        <v>8.9999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N15" s="157">
         <v>25</v>
@@ -16603,7 +16593,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="157">
-        <v>1.7000000000000001E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N16" s="157">
         <v>20</v>

</xml_diff>

<commit_message>
WIP calculated percentage by tier increment
Former-commit-id: c7c5892d5c797878e500ae37a5f510780967fe4d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="165">
   <si>
     <t>[sku]</t>
   </si>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t>NOTA: Añadir las columnas relativas al pet mummy!!!!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC. </t>
+  </si>
+  <si>
+    <t>INC.</t>
+  </si>
+  <si>
+    <t>(how increments a stat in each tier)</t>
   </si>
 </sst>
 </file>
@@ -4366,6 +4375,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4687,6 +4697,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4779,7 +4790,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>206.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4995,6 +5006,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5087,7 +5099,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>140.4</c:v>
+                  <c:v>163.80000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5395,7 +5407,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.7</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5611,6 +5623,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5932,6 +5945,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6253,6 +6267,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6345,7 +6360,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>206.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6561,6 +6576,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6653,7 +6669,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>140.4</c:v>
+                  <c:v>163.80000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6961,7 +6977,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.7</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7177,6 +7193,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7498,6 +7515,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7819,6 +7837,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15467,8 +15486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18239,10 +18258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AC63"/>
+  <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18257,12 +18276,12 @@
     <col min="28" max="28" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="72" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
       <c r="E3" s="179" t="s">
         <v>120</v>
@@ -18280,7 +18299,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D4" s="71"/>
       <c r="E4" s="71">
         <v>1</v>
@@ -18313,7 +18332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="71" t="s">
         <v>121</v>
       </c>
@@ -18357,7 +18376,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="71" t="s">
         <v>122</v>
       </c>
@@ -18401,7 +18420,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="80" t="s">
         <v>123</v>
       </c>
@@ -18448,7 +18467,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="84" t="s">
         <v>147</v>
       </c>
@@ -18465,15 +18484,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>164</v>
+      </c>
+      <c r="V10" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="85"/>
       <c r="D11" s="86" t="s">
         <v>125</v>
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87"/>
@@ -18490,7 +18519,9 @@
       <c r="M11" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="N11" s="74"/>
+      <c r="N11" s="74" t="s">
+        <v>162</v>
+      </c>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="R11" s="77" t="s">
@@ -18505,7 +18536,9 @@
       <c r="U11" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="V11" s="74"/>
+      <c r="V11" s="74" t="s">
+        <v>163</v>
+      </c>
       <c r="W11" s="74"/>
       <c r="X11" s="74"/>
       <c r="Z11" s="70" t="s">
@@ -18520,8 +18553,11 @@
       <c r="AC11" s="74" t="s">
         <v>139</v>
       </c>
+      <c r="AD11" s="74" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="12" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="89"/>
       <c r="D12" s="90"/>
       <c r="E12" s="90"/>
@@ -18543,6 +18579,10 @@
         <f>L12-K12</f>
         <v>100</v>
       </c>
+      <c r="N12">
+        <f>(K12*$L$7)/100</f>
+        <v>3.3</v>
+      </c>
       <c r="R12" s="70" t="s">
         <v>132</v>
       </c>
@@ -18558,6 +18598,10 @@
         <f>T12-S12</f>
         <v>50</v>
       </c>
+      <c r="V12">
+        <f>(S12*$T$7)/100</f>
+        <v>1.7</v>
+      </c>
       <c r="Z12" s="70" t="s">
         <v>132</v>
       </c>
@@ -18573,8 +18617,12 @@
         <f>AB12-AA12</f>
         <v>5.0999999999999996</v>
       </c>
+      <c r="AD12">
+        <f>(AA12*$AB$7)/100</f>
+        <v>0.17169999999999999</v>
+      </c>
     </row>
-    <row r="13" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="89" t="s">
         <v>128</v>
       </c>
@@ -18582,7 +18630,7 @@
         <v>124</v>
       </c>
       <c r="E13" s="91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
@@ -18590,7 +18638,7 @@
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>150</v>
+        <v>206.6</v>
       </c>
       <c r="J13" s="70" t="s">
         <v>135</v>
@@ -18607,6 +18655,10 @@
         <f t="shared" ref="M13:M15" si="0">L13-K13</f>
         <v>150</v>
       </c>
+      <c r="N13">
+        <f>(K13*$L$7)/100</f>
+        <v>4.95</v>
+      </c>
       <c r="R13" s="70" t="s">
         <v>135</v>
       </c>
@@ -18622,6 +18674,10 @@
         <f t="shared" ref="U13:U15" si="1">T13-S13</f>
         <v>60</v>
       </c>
+      <c r="V13">
+        <f t="shared" ref="V13:V15" si="2">(S13*$T$7)/100</f>
+        <v>2.04</v>
+      </c>
       <c r="Z13" s="70" t="s">
         <v>135</v>
       </c>
@@ -18637,8 +18693,12 @@
         <f>AB13-AA13</f>
         <v>5.4000000000000021</v>
       </c>
+      <c r="AD13">
+        <f t="shared" ref="AD13:AD15" si="3">(AA13*$AB$7)/100</f>
+        <v>0.18189999999999998</v>
+      </c>
     </row>
-    <row r="14" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="89" t="s">
         <v>129</v>
       </c>
@@ -18654,7 +18714,7 @@
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>140.4</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="J14" s="70" t="s">
         <v>136</v>
@@ -18671,6 +18731,10 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
+      <c r="N14">
+        <f t="shared" ref="N13:N15" si="4">(K14*$L$7)/100</f>
+        <v>6.6</v>
+      </c>
       <c r="R14" s="70" t="s">
         <v>136</v>
       </c>
@@ -18686,6 +18750,10 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>2.38</v>
+      </c>
       <c r="Z14" s="70" t="s">
         <v>136</v>
       </c>
@@ -18701,8 +18769,12 @@
         <f>AB14-AA14</f>
         <v>5.7000000000000011</v>
       </c>
+      <c r="AD14">
+        <f t="shared" si="3"/>
+        <v>0.1938</v>
+      </c>
     </row>
-    <row r="15" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="89" t="s">
         <v>130</v>
       </c>
@@ -18710,7 +18782,7 @@
         <v>127</v>
       </c>
       <c r="E15" s="91">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
@@ -18718,7 +18790,7 @@
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
-        <v>10.7</v>
+        <v>13.3</v>
       </c>
       <c r="J15" s="70" t="s">
         <v>137</v>
@@ -18735,6 +18807,10 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>8.25</v>
+      </c>
       <c r="R15" s="70" t="s">
         <v>137</v>
       </c>
@@ -18750,6 +18826,10 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>2.72</v>
+      </c>
       <c r="Z15" s="70" t="s">
         <v>137</v>
       </c>
@@ -18765,15 +18845,19 @@
         <f>AB15-AA15</f>
         <v>6</v>
       </c>
+      <c r="AD15">
+        <f t="shared" si="3"/>
+        <v>0.20399999999999999</v>
+      </c>
     </row>
-    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="89"/>
       <c r="D16" s="96" t="s">
         <v>141</v>
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -19187,10 +19271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AC63"/>
+  <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19205,12 +19289,12 @@
     <col min="28" max="28" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="72" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
       <c r="E3" s="179" t="s">
         <v>120</v>
@@ -19228,7 +19312,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D4" s="71"/>
       <c r="E4" s="71">
         <v>1</v>
@@ -19261,7 +19345,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="71" t="s">
         <v>121</v>
       </c>
@@ -19305,7 +19389,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="71" t="s">
         <v>122</v>
       </c>
@@ -19349,7 +19433,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="80" t="s">
         <v>123</v>
       </c>
@@ -19396,7 +19480,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="84" t="s">
         <v>147</v>
       </c>
@@ -19413,8 +19497,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>164</v>
+      </c>
+      <c r="V10" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="85"/>
       <c r="D11" s="86" t="s">
         <v>125</v>
@@ -19438,7 +19532,9 @@
       <c r="M11" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="N11" s="74"/>
+      <c r="N11" s="74" t="s">
+        <v>163</v>
+      </c>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="R11" s="77" t="s">
@@ -19453,7 +19549,9 @@
       <c r="U11" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="V11" s="74"/>
+      <c r="V11" s="74" t="s">
+        <v>163</v>
+      </c>
       <c r="W11" s="74"/>
       <c r="X11" s="74"/>
       <c r="Z11" s="70" t="s">
@@ -19468,8 +19566,11 @@
       <c r="AC11" s="74" t="s">
         <v>139</v>
       </c>
+      <c r="AD11" s="74" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="12" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="89"/>
       <c r="D12" s="90"/>
       <c r="E12" s="90"/>
@@ -19491,6 +19592,10 @@
         <f>L12-K12</f>
         <v>150</v>
       </c>
+      <c r="N12">
+        <f>(K12*$L$7)/100</f>
+        <v>4.95</v>
+      </c>
       <c r="R12" s="70" t="s">
         <v>132</v>
       </c>
@@ -19506,6 +19611,10 @@
         <f>T12-S12</f>
         <v>60</v>
       </c>
+      <c r="V12">
+        <f>(S12*$T$7)/100</f>
+        <v>2.04</v>
+      </c>
       <c r="Z12" s="70" t="s">
         <v>132</v>
       </c>
@@ -19521,8 +19630,12 @@
         <f>AB12-AA12</f>
         <v>6.6999999999999993</v>
       </c>
+      <c r="AD12">
+        <f>(AA12*$AB$7)/100</f>
+        <v>0.2261</v>
+      </c>
     </row>
-    <row r="13" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="89" t="s">
         <v>128</v>
       </c>
@@ -19555,6 +19668,10 @@
         <f t="shared" ref="M13:M15" si="0">L13-K13</f>
         <v>200</v>
       </c>
+      <c r="N13">
+        <f t="shared" ref="N13:N15" si="1">(K13*$L$7)/100</f>
+        <v>6.6</v>
+      </c>
       <c r="R13" s="70" t="s">
         <v>135</v>
       </c>
@@ -19567,8 +19684,12 @@
         <v>210</v>
       </c>
       <c r="U13">
-        <f t="shared" ref="U13:U15" si="1">T13-S13</f>
+        <f t="shared" ref="U13:U15" si="2">T13-S13</f>
         <v>70</v>
+      </c>
+      <c r="V13">
+        <f>(S13*$T$7)/100</f>
+        <v>2.38</v>
       </c>
       <c r="Z13" s="70" t="s">
         <v>135</v>
@@ -19585,8 +19706,12 @@
         <f>AB13-AA13</f>
         <v>7.3000000000000007</v>
       </c>
+      <c r="AD13">
+        <f>(AA13*$AB$7)/100</f>
+        <v>0.24989999999999998</v>
+      </c>
     </row>
-    <row r="14" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="89" t="s">
         <v>129</v>
       </c>
@@ -19619,6 +19744,10 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>8.25</v>
+      </c>
       <c r="R14" s="70" t="s">
         <v>136</v>
       </c>
@@ -19631,8 +19760,12 @@
         <v>240</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ref="V13:V15" si="3">(S14*$T$7)/100</f>
+        <v>2.72</v>
       </c>
       <c r="Z14" s="70" t="s">
         <v>136</v>
@@ -19649,8 +19782,12 @@
         <f>AB14-AA14</f>
         <v>8</v>
       </c>
+      <c r="AD14">
+        <f t="shared" ref="AD13:AD15" si="4">(AA14*$AB$7)/100</f>
+        <v>0.27200000000000002</v>
+      </c>
     </row>
-    <row r="15" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="89" t="s">
         <v>130</v>
       </c>
@@ -19683,6 +19820,10 @@
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
       <c r="R15" s="70" t="s">
         <v>137</v>
       </c>
@@ -19695,8 +19836,12 @@
         <v>270</v>
       </c>
       <c r="U15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="3"/>
+        <v>3.06</v>
       </c>
       <c r="Z15" s="70" t="s">
         <v>137</v>
@@ -19713,8 +19858,12 @@
         <f>AB15-AA15</f>
         <v>8.6999999999999993</v>
       </c>
+      <c r="AD15">
+        <f t="shared" si="4"/>
+        <v>0.29410000000000003</v>
+      </c>
     </row>
-    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="89"/>
       <c r="D16" s="96" t="s">
         <v>141</v>
@@ -20227,15 +20376,15 @@
       </c>
       <c r="G9">
         <f ca="1">Electric!H13</f>
-        <v>150</v>
+        <v>206.6</v>
       </c>
       <c r="H9">
         <f ca="1">Electric!H14</f>
-        <v>140.4</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="I9">
         <f ca="1">Electric!H15</f>
-        <v>10.7</v>
+        <v>13.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP review some values
Former-commit-id: aeb52f3076fe77451f08e60e84bb3da22c36af3d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -15481,8 +15481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="157">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="N15" s="157">
         <v>25</v>
@@ -16607,7 +16607,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="157">
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="N16" s="157">
         <v>20</v>
@@ -16793,7 +16793,7 @@
         <v>9</v>
       </c>
       <c r="X17" s="136">
-        <v>8500</v>
+        <v>10000</v>
       </c>
       <c r="Y17" s="119">
         <v>2</v>
@@ -16946,7 +16946,7 @@
         <v>10</v>
       </c>
       <c r="X18" s="136">
-        <v>15000</v>
+        <v>22000</v>
       </c>
       <c r="Y18" s="119">
         <v>3</v>
@@ -17099,7 +17099,7 @@
         <v>10</v>
       </c>
       <c r="X19" s="136">
-        <v>27000</v>
+        <v>37000</v>
       </c>
       <c r="Y19" s="119">
         <v>4</v>
@@ -17252,7 +17252,7 @@
         <v>10</v>
       </c>
       <c r="X20" s="136">
-        <v>45000</v>
+        <v>65000</v>
       </c>
       <c r="Y20" s="119">
         <v>5</v>
@@ -19269,7 +19269,7 @@
   <dimension ref="C1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
WIP review Helicopter stats
Former-commit-id: 4a7f0102de3a06f5a552c9bda3dc57a734704e5c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -761,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1254,11 +1254,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1731,11 +1759,71 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="104">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2456,46 +2544,6 @@
         </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -4375,6 +4423,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5622,6 +5671,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5943,6 +5993,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6264,6 +6315,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6572,6 +6624,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7243,16 +7296,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>250</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7286,16 +7339,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>250</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7565,16 +7618,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7608,16 +7661,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15163,37 +15216,37 @@
     <tableColumn id="48" name="[friction]" dataDxfId="42"/>
     <tableColumn id="49" name="[gravityModifier]" dataDxfId="41"/>
     <tableColumn id="50" name="[airGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="39"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="37"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="36"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="0"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="39"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="38"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="B3:T6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="31"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="32"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="30"/>
-    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="29"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="28"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="27"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="26"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="25"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="24"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="23"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="22"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="21"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="20"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="19"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="18"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="17"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="16"/>
+    <tableColumn id="5" name="[order]" dataDxfId="31"/>
+    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="30"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="29"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="28"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="27"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="26"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="25"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="24"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="23"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="22"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="21"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="20"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="19"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="18"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="17"/>
     <tableColumn id="65" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15201,14 +15254,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="10"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="9"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="8">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="11"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="10"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15481,8 +15534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16099,10 +16152,10 @@
       <c r="AX12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AY12" s="24" t="s">
+      <c r="AY12" s="183" t="s">
         <v>27</v>
       </c>
-      <c r="AZ12" s="21" t="s">
+      <c r="AZ12" s="28" t="s">
         <v>26</v>
       </c>
       <c r="BA12" s="21" t="s">
@@ -16138,7 +16191,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="156">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="K13" s="157">
         <v>6</v>
@@ -16162,10 +16215,10 @@
         <v>1.4</v>
       </c>
       <c r="R13" s="157">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="S13" s="157">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="T13" s="159">
         <v>10</v>
@@ -16180,7 +16233,7 @@
         <v>9</v>
       </c>
       <c r="X13" s="159">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="Y13" s="138">
         <v>2</v>
@@ -16252,10 +16305,10 @@
       <c r="AX13" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY13" s="106">
+      <c r="AY13" s="184">
         <v>0</v>
       </c>
-      <c r="AZ13" s="161">
+      <c r="AZ13" s="180">
         <v>0</v>
       </c>
       <c r="BA13" s="161">
@@ -16291,7 +16344,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="156">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="K14" s="157">
         <v>7</v>
@@ -16315,10 +16368,10 @@
         <v>1.4</v>
       </c>
       <c r="R14" s="157">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="S14" s="157">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="T14" s="159">
         <v>10</v>
@@ -16333,7 +16386,7 @@
         <v>10</v>
       </c>
       <c r="X14" s="159">
-        <v>45000</v>
+        <v>50000</v>
       </c>
       <c r="Y14" s="138">
         <v>3</v>
@@ -16405,10 +16458,10 @@
       <c r="AX14" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY14" s="106">
+      <c r="AY14" s="184">
         <v>0</v>
       </c>
-      <c r="AZ14" s="161">
+      <c r="AZ14" s="180">
         <v>9</v>
       </c>
       <c r="BA14" s="161">
@@ -16444,7 +16497,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="156">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="K15" s="157">
         <v>7.5</v>
@@ -16468,10 +16521,10 @@
         <v>1.4</v>
       </c>
       <c r="R15" s="157">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="S15" s="157">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="T15" s="159">
         <v>10</v>
@@ -16486,7 +16539,7 @@
         <v>10</v>
       </c>
       <c r="X15" s="159">
-        <v>57000</v>
+        <v>63000</v>
       </c>
       <c r="Y15" s="138">
         <v>4</v>
@@ -16558,10 +16611,10 @@
       <c r="AX15" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY15" s="106">
+      <c r="AY15" s="184">
         <v>0</v>
       </c>
-      <c r="AZ15" s="161">
+      <c r="AZ15" s="180">
         <v>45</v>
       </c>
       <c r="BA15" s="161">
@@ -16598,7 +16651,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="156">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="K16" s="157">
         <v>8</v>
@@ -16622,10 +16675,10 @@
         <v>1.4</v>
       </c>
       <c r="R16" s="157">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="S16" s="157">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="T16" s="159">
         <v>10</v>
@@ -16640,7 +16693,7 @@
         <v>10</v>
       </c>
       <c r="X16" s="159">
-        <v>93000</v>
+        <v>97000</v>
       </c>
       <c r="Y16" s="138">
         <v>5</v>
@@ -16712,10 +16765,10 @@
       <c r="AX16" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY16" s="106">
+      <c r="AY16" s="184">
         <v>0</v>
       </c>
-      <c r="AZ16" s="161">
+      <c r="AZ16" s="180">
         <v>59</v>
       </c>
       <c r="BA16" s="161">
@@ -16865,10 +16918,10 @@
       <c r="AX17" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY17" s="128">
+      <c r="AY17" s="185">
         <v>1.2</v>
       </c>
-      <c r="AZ17" s="162">
+      <c r="AZ17" s="181">
         <v>0</v>
       </c>
       <c r="BA17" s="162">
@@ -17018,10 +17071,10 @@
       <c r="AX18" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY18" s="128">
+      <c r="AY18" s="185">
         <v>1.2</v>
       </c>
-      <c r="AZ18" s="162">
+      <c r="AZ18" s="181">
         <v>9</v>
       </c>
       <c r="BA18" s="162">
@@ -17171,10 +17224,10 @@
       <c r="AX19" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY19" s="128">
+      <c r="AY19" s="185">
         <v>1.2</v>
       </c>
-      <c r="AZ19" s="162">
+      <c r="AZ19" s="181">
         <v>45</v>
       </c>
       <c r="BA19" s="162">
@@ -17324,10 +17377,10 @@
       <c r="AX20" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY20" s="128">
+      <c r="AY20" s="185">
         <v>1.2</v>
       </c>
-      <c r="AZ20" s="162">
+      <c r="AZ20" s="181">
         <v>59</v>
       </c>
       <c r="BA20" s="162">
@@ -17477,10 +17530,10 @@
       <c r="AX21" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY21" s="106">
+      <c r="AY21" s="184">
         <v>1.2</v>
       </c>
-      <c r="AZ21" s="106">
+      <c r="AZ21" s="182">
         <v>0</v>
       </c>
       <c r="BA21" s="106">
@@ -17630,10 +17683,10 @@
       <c r="AX22" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY22" s="106">
+      <c r="AY22" s="184">
         <v>1.2</v>
       </c>
-      <c r="AZ22" s="106">
+      <c r="AZ22" s="182">
         <v>9</v>
       </c>
       <c r="BA22" s="106">
@@ -17783,10 +17836,10 @@
       <c r="AX23" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY23" s="106">
+      <c r="AY23" s="184">
         <v>1.2</v>
       </c>
-      <c r="AZ23" s="106">
+      <c r="AZ23" s="182">
         <v>45</v>
       </c>
       <c r="BA23" s="106">
@@ -17937,10 +17990,10 @@
       <c r="AX24" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="106">
+      <c r="AY24" s="184">
         <v>1.2</v>
       </c>
-      <c r="AZ24" s="106">
+      <c r="AZ24" s="182">
         <v>59</v>
       </c>
       <c r="BA24" s="106">
@@ -18255,7 +18308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -19239,22 +19292,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19269,7 +19322,7 @@
   <dimension ref="C1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19345,16 +19398,16 @@
         <v>121</v>
       </c>
       <c r="E5" s="73">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F5" s="73">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G5" s="73">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="H5" s="73">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="K5" t="s">
         <v>117</v>
@@ -19389,16 +19442,16 @@
         <v>122</v>
       </c>
       <c r="E6" s="73">
+        <v>100</v>
+      </c>
+      <c r="F6" s="73">
         <v>120</v>
       </c>
-      <c r="F6" s="73">
+      <c r="G6" s="73">
         <v>140</v>
       </c>
-      <c r="G6" s="73">
+      <c r="H6" s="73">
         <v>160</v>
-      </c>
-      <c r="H6" s="73">
-        <v>180</v>
       </c>
       <c r="K6" t="s">
         <v>118</v>
@@ -19577,38 +19630,38 @@
       </c>
       <c r="K12">
         <f>E5</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L12">
         <f>E5+E5*(L6/100)</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="M12">
         <f>L12-K12</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="N12">
         <f>(K12*$L$7)/100</f>
-        <v>4.95</v>
+        <v>6.6</v>
       </c>
       <c r="R12" s="70" t="s">
         <v>132</v>
       </c>
       <c r="S12">
         <f>E6</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="T12">
         <f>E6+E6*(T6/100)</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="U12">
         <f>T12-S12</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="V12">
         <f>(S12*$T$7)/100</f>
-        <v>2.04</v>
+        <v>1.7</v>
       </c>
       <c r="Z12" s="70" t="s">
         <v>132</v>
@@ -19646,45 +19699,45 @@
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="J13" s="70" t="s">
         <v>135</v>
       </c>
       <c r="K13">
         <f>F5</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L13">
         <f>F5+F5*(L6/100)</f>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:M15" si="0">L13-K13</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N13">
         <f t="shared" ref="N13:N15" si="1">(K13*$L$7)/100</f>
-        <v>6.6</v>
+        <v>9.9</v>
       </c>
       <c r="R13" s="70" t="s">
         <v>135</v>
       </c>
       <c r="S13">
         <f>F6</f>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="T13">
         <f>F6+F6*(T6/100)</f>
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="U13">
         <f t="shared" ref="U13:U15" si="2">T13-S13</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="V13">
         <f>(S13*$T$7)/100</f>
-        <v>2.38</v>
+        <v>2.04</v>
       </c>
       <c r="Z13" s="70" t="s">
         <v>135</v>
@@ -19722,45 +19775,45 @@
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="J14" s="70" t="s">
         <v>136</v>
       </c>
       <c r="K14">
         <f>G5</f>
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="L14">
         <f>G5+G5*(L6/100)</f>
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>8.25</v>
+        <v>13.2</v>
       </c>
       <c r="R14" s="70" t="s">
         <v>136</v>
       </c>
       <c r="S14">
         <f>G6</f>
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="T14">
         <f>G6+G6*(T6/100)</f>
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="V14">
         <f t="shared" ref="V14:V15" si="3">(S14*$T$7)/100</f>
-        <v>2.72</v>
+        <v>2.38</v>
       </c>
       <c r="Z14" s="70" t="s">
         <v>136</v>
@@ -19805,38 +19858,38 @@
       </c>
       <c r="K15">
         <f>H5</f>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="L15">
         <f>H5+H5*(L6/100)</f>
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>9.9</v>
+        <v>16.5</v>
       </c>
       <c r="R15" s="70" t="s">
         <v>137</v>
       </c>
       <c r="S15">
         <f>H6</f>
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="T15">
         <f>H6+H6*(T6/100)</f>
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="U15">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="V15">
         <f t="shared" si="3"/>
-        <v>3.06</v>
+        <v>2.72</v>
       </c>
       <c r="Z15" s="70" t="s">
         <v>137</v>
@@ -20260,22 +20313,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding prefabs names for results and menu
Former-commit-id: 7b50505b1cd517bdeb87eed3ae35e51a18b454c6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="164">
   <si>
     <t>[sku]</t>
   </si>
@@ -86,22 +86,7 @@
     <t>tier_2</t>
   </si>
   <si>
-    <t>PF_DragonFatMenu</t>
-  </si>
-  <si>
     <t>tier_1</t>
-  </si>
-  <si>
-    <t>PF_DragonReptileResults</t>
-  </si>
-  <si>
-    <t>PF_DragonReptileMenu</t>
-  </si>
-  <si>
-    <t>PF_DragonCrocodileMenu</t>
-  </si>
-  <si>
-    <t>PF_DragonBabyMenu</t>
   </si>
   <si>
     <t>[dotAnimationThreshold]</t>
@@ -522,6 +507,18 @@
   </si>
   <si>
     <t>(how increments a stat in each tier)</t>
+  </si>
+  <si>
+    <t>PF_DragonHelicopterMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonSonicMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonElectricMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonElectricResults</t>
   </si>
 </sst>
 </file>
@@ -1720,6 +1717,24 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1759,24 +1774,6 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1801,15 +1798,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color auto="1"/>
         </right>
         <top style="thin">
@@ -1818,10 +1815,116 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2656,6 +2759,48 @@
         <left style="thin">
           <color auto="1"/>
         </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -3320,160 +3465,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -4423,7 +4414,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4745,7 +4735,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5054,7 +5043,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5671,7 +5659,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5993,7 +5980,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6315,7 +6301,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6624,7 +6609,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7241,7 +7225,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7563,7 +7546,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7885,7 +7867,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15194,59 +15175,59 @@
     <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="64"/>
     <tableColumn id="27" name="[maxAlcohol]" dataDxfId="63"/>
     <tableColumn id="28" name="[alcoholDrain]" dataDxfId="62"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="61"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="60"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="59"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="58"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="57"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="56"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="55"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="54"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="53"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="52"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="51"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="50"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="49"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="48"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="47"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="46"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="45"/>
-    <tableColumn id="46" name="[force]" dataDxfId="44"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="43"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="42"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="41"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="40"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="0"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="39"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="38"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="37"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="3"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="2"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="0"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="1"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="61"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="60"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="59"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="58"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="57"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="56"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="55"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="54"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="53"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="52"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="51"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="50"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="49"/>
+    <tableColumn id="46" name="[force]" dataDxfId="48"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="47"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="46"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="45"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="44"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="43"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="42"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="41"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="B3:T6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="32"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="35"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="31"/>
-    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="30"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="29"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="28"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="27"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="26"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="25"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="24"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="23"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="22"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="21"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="20"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="19"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="18"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="17"/>
+    <tableColumn id="5" name="[order]" dataDxfId="34"/>
+    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="33"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="32"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="31"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="30"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="29"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="28"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="27"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="26"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="25"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="24"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="23"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="22"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="21"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="20"/>
     <tableColumn id="65" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15254,14 +15235,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="11"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="10"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="9">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="16"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="14"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="13"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="12">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15534,8 +15515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15567,7 +15548,7 @@
     <col min="26" max="26" width="23.140625" customWidth="1"/>
     <col min="27" max="27" width="18.85546875" customWidth="1"/>
     <col min="28" max="29" width="24" customWidth="1"/>
-    <col min="30" max="30" width="22.5703125" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" customWidth="1"/>
     <col min="31" max="31" width="30" customWidth="1"/>
     <col min="32" max="32" width="26.7109375" customWidth="1"/>
     <col min="33" max="33" width="14.42578125" customWidth="1"/>
@@ -15608,7 +15589,7 @@
   <sheetData>
     <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -15638,69 +15619,69 @@
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="P2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:54" ht="147" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E3" s="41" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="61" t="s">
+      <c r="M3" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="N3" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="O3" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="P3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="Q3" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="M3" s="58" t="s">
+      <c r="R3" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="S3" s="59" t="s">
         <v>84</v>
-      </c>
-      <c r="O3" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="P3" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q3" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="S3" s="59" t="s">
-        <v>89</v>
       </c>
       <c r="T3" s="52" t="s">
         <v>1</v>
@@ -15711,10 +15692,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E4" s="45">
         <v>0</v>
@@ -15770,10 +15751,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E5" s="45">
         <v>1</v>
@@ -15829,10 +15810,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E6" s="45">
         <v>2</v>
@@ -15944,7 +15925,7 @@
     <row r="9" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -15972,7 +15953,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AW10" s="153" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -16006,7 +15987,7 @@
     </row>
     <row r="12" spans="1:54" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
@@ -16015,76 +15996,76 @@
         <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>69</v>
-      </c>
       <c r="Q12" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AB12" s="26" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="AC12" s="23" t="s">
         <v>10</v>
@@ -16093,37 +16074,37 @@
         <v>11</v>
       </c>
       <c r="AE12" s="22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AF12" s="22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="AG12" s="140" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AH12" s="143" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AI12" s="22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AJ12" s="22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AK12" s="22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AL12" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AM12" s="22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="AN12" s="149" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="AO12" s="147" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AP12" s="27" t="s">
         <v>3</v>
@@ -16132,34 +16113,34 @@
         <v>9</v>
       </c>
       <c r="AR12" s="28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AS12" s="30" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="AT12" s="25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AU12" s="24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="AV12" s="24" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AW12" s="24" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="AX12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="AY12" s="183" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="AY12" s="170" t="s">
+        <v>22</v>
       </c>
       <c r="AZ12" s="28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="BA12" s="21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="BB12" s="24" t="s">
         <v>1</v>
@@ -16170,16 +16151,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="36">
         <v>0</v>
@@ -16248,13 +16229,13 @@
         <v>12</v>
       </c>
       <c r="AC13" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD13" s="102" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE13" s="102" t="s">
-        <v>24</v>
+        <v>152</v>
+      </c>
+      <c r="AD13" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE13" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="AF13" s="38"/>
       <c r="AG13" s="141"/>
@@ -16305,10 +16286,10 @@
       <c r="AX13" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY13" s="184">
+      <c r="AY13" s="171">
         <v>0</v>
       </c>
-      <c r="AZ13" s="180">
+      <c r="AZ13" s="167">
         <v>0</v>
       </c>
       <c r="BA13" s="161">
@@ -16323,13 +16304,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>18</v>
@@ -16401,13 +16382,13 @@
         <v>12</v>
       </c>
       <c r="AC14" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD14" s="102" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE14" s="102" t="s">
-        <v>23</v>
+        <v>152</v>
+      </c>
+      <c r="AD14" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE14" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="AF14" s="38"/>
       <c r="AG14" s="141"/>
@@ -16458,10 +16439,10 @@
       <c r="AX14" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY14" s="184">
+      <c r="AY14" s="171">
         <v>0</v>
       </c>
-      <c r="AZ14" s="180">
+      <c r="AZ14" s="167">
         <v>9</v>
       </c>
       <c r="BA14" s="161">
@@ -16476,13 +16457,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>17</v>
@@ -16554,13 +16535,13 @@
         <v>12</v>
       </c>
       <c r="AC15" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD15" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE15" s="102" t="s">
-        <v>21</v>
+        <v>152</v>
+      </c>
+      <c r="AD15" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE15" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="AF15" s="38"/>
       <c r="AG15" s="141"/>
@@ -16611,10 +16592,10 @@
       <c r="AX15" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY15" s="184">
+      <c r="AY15" s="171">
         <v>0</v>
       </c>
-      <c r="AZ15" s="180">
+      <c r="AZ15" s="167">
         <v>45</v>
       </c>
       <c r="BA15" s="161">
@@ -16630,13 +16611,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F16" s="35" t="s">
         <v>16</v>
@@ -16708,13 +16689,13 @@
         <v>12</v>
       </c>
       <c r="AC16" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD16" s="102" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE16" s="102" t="s">
-        <v>19</v>
+        <v>152</v>
+      </c>
+      <c r="AD16" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE16" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="AF16" s="38"/>
       <c r="AG16" s="141"/>
@@ -16765,10 +16746,10 @@
       <c r="AX16" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY16" s="184">
+      <c r="AY16" s="171">
         <v>0</v>
       </c>
-      <c r="AZ16" s="180">
+      <c r="AZ16" s="167">
         <v>59</v>
       </c>
       <c r="BA16" s="161">
@@ -16783,16 +16764,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="111" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D17" s="112" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="113" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F17" s="114" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="115">
         <v>0</v>
@@ -16861,13 +16842,13 @@
         <v>12</v>
       </c>
       <c r="AC17" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD17" s="122" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE17" s="122" t="s">
-        <v>24</v>
+        <v>150</v>
+      </c>
+      <c r="AD17" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE17" s="123" t="s">
+        <v>163</v>
       </c>
       <c r="AF17" s="123"/>
       <c r="AG17" s="142"/>
@@ -16918,10 +16899,10 @@
       <c r="AX17" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY17" s="185">
+      <c r="AY17" s="172">
         <v>1.2</v>
       </c>
-      <c r="AZ17" s="181">
+      <c r="AZ17" s="168">
         <v>0</v>
       </c>
       <c r="BA17" s="162">
@@ -16936,13 +16917,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="111" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D18" s="112" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="113" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F18" s="114" t="s">
         <v>18</v>
@@ -17014,13 +16995,13 @@
         <v>12</v>
       </c>
       <c r="AC18" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD18" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE18" s="122" t="s">
-        <v>23</v>
+        <v>150</v>
+      </c>
+      <c r="AD18" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE18" s="123" t="s">
+        <v>163</v>
       </c>
       <c r="AF18" s="123"/>
       <c r="AG18" s="142"/>
@@ -17071,10 +17052,10 @@
       <c r="AX18" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY18" s="185">
+      <c r="AY18" s="172">
         <v>1.2</v>
       </c>
-      <c r="AZ18" s="181">
+      <c r="AZ18" s="168">
         <v>9</v>
       </c>
       <c r="BA18" s="162">
@@ -17089,13 +17070,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="111" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D19" s="112" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="113" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F19" s="114" t="s">
         <v>17</v>
@@ -17167,13 +17148,13 @@
         <v>12</v>
       </c>
       <c r="AC19" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD19" s="122" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE19" s="122" t="s">
-        <v>21</v>
+        <v>150</v>
+      </c>
+      <c r="AD19" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE19" s="123" t="s">
+        <v>163</v>
       </c>
       <c r="AF19" s="123"/>
       <c r="AG19" s="142"/>
@@ -17224,10 +17205,10 @@
       <c r="AX19" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY19" s="185">
+      <c r="AY19" s="172">
         <v>1.2</v>
       </c>
-      <c r="AZ19" s="181">
+      <c r="AZ19" s="168">
         <v>45</v>
       </c>
       <c r="BA19" s="162">
@@ -17242,13 +17223,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="111" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D20" s="112" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="113" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F20" s="114" t="s">
         <v>16</v>
@@ -17320,13 +17301,13 @@
         <v>12</v>
       </c>
       <c r="AC20" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD20" s="122" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE20" s="122" t="s">
-        <v>19</v>
+        <v>150</v>
+      </c>
+      <c r="AD20" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE20" s="123" t="s">
+        <v>163</v>
       </c>
       <c r="AF20" s="123"/>
       <c r="AG20" s="142"/>
@@ -17377,10 +17358,10 @@
       <c r="AX20" s="128">
         <v>0.7</v>
       </c>
-      <c r="AY20" s="185">
+      <c r="AY20" s="172">
         <v>1.2</v>
       </c>
-      <c r="AZ20" s="181">
+      <c r="AZ20" s="168">
         <v>59</v>
       </c>
       <c r="BA20" s="162">
@@ -17395,16 +17376,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="36">
         <v>0</v>
@@ -17473,13 +17454,13 @@
         <v>12</v>
       </c>
       <c r="AC21" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD21" s="102" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE21" s="102" t="s">
-        <v>24</v>
+        <v>153</v>
+      </c>
+      <c r="AD21" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE21" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="AF21" s="38"/>
       <c r="AG21" s="141"/>
@@ -17530,10 +17511,10 @@
       <c r="AX21" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY21" s="184">
+      <c r="AY21" s="171">
         <v>1.2</v>
       </c>
-      <c r="AZ21" s="182">
+      <c r="AZ21" s="169">
         <v>0</v>
       </c>
       <c r="BA21" s="106">
@@ -17548,13 +17529,13 @@
         <v>2</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F22" s="35" t="s">
         <v>18</v>
@@ -17626,13 +17607,13 @@
         <v>12</v>
       </c>
       <c r="AC22" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD22" s="102" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE22" s="102" t="s">
-        <v>23</v>
+        <v>153</v>
+      </c>
+      <c r="AD22" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE22" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="AF22" s="38"/>
       <c r="AG22" s="141"/>
@@ -17683,10 +17664,10 @@
       <c r="AX22" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY22" s="184">
+      <c r="AY22" s="171">
         <v>1.2</v>
       </c>
-      <c r="AZ22" s="182">
+      <c r="AZ22" s="169">
         <v>9</v>
       </c>
       <c r="BA22" s="106">
@@ -17701,13 +17682,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D23" s="33" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F23" s="35" t="s">
         <v>17</v>
@@ -17779,13 +17760,13 @@
         <v>12</v>
       </c>
       <c r="AC23" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD23" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE23" s="102" t="s">
-        <v>21</v>
+        <v>153</v>
+      </c>
+      <c r="AD23" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE23" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="AF23" s="38"/>
       <c r="AG23" s="141"/>
@@ -17836,10 +17817,10 @@
       <c r="AX23" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY23" s="184">
+      <c r="AY23" s="171">
         <v>1.2</v>
       </c>
-      <c r="AZ23" s="182">
+      <c r="AZ23" s="169">
         <v>45</v>
       </c>
       <c r="BA23" s="106">
@@ -17855,13 +17836,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D24" s="33" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>16</v>
@@ -17933,13 +17914,13 @@
         <v>12</v>
       </c>
       <c r="AC24" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD24" s="102" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE24" s="102" t="s">
-        <v>19</v>
+        <v>153</v>
+      </c>
+      <c r="AD24" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE24" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="AF24" s="38"/>
       <c r="AG24" s="141"/>
@@ -17990,10 +17971,10 @@
       <c r="AX24" s="106">
         <v>0.7</v>
       </c>
-      <c r="AY24" s="184">
+      <c r="AY24" s="171">
         <v>1.2</v>
       </c>
-      <c r="AZ24" s="182">
+      <c r="AZ24" s="169">
         <v>59</v>
       </c>
       <c r="BA24" s="106">
@@ -18010,49 +17991,49 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="174" t="s">
+      <c r="H25" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="175"/>
-      <c r="J25" s="176" t="s">
+      <c r="I25" s="181"/>
+      <c r="J25" s="182" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="177"/>
-      <c r="L25" s="177"/>
-      <c r="M25" s="177"/>
-      <c r="N25" s="177"/>
-      <c r="O25" s="178"/>
+      <c r="K25" s="183"/>
+      <c r="L25" s="183"/>
+      <c r="M25" s="183"/>
+      <c r="N25" s="183"/>
+      <c r="O25" s="184"/>
       <c r="P25" s="79"/>
-      <c r="Q25" s="170" t="s">
-        <v>145</v>
-      </c>
-      <c r="R25" s="171"/>
-      <c r="S25" s="171"/>
-      <c r="T25" s="171"/>
-      <c r="U25" s="172" t="s">
+      <c r="Q25" s="176" t="s">
+        <v>140</v>
+      </c>
+      <c r="R25" s="177"/>
+      <c r="S25" s="177"/>
+      <c r="T25" s="177"/>
+      <c r="U25" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="173"/>
-      <c r="W25" s="173"/>
-      <c r="X25" s="173"/>
+      <c r="V25" s="179"/>
+      <c r="W25" s="179"/>
+      <c r="X25" s="179"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="167" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI25" s="168"/>
-      <c r="AJ25" s="168"/>
-      <c r="AK25" s="168"/>
-      <c r="AL25" s="168"/>
-      <c r="AM25" s="168"/>
-      <c r="AN25" s="169"/>
+      <c r="AH25" s="173" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI25" s="174"/>
+      <c r="AJ25" s="174"/>
+      <c r="AK25" s="174"/>
+      <c r="AL25" s="174"/>
+      <c r="AM25" s="174"/>
+      <c r="AN25" s="175"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -18065,19 +18046,19 @@
     </row>
     <row r="30" spans="1:54" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F30" s="66" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
@@ -18085,10 +18066,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E31" s="64">
         <v>5</v>
@@ -18103,10 +18084,10 @@
         <v>2</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D32" s="64" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E32" s="64">
         <v>15</v>
@@ -18121,10 +18102,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E33" s="64">
         <v>25</v>
@@ -18139,10 +18120,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D34" s="64" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E34" s="64">
         <v>5</v>
@@ -18157,10 +18138,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D35" s="64" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E35" s="64">
         <v>15</v>
@@ -18175,10 +18156,10 @@
         <v>2</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E36" s="64">
         <v>25</v>
@@ -18193,10 +18174,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E37" s="64">
         <v>5</v>
@@ -18211,10 +18192,10 @@
         <v>2</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E38" s="64">
         <v>15</v>
@@ -18229,10 +18210,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D39" s="68" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E39" s="68">
         <v>25</v>
@@ -18326,25 +18307,25 @@
   <sheetData>
     <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="72" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="179" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
+      <c r="E3" s="185" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
       <c r="J3" s="70" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R3" s="70" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Z3" s="70" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
@@ -18362,19 +18343,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="L4" s="69">
         <v>30</v>
       </c>
       <c r="S4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="T4" s="69">
         <v>30</v>
       </c>
       <c r="AA4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="AB4" s="69">
         <v>30</v>
@@ -18382,7 +18363,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="71" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E5" s="73">
         <v>100</v>
@@ -18397,36 +18378,36 @@
         <v>250</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L5" s="69">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="T5" s="69">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AB5" s="69">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="71" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E6" s="73">
         <v>100</v>
@@ -18441,36 +18422,36 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L6" s="69">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="T6" s="69">
         <v>50</v>
       </c>
       <c r="U6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AB6" s="69">
         <v>50</v>
       </c>
       <c r="AC6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="80" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E7" s="81">
         <v>240</v>
@@ -18485,39 +18466,39 @@
         <v>285</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>3.3</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>1.7</v>
       </c>
       <c r="U7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
         <v>1.7</v>
       </c>
       <c r="AC7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="84" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E8" s="82">
         <v>0</v>
@@ -18534,19 +18515,19 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="V10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AD10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="85"/>
       <c r="D11" s="86" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -18556,53 +18537,53 @@
       <c r="G11" s="87"/>
       <c r="H11" s="88"/>
       <c r="J11" s="70" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K11" s="74" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L11" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="M11" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="M11" s="74" t="s">
-        <v>139</v>
-      </c>
       <c r="N11" s="74" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="R11" s="77" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T11" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="U11" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="U11" s="74" t="s">
-        <v>139</v>
-      </c>
       <c r="V11" s="74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="W11" s="74"/>
       <c r="X11" s="74"/>
       <c r="Z11" s="70" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AA11" s="74" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AB11" s="74" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AC11" s="74" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="AD11" s="74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18613,7 +18594,7 @@
       <c r="G12" s="90"/>
       <c r="H12" s="78"/>
       <c r="J12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -18632,7 +18613,7 @@
         <v>3.3</v>
       </c>
       <c r="R12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -18651,7 +18632,7 @@
         <v>1.7</v>
       </c>
       <c r="Z12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AV17)/'special dragons'!AU17,1)</f>
@@ -18672,24 +18653,24 @@
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="89" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D13" s="90" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E13" s="91">
         <v>1</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>206.6</v>
       </c>
       <c r="J13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -18708,7 +18689,7 @@
         <v>4.95</v>
       </c>
       <c r="R13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -18727,7 +18708,7 @@
         <v>2.04</v>
       </c>
       <c r="Z13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AV18)/'special dragons'!AU18,1)</f>
@@ -18748,24 +18729,24 @@
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="89" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E14" s="91">
         <v>10</v>
       </c>
       <c r="F14" s="90"/>
       <c r="G14" s="75" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>163.80000000000001</v>
       </c>
       <c r="J14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -18784,7 +18765,7 @@
         <v>6.6</v>
       </c>
       <c r="R14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -18803,7 +18784,7 @@
         <v>2.38</v>
       </c>
       <c r="Z14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AV19)/'special dragons'!AU19,1)</f>
@@ -18824,24 +18805,24 @@
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="89" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D15" s="90" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E15" s="91">
         <v>10</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
         <v>13.3</v>
       </c>
       <c r="J15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -18860,7 +18841,7 @@
         <v>8.25</v>
       </c>
       <c r="R15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -18879,7 +18860,7 @@
         <v>2.72</v>
       </c>
       <c r="Z15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AV20)/'special dragons'!AU20,1)</f>
@@ -18901,7 +18882,7 @@
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="89"/>
       <c r="D16" s="96" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
@@ -19292,22 +19273,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19339,25 +19320,25 @@
   <sheetData>
     <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="72" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="179" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
+      <c r="E3" s="185" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
       <c r="J3" s="70" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R3" s="70" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Z3" s="70" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
@@ -19375,19 +19356,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="L4" s="69">
         <v>30</v>
       </c>
       <c r="S4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="T4" s="69">
         <v>30</v>
       </c>
       <c r="AA4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="AB4" s="69">
         <v>30</v>
@@ -19395,7 +19376,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="71" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E5" s="73">
         <v>200</v>
@@ -19410,36 +19391,36 @@
         <v>500</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L5" s="69">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="T5" s="69">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AB5" s="69">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="71" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E6" s="73">
         <v>100</v>
@@ -19454,36 +19435,36 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L6" s="69">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="T6" s="69">
         <v>50</v>
       </c>
       <c r="U6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AB6" s="69">
         <v>50</v>
       </c>
       <c r="AC6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="80" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E7" s="81">
         <v>100</v>
@@ -19498,39 +19479,39 @@
         <v>130</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>3.3</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="S7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>1.7</v>
       </c>
       <c r="U7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AA7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
         <v>1.7</v>
       </c>
       <c r="AC7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="84" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E8" s="82">
         <v>0</v>
@@ -19547,19 +19528,19 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="V10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AD10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="85"/>
       <c r="D11" s="86" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -19569,53 +19550,53 @@
       <c r="G11" s="87"/>
       <c r="H11" s="88"/>
       <c r="J11" s="70" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K11" s="74" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L11" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="M11" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="M11" s="74" t="s">
-        <v>139</v>
-      </c>
       <c r="N11" s="74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="R11" s="77" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T11" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="U11" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="U11" s="74" t="s">
-        <v>139</v>
-      </c>
       <c r="V11" s="74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="W11" s="74"/>
       <c r="X11" s="74"/>
       <c r="Z11" s="70" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AA11" s="74" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AB11" s="74" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AC11" s="74" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="AD11" s="74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19626,7 +19607,7 @@
       <c r="G12" s="90"/>
       <c r="H12" s="78"/>
       <c r="J12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -19645,7 +19626,7 @@
         <v>6.6</v>
       </c>
       <c r="R12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -19664,7 +19645,7 @@
         <v>1.7</v>
       </c>
       <c r="Z12" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AV13)/'special dragons'!AU13,1)</f>
@@ -19685,24 +19666,24 @@
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="89" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D13" s="90" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E13" s="91">
         <v>0</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>200</v>
       </c>
       <c r="J13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -19721,7 +19702,7 @@
         <v>9.9</v>
       </c>
       <c r="R13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -19740,7 +19721,7 @@
         <v>2.04</v>
       </c>
       <c r="Z13" s="70" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AV14)/'special dragons'!AU14,1)</f>
@@ -19761,24 +19742,24 @@
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="89" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E14" s="91">
         <v>0</v>
       </c>
       <c r="F14" s="90"/>
       <c r="G14" s="75" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>100</v>
       </c>
       <c r="J14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -19797,7 +19778,7 @@
         <v>13.2</v>
       </c>
       <c r="R14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -19816,7 +19797,7 @@
         <v>2.38</v>
       </c>
       <c r="Z14" s="70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AV15)/'special dragons'!AU15,1)</f>
@@ -19837,24 +19818,24 @@
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="89" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D15" s="90" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E15" s="91">
         <v>0</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(12+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(12+E11,47,1,1,"special dragons")),1)</f>
         <v>13.3</v>
       </c>
       <c r="J15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -19873,7 +19854,7 @@
         <v>16.5</v>
       </c>
       <c r="R15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -19892,7 +19873,7 @@
         <v>2.72</v>
       </c>
       <c r="Z15" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AV16)/'special dragons'!AU16,1)</f>
@@ -19914,7 +19895,7 @@
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="89"/>
       <c r="D16" s="96" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
@@ -20313,22 +20294,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20353,18 +20334,18 @@
   <sheetData>
     <row r="4" spans="6:9" x14ac:dyDescent="0.25">
       <c r="G4" s="95" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H4" s="95" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I4" s="95" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -20378,7 +20359,7 @@
     </row>
     <row r="6" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G6">
         <v>240</v>
@@ -20392,7 +20373,7 @@
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G7">
         <v>365</v>
@@ -20406,7 +20387,7 @@
     </row>
     <row r="8" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G8">
         <v>410</v>
@@ -20420,7 +20401,7 @@
     </row>
     <row r="9" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G9">
         <f ca="1">Electric!H13</f>

</xml_diff>

<commit_message>
Content - First balancing for the special LAB
Former-commit-id: 58bd572958de45a6bf2673c338225a12c9bdf9b9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
-    <sheet name="Electric" sheetId="11" r:id="rId2"/>
-    <sheet name="Helicopter" sheetId="13" r:id="rId3"/>
-    <sheet name="DATA" sheetId="12" r:id="rId4"/>
+    <sheet name="Special Missions" sheetId="14" r:id="rId2"/>
+    <sheet name="Electric" sheetId="11" r:id="rId3"/>
+    <sheet name="Helicopter" sheetId="13" r:id="rId4"/>
+    <sheet name="DATA" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="189">
   <si>
     <t>[sku]</t>
   </si>
@@ -520,12 +521,87 @@
   <si>
     <t>PF_DragonElectricResults</t>
   </si>
+  <si>
+    <t>[index]</t>
+  </si>
+  <si>
+    <t>[cooldownMinutes]</t>
+  </si>
+  <si>
+    <t>[removeMissionPCCoefA]</t>
+  </si>
+  <si>
+    <t>[removeMissionPCCoefB]</t>
+  </si>
+  <si>
+    <t>[color]</t>
+  </si>
+  <si>
+    <t>TID_MISSION_DIFFICULTY_EASY</t>
+  </si>
+  <si>
+    <t>ffc000</t>
+  </si>
+  <si>
+    <t>TID_MISSION_DIFFICULTY_MEDIUM</t>
+  </si>
+  <si>
+    <t>ff8800</t>
+  </si>
+  <si>
+    <t>TID_MISSION_DIFFICULTY_HARD</t>
+  </si>
+  <si>
+    <t>ff5800</t>
+  </si>
+  <si>
+    <t>[quantityModifier]</t>
+  </si>
+  <si>
+    <t>[missionSCRewardMultiplier]</t>
+  </si>
+  <si>
+    <t>Special Mission Dragon Modifiers Definitions</t>
+  </si>
+  <si>
+    <t>specialDragonTier1</t>
+  </si>
+  <si>
+    <t>specialDragonTier2</t>
+  </si>
+  <si>
+    <t>specialDragonTier3</t>
+  </si>
+  <si>
+    <t>specialDragonTier4</t>
+  </si>
+  <si>
+    <t>SPECIAL MISSION DIFFICULTY DEFINITIONS</t>
+  </si>
+  <si>
+    <t>specialMissionEasy</t>
+  </si>
+  <si>
+    <t>specialMissionMedium</t>
+  </si>
+  <si>
+    <t>specialMissionHard</t>
+  </si>
+  <si>
+    <t>[maxRewardGoldenFragments]</t>
+  </si>
+  <si>
+    <t>{missionSpecialDragonModifiersDefinitions}</t>
+  </si>
+  <si>
+    <t>{specialMissionDifficultyDefinitions}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,8 +669,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="28">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +839,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1283,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1735,6 +1826,46 @@
     <xf numFmtId="0" fontId="7" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1771,6 +1902,9 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1778,155 +1912,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="104">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="125">
     <dxf>
       <fill>
         <patternFill>
@@ -1984,6 +1970,434 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2235,19 +2649,19 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3476,6 +3890,154 @@
         <horizontal style="thin">
           <color auto="1"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -15145,89 +15707,89 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BB24" totalsRowShown="0" headerRowBorderDxfId="111" totalsRowBorderDxfId="110">
   <autoFilter ref="B12:BB24"/>
   <tableColumns count="53">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="88"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="86"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="85"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="84"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="83"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="82"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="81"/>
-    <tableColumn id="10" name="[health]" dataDxfId="80"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="79"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="78"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="77"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="76"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="75"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="74"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="73"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="72"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="71"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="70"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="69"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="68"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="67"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="66"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="65"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="64"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="63"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="62"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="3"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="2"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="0"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="1"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="61"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="60"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="59"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="58"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="57"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="56"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="55"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="54"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="53"/>
-    <tableColumn id="42" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="43" name="[tidDesc]" dataDxfId="51"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="50"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="49"/>
-    <tableColumn id="46" name="[force]" dataDxfId="48"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="47"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="46"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="45"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="44"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="43"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="42"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="41"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="40"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="109"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="108"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="107"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="106"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="105"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="104"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="103"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="102"/>
+    <tableColumn id="10" name="[health]" dataDxfId="101"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="100"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="99"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="98"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="97"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="96"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="95"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="94"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="93"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="92"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="91"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="90"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="89"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="88"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="87"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="86"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="85"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="84"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="83"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="82"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="81"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="80"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="79"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="78"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="77"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="76"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="75"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="74"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="73"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="72"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="71"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="70"/>
+    <tableColumn id="42" name="[tidName]" dataDxfId="69"/>
+    <tableColumn id="43" name="[tidDesc]" dataDxfId="68"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="67"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="66"/>
+    <tableColumn id="46" name="[force]" dataDxfId="65"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="64"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="63"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="62"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="61"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="60"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="59"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="58"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:T6" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53">
   <autoFilter ref="B3:T6"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="35"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="52"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="34"/>
-    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="33"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="32"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="31"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="30"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="29"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="28"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="27"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="26"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="25"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="24"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="23"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="22"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="21"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="20"/>
+    <tableColumn id="5" name="[order]" dataDxfId="51"/>
+    <tableColumn id="7" name="[unlockPriceGoldenFragments]" dataDxfId="50"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="49"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="48"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="47"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="46"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="45"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="44"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="43"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="42"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="41"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="40"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="39"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="38"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="37"/>
     <tableColumn id="65" name="[trackingSku]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15235,18 +15797,50 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="14"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="13"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="12">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="31"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="30"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="29">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="B3:J6"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="7" name="[index]" dataDxfId="24"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="23"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="22"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="21"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="20"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="19"/>
+    <tableColumn id="10" name="[color]" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B11:F15"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="10"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="9"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -15513,10 +16107,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15701,10 +16298,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="46">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G4" s="47">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="H4" s="57">
         <v>30</v>
@@ -15734,7 +16331,7 @@
         <v>50</v>
       </c>
       <c r="Q4" s="55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R4" s="55">
         <v>1</v>
@@ -15760,10 +16357,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="46">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G5" s="47">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="H5" s="57">
         <v>30</v>
@@ -15793,7 +16390,7 @@
         <v>50</v>
       </c>
       <c r="Q5" s="55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R5" s="55">
         <v>1</v>
@@ -15819,10 +16416,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="50">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G6" s="51">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="H6" s="57">
         <v>30</v>
@@ -15852,7 +16449,7 @@
         <v>50</v>
       </c>
       <c r="Q6" s="55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R6" s="55">
         <v>1</v>
@@ -17991,44 +18588,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="180" t="s">
+      <c r="H25" s="200" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="181"/>
-      <c r="J25" s="182" t="s">
+      <c r="I25" s="201"/>
+      <c r="J25" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="183"/>
-      <c r="L25" s="183"/>
-      <c r="M25" s="183"/>
-      <c r="N25" s="183"/>
-      <c r="O25" s="184"/>
+      <c r="K25" s="203"/>
+      <c r="L25" s="203"/>
+      <c r="M25" s="203"/>
+      <c r="N25" s="203"/>
+      <c r="O25" s="204"/>
       <c r="P25" s="79"/>
-      <c r="Q25" s="176" t="s">
+      <c r="Q25" s="196" t="s">
         <v>140</v>
       </c>
-      <c r="R25" s="177"/>
-      <c r="S25" s="177"/>
-      <c r="T25" s="177"/>
-      <c r="U25" s="178" t="s">
+      <c r="R25" s="197"/>
+      <c r="S25" s="197"/>
+      <c r="T25" s="197"/>
+      <c r="U25" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="179"/>
-      <c r="W25" s="179"/>
-      <c r="X25" s="179"/>
+      <c r="V25" s="199"/>
+      <c r="W25" s="199"/>
+      <c r="X25" s="199"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="173" t="s">
+      <c r="AH25" s="193" t="s">
         <v>141</v>
       </c>
-      <c r="AI25" s="174"/>
-      <c r="AJ25" s="174"/>
-      <c r="AK25" s="174"/>
-      <c r="AL25" s="174"/>
-      <c r="AM25" s="174"/>
-      <c r="AN25" s="175"/>
+      <c r="AI25" s="194"/>
+      <c r="AJ25" s="194"/>
+      <c r="AK25" s="194"/>
+      <c r="AL25" s="194"/>
+      <c r="AM25" s="194"/>
+      <c r="AN25" s="195"/>
     </row>
     <row r="27" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
@@ -18232,43 +18829,43 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="103" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="102" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T6">
-    <cfRule type="duplicateValues" dxfId="101" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="100" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="99" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="98" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="97" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB17">
-    <cfRule type="duplicateValues" dxfId="96" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB18:BB20">
-    <cfRule type="duplicateValues" dxfId="95" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB13">
-    <cfRule type="duplicateValues" dxfId="94" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB14:BB16">
-    <cfRule type="duplicateValues" dxfId="93" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB21">
-    <cfRule type="duplicateValues" dxfId="92" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB22:BB24">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -18286,6 +18883,286 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="B1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="16" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="173"/>
+    </row>
+    <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="175" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="175" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="176" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="177" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="177" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="178" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="178" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="179" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="180" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="182" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="182">
+        <v>0</v>
+      </c>
+      <c r="E4" s="183">
+        <v>15</v>
+      </c>
+      <c r="F4" s="183">
+        <v>1</v>
+      </c>
+      <c r="G4" s="184">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="184">
+        <v>1</v>
+      </c>
+      <c r="I4" s="185" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" s="186" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="182" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="182">
+        <v>1</v>
+      </c>
+      <c r="E5" s="183">
+        <v>60</v>
+      </c>
+      <c r="F5" s="183">
+        <v>2</v>
+      </c>
+      <c r="G5" s="184">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="184">
+        <v>1</v>
+      </c>
+      <c r="I5" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" s="186" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="182" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="182">
+        <v>2</v>
+      </c>
+      <c r="E6" s="183">
+        <v>240</v>
+      </c>
+      <c r="F6" s="183">
+        <v>5</v>
+      </c>
+      <c r="G6" s="184">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="184">
+        <v>1</v>
+      </c>
+      <c r="I6" s="185" t="s">
+        <v>173</v>
+      </c>
+      <c r="J6" s="187" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="11" spans="2:13" ht="159" x14ac:dyDescent="0.25">
+      <c r="B11" s="188" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="189" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="189" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="190" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="190" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="192" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="192">
+        <v>1</v>
+      </c>
+      <c r="E12" s="192">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="192" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="192">
+        <v>2</v>
+      </c>
+      <c r="E13" s="192">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="192" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="192">
+        <v>3</v>
+      </c>
+      <c r="E14" s="192">
+        <v>3</v>
+      </c>
+      <c r="F14" s="192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="192" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="192">
+        <v>4</v>
+      </c>
+      <c r="E15" s="192">
+        <v>4</v>
+      </c>
+      <c r="F15" s="192">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:D6">
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
@@ -18312,12 +19189,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="185" t="s">
+      <c r="E3" s="206" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="206"/>
       <c r="J3" s="70" t="s">
         <v>116</v>
       </c>
@@ -19273,22 +20150,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19298,7 +20175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
@@ -19325,12 +20202,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="70"/>
-      <c r="E3" s="185" t="s">
+      <c r="E3" s="206" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="206"/>
       <c r="J3" s="70" t="s">
         <v>116</v>
       </c>
@@ -20294,22 +21171,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20319,7 +21196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F4:I9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Setting stats upgrades steps
Former-commit-id: 0e8e237411abb6f8f122a7827f7e913204d9730e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -4976,6 +4976,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5297,6 +5298,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5389,7 +5391,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>206.6</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5605,6 +5607,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5697,7 +5700,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>163.80000000000001</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6005,7 +6008,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.3</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6221,6 +6224,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6542,6 +6546,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6863,6 +6868,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6955,7 +6961,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>206.6</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7171,6 +7177,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7263,7 +7270,7 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>163.80000000000001</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7571,7 +7578,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.3</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7787,6 +7794,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8108,6 +8116,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8429,6 +8438,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16112,8 +16122,8 @@
   </sheetPr>
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16304,7 +16314,7 @@
         <v>150</v>
       </c>
       <c r="H4" s="57">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I4" s="57">
         <v>0</v>
@@ -16313,7 +16323,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="56">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L4" s="56">
         <v>0</v>
@@ -16322,7 +16332,7 @@
         <v>50</v>
       </c>
       <c r="N4" s="62">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O4" s="62">
         <v>0</v>
@@ -16363,7 +16373,7 @@
         <v>150</v>
       </c>
       <c r="H5" s="57">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I5" s="57">
         <v>0</v>
@@ -16372,7 +16382,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="56">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L5" s="56">
         <v>0</v>
@@ -16381,7 +16391,7 @@
         <v>50</v>
       </c>
       <c r="N5" s="62">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O5" s="62">
         <v>0</v>
@@ -16422,7 +16432,7 @@
         <v>150</v>
       </c>
       <c r="H6" s="57">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I6" s="57">
         <v>0</v>
@@ -16431,7 +16441,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="56">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L6" s="56">
         <v>0</v>
@@ -16440,7 +16450,7 @@
         <v>50</v>
       </c>
       <c r="N6" s="62">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O6" s="62">
         <v>0</v>
@@ -18889,7 +18899,7 @@
   </sheetPr>
   <dimension ref="B1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -19167,7 +19177,7 @@
   <dimension ref="C1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19223,19 +19233,19 @@
         <v>133</v>
       </c>
       <c r="L4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="S4" t="s">
         <v>133</v>
       </c>
       <c r="T4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AA4" t="s">
         <v>133</v>
       </c>
       <c r="AB4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
@@ -19347,7 +19357,7 @@
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="M7" t="s">
         <v>151</v>
@@ -19357,7 +19367,7 @@
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="U7" t="s">
         <v>151</v>
@@ -19367,7 +19377,7 @@
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="AC7" t="s">
         <v>151</v>
@@ -19408,7 +19418,7 @@
       </c>
       <c r="E11" s="87">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="87"/>
@@ -19487,7 +19497,7 @@
       </c>
       <c r="N12">
         <f>(K12*$L$7)/100</f>
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="R12" s="70" t="s">
         <v>127</v>
@@ -19506,7 +19516,7 @@
       </c>
       <c r="V12">
         <f>(S12*$T$7)/100</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="Z12" s="70" t="s">
         <v>127</v>
@@ -19525,7 +19535,7 @@
       </c>
       <c r="AD12">
         <f>(AA12*$AB$7)/100</f>
-        <v>0.17169999999999999</v>
+        <v>0.2525</v>
       </c>
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19536,7 +19546,7 @@
         <v>119</v>
       </c>
       <c r="E13" s="91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="90"/>
       <c r="G13" s="75" t="s">
@@ -19544,7 +19554,7 @@
       </c>
       <c r="H13" s="76">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>206.6</v>
+        <v>100</v>
       </c>
       <c r="J13" s="70" t="s">
         <v>130</v>
@@ -19563,7 +19573,7 @@
       </c>
       <c r="N13">
         <f>(K13*$L$7)/100</f>
-        <v>4.95</v>
+        <v>7.5</v>
       </c>
       <c r="R13" s="70" t="s">
         <v>130</v>
@@ -19582,7 +19592,7 @@
       </c>
       <c r="V13">
         <f t="shared" ref="V13:V15" si="2">(S13*$T$7)/100</f>
-        <v>2.04</v>
+        <v>3</v>
       </c>
       <c r="Z13" s="70" t="s">
         <v>130</v>
@@ -19601,7 +19611,7 @@
       </c>
       <c r="AD13">
         <f t="shared" ref="AD13:AD15" si="3">(AA13*$AB$7)/100</f>
-        <v>0.18189999999999998</v>
+        <v>0.26750000000000002</v>
       </c>
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19612,7 +19622,7 @@
         <v>121</v>
       </c>
       <c r="E14" s="91">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F14" s="90"/>
       <c r="G14" s="75" t="s">
@@ -19620,7 +19630,7 @@
       </c>
       <c r="H14" s="76">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
-        <v>163.80000000000001</v>
+        <v>100</v>
       </c>
       <c r="J14" s="70" t="s">
         <v>131</v>
@@ -19639,7 +19649,7 @@
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N15" si="4">(K14*$L$7)/100</f>
-        <v>6.6</v>
+        <v>10</v>
       </c>
       <c r="R14" s="70" t="s">
         <v>131</v>
@@ -19658,7 +19668,7 @@
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>2.38</v>
+        <v>3.5</v>
       </c>
       <c r="Z14" s="70" t="s">
         <v>131</v>
@@ -19677,7 +19687,7 @@
       </c>
       <c r="AD14">
         <f t="shared" si="3"/>
-        <v>0.1938</v>
+        <v>0.28499999999999998</v>
       </c>
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19688,7 +19698,7 @@
         <v>122</v>
       </c>
       <c r="E15" s="91">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F15" s="90"/>
       <c r="G15" s="75" t="s">
@@ -19696,7 +19706,7 @@
       </c>
       <c r="H15" s="76">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,48,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,47,1,1,"special dragons")),1)</f>
-        <v>13.3</v>
+        <v>10.1</v>
       </c>
       <c r="J15" s="70" t="s">
         <v>132</v>
@@ -19715,7 +19725,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>8.25</v>
+        <v>12.5</v>
       </c>
       <c r="R15" s="70" t="s">
         <v>132</v>
@@ -19734,7 +19744,7 @@
       </c>
       <c r="V15">
         <f t="shared" si="2"/>
-        <v>2.72</v>
+        <v>4</v>
       </c>
       <c r="Z15" s="70" t="s">
         <v>132</v>
@@ -19753,7 +19763,7 @@
       </c>
       <c r="AD15">
         <f t="shared" si="3"/>
-        <v>0.20399999999999999</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
@@ -19763,7 +19773,7 @@
       </c>
       <c r="E16" s="96">
         <f>SUM(E13:E15)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -20179,8 +20189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20236,19 +20246,19 @@
         <v>133</v>
       </c>
       <c r="L4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="S4" t="s">
         <v>133</v>
       </c>
       <c r="T4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AA4" t="s">
         <v>133</v>
       </c>
       <c r="AB4" s="69">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
@@ -20360,7 +20370,7 @@
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="M7" t="s">
         <v>151</v>
@@ -20370,7 +20380,7 @@
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="U7" t="s">
         <v>151</v>
@@ -20380,7 +20390,7 @@
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="AC7" t="s">
         <v>151</v>
@@ -20500,7 +20510,7 @@
       </c>
       <c r="N12">
         <f>(K12*$L$7)/100</f>
-        <v>6.6</v>
+        <v>10</v>
       </c>
       <c r="R12" s="70" t="s">
         <v>127</v>
@@ -20519,7 +20529,7 @@
       </c>
       <c r="V12">
         <f>(S12*$T$7)/100</f>
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="Z12" s="70" t="s">
         <v>127</v>
@@ -20538,7 +20548,7 @@
       </c>
       <c r="AD12">
         <f>(AA12*$AB$7)/100</f>
-        <v>0.2261</v>
+        <v>0.33250000000000002</v>
       </c>
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20576,7 +20586,7 @@
       </c>
       <c r="N13">
         <f t="shared" ref="N13:N15" si="1">(K13*$L$7)/100</f>
-        <v>9.9</v>
+        <v>15</v>
       </c>
       <c r="R13" s="70" t="s">
         <v>130</v>
@@ -20595,7 +20605,7 @@
       </c>
       <c r="V13">
         <f>(S13*$T$7)/100</f>
-        <v>2.04</v>
+        <v>3</v>
       </c>
       <c r="Z13" s="70" t="s">
         <v>130</v>
@@ -20614,7 +20624,7 @@
       </c>
       <c r="AD13">
         <f>(AA13*$AB$7)/100</f>
-        <v>0.24989999999999998</v>
+        <v>0.36749999999999999</v>
       </c>
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20652,7 +20662,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>13.2</v>
+        <v>20</v>
       </c>
       <c r="R14" s="70" t="s">
         <v>131</v>
@@ -20671,7 +20681,7 @@
       </c>
       <c r="V14">
         <f t="shared" ref="V14:V15" si="3">(S14*$T$7)/100</f>
-        <v>2.38</v>
+        <v>3.5</v>
       </c>
       <c r="Z14" s="70" t="s">
         <v>131</v>
@@ -20690,7 +20700,7 @@
       </c>
       <c r="AD14">
         <f t="shared" ref="AD14:AD15" si="4">(AA14*$AB$7)/100</f>
-        <v>0.27200000000000002</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20728,7 +20738,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>25</v>
       </c>
       <c r="R15" s="70" t="s">
         <v>132</v>
@@ -20747,7 +20757,7 @@
       </c>
       <c r="V15">
         <f t="shared" si="3"/>
-        <v>2.72</v>
+        <v>4</v>
       </c>
       <c r="Z15" s="70" t="s">
         <v>132</v>
@@ -20766,7 +20776,7 @@
       </c>
       <c r="AD15">
         <f t="shared" si="4"/>
-        <v>0.29410000000000003</v>
+        <v>0.4325</v>
       </c>
     </row>
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
@@ -21282,15 +21292,15 @@
       </c>
       <c r="G9">
         <f ca="1">Electric!H13</f>
-        <v>206.6</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <f ca="1">Electric!H14</f>
-        <v>163.80000000000001</v>
+        <v>100</v>
       </c>
       <c r="I9">
         <f ca="1">Electric!H15</f>
-        <v>13.3</v>
+        <v>10.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some stats for both dragons
Former-commit-id: 68990e43c0938526ab6ed020eba972d7bd60de73
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -4976,7 +4976,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5298,7 +5297,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5607,7 +5605,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6224,7 +6221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6546,7 +6542,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6868,7 +6863,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7177,7 +7171,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7794,7 +7787,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8116,7 +8108,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8438,7 +8429,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16122,8 +16112,8 @@
   </sheetPr>
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S4" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16782,13 +16772,13 @@
         <v>200</v>
       </c>
       <c r="K13" s="157">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="L13" s="157">
         <v>0</v>
       </c>
       <c r="M13" s="157">
-        <v>8.9999999999999998E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="N13" s="157">
         <v>30</v>
@@ -16821,7 +16811,7 @@
         <v>9</v>
       </c>
       <c r="X13" s="159">
-        <v>40000</v>
+        <v>6000</v>
       </c>
       <c r="Y13" s="138">
         <v>2</v>
@@ -16935,7 +16925,7 @@
         <v>300</v>
       </c>
       <c r="K14" s="157">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="L14" s="157">
         <v>0</v>
@@ -16974,7 +16964,7 @@
         <v>10</v>
       </c>
       <c r="X14" s="159">
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="Y14" s="138">
         <v>3</v>
@@ -17088,7 +17078,7 @@
         <v>400</v>
       </c>
       <c r="K15" s="157">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="L15" s="157">
         <v>0</v>
@@ -17127,7 +17117,7 @@
         <v>10</v>
       </c>
       <c r="X15" s="159">
-        <v>63000</v>
+        <v>85000</v>
       </c>
       <c r="Y15" s="138">
         <v>4</v>
@@ -17242,7 +17232,7 @@
         <v>500</v>
       </c>
       <c r="K16" s="157">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="L16" s="157">
         <v>0</v>
@@ -17281,7 +17271,7 @@
         <v>10</v>
       </c>
       <c r="X16" s="159">
-        <v>97000</v>
+        <v>105000</v>
       </c>
       <c r="Y16" s="138">
         <v>5</v>
@@ -17395,7 +17385,7 @@
         <v>100</v>
       </c>
       <c r="K17" s="135">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="L17" s="135">
         <v>0</v>
@@ -17434,7 +17424,7 @@
         <v>9</v>
       </c>
       <c r="X17" s="136">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="Y17" s="119">
         <v>2</v>
@@ -17548,7 +17538,7 @@
         <v>150</v>
       </c>
       <c r="K18" s="135">
-        <v>1.9</v>
+        <v>2.4</v>
       </c>
       <c r="L18" s="135">
         <v>0</v>
@@ -17587,7 +17577,7 @@
         <v>10</v>
       </c>
       <c r="X18" s="136">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="Y18" s="119">
         <v>3</v>
@@ -17701,7 +17691,7 @@
         <v>200</v>
       </c>
       <c r="K19" s="135">
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="L19" s="135">
         <v>0</v>
@@ -17740,7 +17730,7 @@
         <v>10</v>
       </c>
       <c r="X19" s="136">
-        <v>50000</v>
+        <v>65000</v>
       </c>
       <c r="Y19" s="119">
         <v>4</v>
@@ -17854,7 +17844,7 @@
         <v>250</v>
       </c>
       <c r="K20" s="135">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="L20" s="135">
         <v>0</v>
@@ -17893,7 +17883,7 @@
         <v>10</v>
       </c>
       <c r="X20" s="136">
-        <v>80000</v>
+        <v>95000</v>
       </c>
       <c r="Y20" s="119">
         <v>5</v>

</xml_diff>

<commit_message>
Adding TIDs to replace "boost"
Former-commit-id: 9f2384284ee1ccd6c6c82c2e9ed010f76f6617ff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="215">
   <si>
     <t>[sku]</t>
   </si>
@@ -661,6 +661,18 @@
   </si>
   <si>
     <t>[energyRestartThreshold]</t>
+  </si>
+  <si>
+    <t>[tidBoostAction]</t>
+  </si>
+  <si>
+    <t>[tidBoostReminder]</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_BOOST_ABILITY</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_BOOST_ABILITY</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +1983,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="142">
+  <dxfs count="144">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2201,6 +2213,54 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -16230,104 +16290,106 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="141" totalsRowBorderDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="143" totalsRowBorderDxfId="142">
   <autoFilter ref="B12:AZ24"/>
   <tableColumns count="51">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="139"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="138"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="137"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="136"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="135"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="134"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="133"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="132"/>
-    <tableColumn id="10" name="[health]" dataDxfId="131"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="130"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="129"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="128"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="127"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="126"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="125"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="124"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="123"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="122"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="121"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="120"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="119"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="118"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="117"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="116"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="115"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="114"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="113"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="112"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="111"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="110"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="109"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="108"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="107"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="106"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="105"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="104"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="103"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="102"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="101"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="100"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="99"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="98"/>
-    <tableColumn id="46" name="[force]" dataDxfId="97"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="96"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="95"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="94"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="93"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="92"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="91"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="90"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="89"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="141"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="140"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="139"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="138"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="137"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="136"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="135"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="134"/>
+    <tableColumn id="10" name="[health]" dataDxfId="133"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="132"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="131"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="130"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="129"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="128"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="127"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="126"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="125"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="124"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="123"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="122"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="121"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="120"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="119"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="118"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="117"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="116"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="115"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="114"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="113"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="112"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="111"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="110"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="109"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="108"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="107"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="106"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="105"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="104"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="103"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="102"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="101"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="100"/>
+    <tableColumn id="46" name="[force]" dataDxfId="99"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="98"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="97"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="96"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="95"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="94"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="93"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="92"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:V6" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85">
-  <autoFilter ref="B3:V6"/>
-  <tableColumns count="21">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:X6" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
+  <autoFilter ref="B3:X6"/>
+  <tableColumns count="23">
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="86"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="83"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="82"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="81"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="80"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="79"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="78"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="77"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="76"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="75"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="74"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="73"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="72"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="71"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="70"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="69"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="0"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="24"/>
-    <tableColumn id="65" name="[trackingSku]" dataDxfId="68"/>
+    <tableColumn id="5" name="[order]" dataDxfId="85"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="84"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="83"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="82"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="81"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="80"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="79"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="78"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="77"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="76"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="75"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="74"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="73"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="72"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="71"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="25"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="26"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="0"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="24"/>
+    <tableColumn id="65" name="[trackingSku]" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="69" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="64"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="62"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="61"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="60">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="64"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="63"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="62">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -16336,53 +16398,53 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="B45:M48"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="54"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="53"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="52"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="51"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="50"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="49"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="48"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="47"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="46"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="45"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="58"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="57"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="56"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="55"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="54"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="53"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="52"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="51"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="50"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="49"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="48"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="B3:J6"/>
   <tableColumns count="9">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="7" name="[index]" dataDxfId="41"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="40"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="39"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="38"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="37"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="36"/>
-    <tableColumn id="10" name="[color]" dataDxfId="35"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
+    <tableColumn id="7" name="[index]" dataDxfId="43"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="42"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="41"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="40"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="39"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="38"/>
+    <tableColumn id="10" name="[color]" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="27"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="26"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="25"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="31"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="29"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="28"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16656,8 +16718,8 @@
   </sheetPr>
   <dimension ref="A1:AZ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16830,7 +16892,13 @@
       <c r="U3" s="202" t="s">
         <v>210</v>
       </c>
-      <c r="V3" s="48" t="s">
+      <c r="V3" s="202" t="s">
+        <v>211</v>
+      </c>
+      <c r="W3" s="202" t="s">
+        <v>212</v>
+      </c>
+      <c r="X3" s="48" t="s">
         <v>1</v>
       </c>
     </row>
@@ -16895,7 +16963,11 @@
       <c r="U4" s="49">
         <v>1</v>
       </c>
-      <c r="V4" s="184" t="s">
+      <c r="V4" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="W4" s="49"/>
+      <c r="X4" s="184" t="s">
         <v>4</v>
       </c>
     </row>
@@ -16960,7 +17032,11 @@
       <c r="U5" s="49">
         <v>1</v>
       </c>
-      <c r="V5" s="184" t="s">
+      <c r="V5" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="W5" s="49"/>
+      <c r="X5" s="184" t="s">
         <v>5</v>
       </c>
     </row>
@@ -17025,7 +17101,9 @@
       <c r="U6" s="203">
         <v>1</v>
       </c>
-      <c r="V6" s="185" t="s">
+      <c r="V6" s="203"/>
+      <c r="W6" s="203"/>
+      <c r="X6" s="185" t="s">
         <v>6</v>
       </c>
     </row>
@@ -19476,7 +19554,7 @@
   <conditionalFormatting sqref="C4:D6">
     <cfRule type="duplicateValues" dxfId="22" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V4:V6">
+  <conditionalFormatting sqref="X4:X6">
     <cfRule type="duplicateValues" dxfId="21" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">

</xml_diff>

<commit_message>
New table related to each special dragon "Boost" ability
Former-commit-id: 4a7c4ac501cc5de1d5a15245e2f42ea1da3682de
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="228">
   <si>
     <t>[sku]</t>
   </si>
@@ -679,6 +679,39 @@
   </si>
   <si>
     <t>PF_DragonSonicResults</t>
+  </si>
+  <si>
+    <t>DRAGONS SPECIAL ABILIT DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{dragonStatsDefinitions}</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_STAT_HEALTH</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_STAT_SPEED</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_STAT_ENERGY</t>
+  </si>
+  <si>
+    <t>icon_stat_health</t>
+  </si>
+  <si>
+    <t>icon_stat_speed</t>
+  </si>
+  <si>
+    <t>icon_stat_energy</t>
   </si>
 </sst>
 </file>
@@ -1931,6 +1964,15 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1973,20 +2015,21 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="145">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5562,7 +5605,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6808,7 +6850,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7130,7 +7171,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7452,7 +7492,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7761,7 +7800,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16298,106 +16336,106 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="129" totalsRowBorderDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="130" totalsRowBorderDxfId="129">
   <autoFilter ref="B12:AZ24"/>
   <tableColumns count="51">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="127"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="126"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="125"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="124"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="123"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="122"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="121"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="120"/>
-    <tableColumn id="10" name="[health]" dataDxfId="119"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="118"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="117"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="116"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="115"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="114"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="113"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="112"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="111"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="110"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="109"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="108"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="107"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="106"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="105"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="104"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="103"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="102"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="101"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="100"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="99"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="98"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="97"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="96"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="95"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="94"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="93"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="92"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="91"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="90"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="89"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="88"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="87"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="86"/>
-    <tableColumn id="46" name="[force]" dataDxfId="85"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="84"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="83"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="82"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="81"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="80"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="79"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="78"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="77"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="128"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="127"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="126"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="125"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="124"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="123"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="122"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="121"/>
+    <tableColumn id="10" name="[health]" dataDxfId="120"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="119"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="118"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="117"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="116"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="115"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="114"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="113"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="112"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="111"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="110"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="109"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="108"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="107"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="106"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="105"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="104"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="103"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="102"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="101"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="100"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="99"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="98"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="97"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="96"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="95"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="94"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="93"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="92"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="91"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="90"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="89"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="88"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="87"/>
+    <tableColumn id="46" name="[force]" dataDxfId="86"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="85"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="84"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="83"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="82"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="81"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="80"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="79"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:X6" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:X6" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74">
   <autoFilter ref="B3:X6"/>
   <tableColumns count="23">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="72"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="73"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="71"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="70"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="69"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="68"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="67"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="66"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="65"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="64"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="63"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="62"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="61"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="60"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="59"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="58"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="57"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="56"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="55"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="54"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="53"/>
-    <tableColumn id="65" name="[trackingSku]" dataDxfId="52"/>
+    <tableColumn id="5" name="[order]" dataDxfId="72"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="71"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="70"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="69"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="68"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="67"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="66"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="65"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="64"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="63"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="62"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="61"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="60"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="59"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="58"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="57"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="56"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="55"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="54"/>
+    <tableColumn id="65" name="[trackingSku]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="52" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="B30:F39"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="46"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="45"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="44">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="47"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="46"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="45">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -16406,53 +16444,53 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B45:M48"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="38"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="37"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="36"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="35"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="34"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="33"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="31"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="30"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="29"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="39"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="38"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="37"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="36"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="35"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="34"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="33"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="32"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="31"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="B3:J6"/>
   <tableColumns count="9">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="7" name="[index]" dataDxfId="24"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="23"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="22"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="21"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="20"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="19"/>
-    <tableColumn id="10" name="[color]" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
+    <tableColumn id="7" name="[index]" dataDxfId="25"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="24"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="23"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="22"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="21"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="20"/>
+    <tableColumn id="10" name="[color]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="10"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="9"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="8"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="11"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="10"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16724,10 +16762,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AZ48"/>
+  <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18031,7 +18069,7 @@
       </c>
       <c r="AF17" s="116"/>
       <c r="AG17" s="131"/>
-      <c r="AH17" s="202">
+      <c r="AH17" s="188">
         <v>4.0999999999999996</v>
       </c>
       <c r="AI17" s="116">
@@ -18049,7 +18087,7 @@
       <c r="AM17" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="AN17" s="201">
+      <c r="AN17" s="187">
         <v>10</v>
       </c>
       <c r="AO17" s="142">
@@ -18076,7 +18114,7 @@
       <c r="AV17" s="149">
         <v>0.7</v>
       </c>
-      <c r="AW17" s="200">
+      <c r="AW17" s="186">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX17" s="155">
@@ -18182,7 +18220,7 @@
       </c>
       <c r="AF18" s="116"/>
       <c r="AG18" s="131"/>
-      <c r="AH18" s="202">
+      <c r="AH18" s="188">
         <v>2.2999999999999998</v>
       </c>
       <c r="AI18" s="116">
@@ -18200,7 +18238,7 @@
       <c r="AM18" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="AN18" s="201">
+      <c r="AN18" s="187">
         <v>10</v>
       </c>
       <c r="AO18" s="142">
@@ -18227,7 +18265,7 @@
       <c r="AV18" s="149">
         <v>0.7</v>
       </c>
-      <c r="AW18" s="200">
+      <c r="AW18" s="186">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX18" s="155">
@@ -18333,7 +18371,7 @@
       </c>
       <c r="AF19" s="116"/>
       <c r="AG19" s="131"/>
-      <c r="AH19" s="202">
+      <c r="AH19" s="188">
         <v>2.1</v>
       </c>
       <c r="AI19" s="116">
@@ -18351,7 +18389,7 @@
       <c r="AM19" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="AN19" s="201">
+      <c r="AN19" s="187">
         <v>10</v>
       </c>
       <c r="AO19" s="142">
@@ -18378,7 +18416,7 @@
       <c r="AV19" s="149">
         <v>0.7</v>
       </c>
-      <c r="AW19" s="200">
+      <c r="AW19" s="186">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX19" s="155">
@@ -18484,7 +18522,7 @@
       </c>
       <c r="AF20" s="116"/>
       <c r="AG20" s="131"/>
-      <c r="AH20" s="202">
+      <c r="AH20" s="188">
         <v>2.1</v>
       </c>
       <c r="AI20" s="116">
@@ -18502,7 +18540,7 @@
       <c r="AM20" s="116" t="b">
         <v>1</v>
       </c>
-      <c r="AN20" s="201">
+      <c r="AN20" s="187">
         <v>10</v>
       </c>
       <c r="AO20" s="142">
@@ -18529,7 +18567,7 @@
       <c r="AV20" s="149">
         <v>0.7</v>
       </c>
-      <c r="AW20" s="200">
+      <c r="AW20" s="186">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX20" s="155">
@@ -19154,44 +19192,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="193" t="s">
+      <c r="H25" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="194"/>
-      <c r="J25" s="195" t="s">
+      <c r="I25" s="197"/>
+      <c r="J25" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="196"/>
-      <c r="L25" s="196"/>
-      <c r="M25" s="196"/>
-      <c r="N25" s="196"/>
-      <c r="O25" s="197"/>
+      <c r="K25" s="199"/>
+      <c r="L25" s="199"/>
+      <c r="M25" s="199"/>
+      <c r="N25" s="199"/>
+      <c r="O25" s="200"/>
       <c r="P25" s="73"/>
-      <c r="Q25" s="189" t="s">
+      <c r="Q25" s="192" t="s">
         <v>139</v>
       </c>
-      <c r="R25" s="190"/>
-      <c r="S25" s="190"/>
-      <c r="T25" s="190"/>
-      <c r="U25" s="191" t="s">
+      <c r="R25" s="193"/>
+      <c r="S25" s="193"/>
+      <c r="T25" s="193"/>
+      <c r="U25" s="194" t="s">
         <v>13</v>
       </c>
-      <c r="V25" s="192"/>
-      <c r="W25" s="192"/>
-      <c r="X25" s="192"/>
+      <c r="V25" s="195"/>
+      <c r="W25" s="195"/>
+      <c r="X25" s="195"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="186" t="s">
+      <c r="AH25" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="AI25" s="187"/>
-      <c r="AJ25" s="187"/>
-      <c r="AK25" s="187"/>
-      <c r="AL25" s="187"/>
-      <c r="AM25" s="187"/>
-      <c r="AN25" s="188"/>
+      <c r="AI25" s="190"/>
+      <c r="AJ25" s="190"/>
+      <c r="AK25" s="190"/>
+      <c r="AL25" s="190"/>
+      <c r="AM25" s="190"/>
+      <c r="AN25" s="191"/>
     </row>
     <row r="27" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:52" ht="23.25" x14ac:dyDescent="0.35">
@@ -19548,6 +19586,71 @@
         <v>207</v>
       </c>
     </row>
+    <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="54" spans="2:5" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" s="58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="E56" s="58" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E57" s="58" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="AH25:AN25"/>
@@ -19557,46 +19660,49 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="143" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
+    <cfRule type="duplicateValues" dxfId="143" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:X6">
     <cfRule type="duplicateValues" dxfId="142" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X4:X6">
-    <cfRule type="duplicateValues" dxfId="141" priority="28"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="140" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="139" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="138" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="137" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ17">
+    <cfRule type="duplicateValues" dxfId="137" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AZ18:AZ20">
     <cfRule type="duplicateValues" dxfId="136" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ18:AZ20">
+  <conditionalFormatting sqref="AZ13">
     <cfRule type="duplicateValues" dxfId="135" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ13">
+  <conditionalFormatting sqref="AZ14:AZ16">
     <cfRule type="duplicateValues" dxfId="134" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ14:AZ16">
+  <conditionalFormatting sqref="AZ21">
     <cfRule type="duplicateValues" dxfId="133" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ21">
+  <conditionalFormatting sqref="AZ22:AZ24">
     <cfRule type="duplicateValues" dxfId="132" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ22:AZ24">
+  <conditionalFormatting sqref="C46:C48">
     <cfRule type="duplicateValues" dxfId="131" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:C48">
-    <cfRule type="duplicateValues" dxfId="130" priority="3"/>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -19663,8 +19769,8 @@
       <c r="D2" s="159"/>
       <c r="E2" s="159"/>
       <c r="F2" s="160"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
       <c r="I2" s="159"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -19884,7 +19990,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -19921,12 +20027,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="64"/>
-      <c r="E3" s="199" t="s">
+      <c r="E3" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="199"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
       <c r="J3" s="64" t="s">
         <v>115</v>
       </c>
@@ -20883,22 +20989,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20935,12 +21041,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="64"/>
-      <c r="E3" s="199" t="s">
+      <c r="E3" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="199"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
       <c r="J3" s="64" t="s">
         <v>115</v>
       </c>
@@ -21904,22 +22010,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Increased max. score for Fury in Electric
Former-commit-id: 8292d7b83ad0e9878d391d8bfd3803312cd170bd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16808,8 +16808,8 @@
   </sheetPr>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18110,7 +18110,7 @@
         <v>10</v>
       </c>
       <c r="X17" s="124">
-        <v>22000</v>
+        <v>24000</v>
       </c>
       <c r="Y17" s="112">
         <v>2</v>
@@ -18261,7 +18261,7 @@
         <v>11</v>
       </c>
       <c r="X18" s="124">
-        <v>72000</v>
+        <v>80000</v>
       </c>
       <c r="Y18" s="112">
         <v>3</v>
@@ -18412,7 +18412,7 @@
         <v>11</v>
       </c>
       <c r="X19" s="124">
-        <v>125000</v>
+        <v>150000</v>
       </c>
       <c r="Y19" s="112">
         <v>4</v>
@@ -18563,7 +18563,7 @@
         <v>11</v>
       </c>
       <c r="X20" s="124">
-        <v>235000</v>
+        <v>265000</v>
       </c>
       <c r="Y20" s="112">
         <v>5</v>

</xml_diff>

<commit_message>
Added power upgrades tids
Former-commit-id: 0e8881291fa828d9949550c4c127dcbddc7b7785
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="244">
   <si>
     <t>[sku]</t>
   </si>
@@ -724,13 +724,49 @@
   </si>
   <si>
     <t>TID_DRAGON_SPECIAL_HELICOPTER_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER1_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER2_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER3_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_ELECTRIC_POWER3_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER1_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER2_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER3_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HELICOPTER_POWER3_DESC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +849,12 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -980,7 +1022,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1501,11 +1543,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2027,11 +2078,110 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="145">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2085,6 +2235,126 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2508,16 +2778,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5483,116 +5743,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -16378,163 +16528,165 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="131" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="144" totalsRowBorderDxfId="143">
   <autoFilter ref="B12:AZ24"/>
   <tableColumns count="51">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="129"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="128"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="127"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="126"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="125"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="124"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="123"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="122"/>
-    <tableColumn id="10" name="[health]" dataDxfId="121"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="120"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="119"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="118"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="117"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="116"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="115"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="114"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="113"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="112"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="111"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="110"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="109"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="108"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="107"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="106"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="105"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="104"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="103"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="102"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="101"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="100"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="99"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="98"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="97"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="96"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="95"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="94"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="93"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="92"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="91"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="90"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="89"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="88"/>
-    <tableColumn id="46" name="[force]" dataDxfId="87"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="86"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="85"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="84"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="83"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="82"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="81"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="80"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="79"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="142"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="141"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="140"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="139"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="138"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="137"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="136"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="135"/>
+    <tableColumn id="10" name="[health]" dataDxfId="134"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="133"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="132"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="131"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="130"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="129"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="128"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="127"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="126"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="125"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="124"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="123"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="122"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="121"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="120"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="119"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="118"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="117"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="116"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="115"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="114"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="113"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="112"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="111"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="110"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="109"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="108"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="107"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="106"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="105"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="104"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="103"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="102"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="101"/>
+    <tableColumn id="46" name="[force]" dataDxfId="100"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="99"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="98"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="97"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="96"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="95"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="94"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="93"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:Z6" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:Z6" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88">
   <autoFilter ref="B3:Z6"/>
   <tableColumns count="25">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="74"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="87"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="73"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="72"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="71"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="70"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="69"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="68"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="67"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="66"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="65"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="64"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="63"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="62"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="61"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="60"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="59"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="58"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="57"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="56"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="55"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="54"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="53"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="52"/>
+    <tableColumn id="5" name="[order]" dataDxfId="86"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="85"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="84"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="83"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="82"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="81"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="80"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="79"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="78"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="77"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="76"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="75"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="74"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="73"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="72"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="71"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="70"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="69"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="68"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="67"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="66"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:F39" totalsRowShown="0" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
-  <autoFilter ref="B30:F39"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="46"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="45"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:H39" totalsRowShown="0" headerRowBorderDxfId="64" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+  <autoFilter ref="B30:H39"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="61"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="60"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="59"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="58"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="57">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="4" name="[tidName]" dataDxfId="0"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="B45:M48"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="38"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="37"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="36"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="35"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="34"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="33"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="32"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="31"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="30"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="29"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="51"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="50"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="49"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="48"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="47"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="46"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="45"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="44"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="43"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:J6" totalsRowShown="0" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="B3:J6"/>
   <tableColumns count="9">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="7" name="[index]" dataDxfId="24"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="23"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="22"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="21"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="20"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="19"/>
-    <tableColumn id="10" name="[color]" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[index]" dataDxfId="38"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="37"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="36"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="35"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="34"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="33"/>
+    <tableColumn id="10" name="[color]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="10"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="9"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="8"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="24"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="23"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16808,8 +16960,8 @@
   </sheetPr>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19327,6 +19479,12 @@
       <c r="F30" s="59" t="s">
         <v>71</v>
       </c>
+      <c r="G30" s="205" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="205" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
@@ -19345,6 +19503,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_1</v>
       </c>
+      <c r="G31" s="207" t="s">
+        <v>238</v>
+      </c>
+      <c r="H31" s="209" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -19363,6 +19527,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_2</v>
       </c>
+      <c r="G32" s="207" t="s">
+        <v>239</v>
+      </c>
+      <c r="H32" s="208" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="29" t="s">
@@ -19381,6 +19551,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_helicopter_power_3</v>
       </c>
+      <c r="G33" s="207" t="s">
+        <v>240</v>
+      </c>
+      <c r="H33" s="208" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="29" t="s">
@@ -19399,6 +19575,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_1</v>
       </c>
+      <c r="G34" s="207" t="s">
+        <v>232</v>
+      </c>
+      <c r="H34" s="208" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="29" t="s">
@@ -19417,6 +19599,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_2</v>
       </c>
+      <c r="G35" s="207" t="s">
+        <v>233</v>
+      </c>
+      <c r="H35" s="208" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="29" t="s">
@@ -19435,6 +19623,12 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_electric_power_3</v>
       </c>
+      <c r="G36" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="H36" s="208" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -19453,6 +19647,8 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_1</v>
       </c>
+      <c r="G37" s="206"/>
+      <c r="H37" s="203"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="29" t="s">
@@ -19471,6 +19667,8 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_2</v>
       </c>
+      <c r="G38" s="206"/>
+      <c r="H38" s="203"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="29" t="s">
@@ -19489,6 +19687,8 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_sonic_power_3</v>
       </c>
+      <c r="G39" s="206"/>
+      <c r="H39" s="204"/>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
@@ -19726,37 +19926,37 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="142" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="141" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="140" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="139" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="138" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="137" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ21">
-    <cfRule type="duplicateValues" dxfId="136" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ22:AZ24">
-    <cfRule type="duplicateValues" dxfId="135" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C48">
-    <cfRule type="duplicateValues" dxfId="134" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="duplicateValues" dxfId="133" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4:Z6">
-    <cfRule type="duplicateValues" dxfId="132" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -20044,7 +20244,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -21043,22 +21243,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22064,22 +22264,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated FuryMax for Helicopter
Former-commit-id: 4788fd56e15045af288fe285611711445da8835a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -16960,8 +16960,8 @@
   </sheetPr>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="S4" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17657,7 +17657,7 @@
         <v>10</v>
       </c>
       <c r="X13" s="144">
-        <v>85000</v>
+        <v>90000</v>
       </c>
       <c r="Y13" s="126">
         <v>2</v>
@@ -17808,7 +17808,7 @@
         <v>11</v>
       </c>
       <c r="X14" s="144">
-        <v>150000</v>
+        <v>220000</v>
       </c>
       <c r="Y14" s="126">
         <v>3</v>
@@ -17959,7 +17959,7 @@
         <v>11</v>
       </c>
       <c r="X15" s="144">
-        <v>250000</v>
+        <v>300000</v>
       </c>
       <c r="Y15" s="126">
         <v>4</v>
@@ -18111,7 +18111,7 @@
         <v>11</v>
       </c>
       <c r="X16" s="144">
-        <v>400000</v>
+        <v>550000</v>
       </c>
       <c r="Y16" s="126">
         <v>5</v>

</xml_diff>

<commit_message>
added petScaleMenu (removed petScale)
Former-commit-id: d370a679043a67e85195ce55ac1974477b99cfa3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="249">
   <si>
     <t>[sku]</t>
   </si>
@@ -772,6 +772,9 @@
   </si>
   <si>
     <t>hard</t>
+  </si>
+  <si>
+    <t>[petScaleMenu]</t>
   </si>
 </sst>
 </file>
@@ -16688,7 +16691,7 @@
     <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="72"/>
     <tableColumn id="10" name="[tidBoostAction]" dataDxfId="71"/>
     <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="70"/>
-    <tableColumn id="13" name="[petScale]" dataDxfId="0"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="0"/>
     <tableColumn id="12" name="[tidDesc]" dataDxfId="69"/>
     <tableColumn id="65" name="[tidName]" dataDxfId="68"/>
     <tableColumn id="11" name="[trackingSku]" dataDxfId="67"/>
@@ -17037,8 +17040,8 @@
   </sheetPr>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17218,7 +17221,7 @@
         <v>212</v>
       </c>
       <c r="X3" s="179" t="s">
-        <v>30</v>
+        <v>248</v>
       </c>
       <c r="Y3" s="53" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added columns related to Mummy pet
Former-commit-id: 32e9d3a3c13f456fcb3d032cb09dacebeadcfa68
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Helicopter" sheetId="13" r:id="rId4"/>
     <sheet name="DATA" sheetId="12" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="250">
   <si>
     <t>[sku]</t>
   </si>
@@ -495,9 +495,6 @@
     <t>HELICOPTER</t>
   </si>
   <si>
-    <t>NOTA: Añadir las columnas relativas al pet mummy!!!!!!</t>
-  </si>
-  <si>
     <t xml:space="preserve">INC. </t>
   </si>
   <si>
@@ -772,6 +769,15 @@
   </si>
   <si>
     <t>hard</t>
+  </si>
+  <si>
+    <t>[petScaleMenu]</t>
+  </si>
+  <si>
+    <t>[mummyHealthFactor]</t>
+  </si>
+  <si>
+    <t>[mummyDuration]</t>
   </si>
 </sst>
 </file>
@@ -1569,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="210">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2112,11 +2118,63 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="146">
+  <dxfs count="149">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2172,6 +2230,150 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2632,16 +2834,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5685,116 +5877,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -16580,166 +16662,169 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="134" totalsRowBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:AZ24" totalsRowShown="0" headerRowBorderDxfId="148" totalsRowBorderDxfId="147">
   <autoFilter ref="B12:AZ24"/>
   <tableColumns count="51">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="132"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="131"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="130"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="129"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="128"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="127"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="126"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="125"/>
-    <tableColumn id="10" name="[health]" dataDxfId="124"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="123"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="122"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="121"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="120"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="119"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="118"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="117"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="116"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="115"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="114"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="113"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="112"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="111"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="110"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="109"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="108"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="107"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="106"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="105"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="104"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="103"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="102"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="101"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="100"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="99"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="98"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="97"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="96"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="95"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="94"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="93"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="92"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="91"/>
-    <tableColumn id="46" name="[force]" dataDxfId="90"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="89"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="88"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="87"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="86"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="85"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="84"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="83"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="82"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="146"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="145"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="144"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="143"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="142"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="141"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="140"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="139"/>
+    <tableColumn id="10" name="[health]" dataDxfId="138"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="137"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="136"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="135"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="134"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="133"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="132"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="131"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="130"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="129"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="128"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="127"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="126"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="125"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="124"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="123"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="122"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="121"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="120"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="119"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="118"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="117"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="116"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="115"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="114"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="113"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="112"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="111"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="110"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="109"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="108"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="107"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="106"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="105"/>
+    <tableColumn id="46" name="[force]" dataDxfId="104"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="103"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="102"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="101"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="100"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="99"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="98"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="97"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:Z6" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80" tableBorderDxfId="78">
-  <autoFilter ref="B3:Z6"/>
-  <tableColumns count="25">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94" tableBorderDxfId="92">
+  <autoFilter ref="B3:AC6"/>
+  <tableColumns count="28">
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="91"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="76"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="75"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="74"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="73"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="72"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="71"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="70"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="69"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="68"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="67"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="66"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="65"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="64"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="63"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="62"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="61"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="60"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="59"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="58"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="57"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="55"/>
+    <tableColumn id="5" name="[order]" dataDxfId="90"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="89"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="88"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="87"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="86"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="85"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="84"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="83"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="82"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="81"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="80"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="79"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="78"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="77"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="76"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="75"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="74"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="73"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="72"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="22"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="71"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="70"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="1"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="0"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:H39" totalsRowShown="0" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:H39" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67" totalsRowBorderDxfId="66">
   <autoFilter ref="B30:H39"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="49"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="48"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="47">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="65"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="63"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="62"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="61">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="46"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="45"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="B45:M48"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="39"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="38"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="37"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="36"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="35"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="34"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="33"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="32"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="31"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="30"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="54"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="53"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="52"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="51"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="50"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="49"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="48"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="47"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="46"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="45"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="25"/>
-    <tableColumn id="7" name="[index]" dataDxfId="24"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="23"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="22"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="21"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="20"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="19"/>
-    <tableColumn id="10" name="[color]" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[index]" dataDxfId="39"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="38"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="37"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="36"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="35"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="34"/>
+    <tableColumn id="10" name="[color]" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="10"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="9"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="8"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="27"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="25"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="24"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17013,8 +17098,8 @@
   </sheetPr>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AW10" sqref="AW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17140,7 +17225,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>60</v>
@@ -17182,24 +17267,33 @@
         <v>83</v>
       </c>
       <c r="T3" s="179" t="s">
+        <v>208</v>
+      </c>
+      <c r="U3" s="179" t="s">
         <v>209</v>
       </c>
-      <c r="U3" s="179" t="s">
+      <c r="V3" s="179" t="s">
         <v>210</v>
       </c>
-      <c r="V3" s="179" t="s">
+      <c r="W3" s="179" t="s">
         <v>211</v>
       </c>
-      <c r="W3" s="179" t="s">
-        <v>212</v>
-      </c>
-      <c r="X3" s="53" t="s">
+      <c r="X3" s="179" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="53" t="s">
+      <c r="Z3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="47" t="s">
+      <c r="AA3" s="210" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB3" s="210" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC3" s="47" t="s">
         <v>1</v>
       </c>
     </row>
@@ -17265,16 +17359,25 @@
         <v>1</v>
       </c>
       <c r="V4" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W4" s="48"/>
-      <c r="X4" s="185" t="s">
-        <v>231</v>
+      <c r="X4" s="48">
+        <v>0.6</v>
       </c>
       <c r="Y4" s="185" t="s">
         <v>230</v>
       </c>
-      <c r="Z4" s="40" t="s">
+      <c r="Z4" s="185" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA4" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="AB4" s="211">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="40" t="s">
         <v>70</v>
       </c>
     </row>
@@ -17340,23 +17443,30 @@
         <v>1</v>
       </c>
       <c r="V5" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W5" s="48"/>
-      <c r="X5" s="185" t="s">
-        <v>229</v>
+      <c r="X5" s="48">
+        <v>0.6</v>
       </c>
       <c r="Y5" s="185" t="s">
         <v>228</v>
       </c>
-      <c r="Z5" s="40" t="s">
+      <c r="Z5" s="185" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA5" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="AB5" s="211">
+        <v>25</v>
+      </c>
+      <c r="AC5" s="40" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
-        <v>2</v>
-      </c>
+      <c r="B6" s="44"/>
       <c r="C6" s="45" t="s">
         <v>69</v>
       </c>
@@ -17416,11 +17526,20 @@
       </c>
       <c r="V6" s="180"/>
       <c r="W6" s="180"/>
-      <c r="X6" s="55"/>
-      <c r="Y6" s="55" t="s">
+      <c r="X6" s="180">
+        <v>0.6</v>
+      </c>
+      <c r="Y6" s="55"/>
+      <c r="Z6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="Z6" s="45" t="s">
+      <c r="AA6" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="AB6" s="211">
+        <v>25</v>
+      </c>
+      <c r="AC6" s="45" t="s">
         <v>69</v>
       </c>
     </row>
@@ -17454,9 +17573,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AW10" s="138" t="s">
-        <v>155</v>
-      </c>
+      <c r="AW10" s="138"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -17728,10 +17845,10 @@
         <v>151</v>
       </c>
       <c r="AD13" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE13" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF13" s="36"/>
       <c r="AG13" s="128"/>
@@ -17879,10 +17996,10 @@
         <v>151</v>
       </c>
       <c r="AD14" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE14" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF14" s="36"/>
       <c r="AG14" s="128"/>
@@ -18030,10 +18147,10 @@
         <v>151</v>
       </c>
       <c r="AD15" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE15" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF15" s="36"/>
       <c r="AG15" s="128"/>
@@ -18182,10 +18299,10 @@
         <v>151</v>
       </c>
       <c r="AD16" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AE16" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF16" s="36"/>
       <c r="AG16" s="128"/>
@@ -18315,7 +18432,7 @@
         <v>10</v>
       </c>
       <c r="X17" s="124">
-        <v>24000</v>
+        <v>27000</v>
       </c>
       <c r="Y17" s="112">
         <v>2</v>
@@ -18333,10 +18450,10 @@
         <v>149</v>
       </c>
       <c r="AD17" s="115" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE17" s="115" t="s">
         <v>161</v>
-      </c>
-      <c r="AE17" s="115" t="s">
-        <v>162</v>
       </c>
       <c r="AF17" s="115"/>
       <c r="AG17" s="129"/>
@@ -18466,7 +18583,7 @@
         <v>11</v>
       </c>
       <c r="X18" s="124">
-        <v>80000</v>
+        <v>90000</v>
       </c>
       <c r="Y18" s="112">
         <v>3</v>
@@ -18484,10 +18601,10 @@
         <v>149</v>
       </c>
       <c r="AD18" s="115" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE18" s="115" t="s">
         <v>161</v>
-      </c>
-      <c r="AE18" s="115" t="s">
-        <v>162</v>
       </c>
       <c r="AF18" s="115"/>
       <c r="AG18" s="129"/>
@@ -18617,7 +18734,7 @@
         <v>11</v>
       </c>
       <c r="X19" s="124">
-        <v>150000</v>
+        <v>200000</v>
       </c>
       <c r="Y19" s="112">
         <v>4</v>
@@ -18635,10 +18752,10 @@
         <v>149</v>
       </c>
       <c r="AD19" s="115" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE19" s="115" t="s">
         <v>161</v>
-      </c>
-      <c r="AE19" s="115" t="s">
-        <v>162</v>
       </c>
       <c r="AF19" s="115"/>
       <c r="AG19" s="129"/>
@@ -18768,7 +18885,7 @@
         <v>11</v>
       </c>
       <c r="X20" s="124">
-        <v>265000</v>
+        <v>365000</v>
       </c>
       <c r="Y20" s="112">
         <v>5</v>
@@ -18786,10 +18903,10 @@
         <v>149</v>
       </c>
       <c r="AD20" s="115" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE20" s="115" t="s">
         <v>161</v>
-      </c>
-      <c r="AE20" s="115" t="s">
-        <v>162</v>
       </c>
       <c r="AF20" s="115"/>
       <c r="AG20" s="129"/>
@@ -18852,9 +18969,7 @@
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
-        <v>2</v>
-      </c>
+      <c r="B21" s="29"/>
       <c r="C21" s="30" t="s">
         <v>66</v>
       </c>
@@ -18937,10 +19052,10 @@
         <v>152</v>
       </c>
       <c r="AD21" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE21" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF21" s="36"/>
       <c r="AG21" s="128"/>
@@ -19003,9 +19118,7 @@
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
-        <v>2</v>
-      </c>
+      <c r="B22" s="29"/>
       <c r="C22" s="30" t="s">
         <v>104</v>
       </c>
@@ -19088,10 +19201,10 @@
         <v>152</v>
       </c>
       <c r="AD22" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE22" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF22" s="36"/>
       <c r="AG22" s="128"/>
@@ -19154,9 +19267,7 @@
       </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>2</v>
-      </c>
+      <c r="B23" s="29"/>
       <c r="C23" s="30" t="s">
         <v>105</v>
       </c>
@@ -19239,10 +19350,10 @@
         <v>152</v>
       </c>
       <c r="AD23" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE23" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF23" s="36"/>
       <c r="AG23" s="128"/>
@@ -19306,9 +19417,7 @@
     </row>
     <row r="24" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="29" t="s">
-        <v>2</v>
-      </c>
+      <c r="B24" s="29"/>
       <c r="C24" s="30" t="s">
         <v>106</v>
       </c>
@@ -19391,10 +19500,10 @@
         <v>152</v>
       </c>
       <c r="AD24" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE24" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF24" s="36"/>
       <c r="AG24" s="128"/>
@@ -19557,10 +19666,10 @@
         <v>icon_helicopter_power_1</v>
       </c>
       <c r="G31" s="193" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H31" s="195" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -19581,10 +19690,10 @@
         <v>icon_helicopter_power_2</v>
       </c>
       <c r="G32" s="193" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H32" s="194" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -19605,10 +19714,10 @@
         <v>icon_helicopter_power_3</v>
       </c>
       <c r="G33" s="193" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H33" s="194" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -19629,10 +19738,10 @@
         <v>icon_electric_power_1</v>
       </c>
       <c r="G34" s="193" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H34" s="194" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -19653,10 +19762,10 @@
         <v>icon_electric_power_2</v>
       </c>
       <c r="G35" s="193" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H35" s="194" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -19677,10 +19786,10 @@
         <v>icon_electric_power_3</v>
       </c>
       <c r="G36" s="193" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H36" s="194" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -19746,7 +19855,7 @@
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -19755,28 +19864,28 @@
     </row>
     <row r="45" spans="2:13" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="F45" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="G45" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="G45" s="59" t="s">
+      <c r="H45" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="H45" s="59" t="s">
+      <c r="I45" s="59" t="s">
         <v>194</v>
-      </c>
-      <c r="I45" s="59" t="s">
-        <v>195</v>
       </c>
       <c r="J45" s="59" t="s">
         <v>71</v>
@@ -19796,10 +19905,10 @@
         <v>2</v>
       </c>
       <c r="C46" s="56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D46" s="57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E46" s="57" t="s">
         <v>70</v>
@@ -19817,16 +19926,16 @@
         <v>0</v>
       </c>
       <c r="J46" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="K46" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="K46" s="58" t="s">
-        <v>200</v>
-      </c>
       <c r="L46" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M46" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
@@ -19834,10 +19943,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D47" s="57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E47" s="57" t="s">
         <v>68</v>
@@ -19855,16 +19964,16 @@
         <v>4</v>
       </c>
       <c r="J47" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K47" s="58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L47" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M47" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
@@ -19872,10 +19981,10 @@
         <v>2</v>
       </c>
       <c r="C48" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E48" s="57" t="s">
         <v>69</v>
@@ -19893,22 +20002,22 @@
         <v>0</v>
       </c>
       <c r="J48" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K48" s="58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L48" s="58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M48" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -19916,7 +20025,7 @@
     </row>
     <row r="54" spans="2:5" ht="121.5" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>0</v>
@@ -19933,13 +20042,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D55" s="57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E55" s="57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -19947,13 +20056,13 @@
         <v>2</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D56" s="57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E56" s="57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -19961,13 +20070,13 @@
         <v>2</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -19979,37 +20088,37 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="145" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="144" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="143" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="142" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="141" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="140" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ21">
-    <cfRule type="duplicateValues" dxfId="139" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ22:AZ24">
-    <cfRule type="duplicateValues" dxfId="138" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C48">
-    <cfRule type="duplicateValues" dxfId="137" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="duplicateValues" dxfId="136" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z4:Z6">
-    <cfRule type="duplicateValues" dxfId="135" priority="3"/>
+  <conditionalFormatting sqref="AC4:AC6">
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -20056,7 +20165,7 @@
   <sheetData>
     <row r="1" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -20082,34 +20191,34 @@
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
       <c r="B3" s="159" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" s="159" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="160" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E3" s="160" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="161" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="G3" s="161" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="162" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="161" t="s">
-        <v>185</v>
-      </c>
-      <c r="H3" s="162" t="s">
+      <c r="I3" s="162" t="s">
         <v>165</v>
-      </c>
-      <c r="I3" s="162" t="s">
-        <v>166</v>
       </c>
       <c r="J3" s="163" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -20117,10 +20226,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="166" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4" s="166" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E4" s="166">
         <v>0</v>
@@ -20138,10 +20247,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="169" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="170" t="s">
         <v>168</v>
-      </c>
-      <c r="K4" s="170" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -20149,10 +20258,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="166" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" s="166" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E5" s="166">
         <v>1</v>
@@ -20170,10 +20279,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="169" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" s="170" t="s">
         <v>170</v>
-      </c>
-      <c r="K5" s="170" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -20181,10 +20290,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="166" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6" s="166" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E6" s="166">
         <v>2</v>
@@ -20202,16 +20311,16 @@
         <v>1</v>
       </c>
       <c r="J6" s="169" t="s">
+        <v>171</v>
+      </c>
+      <c r="K6" s="171" t="s">
         <v>172</v>
-      </c>
-      <c r="K6" s="171" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -20221,7 +20330,7 @@
     </row>
     <row r="11" spans="2:13" ht="159" x14ac:dyDescent="0.25">
       <c r="B11" s="172" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="173" t="s">
         <v>0</v>
@@ -20230,10 +20339,10 @@
         <v>12</v>
       </c>
       <c r="E11" s="174" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="174" t="s">
         <v>174</v>
-      </c>
-      <c r="F11" s="174" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -20241,7 +20350,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D12" s="176" t="s">
         <v>19</v>
@@ -20258,7 +20367,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="176" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" s="176" t="s">
         <v>18</v>
@@ -20275,7 +20384,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="176" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D14" s="176" t="s">
         <v>17</v>
@@ -20292,7 +20401,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="176" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D15" s="176" t="s">
         <v>16</v>
@@ -20309,7 +20418,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="29" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -20550,13 +20659,13 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AD10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
@@ -20584,7 +20693,7 @@
         <v>133</v>
       </c>
       <c r="N11" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
@@ -20601,7 +20710,7 @@
         <v>133</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
@@ -20618,7 +20727,7 @@
         <v>133</v>
       </c>
       <c r="AD11" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21308,22 +21417,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21563,13 +21672,13 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AD10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
@@ -21597,7 +21706,7 @@
         <v>133</v>
       </c>
       <c r="N11" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
@@ -21614,7 +21723,7 @@
         <v>133</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
@@ -21631,7 +21740,7 @@
         <v>133</v>
       </c>
       <c r="AD11" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -22329,22 +22438,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated tier 4 for both dragons
Former-commit-id: bb536d4817ed97daedee10e0480fe50f23f1e47c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="253">
   <si>
     <t>[sku]</t>
   </si>
@@ -784,6 +784,9 @@
   </si>
   <si>
     <t>[tidDescShort]</t>
+  </si>
+  <si>
+    <t>Helicopter</t>
   </si>
 </sst>
 </file>
@@ -5975,6 +5978,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6296,6 +6300,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6348,7 +6353,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DATA!$F$5:$F$9</c:f>
+              <c:f>DATA!$M$5:$M$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -6364,14 +6369,14 @@
                   <c:v>Balrog</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Electric</c:v>
+                  <c:v>Helicopter</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DATA!$G$5:$G$9</c:f>
+              <c:f>DATA!$N$5:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6388,7 +6393,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6604,6 +6609,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6656,7 +6662,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DATA!$F$5:$F$9</c:f>
+              <c:f>DATA!$M$5:$M$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -6672,14 +6678,14 @@
                   <c:v>Balrog</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Electric</c:v>
+                  <c:v>Helicopter</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DATA!$H$5:$H$9</c:f>
+              <c:f>DATA!$O$5:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6912,6 +6918,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6964,7 +6971,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DATA!$F$5:$F$9</c:f>
+              <c:f>DATA!$M$5:$M$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -6980,14 +6987,14 @@
                   <c:v>Balrog</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Electric</c:v>
+                  <c:v>Helicopter</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DATA!$I$5:$I$9</c:f>
+              <c:f>DATA!$P$5:$P$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7004,7 +7011,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.1</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7220,6 +7227,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7541,6 +7549,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7862,6 +7871,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8170,6 +8180,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8786,6 +8797,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9107,6 +9119,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9428,6 +9441,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17144,8 +17158,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18300,13 +18314,13 @@
         <v>400</v>
       </c>
       <c r="K16" s="142">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="L16" s="142">
         <v>0</v>
       </c>
       <c r="M16" s="142">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="N16" s="142">
         <v>10</v>
@@ -18916,13 +18930,13 @@
         <v>250</v>
       </c>
       <c r="K20" s="123">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L20" s="123">
         <v>0</v>
       </c>
       <c r="M20" s="123">
-        <v>1.7000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="N20" s="123">
         <v>10</v>
@@ -20539,7 +20553,7 @@
   <dimension ref="C1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21552,8 +21566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22571,18 +22585,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F4:I9"/>
+  <dimension ref="F4:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:16" x14ac:dyDescent="0.25">
       <c r="G4" s="88" t="s">
         <v>143</v>
       </c>
@@ -22592,8 +22607,17 @@
       <c r="I4" s="88" t="s">
         <v>138</v>
       </c>
+      <c r="N4" s="88" t="s">
+        <v>143</v>
+      </c>
+      <c r="O4" s="88" t="s">
+        <v>144</v>
+      </c>
+      <c r="P4" s="88" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="5" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>142</v>
       </c>
@@ -22606,8 +22630,20 @@
       <c r="I5">
         <v>11.15</v>
       </c>
+      <c r="M5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N5">
+        <v>120</v>
+      </c>
+      <c r="O5">
+        <v>112.5</v>
+      </c>
+      <c r="P5">
+        <v>11.15</v>
+      </c>
     </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>145</v>
       </c>
@@ -22620,8 +22656,20 @@
       <c r="I6">
         <v>14.15</v>
       </c>
+      <c r="M6" t="s">
+        <v>145</v>
+      </c>
+      <c r="N6">
+        <v>240</v>
+      </c>
+      <c r="O6">
+        <v>112.5</v>
+      </c>
+      <c r="P6">
+        <v>14.15</v>
+      </c>
     </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>146</v>
       </c>
@@ -22634,8 +22682,20 @@
       <c r="I7">
         <v>14.8</v>
       </c>
+      <c r="M7" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7">
+        <v>365</v>
+      </c>
+      <c r="O7">
+        <v>112.5</v>
+      </c>
+      <c r="P7">
+        <v>14.8</v>
+      </c>
     </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>147</v>
       </c>
@@ -22648,8 +22708,20 @@
       <c r="I8">
         <v>15.25</v>
       </c>
+      <c r="M8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N8">
+        <v>410</v>
+      </c>
+      <c r="O8">
+        <v>112.5</v>
+      </c>
+      <c r="P8">
+        <v>15.25</v>
+      </c>
     </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>148</v>
       </c>
@@ -22664,6 +22736,21 @@
       <c r="I9">
         <f ca="1">Electric!H15</f>
         <v>10.1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>252</v>
+      </c>
+      <c r="N9">
+        <f ca="1">Helicopter!H13</f>
+        <v>175</v>
+      </c>
+      <c r="O9">
+        <f ca="1">Helicopter!H14</f>
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <f ca="1">Helicopter!H15</f>
+        <v>13.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Electric tier 3 modified
Former-commit-id: 20f5baa2504d39b48b00dd87e9311c0fcf4a1dfe
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17158,8 +17158,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18776,7 +18776,7 @@
         <v>200</v>
       </c>
       <c r="K19" s="123">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="L19" s="123">
         <v>0</v>

</xml_diff>

<commit_message>
Electric tier 3 updated (again)
Former-commit-id: f4a70c94daea4f62683f50f99c55a0be224b3558
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5978,7 +5978,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6300,7 +6299,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6609,7 +6607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6918,7 +6915,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7227,7 +7223,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7549,7 +7544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7871,7 +7865,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8180,7 +8173,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8797,7 +8789,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9119,7 +9110,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9441,7 +9431,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17159,7 +17148,7 @@
   <dimension ref="A1:BA57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18782,7 +18771,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="123">
-        <v>1.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="N19" s="123">
         <v>15</v>

</xml_diff>

<commit_message>
Helicopter tier 3 updated
Former-commit-id: fcdda076ae7b4de0edd0bb97f078f5bea217e008
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17147,8 +17147,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18148,13 +18148,13 @@
         <v>300</v>
       </c>
       <c r="K15" s="142">
-        <v>9</v>
+        <v>8.9</v>
       </c>
       <c r="L15" s="142">
         <v>0</v>
       </c>
       <c r="M15" s="142">
-        <v>7.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N15" s="142">
         <v>15</v>

</xml_diff>

<commit_message>
Review tier 2 Electric
Former-commit-id: b52a76a7e933f77f313dca8ea05dfa6b9bb00dd9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17148,7 +17148,7 @@
   <dimension ref="A1:BA57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17867,7 +17867,7 @@
         <v>40</v>
       </c>
       <c r="T13" s="144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U13" s="143">
         <v>9</v>
@@ -18021,7 +18021,7 @@
         <v>40</v>
       </c>
       <c r="T14" s="144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U14" s="143">
         <v>11</v>
@@ -18154,7 +18154,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="142">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="N15" s="142">
         <v>15</v>
@@ -18175,7 +18175,7 @@
         <v>40</v>
       </c>
       <c r="T15" s="144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U15" s="143">
         <v>11.5</v>
@@ -18330,7 +18330,7 @@
         <v>40</v>
       </c>
       <c r="T16" s="144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U16" s="143">
         <v>12</v>
@@ -18611,13 +18611,13 @@
         <v>150</v>
       </c>
       <c r="K18" s="123">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L18" s="123">
         <v>0</v>
       </c>
       <c r="M18" s="123">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N18" s="123">
         <v>20</v>

</xml_diff>

<commit_message>
For electric dragon, increased airGravityModifier
Former-commit-id: 54ec671b7d0ae067069824c65d8b2d3ac405af44
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17147,8 +17147,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="AQ10" workbookViewId="0">
+      <selection activeCell="AV20" sqref="AV20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18564,7 +18564,7 @@
         <v>1.7</v>
       </c>
       <c r="AV17" s="147">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="AW17" s="182">
         <v>1.1000000000000001</v>
@@ -18718,7 +18718,7 @@
         <v>1.7</v>
       </c>
       <c r="AV18" s="147">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="AW18" s="182">
         <v>1.1000000000000001</v>
@@ -18872,7 +18872,7 @@
         <v>1.7</v>
       </c>
       <c r="AV19" s="147">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="AW19" s="182">
         <v>1.1000000000000001</v>
@@ -19026,7 +19026,7 @@
         <v>1.7</v>
       </c>
       <c r="AV20" s="147">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="AW20" s="182">
         <v>1.1000000000000001</v>

</xml_diff>

<commit_message>
Modified petScaleMenu for electric dragon
Former-commit-id: 96fb4f1b1a32dbe57002466cbb69e120874dc970
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17147,8 +17147,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ10" workbookViewId="0">
-      <selection activeCell="AV20" sqref="AV20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17496,7 +17496,7 @@
       </c>
       <c r="W5" s="48"/>
       <c r="X5" s="48">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="Y5" s="185" t="s">
         <v>228</v>

</xml_diff>

<commit_message>
Increased x3 time between beams and decreased score needed to start a Fire rush
Former-commit-id: 46e0cc5e42c893a6e3fc942268c16c2e1192418d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17147,8 +17147,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18496,7 +18496,7 @@
         <v>10</v>
       </c>
       <c r="X17" s="124">
-        <v>27000</v>
+        <v>20000</v>
       </c>
       <c r="Y17" s="112">
         <v>2</v>
@@ -18650,7 +18650,7 @@
         <v>11</v>
       </c>
       <c r="X18" s="124">
-        <v>90000</v>
+        <v>80000</v>
       </c>
       <c r="Y18" s="112">
         <v>3</v>
@@ -18804,7 +18804,7 @@
         <v>11</v>
       </c>
       <c r="X19" s="124">
-        <v>200000</v>
+        <v>180000</v>
       </c>
       <c r="Y19" s="112">
         <v>4</v>
@@ -18958,7 +18958,7 @@
         <v>11</v>
       </c>
       <c r="X20" s="124">
-        <v>365000</v>
+        <v>350000</v>
       </c>
       <c r="Y20" s="112">
         <v>5</v>

</xml_diff>

<commit_message>
Set scale values when dragon collect HUNGRY letters
Former-commit-id: a6a811729fe29ebcd748217ba037cb5fe502f6aa
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -17147,8 +17147,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17905,7 +17905,7 @@
       <c r="AF13" s="36"/>
       <c r="AG13" s="128"/>
       <c r="AH13" s="186">
-        <v>4.0999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="AI13" s="36">
         <v>2</v>
@@ -18059,7 +18059,7 @@
       <c r="AF14" s="36"/>
       <c r="AG14" s="128"/>
       <c r="AH14" s="186">
-        <v>2.2999999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="AI14" s="36">
         <v>2</v>
@@ -18213,7 +18213,7 @@
       <c r="AF15" s="36"/>
       <c r="AG15" s="128"/>
       <c r="AH15" s="186">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="AI15" s="36">
         <v>2</v>
@@ -18368,7 +18368,7 @@
       <c r="AF16" s="36"/>
       <c r="AG16" s="128"/>
       <c r="AH16" s="186">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="AI16" s="36">
         <v>2</v>
@@ -18522,7 +18522,7 @@
       <c r="AF17" s="115"/>
       <c r="AG17" s="129"/>
       <c r="AH17" s="184">
-        <v>4.0999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="AI17" s="115">
         <v>2</v>
@@ -18676,7 +18676,7 @@
       <c r="AF18" s="115"/>
       <c r="AG18" s="129"/>
       <c r="AH18" s="184">
-        <v>2.2999999999999998</v>
+        <v>1.6</v>
       </c>
       <c r="AI18" s="115">
         <v>2</v>
@@ -18830,7 +18830,7 @@
       <c r="AF19" s="115"/>
       <c r="AG19" s="129"/>
       <c r="AH19" s="184">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="AI19" s="115">
         <v>2</v>
@@ -18984,7 +18984,7 @@
       <c r="AF20" s="115"/>
       <c r="AG20" s="129"/>
       <c r="AH20" s="184">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="AI20" s="115">
         <v>2</v>

</xml_diff>

<commit_message>
Renamed Sonic to Hedgehog
Former-commit-id: 69e2c8c6942bffeada9e2a9fd1c81ea0a9007470
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="260">
   <si>
     <t>[sku]</t>
   </si>
@@ -41,18 +41,6 @@
   </si>
   <si>
     <t>[tidName]</t>
-  </si>
-  <si>
-    <t>dragon_baby</t>
-  </si>
-  <si>
-    <t>dragon_crocodile</t>
-  </si>
-  <si>
-    <t>dragon_reptile</t>
-  </si>
-  <si>
-    <t>dragon_fat</t>
   </si>
   <si>
     <t>[order]</t>
@@ -229,16 +217,10 @@
     <t>electric_01</t>
   </si>
   <si>
-    <t>sonic_01</t>
-  </si>
-  <si>
     <t>{specialDragonTierDefinitions}</t>
   </si>
   <si>
     <t>dragon_electric</t>
-  </si>
-  <si>
-    <t>dragon_sonic</t>
   </si>
   <si>
     <t>dragon_helicopter</t>
@@ -307,15 +289,6 @@
     <t>helicopter_power_3</t>
   </si>
   <si>
-    <t>sonic_power_1</t>
-  </si>
-  <si>
-    <t>sonic_power_2</t>
-  </si>
-  <si>
-    <t>sonic_power_3</t>
-  </si>
-  <si>
     <t>[specialDragon]</t>
   </si>
   <si>
@@ -338,15 +311,6 @@
   </si>
   <si>
     <t>electric_04</t>
-  </si>
-  <si>
-    <t>sonic_02</t>
-  </si>
-  <si>
-    <t>sonic_03</t>
-  </si>
-  <si>
-    <t>sonic_04</t>
   </si>
   <si>
     <t>[upgradeLevelToUnlock]</t>
@@ -484,9 +448,6 @@
     <t>PF_DragonHelicopter</t>
   </si>
   <si>
-    <t>PF_DragonSonic</t>
-  </si>
-  <si>
     <t>percentage</t>
   </si>
   <si>
@@ -503,9 +464,6 @@
   </si>
   <si>
     <t>PF_DragonHelicopterMenu</t>
-  </si>
-  <si>
-    <t>PF_DragonSonicMenu</t>
   </si>
   <si>
     <t>PF_DragonElectricMenu</t>
@@ -619,9 +577,6 @@
     <t>dragon_electric_0</t>
   </si>
   <si>
-    <t>dragon_sonic_0</t>
-  </si>
-  <si>
     <t>icon_disguise_0</t>
   </si>
   <si>
@@ -631,22 +586,10 @@
     <t>TID_SKIN_ELECTRIC_0_NAME</t>
   </si>
   <si>
-    <t>TID_DRAGON_SONIC_0_DESC</t>
-  </si>
-  <si>
     <t>TID_DRAGON_HELICOPTER_0_DESC</t>
   </si>
   <si>
     <t>TID_DRAGON_ELECTRIC_0_DESC</t>
-  </si>
-  <si>
-    <t>baby_default</t>
-  </si>
-  <si>
-    <t>baby_chef</t>
-  </si>
-  <si>
-    <t>crocodile_default</t>
   </si>
   <si>
     <t>[unlockPriceGF]</t>
@@ -671,9 +614,6 @@
   </si>
   <si>
     <t>PF_DragonHelicopterResults</t>
-  </si>
-  <si>
-    <t>PF_DragonSonicResults</t>
   </si>
   <si>
     <t>DRAGONS SPECIAL ABILIT DEFINITIONS</t>
@@ -793,34 +733,82 @@
     <t>Sonic</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_BOOST_ABILITY</t>
+    <t>SPECIAL DRAGONS DEFINITIONS</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_NAME</t>
+    <t>dragon_hedgehog</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_DESC</t>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_BOOST_ABILITY</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER1_TITLE</t>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_DESC</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER1_DESC</t>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_NAME</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER2_TITLE</t>
+    <t>hedgehog_01</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER2_DESC</t>
+    <t>hedgehog_02</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER3_TITLE</t>
+    <t>hedgehog_03</t>
   </si>
   <si>
-    <t>TID_DRAGON_SPECIAL_SONIC_POWER3_DESC</t>
+    <t>hedgehog_04</t>
   </si>
   <si>
-    <t>SPECIAL DRAGONS DEFINITIONS</t>
+    <t>PF_DragonHedgehog</t>
+  </si>
+  <si>
+    <t>PF_DragonHedgehogMenu</t>
+  </si>
+  <si>
+    <t>PF_DragonHedgehogResults</t>
+  </si>
+  <si>
+    <t>hedgehog_power_1</t>
+  </si>
+  <si>
+    <t>hedgehog_power_2</t>
+  </si>
+  <si>
+    <t>hedgehog_power_3</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER1_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER2_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER3_TITLE</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_SPECIAL_HEDGEHOG_POWER3_DESC</t>
+  </si>
+  <si>
+    <t>dragon_hedgehog_0</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_HEDGEHOG_0_DESC</t>
+  </si>
+  <si>
+    <t>helicopter_default</t>
+  </si>
+  <si>
+    <t>electric_default</t>
+  </si>
+  <si>
+    <t>hedgehog_default</t>
   </si>
 </sst>
 </file>
@@ -2201,7 +2189,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="159">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -22202,116 +22220,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="144" totalsRowBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="147" totalsRowBorderDxfId="146">
   <autoFilter ref="B12:BA24"/>
   <tableColumns count="52">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="142"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="141"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="140"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="139"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="138"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="137"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="136"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="135"/>
-    <tableColumn id="10" name="[health]" dataDxfId="134"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="133"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="132"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="131"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="130"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="129"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="128"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="127"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="126"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="125"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="124"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="123"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="122"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="121"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="120"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="119"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="118"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="117"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="116"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="115"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="114"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="113"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="112"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="111"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="110"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="109"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="108"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="107"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="106"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="105"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="104"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="103"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="102"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="101"/>
-    <tableColumn id="46" name="[force]" dataDxfId="100"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="99"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="98"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="97"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="96"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="95"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="94"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="93"/>
-    <tableColumn id="6" name="[scaleMenu]" dataDxfId="92"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="91"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="145"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="144"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="143"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="142"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="141"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="140"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="139"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="138"/>
+    <tableColumn id="10" name="[health]" dataDxfId="137"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="136"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="135"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="134"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="133"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="132"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="131"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="130"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="129"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="128"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="127"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="126"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="125"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="124"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="123"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="122"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="121"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="120"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="119"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="118"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="117"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="116"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="115"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="114"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="113"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="112"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="111"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="110"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="109"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="108"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="107"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="106"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="105"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="104"/>
+    <tableColumn id="46" name="[force]" dataDxfId="103"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="102"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="101"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="100"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="99"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="98"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="97"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="96"/>
+    <tableColumn id="6" name="[scaleMenu]" dataDxfId="95"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90">
   <autoFilter ref="B3:AC6"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="86"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="89"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="85"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="84"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="83"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="82"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="81"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="80"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="79"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="78"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="77"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="76"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="75"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="74"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="73"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="72"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="71"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="70"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="69"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="68"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="67"/>
-    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="66"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="65"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="64"/>
-    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="63"/>
-    <tableColumn id="14" name="[mummyDuration]" dataDxfId="62"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="61"/>
+    <tableColumn id="5" name="[order]" dataDxfId="88"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="87"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="86"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="85"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="84"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="83"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="82"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="81"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="80"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="79"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="78"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="77"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="76"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="75"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="74"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="73"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="72"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="71"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="70"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="69"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="68"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="67"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="66"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="65"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="63" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="B30:I39"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="57"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="55"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="54"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="53">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="60"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="59"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="58"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="57"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="56">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="51"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="55"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="54"/>
     <tableColumn id="8" name="[tidDescShort]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -22319,54 +22337,54 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <autoFilter ref="B45:M48"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="45"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="43"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="42"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="41"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="40"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="39"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="38"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="37"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="36"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="35"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="34"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="46"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="45"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="44"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="43"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="42"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="41"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="40"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="39"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="38"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="35" tableBorderDxfId="34">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="29"/>
-    <tableColumn id="7" name="[index]" dataDxfId="28"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="27"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="26"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="25"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="24"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="23"/>
-    <tableColumn id="10" name="[color]" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="32"/>
+    <tableColumn id="7" name="[index]" dataDxfId="31"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="30"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="29"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="28"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="27"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="26"/>
+    <tableColumn id="10" name="[color]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="14"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="13"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="12"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="19"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="17"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="16"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -22640,8 +22658,8 @@
   </sheetPr>
   <dimension ref="A1:BA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22714,7 +22732,7 @@
   <sheetData>
     <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>234</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -22744,96 +22762,96 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="M2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="P2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:53" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H3" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="O3" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="P3" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="Q3" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="R3" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="51" t="s">
+      <c r="S3" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="O3" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="R3" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="S3" s="52" t="s">
-        <v>83</v>
-      </c>
       <c r="T3" s="179" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="U3" s="179" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="V3" s="179" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="W3" s="179" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="X3" s="179" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="Y3" s="53" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="53" t="s">
         <v>3</v>
       </c>
       <c r="AA3" s="192" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="AB3" s="192" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="AC3" s="47" t="s">
         <v>1</v>
@@ -22844,10 +22862,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E4" s="41">
         <v>0</v>
@@ -22901,17 +22919,17 @@
         <v>1</v>
       </c>
       <c r="V4" s="48" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="W4" s="48"/>
       <c r="X4" s="48">
         <v>0.6</v>
       </c>
       <c r="Y4" s="184" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="Z4" s="184" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="AA4" s="193">
         <v>0.4</v>
@@ -22920,7 +22938,7 @@
         <v>25</v>
       </c>
       <c r="AC4" s="40" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
@@ -22928,10 +22946,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E5" s="41">
         <v>1</v>
@@ -22985,17 +23003,17 @@
         <v>1</v>
       </c>
       <c r="V5" s="48" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="W5" s="48"/>
       <c r="X5" s="48">
         <v>0.3</v>
       </c>
       <c r="Y5" s="184" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="Z5" s="184" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="AA5" s="193">
         <v>0.4</v>
@@ -23004,7 +23022,7 @@
         <v>25</v>
       </c>
       <c r="AC5" s="40" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
@@ -23012,10 +23030,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E6" s="41">
         <v>2</v>
@@ -23069,17 +23087,17 @@
         <v>1</v>
       </c>
       <c r="V6" s="48" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="W6" s="180"/>
       <c r="X6" s="206">
         <v>0.6</v>
       </c>
       <c r="Y6" s="55" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="Z6" s="55" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="AA6" s="193">
         <v>0.4</v>
@@ -23088,13 +23106,13 @@
         <v>25</v>
       </c>
       <c r="AC6" s="45" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -23154,157 +23172,157 @@
     </row>
     <row r="12" spans="1:53" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="K12" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AB12" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AC12" s="23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AD12" s="22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AE12" s="22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AF12" s="177" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AG12" s="178" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AH12" s="130" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AI12" s="22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AJ12" s="22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AK12" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AL12" s="22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AM12" s="22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AN12" s="135" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AO12" s="133" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AP12" s="27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="AQ12" s="28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AR12" s="25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AS12" s="24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AT12" s="24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AU12" s="24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AV12" s="24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AW12" s="155" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AX12" s="27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AY12" s="21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AZ12" s="21" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="BA12" s="24" t="s">
         <v>1</v>
@@ -23315,16 +23333,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G13" s="34">
         <v>0</v>
@@ -23393,13 +23411,13 @@
         <v>12</v>
       </c>
       <c r="AC13" s="35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="AD13" s="36" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AE13" s="36" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AF13" s="36"/>
       <c r="AG13" s="128"/>
@@ -23461,7 +23479,7 @@
         <v>1</v>
       </c>
       <c r="BA13" s="146" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
@@ -23469,16 +23487,16 @@
         <v>2</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G14" s="34">
         <v>10</v>
@@ -23547,13 +23565,13 @@
         <v>12</v>
       </c>
       <c r="AC14" s="35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="AD14" s="36" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AE14" s="36" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AF14" s="36"/>
       <c r="AG14" s="128"/>
@@ -23615,7 +23633,7 @@
         <v>1.2</v>
       </c>
       <c r="BA14" s="146" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
@@ -23623,16 +23641,16 @@
         <v>2</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G15" s="34">
         <v>20</v>
@@ -23701,13 +23719,13 @@
         <v>12</v>
       </c>
       <c r="AC15" s="35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="AD15" s="36" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AE15" s="36" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AF15" s="36"/>
       <c r="AG15" s="128"/>
@@ -23769,7 +23787,7 @@
         <v>1.3</v>
       </c>
       <c r="BA15" s="146" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.25">
@@ -23778,16 +23796,16 @@
         <v>2</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G16" s="34">
         <v>30</v>
@@ -23856,13 +23874,13 @@
         <v>12</v>
       </c>
       <c r="AC16" s="35" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="AD16" s="36" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AE16" s="36" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AF16" s="36"/>
       <c r="AG16" s="128"/>
@@ -23924,7 +23942,7 @@
         <v>1.5</v>
       </c>
       <c r="BA16" s="146" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
@@ -23932,16 +23950,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="104" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E17" s="106" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G17" s="108">
         <v>0</v>
@@ -24010,13 +24028,13 @@
         <v>12</v>
       </c>
       <c r="AC17" s="114" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="AD17" s="115" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="AE17" s="115" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="AF17" s="115"/>
       <c r="AG17" s="129"/>
@@ -24078,7 +24096,7 @@
         <v>1</v>
       </c>
       <c r="BA17" s="147" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.25">
@@ -24086,16 +24104,16 @@
         <v>2</v>
       </c>
       <c r="C18" s="104" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18" s="106" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G18" s="108">
         <v>10</v>
@@ -24164,13 +24182,13 @@
         <v>12</v>
       </c>
       <c r="AC18" s="114" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="AD18" s="115" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="AE18" s="115" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="AF18" s="115"/>
       <c r="AG18" s="129"/>
@@ -24232,7 +24250,7 @@
         <v>1.2</v>
       </c>
       <c r="BA18" s="147" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.25">
@@ -24240,16 +24258,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="104" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E19" s="106" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F19" s="107" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G19" s="108">
         <v>20</v>
@@ -24318,13 +24336,13 @@
         <v>12</v>
       </c>
       <c r="AC19" s="114" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="AD19" s="115" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="AE19" s="115" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="AF19" s="115"/>
       <c r="AG19" s="129"/>
@@ -24386,7 +24404,7 @@
         <v>1.3</v>
       </c>
       <c r="BA19" s="147" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.25">
@@ -24394,16 +24412,16 @@
         <v>2</v>
       </c>
       <c r="C20" s="104" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E20" s="106" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F20" s="107" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G20" s="108">
         <v>30</v>
@@ -24472,13 +24490,13 @@
         <v>12</v>
       </c>
       <c r="AC20" s="114" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="AD20" s="115" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="AE20" s="115" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="AF20" s="115"/>
       <c r="AG20" s="129"/>
@@ -24540,7 +24558,7 @@
         <v>1.5</v>
       </c>
       <c r="BA20" s="147" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.25">
@@ -24548,16 +24566,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>66</v>
+        <v>239</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G21" s="34">
         <v>0</v>
@@ -24626,13 +24644,13 @@
         <v>12</v>
       </c>
       <c r="AC21" s="35" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="AD21" s="36" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="AE21" s="36" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="AF21" s="36"/>
       <c r="AG21" s="128"/>
@@ -24690,11 +24708,11 @@
       <c r="AY21" s="99">
         <v>8</v>
       </c>
-      <c r="AZ21" s="146">
+      <c r="AZ21" s="99">
         <v>1</v>
       </c>
-      <c r="BA21" s="98" t="s">
-        <v>4</v>
+      <c r="BA21" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.25">
@@ -24702,16 +24720,16 @@
         <v>2</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>103</v>
+        <v>240</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G22" s="34">
         <v>10</v>
@@ -24780,13 +24798,13 @@
         <v>12</v>
       </c>
       <c r="AC22" s="35" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="AD22" s="36" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="AE22" s="36" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="AF22" s="36"/>
       <c r="AG22" s="128"/>
@@ -24844,11 +24862,11 @@
       <c r="AY22" s="99">
         <v>8</v>
       </c>
-      <c r="AZ22" s="146">
+      <c r="AZ22" s="99">
         <v>1.2</v>
       </c>
-      <c r="BA22" s="98" t="s">
-        <v>5</v>
+      <c r="BA22" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.25">
@@ -24856,16 +24874,16 @@
         <v>2</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G23" s="34">
         <v>20</v>
@@ -24934,13 +24952,13 @@
         <v>12</v>
       </c>
       <c r="AC23" s="35" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="AD23" s="36" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="AE23" s="36" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="AF23" s="36"/>
       <c r="AG23" s="128"/>
@@ -24998,11 +25016,11 @@
       <c r="AY23" s="99">
         <v>15</v>
       </c>
-      <c r="AZ23" s="146">
+      <c r="AZ23" s="99">
         <v>1.3</v>
       </c>
-      <c r="BA23" s="98" t="s">
-        <v>6</v>
+      <c r="BA23" s="118" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25011,16 +25029,16 @@
         <v>2</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>105</v>
+        <v>242</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G24" s="34">
         <v>30</v>
@@ -25089,13 +25107,13 @@
         <v>12</v>
       </c>
       <c r="AC24" s="35" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="AD24" s="36" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="AE24" s="36" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="AF24" s="36"/>
       <c r="AG24" s="128"/>
@@ -25153,11 +25171,11 @@
       <c r="AY24" s="99">
         <v>15</v>
       </c>
-      <c r="AZ24" s="146">
+      <c r="AZ24" s="99">
         <v>1.5</v>
       </c>
-      <c r="BA24" s="98" t="s">
-        <v>7</v>
+      <c r="BA24" s="118" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:53" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -25168,11 +25186,11 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="215" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I25" s="216"/>
       <c r="J25" s="217" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K25" s="218"/>
       <c r="L25" s="218"/>
@@ -25181,13 +25199,13 @@
       <c r="O25" s="219"/>
       <c r="P25" s="72"/>
       <c r="Q25" s="211" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="R25" s="212"/>
       <c r="S25" s="212"/>
       <c r="T25" s="212"/>
       <c r="U25" s="213" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="V25" s="214"/>
       <c r="W25" s="214"/>
@@ -25197,7 +25215,7 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
       <c r="AH25" s="208" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="AI25" s="209"/>
       <c r="AJ25" s="209"/>
@@ -25209,7 +25227,7 @@
     <row r="27" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -25222,28 +25240,28 @@
     </row>
     <row r="30" spans="1:53" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F30" s="59" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G30" s="188" t="s">
         <v>3</v>
       </c>
       <c r="H30" s="188" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I30" s="188" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.25">
@@ -25251,10 +25269,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D31" s="57" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E31" s="57">
         <v>5</v>
@@ -25264,13 +25282,13 @@
         <v>icon_helicopter_power_1</v>
       </c>
       <c r="G31" s="189" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="H31" s="191" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="I31" s="189" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.25">
@@ -25278,10 +25296,10 @@
         <v>2</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E32" s="57">
         <v>15</v>
@@ -25291,13 +25309,13 @@
         <v>icon_helicopter_power_2</v>
       </c>
       <c r="G32" s="189" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="H32" s="190" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="I32" s="189" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -25305,10 +25323,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E33" s="57">
         <v>25</v>
@@ -25318,13 +25336,13 @@
         <v>icon_helicopter_power_3</v>
       </c>
       <c r="G33" s="189" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="H33" s="190" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="I33" s="189" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -25332,10 +25350,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D34" s="57" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E34" s="57">
         <v>5</v>
@@ -25345,13 +25363,13 @@
         <v>icon_electric_power_1</v>
       </c>
       <c r="G34" s="189" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="H34" s="190" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="I34" s="189" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -25359,10 +25377,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D35" s="57" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E35" s="57">
         <v>15</v>
@@ -25372,13 +25390,13 @@
         <v>icon_electric_power_2</v>
       </c>
       <c r="G35" s="189" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="H35" s="190" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="I35" s="189" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -25386,10 +25404,10 @@
         <v>2</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D36" s="57" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E36" s="57">
         <v>25</v>
@@ -25399,13 +25417,13 @@
         <v>icon_electric_power_3</v>
       </c>
       <c r="G36" s="189" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="H36" s="190" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="I36" s="189" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -25413,26 +25431,26 @@
         <v>2</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>92</v>
+        <v>246</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="E37" s="57">
         <v>5</v>
       </c>
       <c r="F37" s="58" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
-        <v>icon_sonic_power_1</v>
+        <v>icon_hedgehog_power_1</v>
       </c>
       <c r="G37" s="203" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H37" s="204" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="I37" s="203" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -25440,26 +25458,26 @@
         <v>2</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>93</v>
+        <v>247</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="E38" s="57">
         <v>15</v>
       </c>
       <c r="F38" s="58" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
-        <v>icon_sonic_power_2</v>
+        <v>icon_hedgehog_power_2</v>
       </c>
       <c r="G38" s="203" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H38" s="204" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="I38" s="203" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -25467,32 +25485,32 @@
         <v>2</v>
       </c>
       <c r="C39" s="60" t="s">
-        <v>94</v>
+        <v>248</v>
       </c>
       <c r="D39" s="61" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="E39" s="61">
         <v>25</v>
       </c>
       <c r="F39" s="58" t="str">
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
-        <v>icon_sonic_power_3</v>
+        <v>icon_hedgehog_power_3</v>
       </c>
       <c r="G39" s="203" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H39" s="207" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="I39" s="203" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -25501,37 +25519,37 @@
     </row>
     <row r="45" spans="2:13" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B45" s="194" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C45" s="195" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="196" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E45" s="197" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F45" s="198" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="G45" s="198" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="H45" s="198" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I45" s="198" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="J45" s="198" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K45" s="198" t="s">
         <v>3</v>
       </c>
       <c r="L45" s="198" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M45" s="198" t="s">
         <v>1</v>
@@ -25542,13 +25560,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="200" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="D46" s="201" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="E46" s="201" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F46" s="202">
         <v>0</v>
@@ -25563,16 +25581,16 @@
         <v>0</v>
       </c>
       <c r="J46" s="202" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="K46" s="202" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="L46" s="202" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="M46" s="202" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
@@ -25580,13 +25598,13 @@
         <v>2</v>
       </c>
       <c r="C47" s="200" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="D47" s="201" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E47" s="201" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F47" s="202">
         <v>1</v>
@@ -25601,16 +25619,16 @@
         <v>4</v>
       </c>
       <c r="J47" s="202" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="K47" s="202" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="L47" s="202" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="M47" s="202" t="s">
-        <v>204</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
@@ -25618,13 +25636,13 @@
         <v>2</v>
       </c>
       <c r="C48" s="200" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="D48" s="201" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="E48" s="201" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="F48" s="202">
         <v>0</v>
@@ -25639,22 +25657,22 @@
         <v>0</v>
       </c>
       <c r="J48" s="202" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="K48" s="202" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="L48" s="202" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="M48" s="202" t="s">
-        <v>205</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -25662,7 +25680,7 @@
     </row>
     <row r="54" spans="2:5" ht="121.5" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>0</v>
@@ -25671,7 +25689,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="47" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -25679,13 +25697,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="56" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D55" s="57" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E55" s="57" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -25693,13 +25711,13 @@
         <v>2</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D56" s="57" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E56" s="57" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -25707,13 +25725,13 @@
         <v>2</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -25725,37 +25743,43 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="155" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="154" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="153" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="152" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="151" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="150" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="duplicateValues" dxfId="149" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA22:BA24">
-    <cfRule type="duplicateValues" dxfId="148" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C48">
-    <cfRule type="duplicateValues" dxfId="147" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="duplicateValues" dxfId="146" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC6">
-    <cfRule type="duplicateValues" dxfId="145" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA22">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA23">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA24">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -25802,7 +25826,7 @@
   <sheetData>
     <row r="1" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -25828,34 +25852,34 @@
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
       <c r="B3" s="159" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C3" s="159" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="160" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="E3" s="160" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F3" s="161" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G3" s="161" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="H3" s="162" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="I3" s="162" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="J3" s="163" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="164" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -25863,10 +25887,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="166" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D4" s="166" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="E4" s="166">
         <v>0</v>
@@ -25884,10 +25908,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="K4" s="170" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -25895,10 +25919,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="166" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D5" s="166" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="E5" s="166">
         <v>1</v>
@@ -25916,10 +25940,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="169" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="K5" s="170" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -25927,10 +25951,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="166" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D6" s="166" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="E6" s="166">
         <v>2</v>
@@ -25948,16 +25972,16 @@
         <v>1</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="K6" s="171" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -25967,19 +25991,19 @@
     </row>
     <row r="11" spans="2:13" ht="159" x14ac:dyDescent="0.25">
       <c r="B11" s="172" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C11" s="173" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="173" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="174" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F11" s="174" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -25987,10 +26011,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="176" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D12" s="176" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" s="176">
         <v>0.7</v>
@@ -26004,10 +26028,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="176" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D13" s="176" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E13" s="176">
         <v>1.5</v>
@@ -26021,10 +26045,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="176" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="D14" s="176" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E14" s="176">
         <v>3</v>
@@ -26038,10 +26062,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="176" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D15" s="176" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E15" s="176">
         <v>4</v>
@@ -26055,7 +26079,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="33" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -26087,25 +26111,25 @@
   <sheetData>
     <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="65" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
       <c r="E3" s="221" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F3" s="221"/>
       <c r="G3" s="221"/>
       <c r="H3" s="221"/>
       <c r="J3" s="63" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="R3" s="63" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
@@ -26123,19 +26147,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="L4" s="62">
         <v>20</v>
       </c>
       <c r="S4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="T4" s="62">
         <v>20</v>
       </c>
       <c r="AA4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="AB4" s="62">
         <v>20</v>
@@ -26143,7 +26167,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="64" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E5" s="66">
         <v>100</v>
@@ -26158,36 +26182,36 @@
         <v>250</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L5" s="62">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="T5" s="62">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AB5" s="62">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="64" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E6" s="66">
         <v>100</v>
@@ -26202,36 +26226,36 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L6" s="62">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="T6" s="62">
         <v>60</v>
       </c>
       <c r="U6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AB6" s="62">
         <v>60</v>
       </c>
       <c r="AC6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="73" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E7" s="74">
         <v>240</v>
@@ -26246,40 +26270,40 @@
         <v>285</v>
       </c>
       <c r="K7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="N7" s="138"/>
       <c r="S7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
         <v>3</v>
       </c>
       <c r="AC7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="77" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E8" s="75">
         <v>0</v>
@@ -26296,19 +26320,19 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="V10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AD10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="78"/>
       <c r="D11" s="79" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E11" s="80">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -26318,53 +26342,53 @@
       <c r="G11" s="80"/>
       <c r="H11" s="81"/>
       <c r="J11" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="67" t="s">
-        <v>126</v>
-      </c>
       <c r="L11" s="67" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="M11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="N11" s="67" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
       <c r="R11" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="S11" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="T11" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="S11" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="67" t="s">
-        <v>127</v>
-      </c>
       <c r="U11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
       <c r="Z11" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="AA11" s="67" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AB11" s="67" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="AC11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AD11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -26375,7 +26399,7 @@
       <c r="G12" s="83"/>
       <c r="H12" s="71"/>
       <c r="J12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -26394,7 +26418,7 @@
         <v>5</v>
       </c>
       <c r="R12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -26413,7 +26437,7 @@
         <v>3</v>
       </c>
       <c r="Z12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AT17)/'special dragons'!AS17,1)</f>
@@ -26434,24 +26458,24 @@
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="82" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D13" s="83" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E13" s="84">
         <v>1</v>
       </c>
       <c r="F13" s="83"/>
       <c r="G13" s="68" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H13" s="69">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>105</v>
       </c>
       <c r="J13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -26470,7 +26494,7 @@
         <v>7.5</v>
       </c>
       <c r="R13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -26489,7 +26513,7 @@
         <v>3.6</v>
       </c>
       <c r="Z13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AT18)/'special dragons'!AS18,1)</f>
@@ -26510,24 +26534,24 @@
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="82" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E14" s="84">
         <v>0</v>
       </c>
       <c r="F14" s="83"/>
       <c r="G14" s="68" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H14" s="69">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>100</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -26546,7 +26570,7 @@
         <v>10</v>
       </c>
       <c r="R14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -26565,7 +26589,7 @@
         <v>4.2</v>
       </c>
       <c r="Z14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AT19)/'special dragons'!AS19,1)</f>
@@ -26586,24 +26610,24 @@
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="82" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" s="84">
         <v>0</v>
       </c>
       <c r="F15" s="83"/>
       <c r="G15" s="68" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H15" s="69">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,46,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,45,1,1,"special dragons")),1)</f>
         <v>10.1</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -26622,7 +26646,7 @@
         <v>12.5</v>
       </c>
       <c r="R15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -26641,7 +26665,7 @@
         <v>4.8</v>
       </c>
       <c r="Z15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AT20)/'special dragons'!AS20,1)</f>
@@ -26663,7 +26687,7 @@
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="82"/>
       <c r="D16" s="89" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E16" s="89">
         <f>SUM(E13:E15)</f>
@@ -27054,22 +27078,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27101,25 +27125,25 @@
   <sheetData>
     <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="65" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
       <c r="E3" s="221" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F3" s="221"/>
       <c r="G3" s="221"/>
       <c r="H3" s="221"/>
       <c r="J3" s="63" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="R3" s="63" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
@@ -27137,19 +27161,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="L4" s="62">
         <v>20</v>
       </c>
       <c r="S4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="T4" s="62">
         <v>20</v>
       </c>
       <c r="AA4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="AB4" s="62">
         <v>20</v>
@@ -27157,7 +27181,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="64" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E5" s="66">
         <v>175</v>
@@ -27172,36 +27196,36 @@
         <v>400</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L5" s="62">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="T5" s="62">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AB5" s="62">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="64" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E6" s="66">
         <v>100</v>
@@ -27216,36 +27240,36 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L6" s="62">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="T6" s="62">
         <v>60</v>
       </c>
       <c r="U6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AB6" s="62">
         <v>60</v>
       </c>
       <c r="AC6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="73" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E7" s="74">
         <v>100</v>
@@ -27260,39 +27284,39 @@
         <v>130</v>
       </c>
       <c r="K7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
         <v>3</v>
       </c>
       <c r="AC7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="77" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E8" s="75">
         <v>0</v>
@@ -27309,19 +27333,19 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="V10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AD10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="78"/>
       <c r="D11" s="79" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E11" s="80">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -27331,53 +27355,53 @@
       <c r="G11" s="80"/>
       <c r="H11" s="81"/>
       <c r="J11" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="67" t="s">
-        <v>126</v>
-      </c>
       <c r="L11" s="67" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="M11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="N11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
       <c r="R11" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="S11" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="T11" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="S11" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="67" t="s">
-        <v>127</v>
-      </c>
       <c r="U11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
       <c r="Z11" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="AA11" s="67" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AB11" s="67" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="AC11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AD11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27388,7 +27412,7 @@
       <c r="G12" s="83"/>
       <c r="H12" s="71"/>
       <c r="J12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -27407,7 +27431,7 @@
         <v>8.75</v>
       </c>
       <c r="R12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -27426,7 +27450,7 @@
         <v>3</v>
       </c>
       <c r="Z12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AT13)/'special dragons'!AS13,1)</f>
@@ -27447,24 +27471,24 @@
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="82" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D13" s="83" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E13" s="84">
         <v>0</v>
       </c>
       <c r="F13" s="83"/>
       <c r="G13" s="68" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H13" s="69">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>175</v>
       </c>
       <c r="J13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -27483,7 +27507,7 @@
         <v>12.5</v>
       </c>
       <c r="R13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -27502,7 +27526,7 @@
         <v>3.6</v>
       </c>
       <c r="Z13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AT14)/'special dragons'!AS14,1)</f>
@@ -27523,24 +27547,24 @@
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="82" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E14" s="84">
         <v>0</v>
       </c>
       <c r="F14" s="83"/>
       <c r="G14" s="68" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H14" s="69">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>100</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -27559,7 +27583,7 @@
         <v>15</v>
       </c>
       <c r="R14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -27578,7 +27602,7 @@
         <v>4.2</v>
       </c>
       <c r="Z14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AT15)/'special dragons'!AS15,1)</f>
@@ -27599,24 +27623,24 @@
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="82" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" s="84">
         <v>0</v>
       </c>
       <c r="F15" s="83"/>
       <c r="G15" s="68" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H15" s="69">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(12+E11,46,1,1,"special dragons")))/INDIRECT(ADDRESS(12+E11,45,1,1,"special dragons")),1)</f>
         <v>13.3</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -27635,7 +27659,7 @@
         <v>20</v>
       </c>
       <c r="R15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -27654,7 +27678,7 @@
         <v>4.8</v>
       </c>
       <c r="Z15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AT16)/'special dragons'!AS16,1)</f>
@@ -27676,7 +27700,7 @@
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="82"/>
       <c r="D16" s="89" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E16" s="89">
         <f>SUM(E13:E15)</f>
@@ -28075,22 +28099,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28122,25 +28146,25 @@
   <sheetData>
     <row r="1" spans="3:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="65" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
       <c r="E3" s="221" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F3" s="221"/>
       <c r="G3" s="221"/>
       <c r="H3" s="221"/>
       <c r="J3" s="63" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="R3" s="63" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.25">
@@ -28158,19 +28182,19 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="L4" s="62">
         <v>20</v>
       </c>
       <c r="S4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="T4" s="62">
         <v>20</v>
       </c>
       <c r="AA4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="AB4" s="62">
         <v>20</v>
@@ -28178,7 +28202,7 @@
     </row>
     <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D5" s="64" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E5" s="66">
         <v>100</v>
@@ -28193,36 +28217,36 @@
         <v>250</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L5" s="62">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="T5" s="62">
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AB5" s="62">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D6" s="64" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E6" s="66">
         <v>100</v>
@@ -28237,36 +28261,36 @@
         <v>160</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L6" s="62">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="S6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="T6" s="62">
         <v>60</v>
       </c>
       <c r="U6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AB6" s="62">
         <v>60</v>
       </c>
       <c r="AC6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="73" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E7" s="74">
         <v>240</v>
@@ -28281,40 +28305,40 @@
         <v>285</v>
       </c>
       <c r="K7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="L7">
         <f>ROUND((L6-L5)/L4,1)</f>
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="N7" s="138"/>
       <c r="S7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="T7">
         <f>ROUND((T6-T5)/T4,1)</f>
         <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="AA7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="AB7">
         <f>ROUND((AB6-AB5)/AB4,1)</f>
         <v>3</v>
       </c>
       <c r="AC7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="77" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E8" s="75">
         <v>0</v>
@@ -28331,19 +28355,19 @@
     </row>
     <row r="10" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="V10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AD10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="78"/>
       <c r="D11" s="79" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E11" s="80">
         <f>IF(E16&lt;F8,1,IF(AND(E16&gt;=F8,E16&lt;G8),2,IF(AND(E16&gt;=G8,E16&lt;H8),3,4)))</f>
@@ -28353,53 +28377,53 @@
       <c r="G11" s="80"/>
       <c r="H11" s="81"/>
       <c r="J11" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="67" t="s">
-        <v>126</v>
-      </c>
       <c r="L11" s="67" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="M11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="N11" s="67" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="O11" s="67"/>
       <c r="P11" s="67"/>
       <c r="R11" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="S11" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="T11" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="S11" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="67" t="s">
-        <v>127</v>
-      </c>
       <c r="U11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
       <c r="Z11" s="63" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="AA11" s="67" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AB11" s="67" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="AC11" s="67" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AD11" s="67" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28410,7 +28434,7 @@
       <c r="G12" s="83"/>
       <c r="H12" s="71"/>
       <c r="J12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="K12">
         <f>E5</f>
@@ -28429,7 +28453,7 @@
         <v>5</v>
       </c>
       <c r="R12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="S12">
         <f>E6</f>
@@ -28448,7 +28472,7 @@
         <v>3</v>
       </c>
       <c r="Z12" s="63" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AT17)/'special dragons'!AS17,1)</f>
@@ -28469,24 +28493,24 @@
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="82" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D13" s="83" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E13" s="84">
         <v>0</v>
       </c>
       <c r="F13" s="83"/>
       <c r="G13" s="68" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H13" s="69">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
         <v>100</v>
       </c>
       <c r="J13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K13">
         <f>F5</f>
@@ -28505,7 +28529,7 @@
         <v>7.5</v>
       </c>
       <c r="R13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="S13">
         <f>F6</f>
@@ -28524,7 +28548,7 @@
         <v>3.6</v>
       </c>
       <c r="Z13" s="63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AT18)/'special dragons'!AS18,1)</f>
@@ -28545,24 +28569,24 @@
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="82" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E14" s="84">
         <v>0</v>
       </c>
       <c r="F14" s="83"/>
       <c r="G14" s="68" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H14" s="69">
         <f ca="1">INDIRECT(ADDRESS(6,4+E11)) + (INDIRECT(ADDRESS(6,4+E11)) *(T7/100) *E14)</f>
         <v>100</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="K14">
         <f>G5</f>
@@ -28581,7 +28605,7 @@
         <v>10</v>
       </c>
       <c r="R14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="S14">
         <f>G6</f>
@@ -28600,7 +28624,7 @@
         <v>4.2</v>
       </c>
       <c r="Z14" s="63" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AT19)/'special dragons'!AS19,1)</f>
@@ -28621,24 +28645,24 @@
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="82" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E15" s="84">
         <v>0</v>
       </c>
       <c r="F15" s="83"/>
       <c r="G15" s="68" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H15" s="69">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(16+E11,46,1,1,"special dragons")))/INDIRECT(ADDRESS(16+E11,45,1,1,"special dragons")),1)</f>
         <v>10.1</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="K15">
         <f>H5</f>
@@ -28657,7 +28681,7 @@
         <v>12.5</v>
       </c>
       <c r="R15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="S15">
         <f>H6</f>
@@ -28676,7 +28700,7 @@
         <v>4.8</v>
       </c>
       <c r="Z15" s="63" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AT20)/'special dragons'!AS20,1)</f>
@@ -28698,7 +28722,7 @@
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="82"/>
       <c r="D16" s="89" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E16" s="89">
         <f>SUM(E13:E15)</f>
@@ -29089,22 +29113,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29130,36 +29154,36 @@
   <sheetData>
     <row r="4" spans="6:23" x14ac:dyDescent="0.25">
       <c r="G4" s="88" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H4" s="88" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="I4" s="88" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="N4" s="88" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="O4" s="88" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="P4" s="88" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="U4" s="88" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="V4" s="88" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="W4" s="88" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -29171,7 +29195,7 @@
         <v>11.15</v>
       </c>
       <c r="M5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="N5">
         <v>120</v>
@@ -29183,7 +29207,7 @@
         <v>11.15</v>
       </c>
       <c r="T5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="U5">
         <v>120</v>
@@ -29197,7 +29221,7 @@
     </row>
     <row r="6" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G6">
         <v>240</v>
@@ -29209,7 +29233,7 @@
         <v>14.15</v>
       </c>
       <c r="M6" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="N6">
         <v>240</v>
@@ -29221,7 +29245,7 @@
         <v>14.15</v>
       </c>
       <c r="T6" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="U6">
         <v>240</v>
@@ -29235,7 +29259,7 @@
     </row>
     <row r="7" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="G7">
         <v>365</v>
@@ -29247,7 +29271,7 @@
         <v>14.8</v>
       </c>
       <c r="M7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="N7">
         <v>365</v>
@@ -29259,7 +29283,7 @@
         <v>14.8</v>
       </c>
       <c r="T7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="U7">
         <v>365</v>
@@ -29273,7 +29297,7 @@
     </row>
     <row r="8" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="G8">
         <v>410</v>
@@ -29285,7 +29309,7 @@
         <v>15.25</v>
       </c>
       <c r="M8" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="N8">
         <v>410</v>
@@ -29297,7 +29321,7 @@
         <v>15.25</v>
       </c>
       <c r="T8" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="U8">
         <v>410</v>
@@ -29311,7 +29335,7 @@
     </row>
     <row r="9" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G9">
         <f ca="1">Electric!H13</f>
@@ -29326,7 +29350,7 @@
         <v>10.1</v>
       </c>
       <c r="M9" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="N9">
         <f ca="1">Helicopter!H13</f>
@@ -29341,7 +29365,7 @@
         <v>13.3</v>
       </c>
       <c r="T9" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="U9">
         <f ca="1">Sonic!H13</f>

</xml_diff>

<commit_message>
adding a new "Hedgehog disguise"
Former-commit-id: 165d2806778bf46a3ed898e4d0bfaf6d1b196872
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="273">
   <si>
     <t>[sku]</t>
   </si>
@@ -846,12 +846,15 @@
   <si>
     <t>SPEED</t>
   </si>
+  <si>
+    <t>dragon_hedgehog_1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,6 +952,19 @@
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1116,7 +1132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1646,11 +1662,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2112,6 +2150,12 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2154,17 +2198,49 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="158">
+  <dxfs count="160">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2246,6 +2322,146 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2705,16 +2921,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5885,136 +6091,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -43997,116 +44073,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="144" totalsRowBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="159" totalsRowBorderDxfId="158">
   <autoFilter ref="B12:BA24"/>
   <tableColumns count="52">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="142"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="141"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="140"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="139"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="138"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="137"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="136"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="135"/>
-    <tableColumn id="10" name="[health]" dataDxfId="134"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="133"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="132"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="131"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="130"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="129"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="128"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="127"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="126"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="125"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="124"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="123"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="122"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="121"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="120"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="119"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="118"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="117"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="116"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="115"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="114"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="113"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="112"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="111"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="110"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="109"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="108"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="107"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="106"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="105"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="104"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="103"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="102"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="101"/>
-    <tableColumn id="46" name="[force]" dataDxfId="100"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="99"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="98"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="97"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="96"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="95"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="94"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="93"/>
-    <tableColumn id="6" name="[scaleMenu]" dataDxfId="92"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="91"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="157"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="156"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="155"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="154"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="153"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="152"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="151"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="150"/>
+    <tableColumn id="10" name="[health]" dataDxfId="149"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="148"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="147"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="146"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="145"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="144"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="143"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="142"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="141"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="140"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="139"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="138"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="137"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="136"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="135"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="134"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="133"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="132"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="131"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="130"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="129"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="128"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="127"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="126"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="125"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="124"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="123"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="122"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="121"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="120"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="119"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="118"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="117"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="116"/>
+    <tableColumn id="46" name="[force]" dataDxfId="115"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="114"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="113"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="112"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="111"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="110"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="109"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="108"/>
+    <tableColumn id="6" name="[scaleMenu]" dataDxfId="107"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102">
   <autoFilter ref="B3:AC6"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="86"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="101"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="85"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="84"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="83"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="82"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="81"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="80"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="79"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="78"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="77"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="76"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="75"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="74"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="73"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="72"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="71"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="70"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="69"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="68"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="67"/>
-    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="66"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="65"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="64"/>
-    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="63"/>
-    <tableColumn id="14" name="[mummyDuration]" dataDxfId="62"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="61"/>
+    <tableColumn id="5" name="[order]" dataDxfId="100"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="99"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="98"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="97"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="96"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="95"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="94"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="93"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="92"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="91"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="90"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="89"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="88"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="87"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="86"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="85"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="84"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="83"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="82"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="81"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="80"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="79"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="78"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="77"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="B30:I39"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="57"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="56"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="55"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="54"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="53">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="72"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="70"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="69"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="68">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="52"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="51"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="67"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="66"/>
     <tableColumn id="8" name="[tidDescShort]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -44114,54 +44190,54 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M48" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
-  <autoFilter ref="B45:M48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M49" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
+  <autoFilter ref="B45:M49"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="45"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="43"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="42"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="41"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="40"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="39"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="38"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="37"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="36"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="35"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="34"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="60"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="59"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="58"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="57"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="56"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="55"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="54"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="53"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="52"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="51"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="50"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="48" tableBorderDxfId="47">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="30"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="29"/>
-    <tableColumn id="7" name="[index]" dataDxfId="28"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="27"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="26"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="25"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="24"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="23"/>
-    <tableColumn id="10" name="[color]" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="46"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="45"/>
+    <tableColumn id="7" name="[index]" dataDxfId="44"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="43"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="42"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="41"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="40"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="39"/>
+    <tableColumn id="10" name="[color]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="14"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="13"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="12"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="30"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="29"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -44433,10 +44509,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:BA57"/>
+  <dimension ref="A1:BA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46894,7 +46970,7 @@
       </c>
       <c r="AF24" s="36"/>
       <c r="AG24" s="115"/>
-      <c r="AH24" s="197">
+      <c r="AH24" s="183">
         <v>1.4</v>
       </c>
       <c r="AI24" s="36">
@@ -46912,7 +46988,7 @@
       <c r="AM24" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="AN24" s="198">
+      <c r="AN24" s="184">
         <v>10</v>
       </c>
       <c r="AO24" s="121">
@@ -46962,44 +47038,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="190" t="s">
+      <c r="H25" s="192" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="191"/>
-      <c r="J25" s="192" t="s">
+      <c r="I25" s="193"/>
+      <c r="J25" s="194" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="193"/>
-      <c r="L25" s="193"/>
-      <c r="M25" s="193"/>
-      <c r="N25" s="193"/>
-      <c r="O25" s="194"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="N25" s="195"/>
+      <c r="O25" s="196"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="186" t="s">
+      <c r="Q25" s="188" t="s">
         <v>126</v>
       </c>
-      <c r="R25" s="187"/>
-      <c r="S25" s="187"/>
-      <c r="T25" s="187"/>
-      <c r="U25" s="188" t="s">
+      <c r="R25" s="189"/>
+      <c r="S25" s="189"/>
+      <c r="T25" s="189"/>
+      <c r="U25" s="190" t="s">
         <v>9</v>
       </c>
-      <c r="V25" s="189"/>
-      <c r="W25" s="189"/>
-      <c r="X25" s="189"/>
+      <c r="V25" s="191"/>
+      <c r="W25" s="191"/>
+      <c r="X25" s="191"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="183" t="s">
+      <c r="AH25" s="185" t="s">
         <v>127</v>
       </c>
-      <c r="AI25" s="184"/>
-      <c r="AJ25" s="184"/>
-      <c r="AK25" s="184"/>
-      <c r="AL25" s="184"/>
-      <c r="AM25" s="184"/>
-      <c r="AN25" s="185"/>
+      <c r="AI25" s="186"/>
+      <c r="AJ25" s="186"/>
+      <c r="AK25" s="186"/>
+      <c r="AL25" s="186"/>
+      <c r="AM25" s="186"/>
+      <c r="AN25" s="187"/>
     </row>
     <row r="27" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
@@ -47446,68 +47522,106 @@
         <v>259</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B52" s="1" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="199" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="200" t="s">
+        <v>272</v>
+      </c>
+      <c r="D49" s="201" t="s">
+        <v>272</v>
+      </c>
+      <c r="E49" s="202" t="s">
+        <v>235</v>
+      </c>
+      <c r="F49" s="203">
+        <v>0</v>
+      </c>
+      <c r="G49" s="204">
+        <v>0</v>
+      </c>
+      <c r="H49" s="204">
+        <v>0</v>
+      </c>
+      <c r="I49" s="204">
+        <v>0</v>
+      </c>
+      <c r="J49" s="204" t="s">
+        <v>182</v>
+      </c>
+      <c r="K49" s="204" t="s">
+        <v>256</v>
+      </c>
+      <c r="L49" s="204" t="s">
+        <v>256</v>
+      </c>
+      <c r="M49" s="204" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="2:5" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="12" t="s">
+    <row r="55" spans="2:13" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="47" t="s">
+      <c r="E55" s="47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="56" t="s">
-        <v>197</v>
-      </c>
-      <c r="D55" s="57" t="s">
-        <v>200</v>
-      </c>
-      <c r="E55" s="57" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D56" s="57" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E56" s="57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="D57" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="E57" s="57" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="D57" s="57" t="s">
+      <c r="D58" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="E57" s="57" t="s">
+      <c r="E58" s="57" t="s">
         <v>205</v>
       </c>
     </row>
@@ -47520,43 +47634,46 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="157" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="156" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="155" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="154" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="153" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="152" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="duplicateValues" dxfId="151" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:C48">
-    <cfRule type="duplicateValues" dxfId="150" priority="10"/>
+  <conditionalFormatting sqref="C46:C49">
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:C57">
-    <cfRule type="duplicateValues" dxfId="149" priority="7"/>
+  <conditionalFormatting sqref="C56:C58">
+    <cfRule type="duplicateValues" dxfId="19" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC6">
-    <cfRule type="duplicateValues" dxfId="148" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA22">
-    <cfRule type="duplicateValues" dxfId="147" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA23">
-    <cfRule type="duplicateValues" dxfId="146" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA24">
-    <cfRule type="duplicateValues" dxfId="145" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -47623,8 +47740,8 @@
       <c r="D2" s="137"/>
       <c r="E2" s="137"/>
       <c r="F2" s="138"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
       <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -47856,7 +47973,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="33" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -47893,12 +48010,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="196" t="s">
+      <c r="E3" s="198" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -48855,22 +48972,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48907,12 +49024,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="196" t="s">
+      <c r="E3" s="198" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -49876,22 +49993,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49928,12 +50045,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="196" t="s">
+      <c r="E3" s="198" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -50890,22 +51007,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
unlock level set to 1
Former-commit-id: 9930664e47cf1a9b303f1b7b49ed3359b6e18019
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -44512,7 +44512,7 @@
   <dimension ref="A1:BA58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47545,7 +47545,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="204" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Content - Change TID titlte name
Former-commit-id: dbd19b4b57dfe098ef042c6e6b0d69102b9e7640
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="376">
   <si>
     <t>[sku]</t>
   </si>
@@ -938,9 +938,6 @@
     <t>PF_TrophyLeague10</t>
   </si>
   <si>
-    <t>TID_LEAGUE_1_NAME</t>
-  </si>
-  <si>
     <t>reward_006</t>
   </si>
   <si>
@@ -1131,6 +1128,36 @@
   </si>
   <si>
     <t>0.10</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_1</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_2</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_3</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_4</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_5</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_6</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_7</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_8</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_9</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_10</t>
   </si>
 </sst>
 </file>
@@ -26774,8 +26801,8 @@
   </sheetPr>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26849,10 +26876,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E4" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F4" s="223">
         <v>1</v>
@@ -26864,7 +26891,7 @@
         <v>292</v>
       </c>
       <c r="I4" s="223" t="s">
-        <v>302</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -26878,10 +26905,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E5" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F5" s="223">
         <v>1</v>
@@ -26893,7 +26920,7 @@
         <v>293</v>
       </c>
       <c r="I5" s="223" t="s">
-        <v>302</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -26907,10 +26934,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E6" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F6" s="223">
         <v>1</v>
@@ -26922,7 +26949,7 @@
         <v>294</v>
       </c>
       <c r="I6" s="223" t="s">
-        <v>302</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -26936,10 +26963,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E7" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F7" s="223">
         <v>1</v>
@@ -26951,7 +26978,7 @@
         <v>295</v>
       </c>
       <c r="I7" s="223" t="s">
-        <v>302</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -26965,10 +26992,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E8" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F8" s="223">
         <v>1</v>
@@ -26980,7 +27007,7 @@
         <v>296</v>
       </c>
       <c r="I8" s="223" t="s">
-        <v>302</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -26994,10 +27021,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E9" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F9" s="223">
         <v>1</v>
@@ -27009,7 +27036,7 @@
         <v>297</v>
       </c>
       <c r="I9" s="223" t="s">
-        <v>302</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -27023,10 +27050,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E10" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F10" s="223">
         <v>1</v>
@@ -27038,7 +27065,7 @@
         <v>298</v>
       </c>
       <c r="I10" s="223" t="s">
-        <v>302</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -27052,10 +27079,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E11" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F11" s="223">
         <v>1</v>
@@ -27067,7 +27094,7 @@
         <v>299</v>
       </c>
       <c r="I11" s="223" t="s">
-        <v>302</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -27081,10 +27108,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E12" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F12" s="223">
         <v>1</v>
@@ -27096,7 +27123,7 @@
         <v>300</v>
       </c>
       <c r="I12" s="223" t="s">
-        <v>302</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -27110,10 +27137,10 @@
         <v>9</v>
       </c>
       <c r="D13" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E13" s="223" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F13" s="223">
         <v>1</v>
@@ -27125,7 +27152,7 @@
         <v>301</v>
       </c>
       <c r="I13" s="223" t="s">
-        <v>302</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -27155,19 +27182,19 @@
         <v>0</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="224" t="s">
         <v>355</v>
-      </c>
-      <c r="G17" s="224" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -27175,13 +27202,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="223" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C18" s="223" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D18" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E18" s="223">
         <v>4000</v>
@@ -27190,7 +27217,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -27198,13 +27225,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="223" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="223" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D19" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E19" s="223">
         <v>8000</v>
@@ -27213,7 +27240,7 @@
         <v>90</v>
       </c>
       <c r="G19" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -27221,13 +27248,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="223" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C20" s="223" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D20" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E20" s="223">
         <v>10000</v>
@@ -27236,7 +27263,7 @@
         <v>50</v>
       </c>
       <c r="G20" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -27244,13 +27271,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="223" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C21" s="223" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D21" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E21" s="223">
         <v>20</v>
@@ -27259,7 +27286,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -27267,13 +27294,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="223" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C22" s="223" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D22" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E22" s="223">
         <v>80</v>
@@ -27282,7 +27309,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -27290,13 +27317,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="223" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C23" s="223" t="s">
         <v>272</v>
       </c>
       <c r="D23" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E23" s="223">
         <v>4000</v>
@@ -27305,7 +27332,7 @@
         <v>100</v>
       </c>
       <c r="G23" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -27313,13 +27340,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="223" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C24" s="223" t="s">
         <v>272</v>
       </c>
       <c r="D24" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E24" s="223">
         <v>8000</v>
@@ -27328,7 +27355,7 @@
         <v>90</v>
       </c>
       <c r="G24" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -27336,13 +27363,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="223" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C25" s="223" t="s">
         <v>272</v>
       </c>
       <c r="D25" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E25" s="223">
         <v>10000</v>
@@ -27351,7 +27378,7 @@
         <v>50</v>
       </c>
       <c r="G25" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -27359,13 +27386,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="223" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C26" s="223" t="s">
         <v>272</v>
       </c>
       <c r="D26" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E26" s="223">
         <v>20</v>
@@ -27374,7 +27401,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -27382,13 +27409,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="223" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" s="223" t="s">
         <v>272</v>
       </c>
       <c r="D27" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E27" s="223">
         <v>80</v>
@@ -27397,7 +27424,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -27405,13 +27432,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="223" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C28" s="223" t="s">
         <v>273</v>
       </c>
       <c r="D28" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E28" s="223">
         <v>12000</v>
@@ -27420,7 +27447,7 @@
         <v>100</v>
       </c>
       <c r="G28" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -27428,13 +27455,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="223" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C29" s="223" t="s">
         <v>273</v>
       </c>
       <c r="D29" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E29" s="223">
         <v>16000</v>
@@ -27443,7 +27470,7 @@
         <v>90</v>
       </c>
       <c r="G29" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -27451,13 +27478,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="223" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C30" s="223" t="s">
         <v>273</v>
       </c>
       <c r="D30" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E30" s="223">
         <v>20000</v>
@@ -27466,7 +27493,7 @@
         <v>50</v>
       </c>
       <c r="G30" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -27474,13 +27501,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="223" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C31" s="223" t="s">
         <v>273</v>
       </c>
       <c r="D31" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E31" s="223">
         <v>30</v>
@@ -27489,7 +27516,7 @@
         <v>10</v>
       </c>
       <c r="G31" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -27497,13 +27524,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="223" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C32" s="223" t="s">
         <v>273</v>
       </c>
       <c r="D32" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E32" s="223">
         <v>100</v>
@@ -27512,7 +27539,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -27520,13 +27547,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="223" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C33" s="223" t="s">
         <v>274</v>
       </c>
       <c r="D33" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E33" s="223">
         <v>21000</v>
@@ -27535,7 +27562,7 @@
         <v>100</v>
       </c>
       <c r="G33" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -27543,13 +27570,13 @@
         <v>2</v>
       </c>
       <c r="B34" s="223" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C34" s="223" t="s">
         <v>274</v>
       </c>
       <c r="D34" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E34" s="223">
         <v>24000</v>
@@ -27558,7 +27585,7 @@
         <v>90</v>
       </c>
       <c r="G34" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -27566,13 +27593,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="223" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C35" s="223" t="s">
         <v>274</v>
       </c>
       <c r="D35" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E35" s="223">
         <v>30000</v>
@@ -27581,7 +27608,7 @@
         <v>50</v>
       </c>
       <c r="G35" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -27589,13 +27616,13 @@
         <v>2</v>
       </c>
       <c r="B36" s="223" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C36" s="223" t="s">
         <v>274</v>
       </c>
       <c r="D36" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E36" s="223">
         <v>50</v>
@@ -27604,7 +27631,7 @@
         <v>10</v>
       </c>
       <c r="G36" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -27612,13 +27639,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="223" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C37" s="223" t="s">
         <v>274</v>
       </c>
       <c r="D37" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E37" s="223">
         <v>110</v>
@@ -27627,7 +27654,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -27635,13 +27662,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="223" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C38" s="223" t="s">
         <v>275</v>
       </c>
       <c r="D38" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E38" s="223">
         <v>32000</v>
@@ -27650,7 +27677,7 @@
         <v>100</v>
       </c>
       <c r="G38" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -27658,13 +27685,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="223" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C39" s="223" t="s">
         <v>275</v>
       </c>
       <c r="D39" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E39" s="223">
         <v>37000</v>
@@ -27673,7 +27700,7 @@
         <v>90</v>
       </c>
       <c r="G39" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -27681,13 +27708,13 @@
         <v>2</v>
       </c>
       <c r="B40" s="223" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C40" s="223" t="s">
         <v>275</v>
       </c>
       <c r="D40" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E40" s="223">
         <v>42000</v>
@@ -27696,7 +27723,7 @@
         <v>50</v>
       </c>
       <c r="G40" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -27704,13 +27731,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="223" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C41" s="223" t="s">
         <v>275</v>
       </c>
       <c r="D41" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E41" s="223">
         <v>60</v>
@@ -27719,7 +27746,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -27727,13 +27754,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="223" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C42" s="223" t="s">
         <v>275</v>
       </c>
       <c r="D42" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E42" s="223">
         <v>120</v>
@@ -27742,7 +27769,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -27750,13 +27777,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="223" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C43" s="223" t="s">
         <v>276</v>
       </c>
       <c r="D43" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E43" s="223">
         <v>43000</v>
@@ -27765,7 +27792,7 @@
         <v>100</v>
       </c>
       <c r="G43" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -27773,13 +27800,13 @@
         <v>2</v>
       </c>
       <c r="B44" s="223" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C44" s="223" t="s">
         <v>276</v>
       </c>
       <c r="D44" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E44" s="223">
         <v>48000</v>
@@ -27788,7 +27815,7 @@
         <v>90</v>
       </c>
       <c r="G44" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -27796,13 +27823,13 @@
         <v>2</v>
       </c>
       <c r="B45" s="223" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C45" s="223" t="s">
         <v>276</v>
       </c>
       <c r="D45" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E45" s="223">
         <v>50000</v>
@@ -27811,7 +27838,7 @@
         <v>50</v>
       </c>
       <c r="G45" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -27819,13 +27846,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="223" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C46" s="223" t="s">
         <v>276</v>
       </c>
       <c r="D46" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E46" s="223">
         <v>70</v>
@@ -27834,7 +27861,7 @@
         <v>10</v>
       </c>
       <c r="G46" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -27842,13 +27869,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="223" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C47" s="223" t="s">
         <v>276</v>
       </c>
       <c r="D47" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E47" s="223">
         <v>130</v>
@@ -27857,7 +27884,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -27865,13 +27892,13 @@
         <v>2</v>
       </c>
       <c r="B48" s="223" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C48" s="223" t="s">
         <v>277</v>
       </c>
       <c r="D48" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E48" s="223">
         <v>52000</v>
@@ -27880,7 +27907,7 @@
         <v>100</v>
       </c>
       <c r="G48" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -27888,13 +27915,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="223" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C49" s="223" t="s">
         <v>277</v>
       </c>
       <c r="D49" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E49" s="223">
         <v>55000</v>
@@ -27903,7 +27930,7 @@
         <v>90</v>
       </c>
       <c r="G49" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -27911,13 +27938,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="223" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C50" s="223" t="s">
         <v>277</v>
       </c>
       <c r="D50" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E50" s="223">
         <v>58000</v>
@@ -27926,7 +27953,7 @@
         <v>50</v>
       </c>
       <c r="G50" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -27934,13 +27961,13 @@
         <v>2</v>
       </c>
       <c r="B51" s="223" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C51" s="223" t="s">
         <v>277</v>
       </c>
       <c r="D51" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E51" s="223">
         <v>80</v>
@@ -27949,7 +27976,7 @@
         <v>10</v>
       </c>
       <c r="G51" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -27957,13 +27984,13 @@
         <v>2</v>
       </c>
       <c r="B52" s="223" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C52" s="223" t="s">
         <v>277</v>
       </c>
       <c r="D52" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E52" s="223">
         <v>140</v>
@@ -27972,7 +27999,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -27980,13 +28007,13 @@
         <v>2</v>
       </c>
       <c r="B53" s="223" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C53" s="223" t="s">
         <v>278</v>
       </c>
       <c r="D53" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E53" s="223">
         <v>60000</v>
@@ -27995,7 +28022,7 @@
         <v>100</v>
       </c>
       <c r="G53" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -28003,13 +28030,13 @@
         <v>2</v>
       </c>
       <c r="B54" s="223" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C54" s="223" t="s">
         <v>278</v>
       </c>
       <c r="D54" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E54" s="223">
         <v>63000</v>
@@ -28018,7 +28045,7 @@
         <v>90</v>
       </c>
       <c r="G54" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -28026,13 +28053,13 @@
         <v>2</v>
       </c>
       <c r="B55" s="223" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C55" s="223" t="s">
         <v>278</v>
       </c>
       <c r="D55" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E55" s="223">
         <v>67000</v>
@@ -28041,7 +28068,7 @@
         <v>50</v>
       </c>
       <c r="G55" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -28049,13 +28076,13 @@
         <v>2</v>
       </c>
       <c r="B56" s="223" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C56" s="223" t="s">
         <v>278</v>
       </c>
       <c r="D56" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E56" s="223">
         <v>90</v>
@@ -28064,7 +28091,7 @@
         <v>10</v>
       </c>
       <c r="G56" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -28072,13 +28099,13 @@
         <v>2</v>
       </c>
       <c r="B57" s="223" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C57" s="223" t="s">
         <v>278</v>
       </c>
       <c r="D57" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E57" s="223">
         <v>150</v>
@@ -28087,7 +28114,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -28095,13 +28122,13 @@
         <v>2</v>
       </c>
       <c r="B58" s="223" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C58" s="223" t="s">
         <v>279</v>
       </c>
       <c r="D58" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E58" s="223">
         <v>70000</v>
@@ -28110,7 +28137,7 @@
         <v>100</v>
       </c>
       <c r="G58" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -28118,13 +28145,13 @@
         <v>2</v>
       </c>
       <c r="B59" s="223" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C59" s="223" t="s">
         <v>279</v>
       </c>
       <c r="D59" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E59" s="223">
         <v>73000</v>
@@ -28133,7 +28160,7 @@
         <v>90</v>
       </c>
       <c r="G59" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -28141,13 +28168,13 @@
         <v>2</v>
       </c>
       <c r="B60" s="223" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C60" s="223" t="s">
         <v>279</v>
       </c>
       <c r="D60" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E60" s="223">
         <v>80000</v>
@@ -28156,7 +28183,7 @@
         <v>50</v>
       </c>
       <c r="G60" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -28164,13 +28191,13 @@
         <v>2</v>
       </c>
       <c r="B61" s="223" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C61" s="223" t="s">
         <v>279</v>
       </c>
       <c r="D61" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E61" s="223">
         <v>100</v>
@@ -28179,7 +28206,7 @@
         <v>10</v>
       </c>
       <c r="G61" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -28187,13 +28214,13 @@
         <v>2</v>
       </c>
       <c r="B62" s="223" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C62" s="223" t="s">
         <v>279</v>
       </c>
       <c r="D62" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E62" s="223">
         <v>160</v>
@@ -28202,7 +28229,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -28210,13 +28237,13 @@
         <v>2</v>
       </c>
       <c r="B63" s="223" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C63" s="223" t="s">
         <v>280</v>
       </c>
       <c r="D63" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E63" s="223">
         <v>82000</v>
@@ -28225,7 +28252,7 @@
         <v>100</v>
       </c>
       <c r="G63" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -28233,13 +28260,13 @@
         <v>2</v>
       </c>
       <c r="B64" s="223" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C64" s="223" t="s">
         <v>280</v>
       </c>
       <c r="D64" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E64" s="223">
         <v>85000</v>
@@ -28248,7 +28275,7 @@
         <v>90</v>
       </c>
       <c r="G64" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -28256,13 +28283,13 @@
         <v>2</v>
       </c>
       <c r="B65" s="223" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C65" s="223" t="s">
         <v>280</v>
       </c>
       <c r="D65" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E65" s="223">
         <v>89000</v>
@@ -28271,7 +28298,7 @@
         <v>50</v>
       </c>
       <c r="G65" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -28279,13 +28306,13 @@
         <v>2</v>
       </c>
       <c r="B66" s="223" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C66" s="223" t="s">
         <v>280</v>
       </c>
       <c r="D66" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E66" s="223">
         <v>110</v>
@@ -28294,7 +28321,7 @@
         <v>10</v>
       </c>
       <c r="G66" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -28302,13 +28329,13 @@
         <v>2</v>
       </c>
       <c r="B67" s="223" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C67" s="223" t="s">
         <v>280</v>
       </c>
       <c r="D67" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E67" s="223">
         <v>170</v>
@@ -28317,7 +28344,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -28325,13 +28352,13 @@
         <v>2</v>
       </c>
       <c r="B68" s="223" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C68" s="223" t="s">
         <v>281</v>
       </c>
       <c r="D68" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E68" s="223">
         <v>92000</v>
@@ -28340,7 +28367,7 @@
         <v>100</v>
       </c>
       <c r="G68" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -28348,13 +28375,13 @@
         <v>2</v>
       </c>
       <c r="B69" s="223" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C69" s="223" t="s">
         <v>281</v>
       </c>
       <c r="D69" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E69" s="223">
         <v>95000</v>
@@ -28363,7 +28390,7 @@
         <v>90</v>
       </c>
       <c r="G69" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -28371,13 +28398,13 @@
         <v>2</v>
       </c>
       <c r="B70" s="223" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C70" s="223" t="s">
         <v>281</v>
       </c>
       <c r="D70" s="223" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E70" s="223">
         <v>120000</v>
@@ -28386,7 +28413,7 @@
         <v>50</v>
       </c>
       <c r="G70" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -28394,13 +28421,13 @@
         <v>2</v>
       </c>
       <c r="B71" s="223" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C71" s="223" t="s">
         <v>281</v>
       </c>
       <c r="D71" s="223" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E71" s="223">
         <v>120</v>
@@ -28409,7 +28436,7 @@
         <v>10</v>
       </c>
       <c r="G71" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -28417,13 +28444,13 @@
         <v>2</v>
       </c>
       <c r="B72" s="226" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C72" s="226" t="s">
         <v>281</v>
       </c>
       <c r="D72" s="226" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E72" s="226">
         <v>180</v>
@@ -28432,7 +28459,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="225" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Content - Add again the league reward to excel
Former-commit-id: e6f5fc6500b8aa30c63b7bdda7b2dbd2848d0af8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
     <sheet name="Special Missions" sheetId="14" r:id="rId2"/>
-    <sheet name="Electric" sheetId="11" r:id="rId3"/>
-    <sheet name="Helicopter" sheetId="13" r:id="rId4"/>
-    <sheet name="Sonic" sheetId="15" r:id="rId5"/>
-    <sheet name="DATA" sheetId="12" r:id="rId6"/>
+    <sheet name="Special Leagues" sheetId="16" r:id="rId3"/>
+    <sheet name="Electric" sheetId="11" r:id="rId4"/>
+    <sheet name="Helicopter" sheetId="13" r:id="rId5"/>
+    <sheet name="Sonic" sheetId="15" r:id="rId6"/>
+    <sheet name="DATA" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="385">
   <si>
     <t>[sku]</t>
   </si>
@@ -849,6 +850,342 @@
   <si>
     <t>dragon_hedgehog_1</t>
   </si>
+  <si>
+    <t>LEAGUES DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{leaguesDefinitions}</t>
+  </si>
+  <si>
+    <t>[demoteScale]</t>
+  </si>
+  <si>
+    <t>[promoteScale]</t>
+  </si>
+  <si>
+    <t>[rewardFactor]</t>
+  </si>
+  <si>
+    <t>[trophyPrefab]</t>
+  </si>
+  <si>
+    <t>league_1</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>icon_league_1</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague1</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_1</t>
+  </si>
+  <si>
+    <t>league_2</t>
+  </si>
+  <si>
+    <t>icon_league_2</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague2</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_2</t>
+  </si>
+  <si>
+    <t>league_3</t>
+  </si>
+  <si>
+    <t>icon_league_3</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague3</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_3</t>
+  </si>
+  <si>
+    <t>league_4</t>
+  </si>
+  <si>
+    <t>icon_league_4</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague4</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_4</t>
+  </si>
+  <si>
+    <t>league_5</t>
+  </si>
+  <si>
+    <t>icon_league_5</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague5</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_5</t>
+  </si>
+  <si>
+    <t>league_6</t>
+  </si>
+  <si>
+    <t>icon_league_6</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague6</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_6</t>
+  </si>
+  <si>
+    <t>league_7</t>
+  </si>
+  <si>
+    <t>icon_league_7</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague7</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_7</t>
+  </si>
+  <si>
+    <t>league_8</t>
+  </si>
+  <si>
+    <t>icon_league_8</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague8</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_8</t>
+  </si>
+  <si>
+    <t>league_9</t>
+  </si>
+  <si>
+    <t>icon_league_9</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague9</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_9</t>
+  </si>
+  <si>
+    <t>league_10</t>
+  </si>
+  <si>
+    <t>icon_league_10</t>
+  </si>
+  <si>
+    <t>PF_TrophyLeague10</t>
+  </si>
+  <si>
+    <t>TID_LEAGUES_TITLE_10</t>
+  </si>
+  <si>
+    <t>LEAGUES REWARDS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{leaguesRewardsDefinitions}</t>
+  </si>
+  <si>
+    <t>[group]</t>
+  </si>
+  <si>
+    <t>[amount]</t>
+  </si>
+  <si>
+    <t>[target]</t>
+  </si>
+  <si>
+    <t>[rsku]</t>
+  </si>
+  <si>
+    <t>reward_001</t>
+  </si>
+  <si>
+    <t>rwd_default</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>reward_002</t>
+  </si>
+  <si>
+    <t>reward_003</t>
+  </si>
+  <si>
+    <t>reward_004</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>reward_005</t>
+  </si>
+  <si>
+    <t>reward_006</t>
+  </si>
+  <si>
+    <t>reward_007</t>
+  </si>
+  <si>
+    <t>reward_008</t>
+  </si>
+  <si>
+    <t>reward_009</t>
+  </si>
+  <si>
+    <t>reward_010</t>
+  </si>
+  <si>
+    <t>reward_011</t>
+  </si>
+  <si>
+    <t>reward_012</t>
+  </si>
+  <si>
+    <t>reward_013</t>
+  </si>
+  <si>
+    <t>reward_014</t>
+  </si>
+  <si>
+    <t>reward_015</t>
+  </si>
+  <si>
+    <t>reward_016</t>
+  </si>
+  <si>
+    <t>reward_017</t>
+  </si>
+  <si>
+    <t>reward_018</t>
+  </si>
+  <si>
+    <t>reward_019</t>
+  </si>
+  <si>
+    <t>reward_020</t>
+  </si>
+  <si>
+    <t>reward_021</t>
+  </si>
+  <si>
+    <t>reward_022</t>
+  </si>
+  <si>
+    <t>reward_023</t>
+  </si>
+  <si>
+    <t>reward_024</t>
+  </si>
+  <si>
+    <t>reward_025</t>
+  </si>
+  <si>
+    <t>reward_026</t>
+  </si>
+  <si>
+    <t>reward_027</t>
+  </si>
+  <si>
+    <t>reward_028</t>
+  </si>
+  <si>
+    <t>reward_029</t>
+  </si>
+  <si>
+    <t>reward_030</t>
+  </si>
+  <si>
+    <t>reward_031</t>
+  </si>
+  <si>
+    <t>reward_032</t>
+  </si>
+  <si>
+    <t>reward_033</t>
+  </si>
+  <si>
+    <t>reward_034</t>
+  </si>
+  <si>
+    <t>reward_035</t>
+  </si>
+  <si>
+    <t>reward_036</t>
+  </si>
+  <si>
+    <t>reward_037</t>
+  </si>
+  <si>
+    <t>reward_038</t>
+  </si>
+  <si>
+    <t>reward_039</t>
+  </si>
+  <si>
+    <t>reward_040</t>
+  </si>
+  <si>
+    <t>reward_041</t>
+  </si>
+  <si>
+    <t>reward_042</t>
+  </si>
+  <si>
+    <t>reward_043</t>
+  </si>
+  <si>
+    <t>reward_044</t>
+  </si>
+  <si>
+    <t>reward_045</t>
+  </si>
+  <si>
+    <t>reward_046</t>
+  </si>
+  <si>
+    <t>reward_047</t>
+  </si>
+  <si>
+    <t>reward_048</t>
+  </si>
+  <si>
+    <t>reward_049</t>
+  </si>
+  <si>
+    <t>reward_050</t>
+  </si>
+  <si>
+    <t>reward_051</t>
+  </si>
+  <si>
+    <t>reward_052</t>
+  </si>
+  <si>
+    <t>reward_053</t>
+  </si>
+  <si>
+    <t>reward_054</t>
+  </si>
+  <si>
+    <t>reward_055</t>
+  </si>
 </sst>
 </file>
 
@@ -959,12 +1296,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1688,7 +2027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2156,6 +2495,24 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2198,29 +2555,373 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="160">
+  <dxfs count="173">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2322,146 +3023,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2921,6 +3482,16 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6091,6 +6662,146 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -44073,116 +44784,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="159" totalsRowBorderDxfId="158">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA24" totalsRowShown="0" headerRowBorderDxfId="158" totalsRowBorderDxfId="157">
   <autoFilter ref="B12:BA24"/>
   <tableColumns count="52">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="157"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="156"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="155"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="154"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="153"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="152"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="151"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="150"/>
-    <tableColumn id="10" name="[health]" dataDxfId="149"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="148"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="147"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="146"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="145"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="144"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="143"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="142"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="141"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="140"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="139"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="138"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="137"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="136"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="135"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="134"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="133"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="132"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="131"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="130"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="129"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="128"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="127"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="126"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="125"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="124"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="123"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="122"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="121"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="120"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="119"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="118"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="117"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="116"/>
-    <tableColumn id="46" name="[force]" dataDxfId="115"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="114"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="113"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="112"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="111"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="110"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="109"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="108"/>
-    <tableColumn id="6" name="[scaleMenu]" dataDxfId="107"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="106"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="156"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="155"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="154"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="153"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="152"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="151"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="150"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="149"/>
+    <tableColumn id="10" name="[health]" dataDxfId="148"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="147"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="146"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="145"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="144"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="143"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="142"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="141"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="140"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="139"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="138"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="137"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="136"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="135"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="134"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="133"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="132"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="131"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="130"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="129"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="128"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="127"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="126"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="125"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="124"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="123"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="122"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="121"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="120"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="119"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="118"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="117"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="116"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="115"/>
+    <tableColumn id="46" name="[force]" dataDxfId="114"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="113"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="112"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="111"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="110"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="109"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="108"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="107"/>
+    <tableColumn id="6" name="[scaleMenu]" dataDxfId="106"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="105" dataDxfId="103" headerRowBorderDxfId="104" tableBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC6" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101">
   <autoFilter ref="B3:AC6"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="101"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="100"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="100"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="99"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="98"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="97"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="96"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="95"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="94"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="93"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="92"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="91"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="90"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="89"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="88"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="87"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="86"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="85"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="84"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="83"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="82"/>
-    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="81"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="80"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="79"/>
-    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="78"/>
-    <tableColumn id="14" name="[mummyDuration]" dataDxfId="77"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="76"/>
+    <tableColumn id="5" name="[order]" dataDxfId="99"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="98"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="97"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="96"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="95"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="94"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="93"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="92"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="91"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="90"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="89"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="88"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="87"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="86"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="85"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="84"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="83"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="82"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="81"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="80"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="79"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="78"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="77"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="76"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B30:I39" totalsRowShown="0" headerRowBorderDxfId="74" tableBorderDxfId="73" totalsRowBorderDxfId="72">
   <autoFilter ref="B30:I39"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="72"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="70"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="69"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="68">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="71"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="70"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="69"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="68"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="67">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="67"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="66"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="66"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="65"/>
     <tableColumn id="8" name="[tidDescShort]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -44190,56 +44901,72 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M49" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B45:M49" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <autoFilter ref="B45:M49"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="60"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="59"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="58"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="57"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="56"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="55"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="54"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="53"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="52"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="51"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="50"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="49"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="59"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="58"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="57"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="56"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="55"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="54"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="53"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="52"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="51"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="50"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="49"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="48" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="46"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="45"/>
-    <tableColumn id="7" name="[index]" dataDxfId="44"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="43"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="42"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="41"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="40"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="39"/>
-    <tableColumn id="10" name="[color]" dataDxfId="38"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="44"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="43"/>
+    <tableColumn id="7" name="[index]" dataDxfId="42"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="41"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="40"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="39"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="38"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="37"/>
+    <tableColumn id="10" name="[color]" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="30"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="29"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="28"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="28"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="27"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:G72" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A17:G72"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="{leaguesRewardsDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="3" name="[group]" dataDxfId="4"/>
+    <tableColumn id="4" name="[type]" dataDxfId="3"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="2"/>
+    <tableColumn id="6" name="[target]" dataDxfId="1"/>
+    <tableColumn id="7" name="[rsku]" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -44511,7 +45238,7 @@
   </sheetPr>
   <dimension ref="A1:BA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
@@ -47038,44 +47765,44 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="192" t="s">
+      <c r="H25" s="198" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="193"/>
-      <c r="J25" s="194" t="s">
+      <c r="I25" s="199"/>
+      <c r="J25" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="195"/>
-      <c r="L25" s="195"/>
-      <c r="M25" s="195"/>
-      <c r="N25" s="195"/>
-      <c r="O25" s="196"/>
+      <c r="K25" s="201"/>
+      <c r="L25" s="201"/>
+      <c r="M25" s="201"/>
+      <c r="N25" s="201"/>
+      <c r="O25" s="202"/>
       <c r="P25" s="72"/>
-      <c r="Q25" s="188" t="s">
+      <c r="Q25" s="194" t="s">
         <v>126</v>
       </c>
-      <c r="R25" s="189"/>
-      <c r="S25" s="189"/>
-      <c r="T25" s="189"/>
-      <c r="U25" s="190" t="s">
+      <c r="R25" s="195"/>
+      <c r="S25" s="195"/>
+      <c r="T25" s="195"/>
+      <c r="U25" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="V25" s="191"/>
-      <c r="W25" s="191"/>
-      <c r="X25" s="191"/>
+      <c r="V25" s="197"/>
+      <c r="W25" s="197"/>
+      <c r="X25" s="197"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
-      <c r="AH25" s="185" t="s">
+      <c r="AH25" s="191" t="s">
         <v>127</v>
       </c>
-      <c r="AI25" s="186"/>
-      <c r="AJ25" s="186"/>
-      <c r="AK25" s="186"/>
-      <c r="AL25" s="186"/>
-      <c r="AM25" s="186"/>
-      <c r="AN25" s="187"/>
+      <c r="AI25" s="192"/>
+      <c r="AJ25" s="192"/>
+      <c r="AK25" s="192"/>
+      <c r="AL25" s="192"/>
+      <c r="AM25" s="192"/>
+      <c r="AN25" s="193"/>
     </row>
     <row r="27" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
@@ -47523,40 +48250,40 @@
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="199" t="s">
+      <c r="B49" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="200" t="s">
+      <c r="C49" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="D49" s="201" t="s">
+      <c r="D49" s="187" t="s">
         <v>272</v>
       </c>
-      <c r="E49" s="202" t="s">
+      <c r="E49" s="188" t="s">
         <v>235</v>
       </c>
-      <c r="F49" s="203">
+      <c r="F49" s="189">
         <v>0</v>
       </c>
-      <c r="G49" s="204">
+      <c r="G49" s="190">
         <v>0</v>
       </c>
-      <c r="H49" s="204">
+      <c r="H49" s="190">
         <v>0</v>
       </c>
-      <c r="I49" s="204">
+      <c r="I49" s="190">
         <v>1</v>
       </c>
-      <c r="J49" s="204" t="s">
+      <c r="J49" s="190" t="s">
         <v>182</v>
       </c>
-      <c r="K49" s="204" t="s">
+      <c r="K49" s="190" t="s">
         <v>256</v>
       </c>
-      <c r="L49" s="204" t="s">
+      <c r="L49" s="190" t="s">
         <v>256</v>
       </c>
-      <c r="M49" s="204" t="s">
+      <c r="M49" s="190" t="s">
         <v>259</v>
       </c>
     </row>
@@ -47634,46 +48361,46 @@
     <mergeCell ref="J25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="27" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="duplicateValues" dxfId="26" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C36">
-    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="duplicateValues" dxfId="24" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39">
-    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C49">
-    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C58">
-    <cfRule type="duplicateValues" dxfId="19" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC6">
-    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA22">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA23">
-    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA24">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D24">
@@ -47740,8 +48467,8 @@
       <c r="D2" s="137"/>
       <c r="E2" s="137"/>
       <c r="F2" s="138"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
       <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -47973,7 +48700,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="14" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -47984,6 +48711,1688 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:I72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="137"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+    </row>
+    <row r="3" spans="1:9" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="206">
+        <v>0</v>
+      </c>
+      <c r="D4" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E4" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" s="206">
+        <v>1</v>
+      </c>
+      <c r="G4" s="206" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="206" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" s="206" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="206">
+        <v>1</v>
+      </c>
+      <c r="D5" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F5" s="206">
+        <v>1</v>
+      </c>
+      <c r="G5" s="206" t="s">
+        <v>285</v>
+      </c>
+      <c r="H5" s="206" t="s">
+        <v>286</v>
+      </c>
+      <c r="I5" s="206" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="206">
+        <v>2</v>
+      </c>
+      <c r="D6" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="206">
+        <v>1</v>
+      </c>
+      <c r="G6" s="206" t="s">
+        <v>289</v>
+      </c>
+      <c r="H6" s="206" t="s">
+        <v>290</v>
+      </c>
+      <c r="I6" s="206" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="206">
+        <v>3</v>
+      </c>
+      <c r="D7" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" s="206">
+        <v>1</v>
+      </c>
+      <c r="G7" s="206" t="s">
+        <v>293</v>
+      </c>
+      <c r="H7" s="206" t="s">
+        <v>294</v>
+      </c>
+      <c r="I7" s="206" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="C8" s="206">
+        <v>4</v>
+      </c>
+      <c r="D8" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E8" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" s="206">
+        <v>1</v>
+      </c>
+      <c r="G8" s="206" t="s">
+        <v>297</v>
+      </c>
+      <c r="H8" s="206" t="s">
+        <v>298</v>
+      </c>
+      <c r="I8" s="206" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="206">
+        <v>5</v>
+      </c>
+      <c r="D9" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" s="206">
+        <v>1</v>
+      </c>
+      <c r="G9" s="206" t="s">
+        <v>301</v>
+      </c>
+      <c r="H9" s="206" t="s">
+        <v>302</v>
+      </c>
+      <c r="I9" s="206" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="206">
+        <v>6</v>
+      </c>
+      <c r="D10" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E10" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="206">
+        <v>1</v>
+      </c>
+      <c r="G10" s="206" t="s">
+        <v>305</v>
+      </c>
+      <c r="H10" s="206" t="s">
+        <v>306</v>
+      </c>
+      <c r="I10" s="206" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="206">
+        <v>7</v>
+      </c>
+      <c r="D11" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E11" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F11" s="206">
+        <v>1</v>
+      </c>
+      <c r="G11" s="206" t="s">
+        <v>309</v>
+      </c>
+      <c r="H11" s="206" t="s">
+        <v>310</v>
+      </c>
+      <c r="I11" s="206" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="206">
+        <v>8</v>
+      </c>
+      <c r="D12" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="206">
+        <v>1</v>
+      </c>
+      <c r="G12" s="206" t="s">
+        <v>313</v>
+      </c>
+      <c r="H12" s="206" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" s="206" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="205" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="206" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" s="206">
+        <v>9</v>
+      </c>
+      <c r="D13" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="206" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="206">
+        <v>1</v>
+      </c>
+      <c r="G13" s="206" t="s">
+        <v>317</v>
+      </c>
+      <c r="H13" s="206" t="s">
+        <v>318</v>
+      </c>
+      <c r="I13" s="206" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="137"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="137"/>
+    </row>
+    <row r="17" spans="1:7" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="207" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="206" t="s">
+        <v>326</v>
+      </c>
+      <c r="C18" s="206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E18" s="206">
+        <v>4000</v>
+      </c>
+      <c r="F18" s="206">
+        <v>100</v>
+      </c>
+      <c r="G18" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="206" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E19" s="206">
+        <v>8000</v>
+      </c>
+      <c r="F19" s="206">
+        <v>90</v>
+      </c>
+      <c r="G19" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="206" t="s">
+        <v>331</v>
+      </c>
+      <c r="C20" s="206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D20" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E20" s="206">
+        <v>10000</v>
+      </c>
+      <c r="F20" s="206">
+        <v>50</v>
+      </c>
+      <c r="G20" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="206" t="s">
+        <v>332</v>
+      </c>
+      <c r="C21" s="206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D21" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E21" s="206">
+        <v>20</v>
+      </c>
+      <c r="F21" s="206">
+        <v>10</v>
+      </c>
+      <c r="G21" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="206" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="206" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E22" s="206">
+        <v>80</v>
+      </c>
+      <c r="F22" s="206">
+        <v>1</v>
+      </c>
+      <c r="G22" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="206" t="s">
+        <v>335</v>
+      </c>
+      <c r="C23" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E23" s="206">
+        <v>4000</v>
+      </c>
+      <c r="F23" s="206">
+        <v>100</v>
+      </c>
+      <c r="G23" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="206" t="s">
+        <v>336</v>
+      </c>
+      <c r="C24" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E24" s="206">
+        <v>8000</v>
+      </c>
+      <c r="F24" s="206">
+        <v>90</v>
+      </c>
+      <c r="G24" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="206" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="D25" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E25" s="206">
+        <v>10000</v>
+      </c>
+      <c r="F25" s="206">
+        <v>50</v>
+      </c>
+      <c r="G25" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="206" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" s="206">
+        <v>20</v>
+      </c>
+      <c r="F26" s="206">
+        <v>10</v>
+      </c>
+      <c r="G26" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="206" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="206" t="s">
+        <v>279</v>
+      </c>
+      <c r="D27" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" s="206">
+        <v>80</v>
+      </c>
+      <c r="F27" s="206">
+        <v>1</v>
+      </c>
+      <c r="G27" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="206" t="s">
+        <v>340</v>
+      </c>
+      <c r="C28" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="D28" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E28" s="206">
+        <v>12000</v>
+      </c>
+      <c r="F28" s="206">
+        <v>100</v>
+      </c>
+      <c r="G28" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="206" t="s">
+        <v>341</v>
+      </c>
+      <c r="C29" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E29" s="206">
+        <v>16000</v>
+      </c>
+      <c r="F29" s="206">
+        <v>90</v>
+      </c>
+      <c r="G29" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="206" t="s">
+        <v>342</v>
+      </c>
+      <c r="C30" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="D30" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E30" s="206">
+        <v>20000</v>
+      </c>
+      <c r="F30" s="206">
+        <v>50</v>
+      </c>
+      <c r="G30" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="206" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="D31" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E31" s="206">
+        <v>30</v>
+      </c>
+      <c r="F31" s="206">
+        <v>10</v>
+      </c>
+      <c r="G31" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="206" t="s">
+        <v>344</v>
+      </c>
+      <c r="C32" s="206" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E32" s="206">
+        <v>100</v>
+      </c>
+      <c r="F32" s="206">
+        <v>1</v>
+      </c>
+      <c r="G32" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="206" t="s">
+        <v>345</v>
+      </c>
+      <c r="C33" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E33" s="206">
+        <v>21000</v>
+      </c>
+      <c r="F33" s="206">
+        <v>100</v>
+      </c>
+      <c r="G33" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="206" t="s">
+        <v>346</v>
+      </c>
+      <c r="C34" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E34" s="206">
+        <v>24000</v>
+      </c>
+      <c r="F34" s="206">
+        <v>90</v>
+      </c>
+      <c r="G34" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="206" t="s">
+        <v>347</v>
+      </c>
+      <c r="C35" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E35" s="206">
+        <v>30000</v>
+      </c>
+      <c r="F35" s="206">
+        <v>50</v>
+      </c>
+      <c r="G35" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="206" t="s">
+        <v>348</v>
+      </c>
+      <c r="C36" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="D36" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E36" s="206">
+        <v>50</v>
+      </c>
+      <c r="F36" s="206">
+        <v>10</v>
+      </c>
+      <c r="G36" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="206" t="s">
+        <v>349</v>
+      </c>
+      <c r="C37" s="206" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E37" s="206">
+        <v>110</v>
+      </c>
+      <c r="F37" s="206">
+        <v>1</v>
+      </c>
+      <c r="G37" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="206" t="s">
+        <v>350</v>
+      </c>
+      <c r="C38" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E38" s="206">
+        <v>32000</v>
+      </c>
+      <c r="F38" s="206">
+        <v>100</v>
+      </c>
+      <c r="G38" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="206" t="s">
+        <v>351</v>
+      </c>
+      <c r="C39" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="D39" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E39" s="206">
+        <v>37000</v>
+      </c>
+      <c r="F39" s="206">
+        <v>90</v>
+      </c>
+      <c r="G39" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="206" t="s">
+        <v>352</v>
+      </c>
+      <c r="C40" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E40" s="206">
+        <v>42000</v>
+      </c>
+      <c r="F40" s="206">
+        <v>50</v>
+      </c>
+      <c r="G40" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="206" t="s">
+        <v>353</v>
+      </c>
+      <c r="C41" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="D41" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" s="206">
+        <v>60</v>
+      </c>
+      <c r="F41" s="206">
+        <v>10</v>
+      </c>
+      <c r="G41" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="206" t="s">
+        <v>354</v>
+      </c>
+      <c r="C42" s="206" t="s">
+        <v>292</v>
+      </c>
+      <c r="D42" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E42" s="206">
+        <v>120</v>
+      </c>
+      <c r="F42" s="206">
+        <v>1</v>
+      </c>
+      <c r="G42" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="206" t="s">
+        <v>355</v>
+      </c>
+      <c r="C43" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="D43" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E43" s="206">
+        <v>43000</v>
+      </c>
+      <c r="F43" s="206">
+        <v>100</v>
+      </c>
+      <c r="G43" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="206" t="s">
+        <v>356</v>
+      </c>
+      <c r="C44" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="D44" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E44" s="206">
+        <v>48000</v>
+      </c>
+      <c r="F44" s="206">
+        <v>90</v>
+      </c>
+      <c r="G44" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="206" t="s">
+        <v>357</v>
+      </c>
+      <c r="C45" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="D45" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E45" s="206">
+        <v>50000</v>
+      </c>
+      <c r="F45" s="206">
+        <v>50</v>
+      </c>
+      <c r="G45" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="206" t="s">
+        <v>358</v>
+      </c>
+      <c r="C46" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="D46" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E46" s="206">
+        <v>70</v>
+      </c>
+      <c r="F46" s="206">
+        <v>10</v>
+      </c>
+      <c r="G46" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="206" t="s">
+        <v>359</v>
+      </c>
+      <c r="C47" s="206" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E47" s="206">
+        <v>130</v>
+      </c>
+      <c r="F47" s="206">
+        <v>1</v>
+      </c>
+      <c r="G47" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="206" t="s">
+        <v>360</v>
+      </c>
+      <c r="C48" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="D48" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E48" s="206">
+        <v>52000</v>
+      </c>
+      <c r="F48" s="206">
+        <v>100</v>
+      </c>
+      <c r="G48" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="206" t="s">
+        <v>361</v>
+      </c>
+      <c r="C49" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="D49" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E49" s="206">
+        <v>55000</v>
+      </c>
+      <c r="F49" s="206">
+        <v>90</v>
+      </c>
+      <c r="G49" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="206" t="s">
+        <v>362</v>
+      </c>
+      <c r="C50" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="D50" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E50" s="206">
+        <v>58000</v>
+      </c>
+      <c r="F50" s="206">
+        <v>50</v>
+      </c>
+      <c r="G50" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="206" t="s">
+        <v>363</v>
+      </c>
+      <c r="C51" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="D51" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E51" s="206">
+        <v>80</v>
+      </c>
+      <c r="F51" s="206">
+        <v>10</v>
+      </c>
+      <c r="G51" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="206" t="s">
+        <v>364</v>
+      </c>
+      <c r="C52" s="206" t="s">
+        <v>300</v>
+      </c>
+      <c r="D52" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E52" s="206">
+        <v>140</v>
+      </c>
+      <c r="F52" s="206">
+        <v>1</v>
+      </c>
+      <c r="G52" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="206" t="s">
+        <v>365</v>
+      </c>
+      <c r="C53" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="D53" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E53" s="206">
+        <v>60000</v>
+      </c>
+      <c r="F53" s="206">
+        <v>100</v>
+      </c>
+      <c r="G53" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="206" t="s">
+        <v>366</v>
+      </c>
+      <c r="C54" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="D54" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E54" s="206">
+        <v>63000</v>
+      </c>
+      <c r="F54" s="206">
+        <v>90</v>
+      </c>
+      <c r="G54" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="206" t="s">
+        <v>367</v>
+      </c>
+      <c r="C55" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="D55" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E55" s="206">
+        <v>67000</v>
+      </c>
+      <c r="F55" s="206">
+        <v>50</v>
+      </c>
+      <c r="G55" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="206" t="s">
+        <v>368</v>
+      </c>
+      <c r="C56" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="D56" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E56" s="206">
+        <v>90</v>
+      </c>
+      <c r="F56" s="206">
+        <v>10</v>
+      </c>
+      <c r="G56" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="206" t="s">
+        <v>369</v>
+      </c>
+      <c r="C57" s="206" t="s">
+        <v>304</v>
+      </c>
+      <c r="D57" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E57" s="206">
+        <v>150</v>
+      </c>
+      <c r="F57" s="206">
+        <v>1</v>
+      </c>
+      <c r="G57" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="206" t="s">
+        <v>370</v>
+      </c>
+      <c r="C58" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="D58" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E58" s="206">
+        <v>70000</v>
+      </c>
+      <c r="F58" s="206">
+        <v>100</v>
+      </c>
+      <c r="G58" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="206" t="s">
+        <v>371</v>
+      </c>
+      <c r="C59" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="D59" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E59" s="206">
+        <v>73000</v>
+      </c>
+      <c r="F59" s="206">
+        <v>90</v>
+      </c>
+      <c r="G59" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="206" t="s">
+        <v>372</v>
+      </c>
+      <c r="C60" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E60" s="206">
+        <v>80000</v>
+      </c>
+      <c r="F60" s="206">
+        <v>50</v>
+      </c>
+      <c r="G60" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="206" t="s">
+        <v>373</v>
+      </c>
+      <c r="C61" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="D61" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E61" s="206">
+        <v>100</v>
+      </c>
+      <c r="F61" s="206">
+        <v>10</v>
+      </c>
+      <c r="G61" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="206" t="s">
+        <v>374</v>
+      </c>
+      <c r="C62" s="206" t="s">
+        <v>308</v>
+      </c>
+      <c r="D62" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E62" s="206">
+        <v>160</v>
+      </c>
+      <c r="F62" s="206">
+        <v>1</v>
+      </c>
+      <c r="G62" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="206" t="s">
+        <v>375</v>
+      </c>
+      <c r="C63" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="D63" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E63" s="206">
+        <v>82000</v>
+      </c>
+      <c r="F63" s="206">
+        <v>100</v>
+      </c>
+      <c r="G63" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="206" t="s">
+        <v>376</v>
+      </c>
+      <c r="C64" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="D64" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E64" s="206">
+        <v>85000</v>
+      </c>
+      <c r="F64" s="206">
+        <v>90</v>
+      </c>
+      <c r="G64" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="206" t="s">
+        <v>377</v>
+      </c>
+      <c r="C65" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="D65" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E65" s="206">
+        <v>89000</v>
+      </c>
+      <c r="F65" s="206">
+        <v>50</v>
+      </c>
+      <c r="G65" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="206" t="s">
+        <v>378</v>
+      </c>
+      <c r="C66" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="D66" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E66" s="206">
+        <v>110</v>
+      </c>
+      <c r="F66" s="206">
+        <v>10</v>
+      </c>
+      <c r="G66" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="206" t="s">
+        <v>379</v>
+      </c>
+      <c r="C67" s="206" t="s">
+        <v>312</v>
+      </c>
+      <c r="D67" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E67" s="206">
+        <v>170</v>
+      </c>
+      <c r="F67" s="206">
+        <v>1</v>
+      </c>
+      <c r="G67" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="206" t="s">
+        <v>380</v>
+      </c>
+      <c r="C68" s="206" t="s">
+        <v>316</v>
+      </c>
+      <c r="D68" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E68" s="206">
+        <v>92000</v>
+      </c>
+      <c r="F68" s="206">
+        <v>100</v>
+      </c>
+      <c r="G68" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="206" t="s">
+        <v>381</v>
+      </c>
+      <c r="C69" s="206" t="s">
+        <v>316</v>
+      </c>
+      <c r="D69" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E69" s="206">
+        <v>95000</v>
+      </c>
+      <c r="F69" s="206">
+        <v>90</v>
+      </c>
+      <c r="G69" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="206" t="s">
+        <v>382</v>
+      </c>
+      <c r="C70" s="206" t="s">
+        <v>316</v>
+      </c>
+      <c r="D70" s="206" t="s">
+        <v>328</v>
+      </c>
+      <c r="E70" s="206">
+        <v>120000</v>
+      </c>
+      <c r="F70" s="206">
+        <v>50</v>
+      </c>
+      <c r="G70" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="206" t="s">
+        <v>383</v>
+      </c>
+      <c r="C71" s="206" t="s">
+        <v>316</v>
+      </c>
+      <c r="D71" s="206" t="s">
+        <v>333</v>
+      </c>
+      <c r="E71" s="206">
+        <v>120</v>
+      </c>
+      <c r="F71" s="206">
+        <v>10</v>
+      </c>
+      <c r="G71" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="209" t="s">
+        <v>384</v>
+      </c>
+      <c r="C72" s="209" t="s">
+        <v>316</v>
+      </c>
+      <c r="D72" s="209" t="s">
+        <v>333</v>
+      </c>
+      <c r="E72" s="209">
+        <v>180</v>
+      </c>
+      <c r="F72" s="206">
+        <v>1</v>
+      </c>
+      <c r="G72" s="208" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B18:B72">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:C13">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
@@ -48010,12 +50419,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="198" t="s">
+      <c r="E3" s="204" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -48972,22 +51381,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48997,7 +51406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
@@ -49024,12 +51433,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="198" t="s">
+      <c r="E3" s="204" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -49993,22 +52402,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50018,7 +52427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
@@ -50045,12 +52454,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="198" t="s">
+      <c r="E3" s="204" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -51007,22 +53416,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51032,7 +53441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:AF33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Check some ice dragon values plus review electric disguises order
Former-commit-id: 3512613a93cd63dfecbc5f677862034d3205e7df
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="special dragons" sheetId="10" r:id="rId1"/>
@@ -58161,8 +58161,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61895,7 +61895,7 @@
         <v>63</v>
       </c>
       <c r="F54" s="58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" s="58">
         <v>600</v>
@@ -67209,7 +67209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WIP ice dragon balance
Former-commit-id: 655a1eac8abfe00f528dda98315ab52e71d43d74
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -7265,6 +7265,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9764,16 +9765,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>650</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>850</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10044,16 +10045,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13857,6 +13858,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16029,16 +16031,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>650</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>850</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16309,16 +16311,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19855,16 +19857,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19898,16 +19900,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20444,6 +20446,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21180,7 +21183,7 @@
                   <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22297,16 +22300,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>650</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>850</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22577,16 +22580,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26350,16 +26353,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>650</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>850</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26630,16 +26633,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -30115,6 +30118,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -30423,6 +30427,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31039,6 +31044,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31322,16 +31328,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>650</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>850</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31602,16 +31608,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>325</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>425</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -32280,6 +32286,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -32392,6 +32399,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -33636,6 +33644,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -33742,6 +33751,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -34987,6 +34997,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -58134,8 +58145,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ7" workbookViewId="0">
-      <selection activeCell="AZ31" sqref="AZ31"/>
+    <sheetView tabSelected="1" topLeftCell="O7" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60765,16 +60776,16 @@
         <v>-2</v>
       </c>
       <c r="J25" s="222">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="K25" s="223">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L25" s="223">
         <v>0</v>
       </c>
       <c r="M25" s="223">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N25" s="223">
         <v>20</v>
@@ -60792,10 +60803,10 @@
         <v>100</v>
       </c>
       <c r="S25" s="223">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T25" s="225">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="U25" s="221">
         <v>11</v>
@@ -60920,16 +60931,16 @@
         <v>0</v>
       </c>
       <c r="J26" s="222">
-        <v>275</v>
+        <v>130</v>
       </c>
       <c r="K26" s="223">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="L26" s="223">
         <v>0</v>
       </c>
       <c r="M26" s="223">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N26" s="223">
         <v>20</v>
@@ -60947,10 +60958,10 @@
         <v>120</v>
       </c>
       <c r="S26" s="223">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T26" s="225">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="U26" s="221">
         <v>13</v>
@@ -61075,16 +61086,16 @@
         <v>0</v>
       </c>
       <c r="J27" s="222">
-        <v>325</v>
+        <v>180</v>
       </c>
       <c r="K27" s="223">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="L27" s="223">
         <v>0</v>
       </c>
       <c r="M27" s="223">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N27" s="223">
         <v>15</v>
@@ -61102,10 +61113,10 @@
         <v>140</v>
       </c>
       <c r="S27" s="223">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T27" s="225">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="U27" s="221">
         <v>14</v>
@@ -61230,16 +61241,16 @@
         <v>0</v>
       </c>
       <c r="J28" s="238">
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="K28" s="239">
-        <v>5.2</v>
+        <v>4.2</v>
       </c>
       <c r="L28" s="239">
         <v>0</v>
       </c>
       <c r="M28" s="239">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N28" s="239">
         <v>10</v>
@@ -61257,10 +61268,10 @@
         <v>160</v>
       </c>
       <c r="S28" s="239">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T28" s="241">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="U28" s="237">
         <v>15</v>
@@ -61881,7 +61892,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="58">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J54" s="58" t="s">
         <v>182</v>
@@ -61995,7 +62006,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" s="259" t="s">
         <v>182</v>
@@ -67187,7 +67198,7 @@
   <dimension ref="C1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67263,16 +67274,16 @@
         <v>102</v>
       </c>
       <c r="E5" s="66">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="F5" s="66">
-        <v>275</v>
+        <v>130</v>
       </c>
       <c r="G5" s="66">
-        <v>325</v>
+        <v>180</v>
       </c>
       <c r="H5" s="66">
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="K5" t="s">
         <v>98</v>
@@ -67502,19 +67513,19 @@
       </c>
       <c r="K12">
         <f>E5</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="L12">
         <f>E5+E5*(L6/100)</f>
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="M12">
         <f>L12-K12</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="N12">
         <f>(K12*$L$7)/100</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="R12" s="63" t="s">
         <v>113</v>
@@ -67571,26 +67582,26 @@
       </c>
       <c r="H13" s="69">
         <f ca="1">INDIRECT(ADDRESS(5,4+E11)) + (INDIRECT(ADDRESS(5,4+E11)) *(L7/100) *E13)</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="J13" s="63" t="s">
         <v>116</v>
       </c>
       <c r="K13">
         <f>F5</f>
-        <v>275</v>
+        <v>130</v>
       </c>
       <c r="L13">
         <f>F5+F5*(L6/100)</f>
-        <v>550</v>
+        <v>260</v>
       </c>
       <c r="M13">
         <f>L13-K13</f>
-        <v>275</v>
+        <v>130</v>
       </c>
       <c r="N13">
         <f>(K13*$L$7)/100</f>
-        <v>13.75</v>
+        <v>6.5</v>
       </c>
       <c r="R13" s="63" t="s">
         <v>116</v>
@@ -67654,19 +67665,19 @@
       </c>
       <c r="K14">
         <f>G5</f>
-        <v>325</v>
+        <v>180</v>
       </c>
       <c r="L14">
         <f>G5+G5*(L6/100)</f>
-        <v>650</v>
+        <v>360</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:M15" si="3">L14-K14</f>
-        <v>325</v>
+        <v>180</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N15" si="4">(K14*$L$7)/100</f>
-        <v>16.25</v>
+        <v>9</v>
       </c>
       <c r="R14" s="63" t="s">
         <v>117</v>
@@ -67730,19 +67741,19 @@
       </c>
       <c r="K15">
         <f>H5</f>
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="L15">
         <f>H5+H5*(L6/100)</f>
-        <v>850</v>
+        <v>460</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>21.25</v>
+        <v>11.5</v>
       </c>
       <c r="R15" s="63" t="s">
         <v>118</v>
@@ -68508,7 +68519,7 @@
       </c>
       <c r="AB9">
         <f ca="1">'Ice Dragon'!$H$13</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="AC9">
         <f ca="1">'Ice Dragon'!$H$14</f>
@@ -68983,19 +68994,19 @@
       </c>
       <c r="G22">
         <f>'Ice Dragon'!L12</f>
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="H22">
         <f>'Ice Dragon'!L13</f>
-        <v>550</v>
+        <v>260</v>
       </c>
       <c r="I22">
         <f>'Ice Dragon'!L14</f>
-        <v>650</v>
+        <v>360</v>
       </c>
       <c r="J22">
         <f>'Ice Dragon'!L15</f>
-        <v>850</v>
+        <v>460</v>
       </c>
       <c r="P22" t="s">
         <v>387</v>
@@ -69051,19 +69062,19 @@
       </c>
       <c r="G23">
         <f>'Ice Dragon'!K12</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="H23">
         <f>'Ice Dragon'!K13</f>
-        <v>275</v>
+        <v>130</v>
       </c>
       <c r="I23">
         <f>'Ice Dragon'!K14</f>
-        <v>325</v>
+        <v>180</v>
       </c>
       <c r="J23">
         <f>'Ice Dragon'!K15</f>
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="P23" t="s">
         <v>388</v>

</xml_diff>

<commit_message>
WIP Ice dragon balancing
Former-commit-id: c1dd2d0ebe8a5863f58dda37c5e7b9915adb8c3c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58111,8 +58111,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="O10" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60772,7 +60772,7 @@
         <v>25</v>
       </c>
       <c r="T25" s="225">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U25" s="221">
         <v>11</v>
@@ -60927,7 +60927,7 @@
         <v>25</v>
       </c>
       <c r="T26" s="225">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U26" s="221">
         <v>13</v>
@@ -61082,7 +61082,7 @@
         <v>25</v>
       </c>
       <c r="T27" s="225">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U27" s="221">
         <v>14</v>
@@ -61237,7 +61237,7 @@
         <v>25</v>
       </c>
       <c r="T28" s="241">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U28" s="237">
         <v>15</v>

</xml_diff>

<commit_message>
WIP ice dragon data
Former-commit-id: 8f1cf470f4a5dddf56888f874832f5617c161e35
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58123,8 +58123,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61246,10 +61246,10 @@
         <v>160</v>
       </c>
       <c r="S28" s="239">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="T28" s="241">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="U28" s="237">
         <v>15</v>
@@ -62155,7 +62155,7 @@
   </sheetPr>
   <dimension ref="B1:M15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WIP Electric and Ice dragon balancing
Former-commit-id: 077304348ae534fc1a6b4fef6b33e5b9ac493200
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -19792,7 +19792,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20114,7 +20113,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20757,7 +20755,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21079,7 +21076,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21388,7 +21384,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21697,7 +21692,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22006,7 +22000,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23247,7 +23240,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23360,7 +23352,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24602,7 +24593,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24709,7 +24699,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25952,7 +25941,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -58126,8 +58114,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59550,10 +59538,10 @@
         <v>100</v>
       </c>
       <c r="S17" s="110">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T17" s="111">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U17" s="109">
         <v>11</v>
@@ -59704,10 +59692,10 @@
         <v>120</v>
       </c>
       <c r="S18" s="110">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T18" s="111">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U18" s="109">
         <v>13</v>
@@ -59834,7 +59822,7 @@
         <v>200</v>
       </c>
       <c r="K19" s="110">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="L19" s="110">
         <v>0</v>
@@ -59858,10 +59846,10 @@
         <v>140</v>
       </c>
       <c r="S19" s="110">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T19" s="111">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U19" s="109">
         <v>14</v>
@@ -59988,7 +59976,7 @@
         <v>250</v>
       </c>
       <c r="K20" s="110">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="L20" s="110">
         <v>0</v>
@@ -60012,10 +60000,10 @@
         <v>160</v>
       </c>
       <c r="S20" s="110">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T20" s="111">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U20" s="109">
         <v>15</v>
@@ -62161,7 +62149,7 @@
   <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Set Ice dragon scale values
Former-commit-id: a105a2d9d6d6be31d77097e942fafbd554fdc09c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58114,8 +58114,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T7" workbookViewId="0">
-      <selection activeCell="R20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60763,7 +60763,7 @@
         <v>0.5</v>
       </c>
       <c r="P25" s="224">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="221">
         <v>1.5</v>
@@ -60867,7 +60867,7 @@
         <v>8</v>
       </c>
       <c r="AZ25" s="232">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BA25" s="234" t="s">
         <v>395</v>
@@ -60918,7 +60918,7 @@
         <v>0.6</v>
       </c>
       <c r="P26" s="224">
-        <v>0.95</v>
+        <v>1.4</v>
       </c>
       <c r="Q26" s="221">
         <v>1.5</v>
@@ -61022,7 +61022,7 @@
         <v>8</v>
       </c>
       <c r="AZ26" s="232">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="BA26" s="235" t="s">
         <v>396</v>
@@ -61073,7 +61073,7 @@
         <v>0.7</v>
       </c>
       <c r="P27" s="224">
-        <v>1.55</v>
+        <v>1.8</v>
       </c>
       <c r="Q27" s="221">
         <v>1.5</v>
@@ -61177,7 +61177,7 @@
         <v>15</v>
       </c>
       <c r="AZ27" s="232">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="BA27" s="235" t="s">
         <v>397</v>
@@ -61230,7 +61230,7 @@
         <v>0.8</v>
       </c>
       <c r="P28" s="240">
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Q28" s="237">
         <v>1.2</v>
@@ -61334,7 +61334,7 @@
         <v>15</v>
       </c>
       <c r="AZ28" s="247">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="BA28" s="249" t="s">
         <v>398</v>

</xml_diff>

<commit_message>
WIP boost speed reduced
Former-commit-id: b797a190494d965a2ba90fc403ebff46a3a035e9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58114,8 +58114,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60766,7 +60766,7 @@
         <v>1</v>
       </c>
       <c r="Q25" s="221">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R25" s="223">
         <v>100</v>
@@ -60921,7 +60921,7 @@
         <v>1.4</v>
       </c>
       <c r="Q26" s="221">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R26" s="223">
         <v>120</v>
@@ -61076,7 +61076,7 @@
         <v>1.8</v>
       </c>
       <c r="Q27" s="221">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="R27" s="223">
         <v>140</v>

</xml_diff>

<commit_message>
Ice dragon XL scale, reduced a bit to make him fit in caves
Former-commit-id: 8e81f10df1c526f5356b38e6857a23b98ebc0e7e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58114,8 +58114,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61230,7 +61230,7 @@
         <v>0.8</v>
       </c>
       <c r="P28" s="240">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q28" s="237">
         <v>1.2</v>

</xml_diff>

<commit_message>
Modified tier limit restrictions so we can have offers
Former-commit-id: b7e8a941f4cdaae559c9869145cb3350ca0179fd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="417">
   <si>
     <t>[sku]</t>
   </si>
@@ -1279,6 +1279,9 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>tier_0</t>
   </si>
 </sst>
 </file>
@@ -58114,8 +58117,8 @@
   </sheetPr>
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58882,7 +58885,7 @@
         <v>64</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="G13" s="34">
         <v>0</v>
@@ -59036,7 +59039,7 @@
         <v>64</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>14</v>
+        <v>416</v>
       </c>
       <c r="G14" s="34">
         <v>10</v>
@@ -59499,7 +59502,7 @@
         <v>63</v>
       </c>
       <c r="F17" s="94" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="G17" s="95">
         <v>0</v>
@@ -59653,7 +59656,7 @@
         <v>63</v>
       </c>
       <c r="F18" s="94" t="s">
-        <v>14</v>
+        <v>416</v>
       </c>
       <c r="G18" s="95">
         <v>10</v>
@@ -60115,7 +60118,7 @@
         <v>235</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="G21" s="34">
         <v>0</v>
@@ -60269,7 +60272,7 @@
         <v>235</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>14</v>
+        <v>416</v>
       </c>
       <c r="G22" s="34">
         <v>10</v>
@@ -60733,7 +60736,7 @@
         <v>391</v>
       </c>
       <c r="F25" s="209" t="s">
-        <v>15</v>
+        <v>416</v>
       </c>
       <c r="G25" s="210">
         <v>0</v>
@@ -60888,7 +60891,7 @@
         <v>391</v>
       </c>
       <c r="F26" s="209" t="s">
-        <v>14</v>
+        <v>416</v>
       </c>
       <c r="G26" s="210">
         <v>10</v>

</xml_diff>

<commit_message>
Ice dragon disguises Fix disguise for Sonic: it was at lv. 1, it is now at lv. 5
Former-commit-id: 6edfaffe6bc29913e5a7561b730e6cd66bfee518
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="423">
   <si>
     <t>[sku]</t>
   </si>
@@ -1283,6 +1283,24 @@
   <si>
     <t>tier_0</t>
   </si>
+  <si>
+    <t>[body_parts]</t>
+  </si>
+  <si>
+    <t>dragon_ice_1</t>
+  </si>
+  <si>
+    <t>dragon_ice_2</t>
+  </si>
+  <si>
+    <t>dragon_ice_3</t>
+  </si>
+  <si>
+    <t>FX_IceSmokeWing_l;FX_IceSmokeWing_r</t>
+  </si>
+  <si>
+    <t>FX_IceSmokeBody</t>
+  </si>
 </sst>
 </file>
 
@@ -2163,7 +2181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2634,9 +2652,6 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2902,7 +2917,133 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="183">
+  <dxfs count="193">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3014,6 +3155,276 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3361,26 +3772,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3841,16 +4232,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -4092,40 +4473,6 @@
         <left style="medium">
           <color auto="1"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -7018,206 +7365,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -57663,116 +57810,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA28" totalsRowShown="0" headerRowBorderDxfId="162" totalsRowBorderDxfId="161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA28" totalsRowShown="0" headerRowBorderDxfId="192" totalsRowBorderDxfId="191">
   <autoFilter ref="B12:BA28"/>
   <tableColumns count="52">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="160"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="159"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="158"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="157"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="156"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="155"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="154"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="153"/>
-    <tableColumn id="10" name="[health]" dataDxfId="152"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="151"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="150"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="149"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="148"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="147"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="146"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="145"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="144"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="143"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="142"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="141"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="140"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="139"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="138"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="137"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="136"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="135"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="134"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="133"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="132"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="131"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="130"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="129"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="128"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="127"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="126"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="125"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="124"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="123"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="122"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="121"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="120"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="119"/>
-    <tableColumn id="46" name="[force]" dataDxfId="118"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="117"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="116"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="115"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="114"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="113"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="112"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="111"/>
-    <tableColumn id="6" name="[scaleMenu]" dataDxfId="110"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="109"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="190"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="189"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="188"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="187"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="186"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="185"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="184"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="183"/>
+    <tableColumn id="10" name="[health]" dataDxfId="182"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="181"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="180"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="179"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="178"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="177"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="176"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="175"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="174"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="173"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="172"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="171"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="170"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="169"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="168"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="167"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="166"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="165"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="164"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="163"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="162"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="161"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="160"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="159"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="158"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="157"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="156"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="155"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="154"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="153"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="152"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="151"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="150"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="149"/>
+    <tableColumn id="46" name="[force]" dataDxfId="148"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="147"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="146"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="145"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="144"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="143"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="142"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="141"/>
+    <tableColumn id="6" name="[scaleMenu]" dataDxfId="140"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="139"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC7" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107" tableBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC7" totalsRowShown="0" headerRowDxfId="138" dataDxfId="136" headerRowBorderDxfId="137" tableBorderDxfId="135">
   <autoFilter ref="B3:AC7"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="104"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="134"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="103"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="102"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="101"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="100"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="99"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="98"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="97"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="96"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="95"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="94"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="93"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="92"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="91"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="90"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="89"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="88"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="87"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="86"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="85"/>
-    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="84"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="83"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="82"/>
-    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="81"/>
-    <tableColumn id="14" name="[mummyDuration]" dataDxfId="80"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="79"/>
+    <tableColumn id="5" name="[order]" dataDxfId="133"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="132"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="131"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="130"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="129"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="128"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="127"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="126"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="125"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="124"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="123"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="122"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="121"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="120"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="119"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="118"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="117"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="116"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="115"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="114"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="113"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="112"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="111"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="110"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:I46" totalsRowShown="0" headerRowBorderDxfId="78" tableBorderDxfId="77" totalsRowBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:I46" totalsRowShown="0" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <autoFilter ref="B34:I46"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="75"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="74"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="73"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="72"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="71">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="105"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="104"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="103"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="102"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="101">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="70"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="69"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="100"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="99"/>
     <tableColumn id="8" name="[tidDescShort]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -57780,70 +57927,71 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B52:M57" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
-  <autoFilter ref="B52:M57"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="63"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="62"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="61"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="60"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="59"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="58"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="57"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="56"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="55"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="54"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="53"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B52:N60" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+  <autoFilter ref="B52:N60"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="93"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="91"/>
+    <tableColumn id="13" name="[body_parts]" dataDxfId="49"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="90"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="0"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="89"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="88"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="87"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="86"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="85"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="84"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="47"/>
-    <tableColumn id="7" name="[index]" dataDxfId="46"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="45"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="44"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="43"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="42"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="41"/>
-    <tableColumn id="10" name="[color]" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="80"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="79"/>
+    <tableColumn id="7" name="[index]" dataDxfId="78"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="77"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="76"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="75"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="74"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="73"/>
+    <tableColumn id="10" name="[color]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="34"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="66"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="64"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="63"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:G72" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:G72" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="A17:G72"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{leaguesRewardsDefinitions}" dataDxfId="22"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
-    <tableColumn id="3" name="[group]" dataDxfId="20"/>
-    <tableColumn id="4" name="[type]" dataDxfId="19"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="18"/>
-    <tableColumn id="6" name="[target]" dataDxfId="17"/>
-    <tableColumn id="7" name="[rsku]" dataDxfId="16"/>
+    <tableColumn id="1" name="{leaguesRewardsDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
+    <tableColumn id="3" name="[group]" dataDxfId="54"/>
+    <tableColumn id="4" name="[type]" dataDxfId="53"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="52"/>
+    <tableColumn id="6" name="[target]" dataDxfId="51"/>
+    <tableColumn id="7" name="[rsku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -58115,10 +58263,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:BA65"/>
+  <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58549,7 +58697,7 @@
         <v>236</v>
       </c>
       <c r="W6" s="160"/>
-      <c r="X6" s="193">
+      <c r="X6" s="192">
         <v>0.6</v>
       </c>
       <c r="Y6" s="55" t="s">
@@ -58578,49 +58726,49 @@
       <c r="D7" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="194">
+      <c r="E7" s="193">
         <v>3</v>
       </c>
       <c r="F7" s="46">
         <v>25</v>
       </c>
-      <c r="G7" s="195">
+      <c r="G7" s="194">
         <v>200</v>
       </c>
-      <c r="H7" s="196">
+      <c r="H7" s="195">
         <v>20</v>
       </c>
-      <c r="I7" s="197">
+      <c r="I7" s="196">
         <v>0</v>
       </c>
-      <c r="J7" s="197">
+      <c r="J7" s="196">
         <v>100</v>
       </c>
-      <c r="K7" s="198">
+      <c r="K7" s="197">
         <v>20</v>
       </c>
-      <c r="L7" s="199">
+      <c r="L7" s="198">
         <v>0</v>
       </c>
-      <c r="M7" s="199">
+      <c r="M7" s="198">
         <v>60</v>
       </c>
-      <c r="N7" s="200">
+      <c r="N7" s="199">
         <v>20</v>
       </c>
-      <c r="O7" s="200">
+      <c r="O7" s="199">
         <v>0</v>
       </c>
-      <c r="P7" s="200">
+      <c r="P7" s="199">
         <v>60</v>
       </c>
       <c r="Q7" s="160">
         <v>25</v>
       </c>
-      <c r="R7" s="201">
+      <c r="R7" s="200">
         <v>1</v>
       </c>
-      <c r="S7" s="201">
+      <c r="S7" s="200">
         <v>0</v>
       </c>
       <c r="T7" s="160">
@@ -58633,22 +58781,22 @@
         <v>392</v>
       </c>
       <c r="W7" s="160"/>
-      <c r="X7" s="193">
+      <c r="X7" s="192">
         <v>0.6</v>
       </c>
-      <c r="Y7" s="202" t="s">
+      <c r="Y7" s="201" t="s">
         <v>393</v>
       </c>
-      <c r="Z7" s="205" t="s">
+      <c r="Z7" s="204" t="s">
         <v>394</v>
       </c>
-      <c r="AA7" s="203">
+      <c r="AA7" s="202">
         <v>0.4</v>
       </c>
-      <c r="AB7" s="203">
+      <c r="AB7" s="202">
         <v>25</v>
       </c>
-      <c r="AC7" s="204" t="s">
+      <c r="AC7" s="203" t="s">
         <v>391</v>
       </c>
     </row>
@@ -60678,7 +60826,7 @@
       <c r="AM24" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="AN24" s="251">
+      <c r="AN24" s="250">
         <v>10</v>
       </c>
       <c r="AO24" s="121">
@@ -60723,466 +60871,466 @@
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="206" t="s">
+      <c r="B25" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="207" t="s">
+      <c r="C25" s="206" t="s">
         <v>395</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="208" t="s">
+      <c r="E25" s="207" t="s">
         <v>391</v>
       </c>
-      <c r="F25" s="209" t="s">
+      <c r="F25" s="208" t="s">
         <v>416</v>
       </c>
-      <c r="G25" s="210">
+      <c r="G25" s="209">
         <v>0</v>
       </c>
-      <c r="H25" s="220">
+      <c r="H25" s="219">
         <v>3</v>
       </c>
-      <c r="I25" s="221">
+      <c r="I25" s="220">
         <v>-2</v>
       </c>
-      <c r="J25" s="222">
+      <c r="J25" s="221">
         <v>75</v>
       </c>
-      <c r="K25" s="223">
+      <c r="K25" s="222">
         <v>2.7</v>
       </c>
-      <c r="L25" s="223">
+      <c r="L25" s="222">
         <v>0</v>
       </c>
-      <c r="M25" s="223">
+      <c r="M25" s="222">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="N25" s="223">
+      <c r="N25" s="222">
         <v>20</v>
       </c>
-      <c r="O25" s="223">
+      <c r="O25" s="222">
         <v>0.5</v>
       </c>
-      <c r="P25" s="224">
+      <c r="P25" s="223">
         <v>1</v>
       </c>
-      <c r="Q25" s="221">
+      <c r="Q25" s="220">
         <v>1.3</v>
       </c>
-      <c r="R25" s="223">
+      <c r="R25" s="222">
         <v>100</v>
       </c>
-      <c r="S25" s="223">
+      <c r="S25" s="222">
         <v>9</v>
       </c>
-      <c r="T25" s="225">
+      <c r="T25" s="224">
         <v>7</v>
       </c>
-      <c r="U25" s="221">
+      <c r="U25" s="220">
         <v>11</v>
       </c>
-      <c r="V25" s="223">
+      <c r="V25" s="222">
         <v>3</v>
       </c>
-      <c r="W25" s="223">
+      <c r="W25" s="222">
         <v>10</v>
       </c>
-      <c r="X25" s="225">
+      <c r="X25" s="224">
         <v>40000</v>
       </c>
-      <c r="Y25" s="226">
+      <c r="Y25" s="225">
         <v>2</v>
       </c>
-      <c r="Z25" s="224">
+      <c r="Z25" s="223">
         <v>0.13</v>
       </c>
-      <c r="AA25" s="224">
+      <c r="AA25" s="223">
         <v>0</v>
       </c>
-      <c r="AB25" s="226">
+      <c r="AB25" s="225">
         <v>12</v>
       </c>
-      <c r="AC25" s="211" t="s">
+      <c r="AC25" s="210" t="s">
         <v>399</v>
       </c>
-      <c r="AD25" s="212" t="s">
+      <c r="AD25" s="211" t="s">
         <v>400</v>
       </c>
-      <c r="AE25" s="212" t="s">
+      <c r="AE25" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF25" s="227"/>
-      <c r="AG25" s="228"/>
-      <c r="AH25" s="229">
+      <c r="AF25" s="226"/>
+      <c r="AG25" s="227"/>
+      <c r="AH25" s="228">
         <v>1.7</v>
       </c>
-      <c r="AI25" s="227">
+      <c r="AI25" s="226">
         <v>2</v>
       </c>
-      <c r="AJ25" s="227">
+      <c r="AJ25" s="226">
         <v>2</v>
       </c>
-      <c r="AK25" s="227" t="b">
+      <c r="AK25" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AL25" s="227" t="b">
+      <c r="AL25" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AM25" s="227" t="b">
+      <c r="AM25" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AN25" s="230">
+      <c r="AN25" s="229">
         <v>10</v>
       </c>
-      <c r="AO25" s="252">
+      <c r="AO25" s="251">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AP25" s="253">
+      <c r="AP25" s="252">
         <v>2E-3</v>
       </c>
-      <c r="AQ25" s="254">
+      <c r="AQ25" s="253">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR25" s="231">
+      <c r="AR25" s="230">
         <v>260</v>
       </c>
-      <c r="AS25" s="232">
+      <c r="AS25" s="231">
         <v>2.5</v>
       </c>
-      <c r="AT25" s="232">
+      <c r="AT25" s="231">
         <v>9.5</v>
       </c>
-      <c r="AU25" s="232">
+      <c r="AU25" s="231">
         <v>1.7</v>
       </c>
-      <c r="AV25" s="232">
+      <c r="AV25" s="231">
         <v>1.2</v>
       </c>
-      <c r="AW25" s="233">
+      <c r="AW25" s="232">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX25" s="232">
+      <c r="AX25" s="231">
         <v>0</v>
       </c>
-      <c r="AY25" s="232">
+      <c r="AY25" s="231">
         <v>8</v>
       </c>
-      <c r="AZ25" s="232">
+      <c r="AZ25" s="231">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BA25" s="234" t="s">
+      <c r="BA25" s="233" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="206" t="s">
+      <c r="B26" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="207" t="s">
+      <c r="C26" s="206" t="s">
         <v>396</v>
       </c>
       <c r="D26" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="208" t="s">
+      <c r="E26" s="207" t="s">
         <v>391</v>
       </c>
-      <c r="F26" s="209" t="s">
+      <c r="F26" s="208" t="s">
         <v>416</v>
       </c>
-      <c r="G26" s="210">
+      <c r="G26" s="209">
         <v>10</v>
       </c>
-      <c r="H26" s="220">
+      <c r="H26" s="219">
         <v>8</v>
       </c>
-      <c r="I26" s="221">
+      <c r="I26" s="220">
         <v>0</v>
       </c>
-      <c r="J26" s="222">
+      <c r="J26" s="221">
         <v>120</v>
       </c>
-      <c r="K26" s="223">
+      <c r="K26" s="222">
         <v>3.4</v>
       </c>
-      <c r="L26" s="223">
+      <c r="L26" s="222">
         <v>0</v>
       </c>
-      <c r="M26" s="223">
+      <c r="M26" s="222">
         <v>0.01</v>
       </c>
-      <c r="N26" s="223">
+      <c r="N26" s="222">
         <v>20</v>
       </c>
-      <c r="O26" s="223">
+      <c r="O26" s="222">
         <v>0.6</v>
       </c>
-      <c r="P26" s="224">
+      <c r="P26" s="223">
         <v>1.4</v>
       </c>
-      <c r="Q26" s="221">
+      <c r="Q26" s="220">
         <v>1.3</v>
       </c>
-      <c r="R26" s="223">
+      <c r="R26" s="222">
         <v>120</v>
       </c>
-      <c r="S26" s="223">
+      <c r="S26" s="222">
         <v>10</v>
       </c>
-      <c r="T26" s="225">
+      <c r="T26" s="224">
         <v>7</v>
       </c>
-      <c r="U26" s="221">
+      <c r="U26" s="220">
         <v>13</v>
       </c>
-      <c r="V26" s="223">
+      <c r="V26" s="222">
         <v>4</v>
       </c>
-      <c r="W26" s="223">
+      <c r="W26" s="222">
         <v>11</v>
       </c>
-      <c r="X26" s="225">
+      <c r="X26" s="224">
         <v>120000</v>
       </c>
-      <c r="Y26" s="226">
+      <c r="Y26" s="225">
         <v>3</v>
       </c>
-      <c r="Z26" s="224">
+      <c r="Z26" s="223">
         <v>0.08</v>
       </c>
-      <c r="AA26" s="224">
+      <c r="AA26" s="223">
         <v>0</v>
       </c>
-      <c r="AB26" s="226">
+      <c r="AB26" s="225">
         <v>12</v>
       </c>
-      <c r="AC26" s="211" t="s">
+      <c r="AC26" s="210" t="s">
         <v>399</v>
       </c>
-      <c r="AD26" s="212" t="s">
+      <c r="AD26" s="211" t="s">
         <v>400</v>
       </c>
-      <c r="AE26" s="212" t="s">
+      <c r="AE26" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF26" s="227"/>
-      <c r="AG26" s="228"/>
-      <c r="AH26" s="229">
+      <c r="AF26" s="226"/>
+      <c r="AG26" s="227"/>
+      <c r="AH26" s="228">
         <v>1.6</v>
       </c>
-      <c r="AI26" s="227">
+      <c r="AI26" s="226">
         <v>2</v>
       </c>
-      <c r="AJ26" s="227">
+      <c r="AJ26" s="226">
         <v>2</v>
       </c>
-      <c r="AK26" s="227" t="b">
+      <c r="AK26" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AL26" s="227" t="b">
+      <c r="AL26" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AM26" s="227" t="b">
+      <c r="AM26" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AN26" s="230">
+      <c r="AN26" s="229">
         <v>10</v>
       </c>
-      <c r="AO26" s="252">
+      <c r="AO26" s="251">
         <v>0.7</v>
       </c>
-      <c r="AP26" s="253">
+      <c r="AP26" s="252">
         <v>1.8E-3</v>
       </c>
-      <c r="AQ26" s="254">
+      <c r="AQ26" s="253">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR26" s="231">
+      <c r="AR26" s="230">
         <v>275</v>
       </c>
-      <c r="AS26" s="232">
+      <c r="AS26" s="231">
         <v>2.5</v>
       </c>
-      <c r="AT26" s="232">
+      <c r="AT26" s="231">
         <v>9.5</v>
       </c>
-      <c r="AU26" s="232">
+      <c r="AU26" s="231">
         <v>1.7</v>
       </c>
-      <c r="AV26" s="232">
+      <c r="AV26" s="231">
         <v>1.2</v>
       </c>
-      <c r="AW26" s="233">
+      <c r="AW26" s="232">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX26" s="232">
+      <c r="AX26" s="231">
         <v>9</v>
       </c>
-      <c r="AY26" s="232">
+      <c r="AY26" s="231">
         <v>8</v>
       </c>
-      <c r="AZ26" s="232">
+      <c r="AZ26" s="231">
         <v>1.3</v>
       </c>
-      <c r="BA26" s="235" t="s">
+      <c r="BA26" s="234" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="206" t="s">
+      <c r="B27" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="207" t="s">
+      <c r="C27" s="206" t="s">
         <v>397</v>
       </c>
       <c r="D27" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="208" t="s">
+      <c r="E27" s="207" t="s">
         <v>391</v>
       </c>
-      <c r="F27" s="209" t="s">
+      <c r="F27" s="208" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="210">
+      <c r="G27" s="209">
         <v>20</v>
       </c>
-      <c r="H27" s="220">
+      <c r="H27" s="219">
         <v>17</v>
       </c>
-      <c r="I27" s="221">
+      <c r="I27" s="220">
         <v>0</v>
       </c>
-      <c r="J27" s="222">
+      <c r="J27" s="221">
         <v>160</v>
       </c>
-      <c r="K27" s="223">
+      <c r="K27" s="222">
         <v>4.3</v>
       </c>
-      <c r="L27" s="223">
+      <c r="L27" s="222">
         <v>0</v>
       </c>
-      <c r="M27" s="223">
+      <c r="M27" s="222">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="N27" s="223">
+      <c r="N27" s="222">
         <v>15</v>
       </c>
-      <c r="O27" s="223">
+      <c r="O27" s="222">
         <v>0.7</v>
       </c>
-      <c r="P27" s="224">
+      <c r="P27" s="223">
         <v>1.8</v>
       </c>
-      <c r="Q27" s="221">
+      <c r="Q27" s="220">
         <v>1.3</v>
       </c>
-      <c r="R27" s="223">
+      <c r="R27" s="222">
         <v>140</v>
       </c>
-      <c r="S27" s="223">
+      <c r="S27" s="222">
         <v>12</v>
       </c>
-      <c r="T27" s="225">
+      <c r="T27" s="224">
         <v>7</v>
       </c>
-      <c r="U27" s="221">
+      <c r="U27" s="220">
         <v>14</v>
       </c>
-      <c r="V27" s="223">
+      <c r="V27" s="222">
         <v>5</v>
       </c>
-      <c r="W27" s="223">
+      <c r="W27" s="222">
         <v>11</v>
       </c>
-      <c r="X27" s="225">
+      <c r="X27" s="224">
         <v>250000</v>
       </c>
-      <c r="Y27" s="226">
+      <c r="Y27" s="225">
         <v>4</v>
       </c>
-      <c r="Z27" s="224">
+      <c r="Z27" s="223">
         <v>0.05</v>
       </c>
-      <c r="AA27" s="224">
+      <c r="AA27" s="223">
         <v>0</v>
       </c>
-      <c r="AB27" s="226">
+      <c r="AB27" s="225">
         <v>12</v>
       </c>
-      <c r="AC27" s="211" t="s">
+      <c r="AC27" s="210" t="s">
         <v>399</v>
       </c>
-      <c r="AD27" s="212" t="s">
+      <c r="AD27" s="211" t="s">
         <v>400</v>
       </c>
-      <c r="AE27" s="212" t="s">
+      <c r="AE27" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF27" s="227"/>
-      <c r="AG27" s="228"/>
-      <c r="AH27" s="229">
+      <c r="AF27" s="226"/>
+      <c r="AG27" s="227"/>
+      <c r="AH27" s="228">
         <v>1.5</v>
       </c>
-      <c r="AI27" s="227">
+      <c r="AI27" s="226">
         <v>2</v>
       </c>
-      <c r="AJ27" s="227">
+      <c r="AJ27" s="226">
         <v>2</v>
       </c>
-      <c r="AK27" s="227" t="b">
+      <c r="AK27" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AL27" s="227" t="b">
+      <c r="AL27" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AM27" s="227" t="b">
+      <c r="AM27" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AN27" s="230">
+      <c r="AN27" s="229">
         <v>10</v>
       </c>
-      <c r="AO27" s="252">
+      <c r="AO27" s="251">
         <v>0.7</v>
       </c>
-      <c r="AP27" s="253">
+      <c r="AP27" s="252">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AQ27" s="254">
+      <c r="AQ27" s="253">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR27" s="231">
+      <c r="AR27" s="230">
         <v>300</v>
       </c>
-      <c r="AS27" s="232">
+      <c r="AS27" s="231">
         <v>2.5</v>
       </c>
-      <c r="AT27" s="232">
+      <c r="AT27" s="231">
         <v>9.5</v>
       </c>
-      <c r="AU27" s="232">
+      <c r="AU27" s="231">
         <v>1.7</v>
       </c>
-      <c r="AV27" s="232">
+      <c r="AV27" s="231">
         <v>1.2</v>
       </c>
-      <c r="AW27" s="233">
+      <c r="AW27" s="232">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX27" s="232">
+      <c r="AX27" s="231">
         <v>45</v>
       </c>
-      <c r="AY27" s="232">
+      <c r="AY27" s="231">
         <v>15</v>
       </c>
-      <c r="AZ27" s="232">
+      <c r="AZ27" s="231">
         <v>1.5</v>
       </c>
-      <c r="BA27" s="235" t="s">
+      <c r="BA27" s="234" t="s">
         <v>397</v>
       </c>
     </row>
@@ -61190,156 +61338,156 @@
       <c r="A28" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="213" t="s">
+      <c r="B28" s="212" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="214" t="s">
+      <c r="C28" s="213" t="s">
         <v>398</v>
       </c>
-      <c r="D28" s="215" t="s">
+      <c r="D28" s="214" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="216" t="s">
+      <c r="E28" s="215" t="s">
         <v>391</v>
       </c>
-      <c r="F28" s="217" t="s">
+      <c r="F28" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="250">
+      <c r="G28" s="249">
         <v>30</v>
       </c>
-      <c r="H28" s="236">
+      <c r="H28" s="235">
         <v>25</v>
       </c>
-      <c r="I28" s="237">
+      <c r="I28" s="236">
         <v>0</v>
       </c>
-      <c r="J28" s="238">
+      <c r="J28" s="237">
         <v>200</v>
       </c>
-      <c r="K28" s="239">
+      <c r="K28" s="238">
         <v>5</v>
       </c>
-      <c r="L28" s="239">
+      <c r="L28" s="238">
         <v>0</v>
       </c>
-      <c r="M28" s="239">
+      <c r="M28" s="238">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="N28" s="239">
+      <c r="N28" s="238">
         <v>10</v>
       </c>
-      <c r="O28" s="239">
+      <c r="O28" s="238">
         <v>0.8</v>
       </c>
-      <c r="P28" s="240">
+      <c r="P28" s="239">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q28" s="237">
+      <c r="Q28" s="236">
         <v>1.2</v>
       </c>
-      <c r="R28" s="239">
+      <c r="R28" s="238">
         <v>160</v>
       </c>
-      <c r="S28" s="239">
+      <c r="S28" s="238">
         <v>14</v>
       </c>
-      <c r="T28" s="241">
+      <c r="T28" s="240">
         <v>7</v>
       </c>
-      <c r="U28" s="237">
+      <c r="U28" s="236">
         <v>15</v>
       </c>
-      <c r="V28" s="239">
+      <c r="V28" s="238">
         <v>6</v>
       </c>
-      <c r="W28" s="239">
+      <c r="W28" s="238">
         <v>11</v>
       </c>
-      <c r="X28" s="241">
+      <c r="X28" s="240">
         <v>550000</v>
       </c>
-      <c r="Y28" s="242">
+      <c r="Y28" s="241">
         <v>5</v>
       </c>
-      <c r="Z28" s="240">
+      <c r="Z28" s="239">
         <v>0.04</v>
       </c>
-      <c r="AA28" s="240">
+      <c r="AA28" s="239">
         <v>0</v>
       </c>
-      <c r="AB28" s="242">
+      <c r="AB28" s="241">
         <v>12</v>
       </c>
-      <c r="AC28" s="218" t="s">
+      <c r="AC28" s="217" t="s">
         <v>399</v>
       </c>
-      <c r="AD28" s="219" t="s">
+      <c r="AD28" s="218" t="s">
         <v>400</v>
       </c>
-      <c r="AE28" s="219" t="s">
+      <c r="AE28" s="218" t="s">
         <v>401</v>
       </c>
-      <c r="AF28" s="227"/>
-      <c r="AG28" s="243"/>
-      <c r="AH28" s="244">
+      <c r="AF28" s="226"/>
+      <c r="AG28" s="242"/>
+      <c r="AH28" s="243">
         <v>1.4</v>
       </c>
-      <c r="AI28" s="227">
+      <c r="AI28" s="226">
         <v>2</v>
       </c>
-      <c r="AJ28" s="227">
+      <c r="AJ28" s="226">
         <v>2</v>
       </c>
-      <c r="AK28" s="227" t="b">
+      <c r="AK28" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AL28" s="227" t="b">
+      <c r="AL28" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AM28" s="227" t="b">
+      <c r="AM28" s="226" t="b">
         <v>1</v>
       </c>
-      <c r="AN28" s="245">
+      <c r="AN28" s="244">
         <v>10</v>
       </c>
-      <c r="AO28" s="252">
+      <c r="AO28" s="251">
         <v>0.7</v>
       </c>
-      <c r="AP28" s="253">
+      <c r="AP28" s="252">
         <v>1.5E-3</v>
       </c>
-      <c r="AQ28" s="254">
+      <c r="AQ28" s="253">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR28" s="246">
+      <c r="AR28" s="245">
         <v>315</v>
       </c>
-      <c r="AS28" s="247">
+      <c r="AS28" s="246">
         <v>2.5</v>
       </c>
-      <c r="AT28" s="247">
+      <c r="AT28" s="246">
         <v>9.5</v>
       </c>
-      <c r="AU28" s="247">
+      <c r="AU28" s="246">
         <v>1.7</v>
       </c>
-      <c r="AV28" s="247">
+      <c r="AV28" s="246">
         <v>1.2</v>
       </c>
-      <c r="AW28" s="248">
+      <c r="AW28" s="247">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX28" s="247">
+      <c r="AX28" s="246">
         <v>59</v>
       </c>
-      <c r="AY28" s="247">
+      <c r="AY28" s="246">
         <v>15</v>
       </c>
-      <c r="AZ28" s="247">
+      <c r="AZ28" s="246">
         <v>1.7</v>
       </c>
-      <c r="BA28" s="249" t="s">
+      <c r="BA28" s="248" t="s">
         <v>398</v>
       </c>
     </row>
@@ -61350,44 +61498,44 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="267" t="s">
+      <c r="H29" s="266" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="268"/>
-      <c r="J29" s="269" t="s">
+      <c r="I29" s="267"/>
+      <c r="J29" s="268" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="270"/>
-      <c r="L29" s="270"/>
-      <c r="M29" s="270"/>
-      <c r="N29" s="270"/>
-      <c r="O29" s="271"/>
+      <c r="K29" s="269"/>
+      <c r="L29" s="269"/>
+      <c r="M29" s="269"/>
+      <c r="N29" s="269"/>
+      <c r="O29" s="270"/>
       <c r="P29" s="72"/>
-      <c r="Q29" s="263" t="s">
+      <c r="Q29" s="262" t="s">
         <v>126</v>
       </c>
-      <c r="R29" s="264"/>
-      <c r="S29" s="264"/>
-      <c r="T29" s="264"/>
-      <c r="U29" s="265" t="s">
+      <c r="R29" s="263"/>
+      <c r="S29" s="263"/>
+      <c r="T29" s="263"/>
+      <c r="U29" s="264" t="s">
         <v>9</v>
       </c>
-      <c r="V29" s="266"/>
-      <c r="W29" s="266"/>
-      <c r="X29" s="266"/>
+      <c r="V29" s="265"/>
+      <c r="W29" s="265"/>
+      <c r="X29" s="265"/>
       <c r="Y29" s="20"/>
       <c r="Z29" s="20"/>
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
-      <c r="AH29" s="260" t="s">
+      <c r="AH29" s="259" t="s">
         <v>127</v>
       </c>
-      <c r="AI29" s="261"/>
-      <c r="AJ29" s="261"/>
-      <c r="AK29" s="261"/>
-      <c r="AL29" s="261"/>
-      <c r="AM29" s="261"/>
-      <c r="AN29" s="262"/>
+      <c r="AI29" s="260"/>
+      <c r="AJ29" s="260"/>
+      <c r="AK29" s="260"/>
+      <c r="AL29" s="260"/>
+      <c r="AM29" s="260"/>
+      <c r="AN29" s="261"/>
     </row>
     <row r="31" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AZ31" t="s">
@@ -61683,7 +61831,7 @@
       <c r="C44" s="56" t="s">
         <v>402</v>
       </c>
-      <c r="D44" s="255" t="s">
+      <c r="D44" s="254" t="s">
         <v>391</v>
       </c>
       <c r="E44" s="57">
@@ -61710,7 +61858,7 @@
       <c r="C45" s="56" t="s">
         <v>403</v>
       </c>
-      <c r="D45" s="255" t="s">
+      <c r="D45" s="254" t="s">
         <v>391</v>
       </c>
       <c r="E45" s="57">
@@ -61731,13 +61879,13 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="256" t="s">
+      <c r="B46" s="255" t="s">
         <v>2</v>
       </c>
       <c r="C46" s="60" t="s">
         <v>404</v>
       </c>
-      <c r="D46" s="257" t="s">
+      <c r="D46" s="256" t="s">
         <v>391</v>
       </c>
       <c r="E46" s="61">
@@ -61747,18 +61895,18 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_ice_power_3</v>
       </c>
-      <c r="G46" s="258" t="s">
+      <c r="G46" s="257" t="s">
         <v>407</v>
       </c>
       <c r="H46" s="177" t="s">
         <v>410</v>
       </c>
-      <c r="I46" s="258" t="s">
+      <c r="I46" s="257" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="49" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
         <v>172</v>
       </c>
@@ -61767,7 +61915,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="52" spans="2:13" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="B52" s="180" t="s">
         <v>173</v>
       </c>
@@ -61777,35 +61925,38 @@
       <c r="D52" s="178" t="s">
         <v>174</v>
       </c>
-      <c r="E52" s="179" t="s">
+      <c r="E52" s="178" t="s">
+        <v>417</v>
+      </c>
+      <c r="F52" s="179" t="s">
         <v>175</v>
       </c>
-      <c r="F52" s="181" t="s">
+      <c r="G52" s="181" t="s">
         <v>176</v>
       </c>
-      <c r="G52" s="181" t="s">
+      <c r="H52" s="181" t="s">
         <v>177</v>
       </c>
-      <c r="H52" s="181" t="s">
+      <c r="I52" s="181" t="s">
         <v>178</v>
       </c>
-      <c r="I52" s="181" t="s">
+      <c r="J52" s="181" t="s">
         <v>179</v>
       </c>
-      <c r="J52" s="181" t="s">
+      <c r="K52" s="181" t="s">
         <v>65</v>
       </c>
-      <c r="K52" s="181" t="s">
+      <c r="L52" s="181" t="s">
         <v>3</v>
       </c>
-      <c r="L52" s="181" t="s">
+      <c r="M52" s="181" t="s">
         <v>5</v>
       </c>
-      <c r="M52" s="181" t="s">
+      <c r="N52" s="181" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="29" t="s">
         <v>2</v>
       </c>
@@ -61815,11 +61966,9 @@
       <c r="D53" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="E53" s="57" t="s">
+      <c r="E53" s="57"/>
+      <c r="F53" s="57" t="s">
         <v>64</v>
-      </c>
-      <c r="F53" s="58">
-        <v>0</v>
       </c>
       <c r="G53" s="58">
         <v>0</v>
@@ -61830,20 +61979,23 @@
       <c r="I53" s="58">
         <v>0</v>
       </c>
-      <c r="J53" s="58" t="s">
+      <c r="J53" s="58">
+        <v>0</v>
+      </c>
+      <c r="K53" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="K53" s="58" t="s">
+      <c r="L53" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="L53" s="58" t="s">
+      <c r="M53" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="M53" s="58" t="s">
+      <c r="N53" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" s="29" t="s">
         <v>2</v>
       </c>
@@ -61853,35 +62005,36 @@
       <c r="D54" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E54" s="57" t="s">
+      <c r="E54" s="57"/>
+      <c r="F54" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="58">
+      <c r="G54" s="58">
         <v>0</v>
       </c>
-      <c r="G54" s="58">
+      <c r="H54" s="58">
         <v>600</v>
-      </c>
-      <c r="H54" s="58">
-        <v>0</v>
       </c>
       <c r="I54" s="58">
         <v>0</v>
       </c>
-      <c r="J54" s="58" t="s">
+      <c r="J54" s="58">
+        <v>0</v>
+      </c>
+      <c r="K54" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="K54" s="58" t="s">
+      <c r="L54" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="L54" s="58" t="s">
+      <c r="M54" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="M54" s="58" t="s">
+      <c r="N54" s="58" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="29" t="s">
         <v>2</v>
       </c>
@@ -61891,11 +62044,9 @@
       <c r="D55" s="57" t="s">
         <v>255</v>
       </c>
-      <c r="E55" s="57" t="s">
+      <c r="E55" s="57"/>
+      <c r="F55" s="57" t="s">
         <v>235</v>
-      </c>
-      <c r="F55" s="58">
-        <v>0</v>
       </c>
       <c r="G55" s="58">
         <v>0</v>
@@ -61906,20 +62057,23 @@
       <c r="I55" s="58">
         <v>0</v>
       </c>
-      <c r="J55" s="58" t="s">
+      <c r="J55" s="58">
+        <v>0</v>
+      </c>
+      <c r="K55" s="58" t="s">
         <v>182</v>
-      </c>
-      <c r="K55" s="58" t="s">
-        <v>256</v>
       </c>
       <c r="L55" s="58" t="s">
         <v>256</v>
       </c>
       <c r="M55" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="N55" s="58" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="182" t="s">
         <v>2</v>
       </c>
@@ -61929,134 +62083,257 @@
       <c r="D56" s="184" t="s">
         <v>272</v>
       </c>
-      <c r="E56" s="185" t="s">
+      <c r="E56" s="184"/>
+      <c r="F56" s="185" t="s">
         <v>235</v>
       </c>
-      <c r="F56" s="186">
+      <c r="G56" s="186">
         <v>0</v>
       </c>
-      <c r="G56" s="187">
+      <c r="H56" s="186">
         <v>0</v>
       </c>
-      <c r="H56" s="187">
+      <c r="I56" s="186">
         <v>0</v>
       </c>
-      <c r="I56" s="187">
-        <v>1</v>
-      </c>
-      <c r="J56" s="187" t="s">
+      <c r="J56" s="186">
+        <v>5</v>
+      </c>
+      <c r="K56" s="186" t="s">
         <v>182</v>
       </c>
-      <c r="K56" s="187" t="s">
+      <c r="L56" s="186" t="s">
         <v>256</v>
       </c>
-      <c r="L56" s="187" t="s">
+      <c r="M56" s="186" t="s">
         <v>256</v>
       </c>
-      <c r="M56" s="187" t="s">
+      <c r="N56" s="186" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="256" t="s">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="255" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="60" t="s">
         <v>411</v>
       </c>
-      <c r="D57" s="257" t="s">
+      <c r="D57" s="256" t="s">
         <v>411</v>
       </c>
-      <c r="E57" s="61" t="s">
+      <c r="E57" s="256"/>
+      <c r="F57" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="F57" s="177">
+      <c r="G57" s="258">
         <v>0</v>
       </c>
-      <c r="G57" s="259">
+      <c r="H57" s="258">
         <v>0</v>
       </c>
-      <c r="H57" s="259">
+      <c r="I57" s="258">
         <v>0</v>
       </c>
-      <c r="I57" s="259">
+      <c r="J57" s="258">
         <v>0</v>
       </c>
-      <c r="J57" s="259" t="s">
+      <c r="K57" s="258" t="s">
         <v>182</v>
       </c>
-      <c r="K57" s="259" t="s">
+      <c r="L57" s="258" t="s">
         <v>413</v>
       </c>
-      <c r="L57" s="259" t="s">
+      <c r="M57" s="258" t="s">
         <v>413</v>
       </c>
-      <c r="M57" s="259" t="s">
+      <c r="N57" s="258" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="59" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B60" s="1" t="s">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="255" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="60" t="s">
+        <v>418</v>
+      </c>
+      <c r="D58" s="256" t="s">
+        <v>411</v>
+      </c>
+      <c r="E58" s="256"/>
+      <c r="F58" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="G58" s="258">
+        <v>0</v>
+      </c>
+      <c r="H58" s="258">
+        <v>0</v>
+      </c>
+      <c r="I58" s="258">
+        <v>0</v>
+      </c>
+      <c r="J58" s="258">
+        <v>5</v>
+      </c>
+      <c r="K58" s="258" t="s">
+        <v>182</v>
+      </c>
+      <c r="L58" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="M58" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="N58" s="258" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="255" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="D59" s="256" t="s">
+        <v>411</v>
+      </c>
+      <c r="E59" s="256" t="s">
+        <v>421</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="G59" s="258">
+        <v>0</v>
+      </c>
+      <c r="H59" s="258">
+        <v>0</v>
+      </c>
+      <c r="I59" s="258">
+        <v>0</v>
+      </c>
+      <c r="J59" s="258">
+        <v>15</v>
+      </c>
+      <c r="K59" s="258" t="s">
+        <v>182</v>
+      </c>
+      <c r="L59" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="M59" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="N59" s="258" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="255" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="D60" s="256" t="s">
+        <v>411</v>
+      </c>
+      <c r="E60" s="256" t="s">
+        <v>422</v>
+      </c>
+      <c r="F60" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="G60" s="258">
+        <v>0</v>
+      </c>
+      <c r="H60" s="258">
+        <v>0</v>
+      </c>
+      <c r="I60" s="258">
+        <v>0</v>
+      </c>
+      <c r="J60" s="258">
+        <v>25</v>
+      </c>
+      <c r="K60" s="258" t="s">
+        <v>182</v>
+      </c>
+      <c r="L60" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="M60" s="258" t="s">
+        <v>413</v>
+      </c>
+      <c r="N60" s="258" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B63" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
     </row>
-    <row r="62" spans="2:13" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+    <row r="65" spans="2:5" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="B65" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="47" t="s">
+      <c r="E65" s="47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="29" t="s">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C66" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="D63" s="57" t="s">
+      <c r="D66" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="E63" s="57" t="s">
+      <c r="E66" s="57" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="29" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C67" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="D64" s="57" t="s">
+      <c r="D67" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="E64" s="57" t="s">
+      <c r="E67" s="57" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="29" t="s">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C68" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="D65" s="57" t="s">
+      <c r="D68" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="E65" s="57" t="s">
+      <c r="E68" s="57" t="s">
         <v>205</v>
       </c>
     </row>
@@ -62069,64 +62346,91 @@
     <mergeCell ref="J29:O29"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="182" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D7">
-    <cfRule type="duplicateValues" dxfId="181" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="duplicateValues" dxfId="180" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="duplicateValues" dxfId="179" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C43">
-    <cfRule type="duplicateValues" dxfId="178" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="177" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="duplicateValues" dxfId="176" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:C57">
-    <cfRule type="duplicateValues" dxfId="175" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63:C65">
-    <cfRule type="duplicateValues" dxfId="174" priority="14"/>
+  <conditionalFormatting sqref="C66:C68">
+    <cfRule type="duplicateValues" dxfId="40" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC7">
-    <cfRule type="duplicateValues" dxfId="173" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA22">
-    <cfRule type="duplicateValues" dxfId="172" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA23">
-    <cfRule type="duplicateValues" dxfId="171" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA24">
-    <cfRule type="duplicateValues" dxfId="170" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="duplicateValues" dxfId="169" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D7">
-    <cfRule type="duplicateValues" dxfId="168" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC7">
-    <cfRule type="duplicateValues" dxfId="167" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C28">
-    <cfRule type="duplicateValues" dxfId="166" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:C46">
-    <cfRule type="duplicateValues" dxfId="165" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="duplicateValues" dxfId="164" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="duplicateValues" dxfId="163" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D28">
@@ -62193,8 +62497,8 @@
       <c r="D2" s="137"/>
       <c r="E2" s="137"/>
       <c r="F2" s="138"/>
-      <c r="G2" s="272"/>
-      <c r="H2" s="272"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
       <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -62426,7 +62730,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="51" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -62508,292 +62812,292 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="188" t="s">
+      <c r="A4" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="189">
+      <c r="C4" s="188">
         <v>0</v>
       </c>
-      <c r="D4" s="189" t="s">
+      <c r="D4" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F4" s="189">
+      <c r="F4" s="188">
         <v>1</v>
       </c>
-      <c r="G4" s="189" t="s">
+      <c r="G4" s="188" t="s">
         <v>281</v>
       </c>
-      <c r="H4" s="189" t="s">
+      <c r="H4" s="188" t="s">
         <v>282</v>
       </c>
-      <c r="I4" s="189" t="s">
+      <c r="I4" s="188" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="188" t="s">
+      <c r="A5" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="189" t="s">
+      <c r="B5" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="189">
+      <c r="C5" s="188">
         <v>1</v>
       </c>
-      <c r="D5" s="189" t="s">
+      <c r="D5" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="189" t="s">
+      <c r="E5" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F5" s="189">
+      <c r="F5" s="188">
         <v>1</v>
       </c>
-      <c r="G5" s="189" t="s">
+      <c r="G5" s="188" t="s">
         <v>285</v>
       </c>
-      <c r="H5" s="189" t="s">
+      <c r="H5" s="188" t="s">
         <v>286</v>
       </c>
-      <c r="I5" s="189" t="s">
+      <c r="I5" s="188" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="188" t="s">
+      <c r="A6" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="189" t="s">
+      <c r="B6" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="C6" s="189">
+      <c r="C6" s="188">
         <v>2</v>
       </c>
-      <c r="D6" s="189" t="s">
+      <c r="D6" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E6" s="189" t="s">
+      <c r="E6" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F6" s="189">
+      <c r="F6" s="188">
         <v>1</v>
       </c>
-      <c r="G6" s="189" t="s">
+      <c r="G6" s="188" t="s">
         <v>289</v>
       </c>
-      <c r="H6" s="189" t="s">
+      <c r="H6" s="188" t="s">
         <v>290</v>
       </c>
-      <c r="I6" s="189" t="s">
+      <c r="I6" s="188" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="188" t="s">
+      <c r="A7" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="189" t="s">
+      <c r="B7" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="C7" s="189">
+      <c r="C7" s="188">
         <v>3</v>
       </c>
-      <c r="D7" s="189" t="s">
+      <c r="D7" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E7" s="189" t="s">
+      <c r="E7" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F7" s="189">
+      <c r="F7" s="188">
         <v>1</v>
       </c>
-      <c r="G7" s="189" t="s">
+      <c r="G7" s="188" t="s">
         <v>293</v>
       </c>
-      <c r="H7" s="189" t="s">
+      <c r="H7" s="188" t="s">
         <v>294</v>
       </c>
-      <c r="I7" s="189" t="s">
+      <c r="I7" s="188" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="188" t="s">
+      <c r="A8" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="189" t="s">
+      <c r="B8" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="C8" s="189">
+      <c r="C8" s="188">
         <v>4</v>
       </c>
-      <c r="D8" s="189" t="s">
+      <c r="D8" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E8" s="189" t="s">
+      <c r="E8" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F8" s="189">
+      <c r="F8" s="188">
         <v>1</v>
       </c>
-      <c r="G8" s="189" t="s">
+      <c r="G8" s="188" t="s">
         <v>297</v>
       </c>
-      <c r="H8" s="189" t="s">
+      <c r="H8" s="188" t="s">
         <v>298</v>
       </c>
-      <c r="I8" s="189" t="s">
+      <c r="I8" s="188" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="188" t="s">
+      <c r="A9" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="189" t="s">
+      <c r="B9" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="C9" s="189">
+      <c r="C9" s="188">
         <v>5</v>
       </c>
-      <c r="D9" s="189" t="s">
+      <c r="D9" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E9" s="189" t="s">
+      <c r="E9" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F9" s="189">
+      <c r="F9" s="188">
         <v>1</v>
       </c>
-      <c r="G9" s="189" t="s">
+      <c r="G9" s="188" t="s">
         <v>301</v>
       </c>
-      <c r="H9" s="189" t="s">
+      <c r="H9" s="188" t="s">
         <v>302</v>
       </c>
-      <c r="I9" s="189" t="s">
+      <c r="I9" s="188" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="188" t="s">
+      <c r="A10" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="189" t="s">
+      <c r="B10" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="C10" s="189">
+      <c r="C10" s="188">
         <v>6</v>
       </c>
-      <c r="D10" s="189" t="s">
+      <c r="D10" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E10" s="189" t="s">
+      <c r="E10" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F10" s="189">
+      <c r="F10" s="188">
         <v>1</v>
       </c>
-      <c r="G10" s="189" t="s">
+      <c r="G10" s="188" t="s">
         <v>305</v>
       </c>
-      <c r="H10" s="189" t="s">
+      <c r="H10" s="188" t="s">
         <v>306</v>
       </c>
-      <c r="I10" s="189" t="s">
+      <c r="I10" s="188" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="188" t="s">
+      <c r="A11" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="189" t="s">
+      <c r="B11" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="C11" s="189">
+      <c r="C11" s="188">
         <v>7</v>
       </c>
-      <c r="D11" s="189" t="s">
+      <c r="D11" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E11" s="189" t="s">
+      <c r="E11" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F11" s="189">
+      <c r="F11" s="188">
         <v>1</v>
       </c>
-      <c r="G11" s="189" t="s">
+      <c r="G11" s="188" t="s">
         <v>309</v>
       </c>
-      <c r="H11" s="189" t="s">
+      <c r="H11" s="188" t="s">
         <v>310</v>
       </c>
-      <c r="I11" s="189" t="s">
+      <c r="I11" s="188" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="188" t="s">
+      <c r="A12" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="189" t="s">
+      <c r="B12" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="C12" s="189">
+      <c r="C12" s="188">
         <v>8</v>
       </c>
-      <c r="D12" s="189" t="s">
+      <c r="D12" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E12" s="189" t="s">
+      <c r="E12" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F12" s="189">
+      <c r="F12" s="188">
         <v>1</v>
       </c>
-      <c r="G12" s="189" t="s">
+      <c r="G12" s="188" t="s">
         <v>313</v>
       </c>
-      <c r="H12" s="189" t="s">
+      <c r="H12" s="188" t="s">
         <v>314</v>
       </c>
-      <c r="I12" s="189" t="s">
+      <c r="I12" s="188" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="188" t="s">
+      <c r="A13" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="189" t="s">
+      <c r="B13" s="188" t="s">
         <v>316</v>
       </c>
-      <c r="C13" s="189">
+      <c r="C13" s="188">
         <v>9</v>
       </c>
-      <c r="D13" s="189" t="s">
+      <c r="D13" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="E13" s="189" t="s">
+      <c r="E13" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="189">
+      <c r="F13" s="188">
         <v>1</v>
       </c>
-      <c r="G13" s="189" t="s">
+      <c r="G13" s="188" t="s">
         <v>317</v>
       </c>
-      <c r="H13" s="189" t="s">
+      <c r="H13" s="188" t="s">
         <v>318</v>
       </c>
-      <c r="I13" s="189" t="s">
+      <c r="I13" s="188" t="s">
         <v>319</v>
       </c>
     </row>
@@ -62835,7 +63139,7 @@
       <c r="F17" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="G17" s="190" t="s">
+      <c r="G17" s="189" t="s">
         <v>325</v>
       </c>
     </row>
@@ -62843,22 +63147,22 @@
       <c r="A18" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="188" t="s">
         <v>326</v>
       </c>
-      <c r="C18" s="189" t="s">
+      <c r="C18" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="D18" s="189" t="s">
+      <c r="D18" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E18" s="189">
+      <c r="E18" s="188">
         <v>4000</v>
       </c>
-      <c r="F18" s="189">
+      <c r="F18" s="188">
         <v>100</v>
       </c>
-      <c r="G18" s="191" t="s">
+      <c r="G18" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62866,22 +63170,22 @@
       <c r="A19" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="189" t="s">
+      <c r="B19" s="188" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="189" t="s">
+      <c r="C19" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="D19" s="189" t="s">
+      <c r="D19" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E19" s="189">
+      <c r="E19" s="188">
         <v>8000</v>
       </c>
-      <c r="F19" s="189">
+      <c r="F19" s="188">
         <v>90</v>
       </c>
-      <c r="G19" s="191" t="s">
+      <c r="G19" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62889,22 +63193,22 @@
       <c r="A20" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="189" t="s">
+      <c r="B20" s="188" t="s">
         <v>331</v>
       </c>
-      <c r="C20" s="189" t="s">
+      <c r="C20" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="D20" s="189" t="s">
+      <c r="D20" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E20" s="189">
+      <c r="E20" s="188">
         <v>10000</v>
       </c>
-      <c r="F20" s="189">
+      <c r="F20" s="188">
         <v>50</v>
       </c>
-      <c r="G20" s="191" t="s">
+      <c r="G20" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62912,22 +63216,22 @@
       <c r="A21" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="189" t="s">
+      <c r="B21" s="188" t="s">
         <v>332</v>
       </c>
-      <c r="C21" s="189" t="s">
+      <c r="C21" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="D21" s="189" t="s">
+      <c r="D21" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E21" s="189">
+      <c r="E21" s="188">
         <v>20</v>
       </c>
-      <c r="F21" s="189">
+      <c r="F21" s="188">
         <v>10</v>
       </c>
-      <c r="G21" s="191" t="s">
+      <c r="G21" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62935,22 +63239,22 @@
       <c r="A22" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="189" t="s">
+      <c r="B22" s="188" t="s">
         <v>334</v>
       </c>
-      <c r="C22" s="189" t="s">
+      <c r="C22" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="D22" s="189" t="s">
+      <c r="D22" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E22" s="189">
+      <c r="E22" s="188">
         <v>80</v>
       </c>
-      <c r="F22" s="189">
+      <c r="F22" s="188">
         <v>1</v>
       </c>
-      <c r="G22" s="191" t="s">
+      <c r="G22" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62958,22 +63262,22 @@
       <c r="A23" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="189" t="s">
+      <c r="B23" s="188" t="s">
         <v>335</v>
       </c>
-      <c r="C23" s="189" t="s">
+      <c r="C23" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="D23" s="189" t="s">
+      <c r="D23" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E23" s="189">
+      <c r="E23" s="188">
         <v>4000</v>
       </c>
-      <c r="F23" s="189">
+      <c r="F23" s="188">
         <v>100</v>
       </c>
-      <c r="G23" s="191" t="s">
+      <c r="G23" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -62981,22 +63285,22 @@
       <c r="A24" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="189" t="s">
+      <c r="B24" s="188" t="s">
         <v>336</v>
       </c>
-      <c r="C24" s="189" t="s">
+      <c r="C24" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="D24" s="189" t="s">
+      <c r="D24" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E24" s="189">
+      <c r="E24" s="188">
         <v>8000</v>
       </c>
-      <c r="F24" s="189">
+      <c r="F24" s="188">
         <v>90</v>
       </c>
-      <c r="G24" s="191" t="s">
+      <c r="G24" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63004,22 +63308,22 @@
       <c r="A25" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="189" t="s">
+      <c r="B25" s="188" t="s">
         <v>337</v>
       </c>
-      <c r="C25" s="189" t="s">
+      <c r="C25" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="D25" s="189" t="s">
+      <c r="D25" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E25" s="189">
+      <c r="E25" s="188">
         <v>10000</v>
       </c>
-      <c r="F25" s="189">
+      <c r="F25" s="188">
         <v>50</v>
       </c>
-      <c r="G25" s="191" t="s">
+      <c r="G25" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63027,22 +63331,22 @@
       <c r="A26" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="189" t="s">
+      <c r="B26" s="188" t="s">
         <v>338</v>
       </c>
-      <c r="C26" s="189" t="s">
+      <c r="C26" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="D26" s="189" t="s">
+      <c r="D26" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E26" s="189">
+      <c r="E26" s="188">
         <v>20</v>
       </c>
-      <c r="F26" s="189">
+      <c r="F26" s="188">
         <v>10</v>
       </c>
-      <c r="G26" s="191" t="s">
+      <c r="G26" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63050,22 +63354,22 @@
       <c r="A27" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="189" t="s">
+      <c r="B27" s="188" t="s">
         <v>339</v>
       </c>
-      <c r="C27" s="189" t="s">
+      <c r="C27" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="D27" s="189" t="s">
+      <c r="D27" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E27" s="189">
+      <c r="E27" s="188">
         <v>80</v>
       </c>
-      <c r="F27" s="189">
+      <c r="F27" s="188">
         <v>1</v>
       </c>
-      <c r="G27" s="191" t="s">
+      <c r="G27" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63073,22 +63377,22 @@
       <c r="A28" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="189" t="s">
+      <c r="B28" s="188" t="s">
         <v>340</v>
       </c>
-      <c r="C28" s="189" t="s">
+      <c r="C28" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="D28" s="189" t="s">
+      <c r="D28" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E28" s="189">
+      <c r="E28" s="188">
         <v>12000</v>
       </c>
-      <c r="F28" s="189">
+      <c r="F28" s="188">
         <v>100</v>
       </c>
-      <c r="G28" s="191" t="s">
+      <c r="G28" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63096,22 +63400,22 @@
       <c r="A29" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="189" t="s">
+      <c r="B29" s="188" t="s">
         <v>341</v>
       </c>
-      <c r="C29" s="189" t="s">
+      <c r="C29" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="D29" s="189" t="s">
+      <c r="D29" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E29" s="189">
+      <c r="E29" s="188">
         <v>16000</v>
       </c>
-      <c r="F29" s="189">
+      <c r="F29" s="188">
         <v>90</v>
       </c>
-      <c r="G29" s="191" t="s">
+      <c r="G29" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63119,22 +63423,22 @@
       <c r="A30" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="189" t="s">
+      <c r="B30" s="188" t="s">
         <v>342</v>
       </c>
-      <c r="C30" s="189" t="s">
+      <c r="C30" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="D30" s="189" t="s">
+      <c r="D30" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="189">
+      <c r="E30" s="188">
         <v>20000</v>
       </c>
-      <c r="F30" s="189">
+      <c r="F30" s="188">
         <v>50</v>
       </c>
-      <c r="G30" s="191" t="s">
+      <c r="G30" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63142,22 +63446,22 @@
       <c r="A31" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="189" t="s">
+      <c r="B31" s="188" t="s">
         <v>343</v>
       </c>
-      <c r="C31" s="189" t="s">
+      <c r="C31" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="D31" s="189" t="s">
+      <c r="D31" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E31" s="189">
+      <c r="E31" s="188">
         <v>30</v>
       </c>
-      <c r="F31" s="189">
+      <c r="F31" s="188">
         <v>10</v>
       </c>
-      <c r="G31" s="191" t="s">
+      <c r="G31" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63165,22 +63469,22 @@
       <c r="A32" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="189" t="s">
+      <c r="B32" s="188" t="s">
         <v>344</v>
       </c>
-      <c r="C32" s="189" t="s">
+      <c r="C32" s="188" t="s">
         <v>284</v>
       </c>
-      <c r="D32" s="189" t="s">
+      <c r="D32" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E32" s="189">
+      <c r="E32" s="188">
         <v>100</v>
       </c>
-      <c r="F32" s="189">
+      <c r="F32" s="188">
         <v>1</v>
       </c>
-      <c r="G32" s="191" t="s">
+      <c r="G32" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63188,22 +63492,22 @@
       <c r="A33" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="189" t="s">
+      <c r="B33" s="188" t="s">
         <v>345</v>
       </c>
-      <c r="C33" s="189" t="s">
+      <c r="C33" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D33" s="189" t="s">
+      <c r="D33" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E33" s="189">
+      <c r="E33" s="188">
         <v>21000</v>
       </c>
-      <c r="F33" s="189">
+      <c r="F33" s="188">
         <v>100</v>
       </c>
-      <c r="G33" s="191" t="s">
+      <c r="G33" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63211,22 +63515,22 @@
       <c r="A34" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="189" t="s">
+      <c r="B34" s="188" t="s">
         <v>346</v>
       </c>
-      <c r="C34" s="189" t="s">
+      <c r="C34" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D34" s="189" t="s">
+      <c r="D34" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E34" s="189">
+      <c r="E34" s="188">
         <v>24000</v>
       </c>
-      <c r="F34" s="189">
+      <c r="F34" s="188">
         <v>90</v>
       </c>
-      <c r="G34" s="191" t="s">
+      <c r="G34" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63234,22 +63538,22 @@
       <c r="A35" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="189" t="s">
+      <c r="B35" s="188" t="s">
         <v>347</v>
       </c>
-      <c r="C35" s="189" t="s">
+      <c r="C35" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D35" s="189" t="s">
+      <c r="D35" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E35" s="189">
+      <c r="E35" s="188">
         <v>30000</v>
       </c>
-      <c r="F35" s="189">
+      <c r="F35" s="188">
         <v>50</v>
       </c>
-      <c r="G35" s="191" t="s">
+      <c r="G35" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63257,22 +63561,22 @@
       <c r="A36" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="189" t="s">
+      <c r="B36" s="188" t="s">
         <v>348</v>
       </c>
-      <c r="C36" s="189" t="s">
+      <c r="C36" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D36" s="189" t="s">
+      <c r="D36" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E36" s="189">
+      <c r="E36" s="188">
         <v>50</v>
       </c>
-      <c r="F36" s="189">
+      <c r="F36" s="188">
         <v>10</v>
       </c>
-      <c r="G36" s="191" t="s">
+      <c r="G36" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63280,22 +63584,22 @@
       <c r="A37" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="189" t="s">
+      <c r="B37" s="188" t="s">
         <v>349</v>
       </c>
-      <c r="C37" s="189" t="s">
+      <c r="C37" s="188" t="s">
         <v>288</v>
       </c>
-      <c r="D37" s="189" t="s">
+      <c r="D37" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E37" s="189">
+      <c r="E37" s="188">
         <v>110</v>
       </c>
-      <c r="F37" s="189">
+      <c r="F37" s="188">
         <v>1</v>
       </c>
-      <c r="G37" s="191" t="s">
+      <c r="G37" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63303,22 +63607,22 @@
       <c r="A38" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="189" t="s">
+      <c r="B38" s="188" t="s">
         <v>350</v>
       </c>
-      <c r="C38" s="189" t="s">
+      <c r="C38" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="D38" s="189" t="s">
+      <c r="D38" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E38" s="189">
+      <c r="E38" s="188">
         <v>32000</v>
       </c>
-      <c r="F38" s="189">
+      <c r="F38" s="188">
         <v>100</v>
       </c>
-      <c r="G38" s="191" t="s">
+      <c r="G38" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63326,22 +63630,22 @@
       <c r="A39" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="189" t="s">
+      <c r="B39" s="188" t="s">
         <v>351</v>
       </c>
-      <c r="C39" s="189" t="s">
+      <c r="C39" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="D39" s="189" t="s">
+      <c r="D39" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E39" s="189">
+      <c r="E39" s="188">
         <v>37000</v>
       </c>
-      <c r="F39" s="189">
+      <c r="F39" s="188">
         <v>90</v>
       </c>
-      <c r="G39" s="191" t="s">
+      <c r="G39" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63349,22 +63653,22 @@
       <c r="A40" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="189" t="s">
+      <c r="B40" s="188" t="s">
         <v>352</v>
       </c>
-      <c r="C40" s="189" t="s">
+      <c r="C40" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="D40" s="189" t="s">
+      <c r="D40" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E40" s="189">
+      <c r="E40" s="188">
         <v>42000</v>
       </c>
-      <c r="F40" s="189">
+      <c r="F40" s="188">
         <v>50</v>
       </c>
-      <c r="G40" s="191" t="s">
+      <c r="G40" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63372,22 +63676,22 @@
       <c r="A41" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="189" t="s">
+      <c r="B41" s="188" t="s">
         <v>353</v>
       </c>
-      <c r="C41" s="189" t="s">
+      <c r="C41" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="D41" s="189" t="s">
+      <c r="D41" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E41" s="189">
+      <c r="E41" s="188">
         <v>60</v>
       </c>
-      <c r="F41" s="189">
+      <c r="F41" s="188">
         <v>10</v>
       </c>
-      <c r="G41" s="191" t="s">
+      <c r="G41" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63395,22 +63699,22 @@
       <c r="A42" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="189" t="s">
+      <c r="B42" s="188" t="s">
         <v>354</v>
       </c>
-      <c r="C42" s="189" t="s">
+      <c r="C42" s="188" t="s">
         <v>292</v>
       </c>
-      <c r="D42" s="189" t="s">
+      <c r="D42" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E42" s="189">
+      <c r="E42" s="188">
         <v>120</v>
       </c>
-      <c r="F42" s="189">
+      <c r="F42" s="188">
         <v>1</v>
       </c>
-      <c r="G42" s="191" t="s">
+      <c r="G42" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63418,22 +63722,22 @@
       <c r="A43" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="189" t="s">
+      <c r="B43" s="188" t="s">
         <v>355</v>
       </c>
-      <c r="C43" s="189" t="s">
+      <c r="C43" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="D43" s="189" t="s">
+      <c r="D43" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E43" s="189">
+      <c r="E43" s="188">
         <v>43000</v>
       </c>
-      <c r="F43" s="189">
+      <c r="F43" s="188">
         <v>100</v>
       </c>
-      <c r="G43" s="191" t="s">
+      <c r="G43" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63441,22 +63745,22 @@
       <c r="A44" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="189" t="s">
+      <c r="B44" s="188" t="s">
         <v>356</v>
       </c>
-      <c r="C44" s="189" t="s">
+      <c r="C44" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="D44" s="189" t="s">
+      <c r="D44" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E44" s="189">
+      <c r="E44" s="188">
         <v>48000</v>
       </c>
-      <c r="F44" s="189">
+      <c r="F44" s="188">
         <v>90</v>
       </c>
-      <c r="G44" s="191" t="s">
+      <c r="G44" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63464,22 +63768,22 @@
       <c r="A45" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="189" t="s">
+      <c r="B45" s="188" t="s">
         <v>357</v>
       </c>
-      <c r="C45" s="189" t="s">
+      <c r="C45" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="D45" s="189" t="s">
+      <c r="D45" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E45" s="189">
+      <c r="E45" s="188">
         <v>50000</v>
       </c>
-      <c r="F45" s="189">
+      <c r="F45" s="188">
         <v>50</v>
       </c>
-      <c r="G45" s="191" t="s">
+      <c r="G45" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63487,22 +63791,22 @@
       <c r="A46" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="189" t="s">
+      <c r="B46" s="188" t="s">
         <v>358</v>
       </c>
-      <c r="C46" s="189" t="s">
+      <c r="C46" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="D46" s="189" t="s">
+      <c r="D46" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E46" s="189">
+      <c r="E46" s="188">
         <v>70</v>
       </c>
-      <c r="F46" s="189">
+      <c r="F46" s="188">
         <v>10</v>
       </c>
-      <c r="G46" s="191" t="s">
+      <c r="G46" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63510,22 +63814,22 @@
       <c r="A47" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="189" t="s">
+      <c r="B47" s="188" t="s">
         <v>359</v>
       </c>
-      <c r="C47" s="189" t="s">
+      <c r="C47" s="188" t="s">
         <v>296</v>
       </c>
-      <c r="D47" s="189" t="s">
+      <c r="D47" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E47" s="189">
+      <c r="E47" s="188">
         <v>130</v>
       </c>
-      <c r="F47" s="189">
+      <c r="F47" s="188">
         <v>1</v>
       </c>
-      <c r="G47" s="191" t="s">
+      <c r="G47" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63533,22 +63837,22 @@
       <c r="A48" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="189" t="s">
+      <c r="B48" s="188" t="s">
         <v>360</v>
       </c>
-      <c r="C48" s="189" t="s">
+      <c r="C48" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="D48" s="189" t="s">
+      <c r="D48" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E48" s="189">
+      <c r="E48" s="188">
         <v>52000</v>
       </c>
-      <c r="F48" s="189">
+      <c r="F48" s="188">
         <v>100</v>
       </c>
-      <c r="G48" s="191" t="s">
+      <c r="G48" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63556,22 +63860,22 @@
       <c r="A49" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="189" t="s">
+      <c r="B49" s="188" t="s">
         <v>361</v>
       </c>
-      <c r="C49" s="189" t="s">
+      <c r="C49" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="D49" s="189" t="s">
+      <c r="D49" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E49" s="189">
+      <c r="E49" s="188">
         <v>55000</v>
       </c>
-      <c r="F49" s="189">
+      <c r="F49" s="188">
         <v>90</v>
       </c>
-      <c r="G49" s="191" t="s">
+      <c r="G49" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63579,22 +63883,22 @@
       <c r="A50" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="189" t="s">
+      <c r="B50" s="188" t="s">
         <v>362</v>
       </c>
-      <c r="C50" s="189" t="s">
+      <c r="C50" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="D50" s="189" t="s">
+      <c r="D50" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E50" s="189">
+      <c r="E50" s="188">
         <v>58000</v>
       </c>
-      <c r="F50" s="189">
+      <c r="F50" s="188">
         <v>50</v>
       </c>
-      <c r="G50" s="191" t="s">
+      <c r="G50" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63602,22 +63906,22 @@
       <c r="A51" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="189" t="s">
+      <c r="B51" s="188" t="s">
         <v>363</v>
       </c>
-      <c r="C51" s="189" t="s">
+      <c r="C51" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="D51" s="189" t="s">
+      <c r="D51" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E51" s="189">
+      <c r="E51" s="188">
         <v>80</v>
       </c>
-      <c r="F51" s="189">
+      <c r="F51" s="188">
         <v>10</v>
       </c>
-      <c r="G51" s="191" t="s">
+      <c r="G51" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63625,22 +63929,22 @@
       <c r="A52" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="189" t="s">
+      <c r="B52" s="188" t="s">
         <v>364</v>
       </c>
-      <c r="C52" s="189" t="s">
+      <c r="C52" s="188" t="s">
         <v>300</v>
       </c>
-      <c r="D52" s="189" t="s">
+      <c r="D52" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E52" s="189">
+      <c r="E52" s="188">
         <v>140</v>
       </c>
-      <c r="F52" s="189">
+      <c r="F52" s="188">
         <v>1</v>
       </c>
-      <c r="G52" s="191" t="s">
+      <c r="G52" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63648,22 +63952,22 @@
       <c r="A53" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="189" t="s">
+      <c r="B53" s="188" t="s">
         <v>365</v>
       </c>
-      <c r="C53" s="189" t="s">
+      <c r="C53" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="D53" s="189" t="s">
+      <c r="D53" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E53" s="189">
+      <c r="E53" s="188">
         <v>60000</v>
       </c>
-      <c r="F53" s="189">
+      <c r="F53" s="188">
         <v>100</v>
       </c>
-      <c r="G53" s="191" t="s">
+      <c r="G53" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63671,22 +63975,22 @@
       <c r="A54" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="189" t="s">
+      <c r="B54" s="188" t="s">
         <v>366</v>
       </c>
-      <c r="C54" s="189" t="s">
+      <c r="C54" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="D54" s="189" t="s">
+      <c r="D54" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E54" s="189">
+      <c r="E54" s="188">
         <v>63000</v>
       </c>
-      <c r="F54" s="189">
+      <c r="F54" s="188">
         <v>90</v>
       </c>
-      <c r="G54" s="191" t="s">
+      <c r="G54" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63694,22 +63998,22 @@
       <c r="A55" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="189" t="s">
+      <c r="B55" s="188" t="s">
         <v>367</v>
       </c>
-      <c r="C55" s="189" t="s">
+      <c r="C55" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="D55" s="189" t="s">
+      <c r="D55" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E55" s="189">
+      <c r="E55" s="188">
         <v>67000</v>
       </c>
-      <c r="F55" s="189">
+      <c r="F55" s="188">
         <v>50</v>
       </c>
-      <c r="G55" s="191" t="s">
+      <c r="G55" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63717,22 +64021,22 @@
       <c r="A56" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="189" t="s">
+      <c r="B56" s="188" t="s">
         <v>368</v>
       </c>
-      <c r="C56" s="189" t="s">
+      <c r="C56" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="D56" s="189" t="s">
+      <c r="D56" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E56" s="189">
+      <c r="E56" s="188">
         <v>90</v>
       </c>
-      <c r="F56" s="189">
+      <c r="F56" s="188">
         <v>10</v>
       </c>
-      <c r="G56" s="191" t="s">
+      <c r="G56" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63740,22 +64044,22 @@
       <c r="A57" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="189" t="s">
+      <c r="B57" s="188" t="s">
         <v>369</v>
       </c>
-      <c r="C57" s="189" t="s">
+      <c r="C57" s="188" t="s">
         <v>304</v>
       </c>
-      <c r="D57" s="189" t="s">
+      <c r="D57" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E57" s="189">
+      <c r="E57" s="188">
         <v>150</v>
       </c>
-      <c r="F57" s="189">
+      <c r="F57" s="188">
         <v>1</v>
       </c>
-      <c r="G57" s="191" t="s">
+      <c r="G57" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63763,22 +64067,22 @@
       <c r="A58" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="189" t="s">
+      <c r="B58" s="188" t="s">
         <v>370</v>
       </c>
-      <c r="C58" s="189" t="s">
+      <c r="C58" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="D58" s="189" t="s">
+      <c r="D58" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E58" s="189">
+      <c r="E58" s="188">
         <v>70000</v>
       </c>
-      <c r="F58" s="189">
+      <c r="F58" s="188">
         <v>100</v>
       </c>
-      <c r="G58" s="191" t="s">
+      <c r="G58" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63786,22 +64090,22 @@
       <c r="A59" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="189" t="s">
+      <c r="B59" s="188" t="s">
         <v>371</v>
       </c>
-      <c r="C59" s="189" t="s">
+      <c r="C59" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="D59" s="189" t="s">
+      <c r="D59" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E59" s="189">
+      <c r="E59" s="188">
         <v>73000</v>
       </c>
-      <c r="F59" s="189">
+      <c r="F59" s="188">
         <v>90</v>
       </c>
-      <c r="G59" s="191" t="s">
+      <c r="G59" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63809,22 +64113,22 @@
       <c r="A60" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="189" t="s">
+      <c r="B60" s="188" t="s">
         <v>372</v>
       </c>
-      <c r="C60" s="189" t="s">
+      <c r="C60" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="D60" s="189" t="s">
+      <c r="D60" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E60" s="189">
+      <c r="E60" s="188">
         <v>80000</v>
       </c>
-      <c r="F60" s="189">
+      <c r="F60" s="188">
         <v>50</v>
       </c>
-      <c r="G60" s="191" t="s">
+      <c r="G60" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63832,22 +64136,22 @@
       <c r="A61" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="189" t="s">
+      <c r="B61" s="188" t="s">
         <v>373</v>
       </c>
-      <c r="C61" s="189" t="s">
+      <c r="C61" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="D61" s="189" t="s">
+      <c r="D61" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E61" s="189">
+      <c r="E61" s="188">
         <v>100</v>
       </c>
-      <c r="F61" s="189">
+      <c r="F61" s="188">
         <v>10</v>
       </c>
-      <c r="G61" s="191" t="s">
+      <c r="G61" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63855,22 +64159,22 @@
       <c r="A62" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="189" t="s">
+      <c r="B62" s="188" t="s">
         <v>374</v>
       </c>
-      <c r="C62" s="189" t="s">
+      <c r="C62" s="188" t="s">
         <v>308</v>
       </c>
-      <c r="D62" s="189" t="s">
+      <c r="D62" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E62" s="189">
+      <c r="E62" s="188">
         <v>160</v>
       </c>
-      <c r="F62" s="189">
+      <c r="F62" s="188">
         <v>1</v>
       </c>
-      <c r="G62" s="191" t="s">
+      <c r="G62" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63878,22 +64182,22 @@
       <c r="A63" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="189" t="s">
+      <c r="B63" s="188" t="s">
         <v>375</v>
       </c>
-      <c r="C63" s="189" t="s">
+      <c r="C63" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="D63" s="189" t="s">
+      <c r="D63" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E63" s="189">
+      <c r="E63" s="188">
         <v>82000</v>
       </c>
-      <c r="F63" s="189">
+      <c r="F63" s="188">
         <v>100</v>
       </c>
-      <c r="G63" s="191" t="s">
+      <c r="G63" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63901,22 +64205,22 @@
       <c r="A64" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="189" t="s">
+      <c r="B64" s="188" t="s">
         <v>376</v>
       </c>
-      <c r="C64" s="189" t="s">
+      <c r="C64" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="D64" s="189" t="s">
+      <c r="D64" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E64" s="189">
+      <c r="E64" s="188">
         <v>85000</v>
       </c>
-      <c r="F64" s="189">
+      <c r="F64" s="188">
         <v>90</v>
       </c>
-      <c r="G64" s="191" t="s">
+      <c r="G64" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63924,22 +64228,22 @@
       <c r="A65" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="189" t="s">
+      <c r="B65" s="188" t="s">
         <v>377</v>
       </c>
-      <c r="C65" s="189" t="s">
+      <c r="C65" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="D65" s="189" t="s">
+      <c r="D65" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E65" s="189">
+      <c r="E65" s="188">
         <v>89000</v>
       </c>
-      <c r="F65" s="189">
+      <c r="F65" s="188">
         <v>50</v>
       </c>
-      <c r="G65" s="191" t="s">
+      <c r="G65" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63947,22 +64251,22 @@
       <c r="A66" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="189" t="s">
+      <c r="B66" s="188" t="s">
         <v>378</v>
       </c>
-      <c r="C66" s="189" t="s">
+      <c r="C66" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="D66" s="189" t="s">
+      <c r="D66" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E66" s="189">
+      <c r="E66" s="188">
         <v>110</v>
       </c>
-      <c r="F66" s="189">
+      <c r="F66" s="188">
         <v>10</v>
       </c>
-      <c r="G66" s="191" t="s">
+      <c r="G66" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63970,22 +64274,22 @@
       <c r="A67" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="189" t="s">
+      <c r="B67" s="188" t="s">
         <v>379</v>
       </c>
-      <c r="C67" s="189" t="s">
+      <c r="C67" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="D67" s="189" t="s">
+      <c r="D67" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E67" s="189">
+      <c r="E67" s="188">
         <v>170</v>
       </c>
-      <c r="F67" s="189">
+      <c r="F67" s="188">
         <v>1</v>
       </c>
-      <c r="G67" s="191" t="s">
+      <c r="G67" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -63993,22 +64297,22 @@
       <c r="A68" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="189" t="s">
+      <c r="B68" s="188" t="s">
         <v>380</v>
       </c>
-      <c r="C68" s="189" t="s">
+      <c r="C68" s="188" t="s">
         <v>316</v>
       </c>
-      <c r="D68" s="189" t="s">
+      <c r="D68" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E68" s="189">
+      <c r="E68" s="188">
         <v>92000</v>
       </c>
-      <c r="F68" s="189">
+      <c r="F68" s="188">
         <v>100</v>
       </c>
-      <c r="G68" s="191" t="s">
+      <c r="G68" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -64016,22 +64320,22 @@
       <c r="A69" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="189" t="s">
+      <c r="B69" s="188" t="s">
         <v>381</v>
       </c>
-      <c r="C69" s="189" t="s">
+      <c r="C69" s="188" t="s">
         <v>316</v>
       </c>
-      <c r="D69" s="189" t="s">
+      <c r="D69" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E69" s="189">
+      <c r="E69" s="188">
         <v>95000</v>
       </c>
-      <c r="F69" s="189">
+      <c r="F69" s="188">
         <v>90</v>
       </c>
-      <c r="G69" s="191" t="s">
+      <c r="G69" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -64039,22 +64343,22 @@
       <c r="A70" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B70" s="189" t="s">
+      <c r="B70" s="188" t="s">
         <v>382</v>
       </c>
-      <c r="C70" s="189" t="s">
+      <c r="C70" s="188" t="s">
         <v>316</v>
       </c>
-      <c r="D70" s="189" t="s">
+      <c r="D70" s="188" t="s">
         <v>328</v>
       </c>
-      <c r="E70" s="189">
+      <c r="E70" s="188">
         <v>120000</v>
       </c>
-      <c r="F70" s="189">
+      <c r="F70" s="188">
         <v>50</v>
       </c>
-      <c r="G70" s="191" t="s">
+      <c r="G70" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -64062,22 +64366,22 @@
       <c r="A71" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="189" t="s">
+      <c r="B71" s="188" t="s">
         <v>383</v>
       </c>
-      <c r="C71" s="189" t="s">
+      <c r="C71" s="188" t="s">
         <v>316</v>
       </c>
-      <c r="D71" s="189" t="s">
+      <c r="D71" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="E71" s="189">
+      <c r="E71" s="188">
         <v>120</v>
       </c>
-      <c r="F71" s="189">
+      <c r="F71" s="188">
         <v>10</v>
       </c>
-      <c r="G71" s="191" t="s">
+      <c r="G71" s="190" t="s">
         <v>329</v>
       </c>
     </row>
@@ -64085,31 +64389,31 @@
       <c r="A72" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="192" t="s">
+      <c r="B72" s="191" t="s">
         <v>384</v>
       </c>
-      <c r="C72" s="192" t="s">
+      <c r="C72" s="191" t="s">
         <v>316</v>
       </c>
-      <c r="D72" s="192" t="s">
+      <c r="D72" s="191" t="s">
         <v>333</v>
       </c>
-      <c r="E72" s="192">
+      <c r="E72" s="191">
         <v>180</v>
       </c>
-      <c r="F72" s="189">
+      <c r="F72" s="188">
         <v>1</v>
       </c>
-      <c r="G72" s="191" t="s">
+      <c r="G72" s="190" t="s">
         <v>329</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:B72">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C13">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -64145,12 +64449,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="273" t="s">
+      <c r="E3" s="272" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="273"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="273"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="272"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -65107,22 +65411,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -65159,12 +65463,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="273" t="s">
+      <c r="E3" s="272" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="273"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="273"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="272"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -66128,22 +66432,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -66180,12 +66484,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="273" t="s">
+      <c r="E3" s="272" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="273"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="273"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="272"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -67142,22 +67446,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67194,12 +67498,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="273" t="s">
+      <c r="E3" s="272" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="273"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="273"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="272"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -68165,22 +68469,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Missing a body part
Former-commit-id: 850cc9a5c9af27a58114ac6e29c4f304cee89398
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -1299,7 +1299,7 @@
     <t>FX_IceSmokeWing_l;FX_IceSmokeWing_r</t>
   </si>
   <si>
-    <t>FX_IceSmokeBody</t>
+    <t>FX_IceSmokeWing_l;FX_IceSmokeWing_r;FX_IceSmokeBody</t>
   </si>
 </sst>
 </file>
@@ -2919,132 +2919,6 @@
   </cellStyles>
   <dxfs count="193">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -3155,276 +3029,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3772,6 +3376,26 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4232,6 +3856,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -4484,6 +4118,42 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -4513,6 +4183,46 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -7365,6 +7075,296 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -57810,116 +57810,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA28" totalsRowShown="0" headerRowBorderDxfId="192" totalsRowBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B12:BA28" totalsRowShown="0" headerRowBorderDxfId="163" totalsRowBorderDxfId="162">
   <autoFilter ref="B12:BA28"/>
   <tableColumns count="52">
-    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="190"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="189"/>
-    <tableColumn id="3" name="[tier]" dataDxfId="188"/>
-    <tableColumn id="4" name="[specialDragon]" dataDxfId="187"/>
-    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="186"/>
-    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="185"/>
-    <tableColumn id="8" name="[defaultSize]" dataDxfId="184"/>
-    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="183"/>
-    <tableColumn id="10" name="[health]" dataDxfId="182"/>
-    <tableColumn id="11" name="[healthDrain]" dataDxfId="181"/>
-    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="180"/>
-    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="179"/>
-    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="178"/>
-    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="177"/>
-    <tableColumn id="16" name="[scale]" dataDxfId="176"/>
-    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="175"/>
-    <tableColumn id="18" name="[energyBase]" dataDxfId="174"/>
-    <tableColumn id="19" name="[energyDrain]" dataDxfId="173"/>
-    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="172"/>
-    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="171"/>
-    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="170"/>
-    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="169"/>
-    <tableColumn id="24" name="[furyMax]" dataDxfId="168"/>
-    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="167"/>
-    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="166"/>
-    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="165"/>
-    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="164"/>
-    <tableColumn id="29" name="[gamePrefab]" dataDxfId="163"/>
-    <tableColumn id="30" name="[menuPrefab]" dataDxfId="162"/>
-    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="161"/>
-    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="160"/>
-    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="159"/>
-    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="158"/>
-    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="157"/>
-    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="156"/>
-    <tableColumn id="37" name="[invincible]" dataDxfId="155"/>
-    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="154"/>
-    <tableColumn id="39" name="[eatEverything]" dataDxfId="153"/>
-    <tableColumn id="40" name="[modeDuration]" dataDxfId="152"/>
-    <tableColumn id="41" name="[petScale]" dataDxfId="151"/>
-    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="150"/>
-    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="149"/>
-    <tableColumn id="46" name="[force]" dataDxfId="148"/>
-    <tableColumn id="47" name="[mass]" dataDxfId="147"/>
-    <tableColumn id="48" name="[friction]" dataDxfId="146"/>
-    <tableColumn id="49" name="[gravityModifier]" dataDxfId="145"/>
-    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="144"/>
-    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="143"/>
-    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="142"/>
-    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="141"/>
-    <tableColumn id="6" name="[scaleMenu]" dataDxfId="140"/>
-    <tableColumn id="54" name="[trackingSku]" dataDxfId="139"/>
+    <tableColumn id="1" name="{specialDragonTierDefinitions}" dataDxfId="161"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="160"/>
+    <tableColumn id="3" name="[tier]" dataDxfId="159"/>
+    <tableColumn id="4" name="[specialDragon]" dataDxfId="158"/>
+    <tableColumn id="5" name="[mainProgressionRestriction]" dataDxfId="157"/>
+    <tableColumn id="7" name="[upgradeLevelToUnlock]" dataDxfId="156"/>
+    <tableColumn id="8" name="[defaultSize]" dataDxfId="155"/>
+    <tableColumn id="9" name="[cameraFrameWidthModifier]" dataDxfId="154"/>
+    <tableColumn id="10" name="[health]" dataDxfId="153"/>
+    <tableColumn id="11" name="[healthDrain]" dataDxfId="152"/>
+    <tableColumn id="12" name="[healthDrainSpacePlus]" dataDxfId="151"/>
+    <tableColumn id="13" name="[healthDrainAmpPerSecond]" dataDxfId="150"/>
+    <tableColumn id="14" name="[sessionStartHealthDrainTime]" dataDxfId="149"/>
+    <tableColumn id="15" name="[sessionStartHealthDrainModifier]" dataDxfId="148"/>
+    <tableColumn id="16" name="[scale]" dataDxfId="147"/>
+    <tableColumn id="17" name="[boostMultiplier]" dataDxfId="146"/>
+    <tableColumn id="18" name="[energyBase]" dataDxfId="145"/>
+    <tableColumn id="19" name="[energyDrain]" dataDxfId="144"/>
+    <tableColumn id="20" name="[energyRefillRate]" dataDxfId="143"/>
+    <tableColumn id="21" name="[furyBaseLength]" dataDxfId="142"/>
+    <tableColumn id="22" name="[furyScoreMultiplier]" dataDxfId="141"/>
+    <tableColumn id="23" name="[furyBaseDuration]" dataDxfId="140"/>
+    <tableColumn id="24" name="[furyMax]" dataDxfId="139"/>
+    <tableColumn id="25" name="[scoreTextThresholdMultiplier]" dataDxfId="138"/>
+    <tableColumn id="26" name="[eatSpeedFactor]" dataDxfId="137"/>
+    <tableColumn id="27" name="[maxAlcohol]" dataDxfId="136"/>
+    <tableColumn id="28" name="[alcoholDrain]" dataDxfId="135"/>
+    <tableColumn id="29" name="[gamePrefab]" dataDxfId="134"/>
+    <tableColumn id="30" name="[menuPrefab]" dataDxfId="133"/>
+    <tableColumn id="31" name="[resultsPrefab]" dataDxfId="132"/>
+    <tableColumn id="32" name="[shadowFromDragon]" dataDxfId="131"/>
+    <tableColumn id="33" name="[revealFromDragon]" dataDxfId="130"/>
+    <tableColumn id="34" name="[sizeUpMultiplier]" dataDxfId="129"/>
+    <tableColumn id="35" name="[speedUpMultiplier]" dataDxfId="128"/>
+    <tableColumn id="36" name="[biteUpMultiplier]" dataDxfId="127"/>
+    <tableColumn id="37" name="[invincible]" dataDxfId="126"/>
+    <tableColumn id="38" name="[infiniteBoost]" dataDxfId="125"/>
+    <tableColumn id="39" name="[eatEverything]" dataDxfId="124"/>
+    <tableColumn id="40" name="[modeDuration]" dataDxfId="123"/>
+    <tableColumn id="41" name="[petScale]" dataDxfId="122"/>
+    <tableColumn id="44" name="[statsBarRatio]" dataDxfId="121"/>
+    <tableColumn id="45" name="[furyBarRatio]" dataDxfId="120"/>
+    <tableColumn id="46" name="[force]" dataDxfId="119"/>
+    <tableColumn id="47" name="[mass]" dataDxfId="118"/>
+    <tableColumn id="48" name="[friction]" dataDxfId="117"/>
+    <tableColumn id="49" name="[gravityModifier]" dataDxfId="116"/>
+    <tableColumn id="50" name="[airGravityModifier]" dataDxfId="115"/>
+    <tableColumn id="51" name="[waterGravityModifier]" dataDxfId="114"/>
+    <tableColumn id="52" name="[damageAnimationThreshold]" dataDxfId="113"/>
+    <tableColumn id="53" name="[dotAnimationThreshold]" dataDxfId="112"/>
+    <tableColumn id="6" name="[scaleMenu]" dataDxfId="111"/>
+    <tableColumn id="54" name="[trackingSku]" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC7" totalsRowShown="0" headerRowDxfId="138" dataDxfId="136" headerRowBorderDxfId="137" tableBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B3:AC7" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106">
   <autoFilter ref="B3:AC7"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="134"/>
+    <tableColumn id="1" name="{specialDragonDefinitions}" dataDxfId="105"/>
     <tableColumn id="2" name="[sku]"/>
     <tableColumn id="3" name="[type]"/>
-    <tableColumn id="5" name="[order]" dataDxfId="133"/>
-    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="132"/>
-    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="131"/>
-    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="130"/>
-    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="129"/>
-    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="128"/>
-    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="127"/>
-    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="126"/>
-    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="125"/>
-    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="124"/>
-    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="123"/>
-    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="122"/>
-    <tableColumn id="76" name="[stepPrice]" dataDxfId="121"/>
-    <tableColumn id="77" name="[priceCoefA]" dataDxfId="120"/>
-    <tableColumn id="75" name="[priceCoefB]" dataDxfId="119"/>
-    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="118"/>
-    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="117"/>
-    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="116"/>
-    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="115"/>
-    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="114"/>
-    <tableColumn id="12" name="[tidDesc]" dataDxfId="113"/>
-    <tableColumn id="65" name="[tidName]" dataDxfId="112"/>
-    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="111"/>
-    <tableColumn id="14" name="[mummyDuration]" dataDxfId="110"/>
-    <tableColumn id="11" name="[trackingSku]" dataDxfId="109"/>
+    <tableColumn id="5" name="[order]" dataDxfId="104"/>
+    <tableColumn id="7" name="[unlockPriceGF]" dataDxfId="103"/>
+    <tableColumn id="8" name="[unlockPricePC]" dataDxfId="102"/>
+    <tableColumn id="66" name="[hpBonusSteps]" dataDxfId="101"/>
+    <tableColumn id="69" name="[hpBonusMin]" dataDxfId="100"/>
+    <tableColumn id="70" name="[hpBonusMax]" dataDxfId="99"/>
+    <tableColumn id="72" name="[speedBonusSteps]" dataDxfId="98"/>
+    <tableColumn id="73" name="[speedBonusMin]" dataDxfId="97"/>
+    <tableColumn id="74" name="[speedBonusMax]" dataDxfId="96"/>
+    <tableColumn id="71" name="[boostBonusSteps]" dataDxfId="95"/>
+    <tableColumn id="68" name="[boostBonusMin]" dataDxfId="94"/>
+    <tableColumn id="67" name="[boostBonusMax]" dataDxfId="93"/>
+    <tableColumn id="76" name="[stepPrice]" dataDxfId="92"/>
+    <tableColumn id="77" name="[priceCoefA]" dataDxfId="91"/>
+    <tableColumn id="75" name="[priceCoefB]" dataDxfId="90"/>
+    <tableColumn id="6" name="[energyRequiredToBoost]" dataDxfId="89"/>
+    <tableColumn id="4" name="[energyRestartThreshold]" dataDxfId="88"/>
+    <tableColumn id="10" name="[tidBoostAction]" dataDxfId="87"/>
+    <tableColumn id="9" name="[tidBoostReminder]" dataDxfId="86"/>
+    <tableColumn id="13" name="[petScaleMenu]" dataDxfId="85"/>
+    <tableColumn id="12" name="[tidDesc]" dataDxfId="84"/>
+    <tableColumn id="65" name="[tidName]" dataDxfId="83"/>
+    <tableColumn id="15" name="[mummyHealthFactor]" dataDxfId="82"/>
+    <tableColumn id="14" name="[mummyDuration]" dataDxfId="81"/>
+    <tableColumn id="11" name="[trackingSku]" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:I46" totalsRowShown="0" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:I46" totalsRowShown="0" headerRowBorderDxfId="79" tableBorderDxfId="78" totalsRowBorderDxfId="77">
   <autoFilter ref="B34:I46"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="105"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="104"/>
-    <tableColumn id="3" name="[specialDragon]" dataDxfId="103"/>
-    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="102"/>
-    <tableColumn id="5" name="[icon]" dataDxfId="101">
+    <tableColumn id="1" name="{specialDragonPowerDefinitions}" dataDxfId="76"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="75"/>
+    <tableColumn id="3" name="[specialDragon]" dataDxfId="74"/>
+    <tableColumn id="6" name="[upgradeLevelToUnlock]" dataDxfId="73"/>
+    <tableColumn id="5" name="[icon]" dataDxfId="72">
       <calculatedColumnFormula>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="[tidName]" dataDxfId="100"/>
-    <tableColumn id="7" name="[tidDesc]" dataDxfId="99"/>
+    <tableColumn id="4" name="[tidName]" dataDxfId="71"/>
+    <tableColumn id="7" name="[tidDesc]" dataDxfId="70"/>
     <tableColumn id="8" name="[tidDescShort]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -57927,71 +57927,71 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B52:N60" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B52:N60" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
   <autoFilter ref="B52:N60"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="93"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="92"/>
-    <tableColumn id="3" name="[skin]" dataDxfId="91"/>
-    <tableColumn id="13" name="[body_parts]" dataDxfId="49"/>
-    <tableColumn id="6" name="[dragonSku]" dataDxfId="90"/>
-    <tableColumn id="5" name="[shopOrder]" dataDxfId="0"/>
-    <tableColumn id="4" name="[priceSC]" dataDxfId="89"/>
-    <tableColumn id="7" name="[priceHC]" dataDxfId="88"/>
-    <tableColumn id="8" name="[unlockLevel]" dataDxfId="87"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="86"/>
-    <tableColumn id="10" name="[tidName]" dataDxfId="85"/>
-    <tableColumn id="11" name="[tidDesc]" dataDxfId="84"/>
-    <tableColumn id="12" name="[trackingSku]" dataDxfId="83"/>
+    <tableColumn id="1" name="{specialDisguisesDefinitions}" dataDxfId="64"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="3" name="[skin]" dataDxfId="62"/>
+    <tableColumn id="13" name="[body_parts]" dataDxfId="61"/>
+    <tableColumn id="6" name="[dragonSku]" dataDxfId="60"/>
+    <tableColumn id="5" name="[shopOrder]" dataDxfId="59"/>
+    <tableColumn id="4" name="[priceSC]" dataDxfId="58"/>
+    <tableColumn id="7" name="[priceHC]" dataDxfId="57"/>
+    <tableColumn id="8" name="[unlockLevel]" dataDxfId="56"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="55"/>
+    <tableColumn id="10" name="[tidName]" dataDxfId="54"/>
+    <tableColumn id="11" name="[tidDesc]" dataDxfId="53"/>
+    <tableColumn id="12" name="[trackingSku]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="82" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B3:K6" totalsRowShown="0" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="B3:K6"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{specialMissionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="80"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="79"/>
-    <tableColumn id="7" name="[index]" dataDxfId="78"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="77"/>
-    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="76"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="75"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="74"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="73"/>
-    <tableColumn id="10" name="[color]" dataDxfId="72"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="47"/>
+    <tableColumn id="7" name="[index]" dataDxfId="46"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="45"/>
+    <tableColumn id="9" name="[maxRewardGoldenFragments]" dataDxfId="44"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="43"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="42"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="41"/>
+    <tableColumn id="10" name="[color]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table13303132" displayName="Table13303132" ref="B11:F15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B11:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="66"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="4" name="[tier]" dataDxfId="64"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="63"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="62"/>
+    <tableColumn id="1" name="{missionSpecialDragonModifiersDefinitions}" dataDxfId="34"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="4" name="[tier]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:G72" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:G72" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A17:G72"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{leaguesRewardsDefinitions}" dataDxfId="56"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
-    <tableColumn id="3" name="[group]" dataDxfId="54"/>
-    <tableColumn id="4" name="[type]" dataDxfId="53"/>
-    <tableColumn id="5" name="[amount]" dataDxfId="52"/>
-    <tableColumn id="6" name="[target]" dataDxfId="51"/>
-    <tableColumn id="7" name="[rsku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{leaguesRewardsDefinitions}" dataDxfId="22"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
+    <tableColumn id="3" name="[group]" dataDxfId="20"/>
+    <tableColumn id="4" name="[type]" dataDxfId="19"/>
+    <tableColumn id="5" name="[amount]" dataDxfId="18"/>
+    <tableColumn id="6" name="[target]" dataDxfId="17"/>
+    <tableColumn id="7" name="[rsku]" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -58266,7 +58266,7 @@
   <dimension ref="A1:BA68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62346,91 +62346,91 @@
     <mergeCell ref="J29:O29"/>
   </mergeCells>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="48" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D7">
-    <cfRule type="duplicateValues" dxfId="47" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="duplicateValues" dxfId="46" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="duplicateValues" dxfId="45" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C43">
-    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C24">
-    <cfRule type="duplicateValues" dxfId="43" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="duplicateValues" dxfId="42" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:C57">
-    <cfRule type="duplicateValues" dxfId="41" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C68">
-    <cfRule type="duplicateValues" dxfId="40" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC7">
-    <cfRule type="duplicateValues" dxfId="39" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA22">
-    <cfRule type="duplicateValues" dxfId="38" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA23">
-    <cfRule type="duplicateValues" dxfId="37" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA24">
-    <cfRule type="duplicateValues" dxfId="36" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="duplicateValues" dxfId="35" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D7">
-    <cfRule type="duplicateValues" dxfId="34" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC7">
-    <cfRule type="duplicateValues" dxfId="33" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C28">
-    <cfRule type="duplicateValues" dxfId="32" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:C46">
-    <cfRule type="duplicateValues" dxfId="31" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="duplicateValues" dxfId="29" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D13:D28">
@@ -62730,7 +62730,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
-    <cfRule type="duplicateValues" dxfId="28" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -64410,10 +64410,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:B72">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C13">
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -65411,22 +65411,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -66432,22 +66432,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67446,22 +67446,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -68469,22 +68469,22 @@
     <mergeCell ref="E3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>E13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$E$13&gt;$L$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$E$14&gt;$T$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E$15&gt;$AB$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[TEXTS] finals for 1.26 Last changes in Ice dragon balancing
Former-commit-id: 259602de6a7178ec68fd08e7763f3c75a50c72dc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -2181,7 +2181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2751,109 +2751,19 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2912,6 +2822,81 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12610,16 +12595,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12890,16 +12875,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13678,6 +13663,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14320,6 +14306,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14641,6 +14628,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14962,6 +14950,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15270,6 +15259,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15886,6 +15876,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17129,6 +17120,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17241,6 +17233,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18485,6 +18478,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18591,6 +18585,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18874,16 +18869,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19154,16 +19149,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19836,6 +19831,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19942,6 +19938,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20263,6 +20260,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20905,6 +20903,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20959,16 +20958,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21002,16 +21001,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.6</c:v>
+                  <c:v>7.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6</c:v>
+                  <c:v>8.9000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.8999999999999986</c:v>
+                  <c:v>9.1000000000000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21226,6 +21225,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21534,6 +21534,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21842,6 +21843,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21934,7 +21936,7 @@
                   <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22150,6 +22152,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23390,6 +23393,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23502,6 +23506,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24743,6 +24748,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24849,6 +24855,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25129,16 +25136,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25409,16 +25416,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26091,6 +26098,7 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29177,16 +29185,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -29457,16 +29465,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34155,16 +34163,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17.5</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.5</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.2</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34435,16 +34443,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.9</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.6</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -58265,8 +58273,8 @@
   </sheetPr>
   <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58481,7 +58489,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="43">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H4" s="50">
         <v>20</v>
@@ -60012,7 +60020,7 @@
         <v>10</v>
       </c>
       <c r="X19" s="111">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="Y19" s="99">
         <v>4</v>
@@ -60166,7 +60174,7 @@
         <v>9</v>
       </c>
       <c r="X20" s="111">
-        <v>500000</v>
+        <v>600000</v>
       </c>
       <c r="Y20" s="99">
         <v>5</v>
@@ -60826,7 +60834,7 @@
       <c r="AM24" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="AN24" s="250">
+      <c r="AN24" s="223">
         <v>10</v>
       </c>
       <c r="AO24" s="121">
@@ -60889,67 +60897,67 @@
       <c r="G25" s="209">
         <v>0</v>
       </c>
-      <c r="H25" s="219">
+      <c r="H25" s="243">
         <v>3</v>
       </c>
-      <c r="I25" s="220">
+      <c r="I25" s="244">
         <v>-2</v>
       </c>
-      <c r="J25" s="221">
+      <c r="J25" s="247">
         <v>75</v>
       </c>
-      <c r="K25" s="222">
-        <v>2.7</v>
-      </c>
-      <c r="L25" s="222">
+      <c r="K25" s="248">
+        <v>2.6</v>
+      </c>
+      <c r="L25" s="248">
         <v>0</v>
       </c>
-      <c r="M25" s="222">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="N25" s="222">
+      <c r="M25" s="248">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="N25" s="248">
         <v>20</v>
       </c>
-      <c r="O25" s="222">
+      <c r="O25" s="248">
         <v>0.5</v>
       </c>
-      <c r="P25" s="223">
+      <c r="P25" s="251">
         <v>1</v>
       </c>
-      <c r="Q25" s="220">
-        <v>1.3</v>
-      </c>
-      <c r="R25" s="222">
+      <c r="Q25" s="244">
+        <v>1.45</v>
+      </c>
+      <c r="R25" s="248">
         <v>100</v>
       </c>
-      <c r="S25" s="222">
+      <c r="S25" s="248">
         <v>9</v>
       </c>
-      <c r="T25" s="224">
+      <c r="T25" s="252">
         <v>7</v>
       </c>
-      <c r="U25" s="220">
+      <c r="U25" s="244">
         <v>11</v>
       </c>
-      <c r="V25" s="222">
+      <c r="V25" s="248">
         <v>3</v>
       </c>
-      <c r="W25" s="222">
+      <c r="W25" s="248">
         <v>10</v>
       </c>
-      <c r="X25" s="224">
-        <v>40000</v>
-      </c>
-      <c r="Y25" s="225">
+      <c r="X25" s="252">
+        <v>25000</v>
+      </c>
+      <c r="Y25" s="255">
         <v>2</v>
       </c>
-      <c r="Z25" s="223">
+      <c r="Z25" s="251">
         <v>0.13</v>
       </c>
-      <c r="AA25" s="223">
+      <c r="AA25" s="251">
         <v>0</v>
       </c>
-      <c r="AB25" s="225">
+      <c r="AB25" s="255">
         <v>12</v>
       </c>
       <c r="AC25" s="210" t="s">
@@ -60961,66 +60969,66 @@
       <c r="AE25" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF25" s="226"/>
-      <c r="AG25" s="227"/>
-      <c r="AH25" s="228">
+      <c r="AF25" s="219"/>
+      <c r="AG25" s="220"/>
+      <c r="AH25" s="257">
         <v>1.7</v>
       </c>
-      <c r="AI25" s="226">
+      <c r="AI25" s="210">
         <v>2</v>
       </c>
-      <c r="AJ25" s="226">
+      <c r="AJ25" s="210">
         <v>2</v>
       </c>
-      <c r="AK25" s="226" t="b">
+      <c r="AK25" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AL25" s="226" t="b">
+      <c r="AL25" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AM25" s="226" t="b">
+      <c r="AM25" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN25" s="229">
+      <c r="AN25" s="258">
         <v>10</v>
       </c>
-      <c r="AO25" s="251">
+      <c r="AO25" s="122">
         <v>0.55999999999999994</v>
       </c>
-      <c r="AP25" s="252">
+      <c r="AP25" s="132">
         <v>2E-3</v>
       </c>
-      <c r="AQ25" s="253">
+      <c r="AQ25" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR25" s="230">
-        <v>260</v>
-      </c>
-      <c r="AS25" s="231">
+      <c r="AR25" s="261">
+        <v>310</v>
+      </c>
+      <c r="AS25" s="188">
         <v>2.5</v>
       </c>
-      <c r="AT25" s="231">
+      <c r="AT25" s="188">
         <v>9.5</v>
       </c>
-      <c r="AU25" s="231">
+      <c r="AU25" s="188">
         <v>1.7</v>
       </c>
-      <c r="AV25" s="231">
+      <c r="AV25" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW25" s="232">
+      <c r="AW25" s="262">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX25" s="231">
+      <c r="AX25" s="188">
         <v>0</v>
       </c>
-      <c r="AY25" s="231">
+      <c r="AY25" s="188">
         <v>8</v>
       </c>
-      <c r="AZ25" s="231">
+      <c r="AZ25" s="188">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BA25" s="233" t="s">
+      <c r="BA25" s="263" t="s">
         <v>395</v>
       </c>
     </row>
@@ -61044,67 +61052,67 @@
       <c r="G26" s="209">
         <v>10</v>
       </c>
-      <c r="H26" s="219">
+      <c r="H26" s="243">
         <v>8</v>
       </c>
-      <c r="I26" s="220">
+      <c r="I26" s="244">
         <v>0</v>
       </c>
-      <c r="J26" s="221">
+      <c r="J26" s="247">
         <v>120</v>
       </c>
-      <c r="K26" s="222">
-        <v>3.4</v>
-      </c>
-      <c r="L26" s="222">
+      <c r="K26" s="248">
+        <v>3.3</v>
+      </c>
+      <c r="L26" s="248">
         <v>0</v>
       </c>
-      <c r="M26" s="222">
-        <v>0.01</v>
-      </c>
-      <c r="N26" s="222">
+      <c r="M26" s="248">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N26" s="248">
         <v>20</v>
       </c>
-      <c r="O26" s="222">
+      <c r="O26" s="248">
         <v>0.6</v>
       </c>
-      <c r="P26" s="223">
+      <c r="P26" s="251">
         <v>1.4</v>
       </c>
-      <c r="Q26" s="220">
-        <v>1.3</v>
-      </c>
-      <c r="R26" s="222">
+      <c r="Q26" s="244">
+        <v>1.45</v>
+      </c>
+      <c r="R26" s="248">
         <v>120</v>
       </c>
-      <c r="S26" s="222">
+      <c r="S26" s="248">
         <v>10</v>
       </c>
-      <c r="T26" s="224">
+      <c r="T26" s="252">
         <v>7</v>
       </c>
-      <c r="U26" s="220">
+      <c r="U26" s="244">
         <v>13</v>
       </c>
-      <c r="V26" s="222">
+      <c r="V26" s="248">
         <v>4</v>
       </c>
-      <c r="W26" s="222">
+      <c r="W26" s="248">
         <v>11</v>
       </c>
-      <c r="X26" s="224">
-        <v>120000</v>
-      </c>
-      <c r="Y26" s="225">
+      <c r="X26" s="252">
+        <v>90000</v>
+      </c>
+      <c r="Y26" s="255">
         <v>3</v>
       </c>
-      <c r="Z26" s="223">
+      <c r="Z26" s="251">
         <v>0.08</v>
       </c>
-      <c r="AA26" s="223">
+      <c r="AA26" s="251">
         <v>0</v>
       </c>
-      <c r="AB26" s="225">
+      <c r="AB26" s="255">
         <v>12</v>
       </c>
       <c r="AC26" s="210" t="s">
@@ -61116,66 +61124,66 @@
       <c r="AE26" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF26" s="226"/>
-      <c r="AG26" s="227"/>
-      <c r="AH26" s="228">
+      <c r="AF26" s="219"/>
+      <c r="AG26" s="220"/>
+      <c r="AH26" s="257">
         <v>1.6</v>
       </c>
-      <c r="AI26" s="226">
+      <c r="AI26" s="210">
         <v>2</v>
       </c>
-      <c r="AJ26" s="226">
+      <c r="AJ26" s="210">
         <v>2</v>
       </c>
-      <c r="AK26" s="226" t="b">
+      <c r="AK26" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AL26" s="226" t="b">
+      <c r="AL26" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AM26" s="226" t="b">
+      <c r="AM26" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN26" s="229">
+      <c r="AN26" s="258">
         <v>10</v>
       </c>
-      <c r="AO26" s="251">
+      <c r="AO26" s="122">
         <v>0.7</v>
       </c>
-      <c r="AP26" s="252">
+      <c r="AP26" s="132">
         <v>1.8E-3</v>
       </c>
-      <c r="AQ26" s="253">
+      <c r="AQ26" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR26" s="230">
-        <v>275</v>
-      </c>
-      <c r="AS26" s="231">
+      <c r="AR26" s="261">
+        <v>325</v>
+      </c>
+      <c r="AS26" s="188">
         <v>2.5</v>
       </c>
-      <c r="AT26" s="231">
+      <c r="AT26" s="188">
         <v>9.5</v>
       </c>
-      <c r="AU26" s="231">
+      <c r="AU26" s="188">
         <v>1.7</v>
       </c>
-      <c r="AV26" s="231">
+      <c r="AV26" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW26" s="232">
+      <c r="AW26" s="262">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX26" s="231">
+      <c r="AX26" s="188">
         <v>9</v>
       </c>
-      <c r="AY26" s="231">
+      <c r="AY26" s="188">
         <v>8</v>
       </c>
-      <c r="AZ26" s="231">
+      <c r="AZ26" s="188">
         <v>1.3</v>
       </c>
-      <c r="BA26" s="234" t="s">
+      <c r="BA26" s="264" t="s">
         <v>396</v>
       </c>
     </row>
@@ -61199,67 +61207,67 @@
       <c r="G27" s="209">
         <v>20</v>
       </c>
-      <c r="H27" s="219">
+      <c r="H27" s="243">
         <v>17</v>
       </c>
-      <c r="I27" s="220">
+      <c r="I27" s="244">
         <v>0</v>
       </c>
-      <c r="J27" s="221">
+      <c r="J27" s="247">
         <v>160</v>
       </c>
-      <c r="K27" s="222">
-        <v>4.3</v>
-      </c>
-      <c r="L27" s="222">
+      <c r="K27" s="248">
+        <v>4.2</v>
+      </c>
+      <c r="L27" s="248">
         <v>0</v>
       </c>
-      <c r="M27" s="222">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="N27" s="222">
+      <c r="M27" s="248">
+        <v>1.2E-2</v>
+      </c>
+      <c r="N27" s="248">
         <v>15</v>
       </c>
-      <c r="O27" s="222">
+      <c r="O27" s="248">
         <v>0.7</v>
       </c>
-      <c r="P27" s="223">
+      <c r="P27" s="251">
         <v>1.8</v>
       </c>
-      <c r="Q27" s="220">
-        <v>1.3</v>
-      </c>
-      <c r="R27" s="222">
+      <c r="Q27" s="244">
+        <v>1.45</v>
+      </c>
+      <c r="R27" s="248">
         <v>140</v>
       </c>
-      <c r="S27" s="222">
+      <c r="S27" s="248">
         <v>12</v>
       </c>
-      <c r="T27" s="224">
+      <c r="T27" s="252">
         <v>7</v>
       </c>
-      <c r="U27" s="220">
+      <c r="U27" s="244">
         <v>14</v>
       </c>
-      <c r="V27" s="222">
+      <c r="V27" s="248">
         <v>5</v>
       </c>
-      <c r="W27" s="222">
+      <c r="W27" s="248">
         <v>11</v>
       </c>
-      <c r="X27" s="224">
-        <v>250000</v>
-      </c>
-      <c r="Y27" s="225">
+      <c r="X27" s="252">
+        <v>200000</v>
+      </c>
+      <c r="Y27" s="255">
         <v>4</v>
       </c>
-      <c r="Z27" s="223">
+      <c r="Z27" s="251">
         <v>0.05</v>
       </c>
-      <c r="AA27" s="223">
+      <c r="AA27" s="251">
         <v>0</v>
       </c>
-      <c r="AB27" s="225">
+      <c r="AB27" s="255">
         <v>12</v>
       </c>
       <c r="AC27" s="210" t="s">
@@ -61271,66 +61279,66 @@
       <c r="AE27" s="211" t="s">
         <v>401</v>
       </c>
-      <c r="AF27" s="226"/>
-      <c r="AG27" s="227"/>
-      <c r="AH27" s="228">
+      <c r="AF27" s="219"/>
+      <c r="AG27" s="220"/>
+      <c r="AH27" s="257">
         <v>1.5</v>
       </c>
-      <c r="AI27" s="226">
+      <c r="AI27" s="210">
         <v>2</v>
       </c>
-      <c r="AJ27" s="226">
+      <c r="AJ27" s="210">
         <v>2</v>
       </c>
-      <c r="AK27" s="226" t="b">
+      <c r="AK27" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AL27" s="226" t="b">
+      <c r="AL27" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AM27" s="226" t="b">
+      <c r="AM27" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN27" s="229">
+      <c r="AN27" s="258">
         <v>10</v>
       </c>
-      <c r="AO27" s="251">
+      <c r="AO27" s="122">
         <v>0.7</v>
       </c>
-      <c r="AP27" s="252">
+      <c r="AP27" s="132">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AQ27" s="253">
+      <c r="AQ27" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR27" s="230">
-        <v>300</v>
-      </c>
-      <c r="AS27" s="231">
+      <c r="AR27" s="261">
+        <v>350</v>
+      </c>
+      <c r="AS27" s="188">
         <v>2.5</v>
       </c>
-      <c r="AT27" s="231">
+      <c r="AT27" s="188">
         <v>9.5</v>
       </c>
-      <c r="AU27" s="231">
+      <c r="AU27" s="188">
         <v>1.7</v>
       </c>
-      <c r="AV27" s="231">
+      <c r="AV27" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW27" s="232">
+      <c r="AW27" s="262">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX27" s="231">
+      <c r="AX27" s="188">
         <v>45</v>
       </c>
-      <c r="AY27" s="231">
+      <c r="AY27" s="188">
         <v>15</v>
       </c>
-      <c r="AZ27" s="231">
+      <c r="AZ27" s="188">
         <v>1.5</v>
       </c>
-      <c r="BA27" s="234" t="s">
+      <c r="BA27" s="264" t="s">
         <v>397</v>
       </c>
     </row>
@@ -61353,70 +61361,70 @@
       <c r="F28" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="249">
+      <c r="G28" s="222">
         <v>30</v>
       </c>
-      <c r="H28" s="235">
+      <c r="H28" s="245">
         <v>25</v>
       </c>
-      <c r="I28" s="236">
+      <c r="I28" s="246">
         <v>0</v>
       </c>
-      <c r="J28" s="237">
+      <c r="J28" s="249">
         <v>200</v>
       </c>
-      <c r="K28" s="238">
+      <c r="K28" s="250">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L28" s="250">
+        <v>0</v>
+      </c>
+      <c r="M28" s="250">
+        <v>1.52E-2</v>
+      </c>
+      <c r="N28" s="250">
+        <v>10</v>
+      </c>
+      <c r="O28" s="250">
+        <v>0.8</v>
+      </c>
+      <c r="P28" s="253">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q28" s="246">
+        <v>1.45</v>
+      </c>
+      <c r="R28" s="250">
+        <v>160</v>
+      </c>
+      <c r="S28" s="250">
+        <v>14</v>
+      </c>
+      <c r="T28" s="254">
+        <v>7</v>
+      </c>
+      <c r="U28" s="246">
+        <v>15</v>
+      </c>
+      <c r="V28" s="250">
+        <v>6</v>
+      </c>
+      <c r="W28" s="250">
+        <v>11</v>
+      </c>
+      <c r="X28" s="254">
+        <v>400000</v>
+      </c>
+      <c r="Y28" s="256">
         <v>5</v>
       </c>
-      <c r="L28" s="238">
+      <c r="Z28" s="253">
+        <v>0.04</v>
+      </c>
+      <c r="AA28" s="253">
         <v>0</v>
       </c>
-      <c r="M28" s="238">
-        <v>1.5599999999999999E-2</v>
-      </c>
-      <c r="N28" s="238">
-        <v>10</v>
-      </c>
-      <c r="O28" s="238">
-        <v>0.8</v>
-      </c>
-      <c r="P28" s="239">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q28" s="236">
-        <v>1.2</v>
-      </c>
-      <c r="R28" s="238">
-        <v>160</v>
-      </c>
-      <c r="S28" s="238">
-        <v>14</v>
-      </c>
-      <c r="T28" s="240">
-        <v>7</v>
-      </c>
-      <c r="U28" s="236">
-        <v>15</v>
-      </c>
-      <c r="V28" s="238">
-        <v>6</v>
-      </c>
-      <c r="W28" s="238">
-        <v>11</v>
-      </c>
-      <c r="X28" s="240">
-        <v>550000</v>
-      </c>
-      <c r="Y28" s="241">
-        <v>5</v>
-      </c>
-      <c r="Z28" s="239">
-        <v>0.04</v>
-      </c>
-      <c r="AA28" s="239">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="241">
+      <c r="AB28" s="256">
         <v>12</v>
       </c>
       <c r="AC28" s="217" t="s">
@@ -61428,66 +61436,66 @@
       <c r="AE28" s="218" t="s">
         <v>401</v>
       </c>
-      <c r="AF28" s="226"/>
-      <c r="AG28" s="242"/>
-      <c r="AH28" s="243">
+      <c r="AF28" s="219"/>
+      <c r="AG28" s="221"/>
+      <c r="AH28" s="259">
         <v>1.4</v>
       </c>
-      <c r="AI28" s="226">
+      <c r="AI28" s="210">
         <v>2</v>
       </c>
-      <c r="AJ28" s="226">
+      <c r="AJ28" s="210">
         <v>2</v>
       </c>
-      <c r="AK28" s="226" t="b">
+      <c r="AK28" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AL28" s="226" t="b">
+      <c r="AL28" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AM28" s="226" t="b">
+      <c r="AM28" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN28" s="244">
+      <c r="AN28" s="260">
         <v>10</v>
       </c>
-      <c r="AO28" s="251">
+      <c r="AO28" s="122">
         <v>0.7</v>
       </c>
-      <c r="AP28" s="252">
+      <c r="AP28" s="132">
         <v>1.5E-3</v>
       </c>
-      <c r="AQ28" s="253">
+      <c r="AQ28" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR28" s="245">
-        <v>315</v>
-      </c>
-      <c r="AS28" s="246">
+      <c r="AR28" s="265">
+        <v>365</v>
+      </c>
+      <c r="AS28" s="191">
         <v>2.5</v>
       </c>
-      <c r="AT28" s="246">
+      <c r="AT28" s="191">
         <v>9.5</v>
       </c>
-      <c r="AU28" s="246">
+      <c r="AU28" s="191">
         <v>1.7</v>
       </c>
-      <c r="AV28" s="246">
+      <c r="AV28" s="191">
         <v>1.2</v>
       </c>
-      <c r="AW28" s="247">
+      <c r="AW28" s="266">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AX28" s="246">
+      <c r="AX28" s="191">
         <v>59</v>
       </c>
-      <c r="AY28" s="246">
+      <c r="AY28" s="191">
         <v>15</v>
       </c>
-      <c r="AZ28" s="246">
+      <c r="AZ28" s="191">
         <v>1.7</v>
       </c>
-      <c r="BA28" s="248" t="s">
+      <c r="BA28" s="267" t="s">
         <v>398</v>
       </c>
     </row>
@@ -61498,44 +61506,44 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="266" t="s">
+      <c r="H29" s="236" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="267"/>
-      <c r="J29" s="268" t="s">
+      <c r="I29" s="237"/>
+      <c r="J29" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="269"/>
-      <c r="L29" s="269"/>
-      <c r="M29" s="269"/>
-      <c r="N29" s="269"/>
-      <c r="O29" s="270"/>
+      <c r="K29" s="239"/>
+      <c r="L29" s="239"/>
+      <c r="M29" s="239"/>
+      <c r="N29" s="239"/>
+      <c r="O29" s="240"/>
       <c r="P29" s="72"/>
-      <c r="Q29" s="262" t="s">
+      <c r="Q29" s="232" t="s">
         <v>126</v>
       </c>
-      <c r="R29" s="263"/>
-      <c r="S29" s="263"/>
-      <c r="T29" s="263"/>
-      <c r="U29" s="264" t="s">
+      <c r="R29" s="233"/>
+      <c r="S29" s="233"/>
+      <c r="T29" s="233"/>
+      <c r="U29" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="V29" s="265"/>
-      <c r="W29" s="265"/>
-      <c r="X29" s="265"/>
+      <c r="V29" s="235"/>
+      <c r="W29" s="235"/>
+      <c r="X29" s="235"/>
       <c r="Y29" s="20"/>
       <c r="Z29" s="20"/>
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
-      <c r="AH29" s="259" t="s">
+      <c r="AH29" s="229" t="s">
         <v>127</v>
       </c>
-      <c r="AI29" s="260"/>
-      <c r="AJ29" s="260"/>
-      <c r="AK29" s="260"/>
-      <c r="AL29" s="260"/>
-      <c r="AM29" s="260"/>
-      <c r="AN29" s="261"/>
+      <c r="AI29" s="230"/>
+      <c r="AJ29" s="230"/>
+      <c r="AK29" s="230"/>
+      <c r="AL29" s="230"/>
+      <c r="AM29" s="230"/>
+      <c r="AN29" s="231"/>
     </row>
     <row r="31" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AZ31" t="s">
@@ -61831,7 +61839,7 @@
       <c r="C44" s="56" t="s">
         <v>402</v>
       </c>
-      <c r="D44" s="254" t="s">
+      <c r="D44" s="224" t="s">
         <v>391</v>
       </c>
       <c r="E44" s="57">
@@ -61858,7 +61866,7 @@
       <c r="C45" s="56" t="s">
         <v>403</v>
       </c>
-      <c r="D45" s="254" t="s">
+      <c r="D45" s="224" t="s">
         <v>391</v>
       </c>
       <c r="E45" s="57">
@@ -61879,13 +61887,13 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="255" t="s">
+      <c r="B46" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C46" s="60" t="s">
         <v>404</v>
       </c>
-      <c r="D46" s="256" t="s">
+      <c r="D46" s="226" t="s">
         <v>391</v>
       </c>
       <c r="E46" s="61">
@@ -61895,13 +61903,13 @@
         <f>CONCATENATE("icon_",Table1[[#This Row],['[sku']]])</f>
         <v>icon_ice_power_3</v>
       </c>
-      <c r="G46" s="257" t="s">
+      <c r="G46" s="227" t="s">
         <v>407</v>
       </c>
       <c r="H46" s="177" t="s">
         <v>410</v>
       </c>
-      <c r="I46" s="257" t="s">
+      <c r="I46" s="227" t="s">
         <v>407</v>
       </c>
     </row>
@@ -62113,162 +62121,162 @@
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="255" t="s">
+      <c r="B57" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="60" t="s">
         <v>411</v>
       </c>
-      <c r="D57" s="256" t="s">
+      <c r="D57" s="226" t="s">
         <v>411</v>
       </c>
-      <c r="E57" s="256"/>
+      <c r="E57" s="226"/>
       <c r="F57" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="G57" s="258">
+      <c r="G57" s="228">
         <v>0</v>
       </c>
-      <c r="H57" s="258">
+      <c r="H57" s="228">
         <v>0</v>
       </c>
-      <c r="I57" s="258">
+      <c r="I57" s="228">
         <v>0</v>
       </c>
-      <c r="J57" s="258">
+      <c r="J57" s="228">
         <v>0</v>
       </c>
-      <c r="K57" s="258" t="s">
+      <c r="K57" s="228" t="s">
         <v>182</v>
       </c>
-      <c r="L57" s="258" t="s">
+      <c r="L57" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="M57" s="258" t="s">
+      <c r="M57" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="N57" s="258" t="s">
+      <c r="N57" s="228" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="255" t="s">
+      <c r="B58" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C58" s="60" t="s">
         <v>418</v>
       </c>
-      <c r="D58" s="256" t="s">
+      <c r="D58" s="226" t="s">
         <v>411</v>
       </c>
-      <c r="E58" s="256"/>
+      <c r="E58" s="226"/>
       <c r="F58" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="G58" s="258">
+      <c r="G58" s="228">
         <v>0</v>
       </c>
-      <c r="H58" s="258">
+      <c r="H58" s="228">
         <v>0</v>
       </c>
-      <c r="I58" s="258">
+      <c r="I58" s="228">
         <v>0</v>
       </c>
-      <c r="J58" s="258">
+      <c r="J58" s="228">
         <v>5</v>
       </c>
-      <c r="K58" s="258" t="s">
+      <c r="K58" s="228" t="s">
         <v>182</v>
       </c>
-      <c r="L58" s="258" t="s">
+      <c r="L58" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="M58" s="258" t="s">
+      <c r="M58" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="N58" s="258" t="s">
+      <c r="N58" s="228" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="255" t="s">
+      <c r="B59" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C59" s="60" t="s">
         <v>419</v>
       </c>
-      <c r="D59" s="256" t="s">
+      <c r="D59" s="226" t="s">
         <v>411</v>
       </c>
-      <c r="E59" s="256" t="s">
+      <c r="E59" s="226" t="s">
         <v>421</v>
       </c>
       <c r="F59" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="G59" s="258">
+      <c r="G59" s="228">
         <v>0</v>
       </c>
-      <c r="H59" s="258">
+      <c r="H59" s="228">
         <v>0</v>
       </c>
-      <c r="I59" s="258">
+      <c r="I59" s="228">
         <v>0</v>
       </c>
-      <c r="J59" s="258">
+      <c r="J59" s="228">
         <v>15</v>
       </c>
-      <c r="K59" s="258" t="s">
+      <c r="K59" s="228" t="s">
         <v>182</v>
       </c>
-      <c r="L59" s="258" t="s">
+      <c r="L59" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="M59" s="258" t="s">
+      <c r="M59" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="N59" s="258" t="s">
+      <c r="N59" s="228" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="255" t="s">
+      <c r="B60" s="225" t="s">
         <v>2</v>
       </c>
       <c r="C60" s="60" t="s">
         <v>420</v>
       </c>
-      <c r="D60" s="256" t="s">
+      <c r="D60" s="226" t="s">
         <v>411</v>
       </c>
-      <c r="E60" s="256" t="s">
+      <c r="E60" s="226" t="s">
         <v>422</v>
       </c>
       <c r="F60" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="G60" s="258">
+      <c r="G60" s="228">
         <v>0</v>
       </c>
-      <c r="H60" s="258">
+      <c r="H60" s="228">
         <v>0</v>
       </c>
-      <c r="I60" s="258">
+      <c r="I60" s="228">
         <v>0</v>
       </c>
-      <c r="J60" s="258">
+      <c r="J60" s="228">
         <v>25</v>
       </c>
-      <c r="K60" s="258" t="s">
+      <c r="K60" s="228" t="s">
         <v>182</v>
       </c>
-      <c r="L60" s="258" t="s">
+      <c r="L60" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="M60" s="258" t="s">
+      <c r="M60" s="228" t="s">
         <v>413</v>
       </c>
-      <c r="N60" s="258" t="s">
+      <c r="N60" s="228" t="s">
         <v>412</v>
       </c>
     </row>
@@ -62497,8 +62505,8 @@
       <c r="D2" s="137"/>
       <c r="E2" s="137"/>
       <c r="F2" s="138"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
+      <c r="G2" s="241"/>
+      <c r="H2" s="241"/>
       <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -64449,12 +64457,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="272" t="s">
+      <c r="E3" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
+      <c r="F3" s="242"/>
+      <c r="G3" s="242"/>
+      <c r="H3" s="242"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -65463,12 +65471,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="272" t="s">
+      <c r="E3" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
+      <c r="F3" s="242"/>
+      <c r="G3" s="242"/>
+      <c r="H3" s="242"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -66484,12 +66492,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="272" t="s">
+      <c r="E3" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
+      <c r="F3" s="242"/>
+      <c r="G3" s="242"/>
+      <c r="H3" s="242"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -67475,8 +67483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67498,12 +67506,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="272" t="s">
+      <c r="E3" s="242" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="272"/>
-      <c r="H3" s="272"/>
+      <c r="F3" s="242"/>
+      <c r="G3" s="242"/>
+      <c r="H3" s="242"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -67643,16 +67651,16 @@
         <v>104</v>
       </c>
       <c r="E7" s="74">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="F7" s="74">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="G7" s="74">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="H7" s="74">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="J7" t="s">
         <v>390</v>
@@ -67829,19 +67837,19 @@
       </c>
       <c r="AA12">
         <f>ROUND((E7/'special dragons'!AT17)/'special dragons'!AS17,1)</f>
-        <v>10.9</v>
+        <v>13.1</v>
       </c>
       <c r="AB12">
         <f>ROUND(((E7+E7*(AB6/100))/'special dragons'!AT17)/'special dragons'!AS17,1)</f>
-        <v>17.5</v>
+        <v>20.9</v>
       </c>
       <c r="AC12">
         <f>AB12-AA12</f>
-        <v>6.6</v>
+        <v>7.7999999999999989</v>
       </c>
       <c r="AD12">
         <f>(AA12*$AB$7)/100</f>
-        <v>0.32700000000000001</v>
+        <v>0.39299999999999996</v>
       </c>
     </row>
     <row r="13" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -67905,19 +67913,19 @@
       </c>
       <c r="AA13">
         <f>ROUND((F7/'special dragons'!AT18)/'special dragons'!AS18,1)</f>
-        <v>11.6</v>
+        <v>13.7</v>
       </c>
       <c r="AB13">
         <f>ROUND(((F7+F7*(AB6/100))/'special dragons'!AT18)/'special dragons'!AS18,1)</f>
-        <v>18.5</v>
+        <v>21.9</v>
       </c>
       <c r="AC13">
         <f>AB13-AA13</f>
-        <v>6.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AD13">
         <f t="shared" ref="AD13:AD15" si="2">(AA13*$AB$7)/100</f>
-        <v>0.34799999999999998</v>
+        <v>0.41099999999999992</v>
       </c>
     </row>
     <row r="14" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -67981,19 +67989,19 @@
       </c>
       <c r="AA14">
         <f>ROUND((G7/'special dragons'!AT19)/'special dragons'!AS19,1)</f>
-        <v>12.6</v>
+        <v>14.7</v>
       </c>
       <c r="AB14">
         <f>ROUND(((G7+G7*(AB6/100))/'special dragons'!AT19)/'special dragons'!AS19,1)</f>
-        <v>20.2</v>
+        <v>23.6</v>
       </c>
       <c r="AC14">
         <f>AB14-AA14</f>
-        <v>7.6</v>
+        <v>8.9000000000000021</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>0.37799999999999995</v>
+        <v>0.44099999999999995</v>
       </c>
     </row>
     <row r="15" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -68012,7 +68020,7 @@
       </c>
       <c r="H15" s="69">
         <f ca="1">ROUND(((INDIRECT(ADDRESS(7,4+E11)) + (INDIRECT(ADDRESS(7,4+E11)) *(AB7/100) *E15))/INDIRECT(ADDRESS(24+E11,46,1,1,"special dragons")))/INDIRECT(ADDRESS(24+E11,45,1,1,"special dragons")),1)</f>
-        <v>10.9</v>
+        <v>13.1</v>
       </c>
       <c r="J15" s="63" t="s">
         <v>118</v>
@@ -68057,19 +68065,19 @@
       </c>
       <c r="AA15">
         <f>ROUND((H7/'special dragons'!AT20)/'special dragons'!AS20,1)</f>
-        <v>13.3</v>
+        <v>15.2</v>
       </c>
       <c r="AB15">
         <f>ROUND(((H7+H7*(AB6/100))/'special dragons'!AT20)/'special dragons'!AS20,1)</f>
-        <v>21.2</v>
+        <v>24.3</v>
       </c>
       <c r="AC15">
         <f>AB15-AA15</f>
-        <v>7.8999999999999986</v>
+        <v>9.1000000000000014</v>
       </c>
       <c r="AD15">
         <f t="shared" si="2"/>
-        <v>0.39900000000000008</v>
+        <v>0.45599999999999996</v>
       </c>
     </row>
     <row r="16" spans="3:30" x14ac:dyDescent="0.25">
@@ -68805,7 +68813,7 @@
       </c>
       <c r="AD9">
         <f ca="1">'Ice Dragon'!$H$15</f>
-        <v>10.9</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="15" spans="5:32" x14ac:dyDescent="0.25">
@@ -69316,19 +69324,19 @@
       </c>
       <c r="AC22">
         <f>'Ice Dragon'!AB12</f>
-        <v>17.5</v>
+        <v>20.9</v>
       </c>
       <c r="AD22">
         <f>'Ice Dragon'!AB13</f>
-        <v>18.5</v>
+        <v>21.9</v>
       </c>
       <c r="AE22">
         <f>'Ice Dragon'!AB14</f>
-        <v>20.2</v>
+        <v>23.6</v>
       </c>
       <c r="AF22">
         <f>'Ice Dragon'!AB15</f>
-        <v>21.2</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="23" spans="5:32" x14ac:dyDescent="0.25">
@@ -69384,19 +69392,19 @@
       </c>
       <c r="AC23">
         <f>'Ice Dragon'!AA12</f>
-        <v>10.9</v>
+        <v>13.1</v>
       </c>
       <c r="AD23">
         <f>'Ice Dragon'!AA13</f>
-        <v>11.6</v>
+        <v>13.7</v>
       </c>
       <c r="AE23">
         <f>'Ice Dragon'!AA14</f>
-        <v>12.6</v>
+        <v>14.7</v>
       </c>
       <c r="AF23">
         <f>'Ice Dragon'!AA15</f>
-        <v>13.3</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="25" spans="5:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rats have the freeze effect and last ice dragon drain changes
Former-commit-id: 4bead28a1a68ae5a27a635c70b8f5fc1f97333c4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58273,8 +58273,8 @@
   </sheetPr>
   <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60913,7 +60913,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="248">
-        <v>6.1999999999999998E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="N25" s="248">
         <v>20</v>
@@ -61068,7 +61068,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="248">
-        <v>8.0000000000000002E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="N26" s="248">
         <v>20</v>
@@ -61223,7 +61223,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="248">
-        <v>1.2E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N27" s="248">
         <v>15</v>
@@ -61380,7 +61380,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="250">
-        <v>1.52E-2</v>
+        <v>1.55E-2</v>
       </c>
       <c r="N28" s="250">
         <v>10</v>

</xml_diff>

<commit_message>
Ice dragon a bit stronger
Former-commit-id: 40c30c7a1df2172f66e44c0ec558a784aa4c3b9d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -2781,48 +2781,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2897,6 +2855,48 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13663,7 +13663,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14306,7 +14305,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14628,7 +14626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14950,7 +14947,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15259,7 +15255,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15876,7 +15871,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17120,7 +17114,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17233,7 +17226,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18478,7 +18470,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18585,7 +18576,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19831,7 +19821,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19938,7 +19927,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20260,7 +20248,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20903,7 +20890,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21225,7 +21211,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21534,7 +21519,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21843,7 +21827,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22152,7 +22135,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23393,7 +23375,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23506,7 +23487,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24748,7 +24728,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24855,7 +24834,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26098,7 +26076,6 @@
         <c:idx val="16"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -58273,8 +58250,8 @@
   </sheetPr>
   <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60897,67 +60874,67 @@
       <c r="G25" s="209">
         <v>0</v>
       </c>
-      <c r="H25" s="243">
+      <c r="H25" s="229">
         <v>3</v>
       </c>
-      <c r="I25" s="244">
+      <c r="I25" s="230">
         <v>-2</v>
       </c>
-      <c r="J25" s="247">
+      <c r="J25" s="233">
         <v>75</v>
       </c>
-      <c r="K25" s="248">
+      <c r="K25" s="234">
         <v>2.6</v>
       </c>
-      <c r="L25" s="248">
+      <c r="L25" s="234">
         <v>0</v>
       </c>
-      <c r="M25" s="248">
+      <c r="M25" s="234">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="N25" s="248">
+      <c r="N25" s="234">
         <v>20</v>
       </c>
-      <c r="O25" s="248">
+      <c r="O25" s="234">
         <v>0.5</v>
       </c>
-      <c r="P25" s="251">
+      <c r="P25" s="237">
         <v>1</v>
       </c>
-      <c r="Q25" s="244">
+      <c r="Q25" s="230">
         <v>1.45</v>
       </c>
-      <c r="R25" s="248">
+      <c r="R25" s="234">
         <v>100</v>
       </c>
-      <c r="S25" s="248">
+      <c r="S25" s="234">
         <v>9</v>
       </c>
-      <c r="T25" s="252">
+      <c r="T25" s="238">
         <v>7</v>
       </c>
-      <c r="U25" s="244">
+      <c r="U25" s="230">
         <v>11</v>
       </c>
-      <c r="V25" s="248">
+      <c r="V25" s="234">
         <v>3</v>
       </c>
-      <c r="W25" s="248">
+      <c r="W25" s="234">
         <v>10</v>
       </c>
-      <c r="X25" s="252">
-        <v>25000</v>
-      </c>
-      <c r="Y25" s="255">
+      <c r="X25" s="238">
+        <v>22000</v>
+      </c>
+      <c r="Y25" s="241">
         <v>2</v>
       </c>
-      <c r="Z25" s="251">
+      <c r="Z25" s="237">
         <v>0.13</v>
       </c>
-      <c r="AA25" s="251">
+      <c r="AA25" s="237">
         <v>0</v>
       </c>
-      <c r="AB25" s="255">
+      <c r="AB25" s="241">
         <v>12</v>
       </c>
       <c r="AC25" s="210" t="s">
@@ -60971,7 +60948,7 @@
       </c>
       <c r="AF25" s="219"/>
       <c r="AG25" s="220"/>
-      <c r="AH25" s="257">
+      <c r="AH25" s="243">
         <v>1.7</v>
       </c>
       <c r="AI25" s="210">
@@ -60989,7 +60966,7 @@
       <c r="AM25" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN25" s="258">
+      <c r="AN25" s="244">
         <v>10</v>
       </c>
       <c r="AO25" s="122">
@@ -61001,7 +60978,7 @@
       <c r="AQ25" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR25" s="261">
+      <c r="AR25" s="247">
         <v>310</v>
       </c>
       <c r="AS25" s="188">
@@ -61016,7 +60993,7 @@
       <c r="AV25" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW25" s="262">
+      <c r="AW25" s="248">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX25" s="188">
@@ -61028,7 +61005,7 @@
       <c r="AZ25" s="188">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BA25" s="263" t="s">
+      <c r="BA25" s="249" t="s">
         <v>395</v>
       </c>
     </row>
@@ -61052,67 +61029,67 @@
       <c r="G26" s="209">
         <v>10</v>
       </c>
-      <c r="H26" s="243">
+      <c r="H26" s="229">
         <v>8</v>
       </c>
-      <c r="I26" s="244">
+      <c r="I26" s="230">
         <v>0</v>
       </c>
-      <c r="J26" s="247">
+      <c r="J26" s="233">
         <v>120</v>
       </c>
-      <c r="K26" s="248">
+      <c r="K26" s="234">
         <v>3.3</v>
       </c>
-      <c r="L26" s="248">
+      <c r="L26" s="234">
         <v>0</v>
       </c>
-      <c r="M26" s="248">
+      <c r="M26" s="234">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="N26" s="248">
+      <c r="N26" s="234">
         <v>20</v>
       </c>
-      <c r="O26" s="248">
+      <c r="O26" s="234">
         <v>0.6</v>
       </c>
-      <c r="P26" s="251">
+      <c r="P26" s="237">
         <v>1.4</v>
       </c>
-      <c r="Q26" s="244">
+      <c r="Q26" s="230">
         <v>1.45</v>
       </c>
-      <c r="R26" s="248">
+      <c r="R26" s="234">
         <v>120</v>
       </c>
-      <c r="S26" s="248">
+      <c r="S26" s="234">
         <v>10</v>
       </c>
-      <c r="T26" s="252">
+      <c r="T26" s="238">
         <v>7</v>
       </c>
-      <c r="U26" s="244">
+      <c r="U26" s="230">
         <v>13</v>
       </c>
-      <c r="V26" s="248">
+      <c r="V26" s="234">
         <v>4</v>
       </c>
-      <c r="W26" s="248">
+      <c r="W26" s="234">
         <v>11</v>
       </c>
-      <c r="X26" s="252">
-        <v>90000</v>
-      </c>
-      <c r="Y26" s="255">
+      <c r="X26" s="238">
+        <v>85000</v>
+      </c>
+      <c r="Y26" s="241">
         <v>3</v>
       </c>
-      <c r="Z26" s="251">
+      <c r="Z26" s="237">
         <v>0.08</v>
       </c>
-      <c r="AA26" s="251">
+      <c r="AA26" s="237">
         <v>0</v>
       </c>
-      <c r="AB26" s="255">
+      <c r="AB26" s="241">
         <v>12</v>
       </c>
       <c r="AC26" s="210" t="s">
@@ -61126,7 +61103,7 @@
       </c>
       <c r="AF26" s="219"/>
       <c r="AG26" s="220"/>
-      <c r="AH26" s="257">
+      <c r="AH26" s="243">
         <v>1.6</v>
       </c>
       <c r="AI26" s="210">
@@ -61144,7 +61121,7 @@
       <c r="AM26" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN26" s="258">
+      <c r="AN26" s="244">
         <v>10</v>
       </c>
       <c r="AO26" s="122">
@@ -61156,7 +61133,7 @@
       <c r="AQ26" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR26" s="261">
+      <c r="AR26" s="247">
         <v>325</v>
       </c>
       <c r="AS26" s="188">
@@ -61171,7 +61148,7 @@
       <c r="AV26" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW26" s="262">
+      <c r="AW26" s="248">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX26" s="188">
@@ -61183,7 +61160,7 @@
       <c r="AZ26" s="188">
         <v>1.3</v>
       </c>
-      <c r="BA26" s="264" t="s">
+      <c r="BA26" s="250" t="s">
         <v>396</v>
       </c>
     </row>
@@ -61207,67 +61184,67 @@
       <c r="G27" s="209">
         <v>20</v>
       </c>
-      <c r="H27" s="243">
+      <c r="H27" s="229">
         <v>17</v>
       </c>
-      <c r="I27" s="244">
+      <c r="I27" s="230">
         <v>0</v>
       </c>
-      <c r="J27" s="247">
+      <c r="J27" s="233">
         <v>160</v>
       </c>
-      <c r="K27" s="248">
+      <c r="K27" s="234">
         <v>4.0999999999999996</v>
       </c>
-      <c r="L27" s="248">
+      <c r="L27" s="234">
         <v>0</v>
       </c>
-      <c r="M27" s="248">
+      <c r="M27" s="234">
         <v>1.4E-2</v>
       </c>
-      <c r="N27" s="248">
+      <c r="N27" s="234">
         <v>15</v>
       </c>
-      <c r="O27" s="248">
+      <c r="O27" s="234">
         <v>0.7</v>
       </c>
-      <c r="P27" s="251">
+      <c r="P27" s="237">
         <v>1.8</v>
       </c>
-      <c r="Q27" s="244">
+      <c r="Q27" s="230">
         <v>1.45</v>
       </c>
-      <c r="R27" s="248">
+      <c r="R27" s="234">
         <v>140</v>
       </c>
-      <c r="S27" s="248">
+      <c r="S27" s="234">
         <v>12</v>
       </c>
-      <c r="T27" s="252">
+      <c r="T27" s="238">
         <v>7</v>
       </c>
-      <c r="U27" s="244">
+      <c r="U27" s="230">
         <v>14</v>
       </c>
-      <c r="V27" s="248">
+      <c r="V27" s="234">
         <v>5</v>
       </c>
-      <c r="W27" s="248">
+      <c r="W27" s="234">
         <v>11</v>
       </c>
-      <c r="X27" s="252">
-        <v>200000</v>
-      </c>
-      <c r="Y27" s="255">
+      <c r="X27" s="238">
+        <v>180000</v>
+      </c>
+      <c r="Y27" s="241">
         <v>4</v>
       </c>
-      <c r="Z27" s="251">
+      <c r="Z27" s="237">
         <v>0.05</v>
       </c>
-      <c r="AA27" s="251">
+      <c r="AA27" s="237">
         <v>0</v>
       </c>
-      <c r="AB27" s="255">
+      <c r="AB27" s="241">
         <v>12</v>
       </c>
       <c r="AC27" s="210" t="s">
@@ -61281,7 +61258,7 @@
       </c>
       <c r="AF27" s="219"/>
       <c r="AG27" s="220"/>
-      <c r="AH27" s="257">
+      <c r="AH27" s="243">
         <v>1.5</v>
       </c>
       <c r="AI27" s="210">
@@ -61299,7 +61276,7 @@
       <c r="AM27" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN27" s="258">
+      <c r="AN27" s="244">
         <v>10</v>
       </c>
       <c r="AO27" s="122">
@@ -61311,7 +61288,7 @@
       <c r="AQ27" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR27" s="261">
+      <c r="AR27" s="247">
         <v>350</v>
       </c>
       <c r="AS27" s="188">
@@ -61326,7 +61303,7 @@
       <c r="AV27" s="188">
         <v>1.2</v>
       </c>
-      <c r="AW27" s="262">
+      <c r="AW27" s="248">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX27" s="188">
@@ -61338,7 +61315,7 @@
       <c r="AZ27" s="188">
         <v>1.5</v>
       </c>
-      <c r="BA27" s="264" t="s">
+      <c r="BA27" s="250" t="s">
         <v>397</v>
       </c>
     </row>
@@ -61364,67 +61341,67 @@
       <c r="G28" s="222">
         <v>30</v>
       </c>
-      <c r="H28" s="245">
+      <c r="H28" s="231">
         <v>25</v>
       </c>
-      <c r="I28" s="246">
+      <c r="I28" s="232">
         <v>0</v>
       </c>
-      <c r="J28" s="249">
+      <c r="J28" s="235">
         <v>200</v>
       </c>
-      <c r="K28" s="250">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="L28" s="250">
+      <c r="K28" s="236">
+        <v>4.7</v>
+      </c>
+      <c r="L28" s="236">
         <v>0</v>
       </c>
-      <c r="M28" s="250">
-        <v>1.55E-2</v>
-      </c>
-      <c r="N28" s="250">
+      <c r="M28" s="236">
+        <v>1.52E-2</v>
+      </c>
+      <c r="N28" s="236">
         <v>10</v>
       </c>
-      <c r="O28" s="250">
+      <c r="O28" s="236">
         <v>0.8</v>
       </c>
-      <c r="P28" s="253">
+      <c r="P28" s="239">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q28" s="246">
+      <c r="Q28" s="232">
         <v>1.45</v>
       </c>
-      <c r="R28" s="250">
+      <c r="R28" s="236">
         <v>160</v>
       </c>
-      <c r="S28" s="250">
+      <c r="S28" s="236">
         <v>14</v>
       </c>
-      <c r="T28" s="254">
+      <c r="T28" s="240">
         <v>7</v>
       </c>
-      <c r="U28" s="246">
+      <c r="U28" s="232">
         <v>15</v>
       </c>
-      <c r="V28" s="250">
+      <c r="V28" s="236">
         <v>6</v>
       </c>
-      <c r="W28" s="250">
+      <c r="W28" s="236">
         <v>11</v>
       </c>
-      <c r="X28" s="254">
-        <v>400000</v>
-      </c>
-      <c r="Y28" s="256">
+      <c r="X28" s="240">
+        <v>380000</v>
+      </c>
+      <c r="Y28" s="242">
         <v>5</v>
       </c>
-      <c r="Z28" s="253">
+      <c r="Z28" s="239">
         <v>0.04</v>
       </c>
-      <c r="AA28" s="253">
+      <c r="AA28" s="239">
         <v>0</v>
       </c>
-      <c r="AB28" s="256">
+      <c r="AB28" s="242">
         <v>12</v>
       </c>
       <c r="AC28" s="217" t="s">
@@ -61438,7 +61415,7 @@
       </c>
       <c r="AF28" s="219"/>
       <c r="AG28" s="221"/>
-      <c r="AH28" s="259">
+      <c r="AH28" s="245">
         <v>1.4</v>
       </c>
       <c r="AI28" s="210">
@@ -61456,7 +61433,7 @@
       <c r="AM28" s="210" t="b">
         <v>1</v>
       </c>
-      <c r="AN28" s="260">
+      <c r="AN28" s="246">
         <v>10</v>
       </c>
       <c r="AO28" s="122">
@@ -61468,7 +61445,7 @@
       <c r="AQ28" s="133">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AR28" s="265">
+      <c r="AR28" s="251">
         <v>365</v>
       </c>
       <c r="AS28" s="191">
@@ -61483,7 +61460,7 @@
       <c r="AV28" s="191">
         <v>1.2</v>
       </c>
-      <c r="AW28" s="266">
+      <c r="AW28" s="252">
         <v>1.1000000000000001</v>
       </c>
       <c r="AX28" s="191">
@@ -61495,7 +61472,7 @@
       <c r="AZ28" s="191">
         <v>1.7</v>
       </c>
-      <c r="BA28" s="267" t="s">
+      <c r="BA28" s="253" t="s">
         <v>398</v>
       </c>
     </row>
@@ -61506,44 +61483,44 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="236" t="s">
+      <c r="H29" s="261" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="237"/>
-      <c r="J29" s="238" t="s">
+      <c r="I29" s="262"/>
+      <c r="J29" s="263" t="s">
         <v>10</v>
       </c>
-      <c r="K29" s="239"/>
-      <c r="L29" s="239"/>
-      <c r="M29" s="239"/>
-      <c r="N29" s="239"/>
-      <c r="O29" s="240"/>
+      <c r="K29" s="264"/>
+      <c r="L29" s="264"/>
+      <c r="M29" s="264"/>
+      <c r="N29" s="264"/>
+      <c r="O29" s="265"/>
       <c r="P29" s="72"/>
-      <c r="Q29" s="232" t="s">
+      <c r="Q29" s="257" t="s">
         <v>126</v>
       </c>
-      <c r="R29" s="233"/>
-      <c r="S29" s="233"/>
-      <c r="T29" s="233"/>
-      <c r="U29" s="234" t="s">
+      <c r="R29" s="258"/>
+      <c r="S29" s="258"/>
+      <c r="T29" s="258"/>
+      <c r="U29" s="259" t="s">
         <v>9</v>
       </c>
-      <c r="V29" s="235"/>
-      <c r="W29" s="235"/>
-      <c r="X29" s="235"/>
+      <c r="V29" s="260"/>
+      <c r="W29" s="260"/>
+      <c r="X29" s="260"/>
       <c r="Y29" s="20"/>
       <c r="Z29" s="20"/>
       <c r="AA29" s="20"/>
       <c r="AB29" s="20"/>
-      <c r="AH29" s="229" t="s">
+      <c r="AH29" s="254" t="s">
         <v>127</v>
       </c>
-      <c r="AI29" s="230"/>
-      <c r="AJ29" s="230"/>
-      <c r="AK29" s="230"/>
-      <c r="AL29" s="230"/>
-      <c r="AM29" s="230"/>
-      <c r="AN29" s="231"/>
+      <c r="AI29" s="255"/>
+      <c r="AJ29" s="255"/>
+      <c r="AK29" s="255"/>
+      <c r="AL29" s="255"/>
+      <c r="AM29" s="255"/>
+      <c r="AN29" s="256"/>
     </row>
     <row r="31" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AZ31" t="s">
@@ -62505,8 +62482,8 @@
       <c r="D2" s="137"/>
       <c r="E2" s="137"/>
       <c r="F2" s="138"/>
-      <c r="G2" s="241"/>
-      <c r="H2" s="241"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
       <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:13" ht="172.5" x14ac:dyDescent="0.25">
@@ -64457,12 +64434,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="242" t="s">
+      <c r="E3" s="267" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
+      <c r="F3" s="267"/>
+      <c r="G3" s="267"/>
+      <c r="H3" s="267"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -65471,12 +65448,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="242" t="s">
+      <c r="E3" s="267" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
+      <c r="F3" s="267"/>
+      <c r="G3" s="267"/>
+      <c r="H3" s="267"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -66492,12 +66469,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="242" t="s">
+      <c r="E3" s="267" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
+      <c r="F3" s="267"/>
+      <c r="G3" s="267"/>
+      <c r="H3" s="267"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>
@@ -67506,12 +67483,12 @@
     </row>
     <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D3" s="63"/>
-      <c r="E3" s="242" t="s">
+      <c r="E3" s="267" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
+      <c r="F3" s="267"/>
+      <c r="G3" s="267"/>
+      <c r="H3" s="267"/>
       <c r="J3" s="63" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Content - Change price for Mecha dragon to 150
Former-commit-id: 640a2e5567fc55c6898c255c52f492b12bae611e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58250,8 +58250,8 @@
   </sheetPr>
   <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S7" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58466,7 +58466,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="43">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="H4" s="50">
         <v>20</v>

</xml_diff>

<commit_message>
WIP setting dragon sizes
Former-commit-id: 8599980d6c142a14514e91f34ccc689e92957e4c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
+++ b/Docs/Content/HungryDragonContent_SpecialDragons.xlsx
@@ -58591,8 +58591,8 @@
   </sheetPr>
   <dimension ref="A1:BA77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P67" sqref="P67"/>
+    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61946,7 +61946,7 @@
         <v>0.5</v>
       </c>
       <c r="P30" s="273">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="Q30" s="270">
         <v>1.5</v>
@@ -61955,10 +61955,10 @@
         <v>100</v>
       </c>
       <c r="S30" s="272">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="T30" s="274">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U30" s="270">
         <v>9</v>
@@ -61976,7 +61976,7 @@
         <v>2</v>
       </c>
       <c r="Z30" s="273">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="AA30" s="273">
         <v>0</v>
@@ -62077,7 +62077,7 @@
         <v>10</v>
       </c>
       <c r="H31" s="269">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I31" s="270">
         <v>0</v>
@@ -62101,7 +62101,7 @@
         <v>0.6</v>
       </c>
       <c r="P31" s="273">
-        <v>1.25</v>
+        <v>1.65</v>
       </c>
       <c r="Q31" s="270">
         <v>1.5</v>
@@ -62110,10 +62110,10 @@
         <v>120</v>
       </c>
       <c r="S31" s="272">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="T31" s="274">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U31" s="270">
         <v>11</v>
@@ -62131,7 +62131,7 @@
         <v>3</v>
       </c>
       <c r="Z31" s="273">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="AA31" s="273">
         <v>0</v>
@@ -62232,7 +62232,7 @@
         <v>20</v>
       </c>
       <c r="H32" s="269">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I32" s="270">
         <v>0</v>
@@ -62256,7 +62256,7 @@
         <v>0.7</v>
       </c>
       <c r="P32" s="273">
-        <v>1.65</v>
+        <v>2.15</v>
       </c>
       <c r="Q32" s="270">
         <v>1.5</v>
@@ -62265,10 +62265,10 @@
         <v>140</v>
       </c>
       <c r="S32" s="272">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="T32" s="274">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U32" s="270">
         <v>11.5</v>
@@ -62286,7 +62286,7 @@
         <v>4</v>
       </c>
       <c r="Z32" s="273">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="AA32" s="273">
         <v>0</v>
@@ -62387,7 +62387,7 @@
         <v>30</v>
       </c>
       <c r="H33" s="269">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I33" s="270">
         <v>0</v>
@@ -62411,7 +62411,7 @@
         <v>0.8</v>
       </c>
       <c r="P33" s="273">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="Q33" s="270">
         <v>1.5</v>
@@ -62420,10 +62420,10 @@
         <v>160</v>
       </c>
       <c r="S33" s="272">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="T33" s="274">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U33" s="270">
         <v>12</v>
@@ -62441,7 +62441,7 @@
         <v>5</v>
       </c>
       <c r="Z33" s="273">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="AA33" s="273">
         <v>0</v>

</xml_diff>